<commit_message>
Configure the web server to have pretty URLs
</commit_message>
<xml_diff>
--- a/me/2.routing.xlsx
+++ b/me/2.routing.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\build-php-mvc-framework\me\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4A3F491-85DA-4DE8-A84E-4706CE253168}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{175E3279-08BC-4718-821E-6A549FD18A15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="central entry point" sheetId="1" r:id="rId1"/>
+    <sheet name="Configure URLs" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="47">
   <si>
     <t>Create a central entry point to the framework: the front controller</t>
   </si>
@@ -134,6 +135,138 @@
       </rPr>
       <t>;</t>
     </r>
+  </si>
+  <si>
+    <t>Configure the web server to have pretty URLs</t>
+  </si>
+  <si>
+    <t>.htaccess</t>
+  </si>
+  <si>
+    <t>new</t>
+  </si>
+  <si>
+    <t>build-php-mvc-framework\public\.htaccess</t>
+  </si>
+  <si>
+    <t># Remove the question mark from the request but maintain the query string</t>
+  </si>
+  <si>
+    <t>RewriteEngine On</t>
+  </si>
+  <si>
+    <t>RewriteBase /</t>
+  </si>
+  <si>
+    <t>RewriteCond %{REQUEST_FILENAME} !-f</t>
+  </si>
+  <si>
+    <t>RewriteCond %{REQUEST_FILENAME} !-d</t>
+  </si>
+  <si>
+    <t>If the requested filename is not a directory,</t>
+  </si>
+  <si>
+    <t>and if the requested filename is not a regular file that exists,</t>
+  </si>
+  <si>
+    <t>Thì sẽ rewrite URL bằng cách:</t>
+  </si>
+  <si>
+    <t>Take the whole request filename and provide it as the value of a "url" query parameter to index.php.</t>
+  </si>
+  <si>
+    <t>Append any query string from the original URL as further query parameters (QSA), and stop</t>
+  </si>
+  <si>
+    <t>processing this .htaccess file (L).</t>
+  </si>
+  <si>
+    <t>Default của webserver là load index.php và để bảo mật url hơn thì mình ko cần viết index.php vào trong url  thì nó vẫn load trang index.php như bình thường</t>
+  </si>
+  <si>
+    <t>Mình cũng có thể bỏ dấu ? Ở vị trí đầu tiên của querystring</t>
+  </si>
+  <si>
+    <r>
+      <t>RewriteRule ^(.*)$ index.php?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>$1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> [L,QSA]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>http://localhost/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>product/list?page=1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>http://localhost/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>index.php</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>?product/list?page=1</t>
+    </r>
+  </si>
+  <si>
+    <t>Remove index.php, mình vẫn nhận được kết quả "product/list?page=1" như vậy</t>
+  </si>
+  <si>
+    <t>Remove dấu ? Ở vị trí đầu tiên, mình vẫn nhận được kết quả "product/list?page=1" như vậy</t>
   </si>
 </sst>
 </file>
@@ -262,7 +395,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -275,6 +408,19 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -560,6 +706,920 @@
         <a:xfrm flipH="1">
           <a:off x="2019300" y="19583400"/>
           <a:ext cx="714375" cy="552450"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="Straight Arrow Connector 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3EC77B06-D880-040B-8C73-3EB13D406287}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="685800" y="4905375"/>
+          <a:ext cx="9525" cy="1123950"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="Straight Arrow Connector 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A4AEFD13-5869-7DAE-80B0-2B71AF2EF6EB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="809625" y="5105400"/>
+          <a:ext cx="9525" cy="504825"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="7" name="Straight Arrow Connector 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0EB7FDD4-7B2A-C50A-AC2F-6D502B73B30E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="1362075" y="10429875"/>
+          <a:ext cx="676275" cy="1085850"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>494106</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>152131</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{39F69445-DE3D-8A63-3A0F-E014C516C428}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="695325" y="1047750"/>
+          <a:ext cx="9552381" cy="2152381"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>160786</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>56890</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D1F8D2CA-80FD-67D7-0D95-7DEE6FFECA3E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="800100" y="3886200"/>
+          <a:ext cx="9114286" cy="2076190"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>113687</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>47481</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3FFAF926-B017-A163-C622-0BBD7547D075}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="695325" y="12992100"/>
+          <a:ext cx="4904762" cy="1152381"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="13" name="Straight Arrow Connector 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{57EDABBB-B232-7813-538E-0169A8944063}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="1371600" y="12896850"/>
+          <a:ext cx="390525" cy="1819275"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>151784</xdr:colOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>104611</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A939BF46-5111-0DDD-7DED-548DBFC186DB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="714375" y="15173325"/>
+          <a:ext cx="4923809" cy="1314286"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="16" name="Straight Arrow Connector 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{87CDD0C3-7FC6-83C1-FD57-14779E34E2B6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="2038350" y="13839825"/>
+          <a:ext cx="1581150" cy="904875"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="18" name="Straight Arrow Connector 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D2335396-F5AB-2013-0A18-35A416F78BD5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="2066925" y="14849475"/>
+          <a:ext cx="1552575" cy="1085850"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>78</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>89</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="20" name="Straight Arrow Connector 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4CE227DE-B980-2A28-B0FE-3B96C273D949}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="1428750" y="15039975"/>
+          <a:ext cx="228600" cy="1962150"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>90</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>113688</xdr:colOff>
+      <xdr:row>96</xdr:row>
+      <xdr:rowOff>85581</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="21" name="Picture 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{44CCE648-8167-3307-D418-FBE3F6096C5F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="704850" y="17221200"/>
+          <a:ext cx="4895238" cy="1152381"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>89</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="23" name="Straight Arrow Connector 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2B8D68DA-05AE-A86B-2416-05C8E464215C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="2190750" y="16049625"/>
+          <a:ext cx="2057400" cy="971550"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>89</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>94</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="25" name="Straight Arrow Connector 24">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{26D743FE-EDF8-4738-EE70-0B4A749504E3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="2095500" y="17125950"/>
+          <a:ext cx="2171700" cy="876300"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="27" name="Straight Arrow Connector 26">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6A41E1AB-1CE4-3019-A5F2-C9BCCDED4604}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2114550" y="3771900"/>
+          <a:ext cx="238125" cy="276225"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="29" name="Straight Arrow Connector 28">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D570E1F9-15E4-8DD5-76EE-B1FA36DF0D60}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2095500" y="3781425"/>
+          <a:ext cx="5305425" cy="381000"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="31" name="Straight Arrow Connector 30">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E7FC95FC-536C-734E-F332-F67A69A857F6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="2466975" y="904875"/>
+          <a:ext cx="9525" cy="428625"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="33" name="Straight Arrow Connector 32">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BDBAD1EC-FE0B-E501-3B79-C82DC9B799AA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2486025" y="914400"/>
+          <a:ext cx="5153025" cy="400050"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -853,8 +1913,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:T101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="O97" sqref="O97"/>
+    <sheetView topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="A81" sqref="A81:F91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1351,4 +2411,1039 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0EE5C4F-42B3-4F42-80A8-CAE45B1514F0}">
+  <dimension ref="A2:Q97"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="O100" sqref="O100"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="3"/>
+    </row>
+    <row r="6" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B6" s="4"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="22"/>
+      <c r="I6" s="22"/>
+      <c r="J6" s="22"/>
+      <c r="K6" s="22"/>
+      <c r="L6" s="22"/>
+      <c r="M6" s="22"/>
+      <c r="N6" s="22"/>
+      <c r="O6" s="22"/>
+      <c r="P6" s="22"/>
+      <c r="Q6" s="5"/>
+    </row>
+    <row r="7" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B7" s="4"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="22"/>
+      <c r="I7" s="22"/>
+      <c r="J7" s="22"/>
+      <c r="K7" s="22"/>
+      <c r="L7" s="22"/>
+      <c r="M7" s="22"/>
+      <c r="N7" s="22"/>
+      <c r="O7" s="22"/>
+      <c r="P7" s="22"/>
+      <c r="Q7" s="5"/>
+    </row>
+    <row r="8" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B8" s="4"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="22"/>
+      <c r="I8" s="22"/>
+      <c r="J8" s="22"/>
+      <c r="K8" s="22"/>
+      <c r="L8" s="22"/>
+      <c r="M8" s="22"/>
+      <c r="N8" s="22"/>
+      <c r="O8" s="22"/>
+      <c r="P8" s="22"/>
+      <c r="Q8" s="5"/>
+    </row>
+    <row r="9" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B9" s="4"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="22"/>
+      <c r="I9" s="22"/>
+      <c r="J9" s="22"/>
+      <c r="K9" s="22"/>
+      <c r="L9" s="22"/>
+      <c r="M9" s="22"/>
+      <c r="N9" s="22"/>
+      <c r="O9" s="22"/>
+      <c r="P9" s="22"/>
+      <c r="Q9" s="5"/>
+    </row>
+    <row r="10" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B10" s="4"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22"/>
+      <c r="I10" s="22"/>
+      <c r="J10" s="22"/>
+      <c r="K10" s="22"/>
+      <c r="L10" s="22"/>
+      <c r="M10" s="22"/>
+      <c r="N10" s="22"/>
+      <c r="O10" s="22"/>
+      <c r="P10" s="22"/>
+      <c r="Q10" s="5"/>
+    </row>
+    <row r="11" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B11" s="4"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="22"/>
+      <c r="I11" s="22"/>
+      <c r="J11" s="22"/>
+      <c r="K11" s="22"/>
+      <c r="L11" s="22"/>
+      <c r="M11" s="22"/>
+      <c r="N11" s="22"/>
+      <c r="O11" s="22"/>
+      <c r="P11" s="22"/>
+      <c r="Q11" s="5"/>
+    </row>
+    <row r="12" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B12" s="4"/>
+      <c r="C12" s="22"/>
+      <c r="D12" s="22"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="22"/>
+      <c r="H12" s="22"/>
+      <c r="I12" s="22"/>
+      <c r="J12" s="22"/>
+      <c r="K12" s="22"/>
+      <c r="L12" s="22"/>
+      <c r="M12" s="22"/>
+      <c r="N12" s="22"/>
+      <c r="O12" s="22"/>
+      <c r="P12" s="22"/>
+      <c r="Q12" s="5"/>
+    </row>
+    <row r="13" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B13" s="4"/>
+      <c r="C13" s="22"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="22"/>
+      <c r="G13" s="22"/>
+      <c r="H13" s="22"/>
+      <c r="I13" s="22"/>
+      <c r="J13" s="22"/>
+      <c r="K13" s="22"/>
+      <c r="L13" s="22"/>
+      <c r="M13" s="22"/>
+      <c r="N13" s="22"/>
+      <c r="O13" s="22"/>
+      <c r="P13" s="22"/>
+      <c r="Q13" s="5"/>
+    </row>
+    <row r="14" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B14" s="4"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="22"/>
+      <c r="F14" s="22"/>
+      <c r="G14" s="22"/>
+      <c r="H14" s="22"/>
+      <c r="I14" s="22"/>
+      <c r="J14" s="22"/>
+      <c r="K14" s="22"/>
+      <c r="L14" s="22"/>
+      <c r="M14" s="22"/>
+      <c r="N14" s="22"/>
+      <c r="O14" s="22"/>
+      <c r="P14" s="22"/>
+      <c r="Q14" s="5"/>
+    </row>
+    <row r="15" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B15" s="4"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="22"/>
+      <c r="F15" s="22"/>
+      <c r="G15" s="22"/>
+      <c r="H15" s="22"/>
+      <c r="I15" s="22"/>
+      <c r="J15" s="22"/>
+      <c r="K15" s="22"/>
+      <c r="L15" s="22"/>
+      <c r="M15" s="22"/>
+      <c r="N15" s="22"/>
+      <c r="O15" s="22"/>
+      <c r="P15" s="22"/>
+      <c r="Q15" s="5"/>
+    </row>
+    <row r="16" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B16" s="4"/>
+      <c r="C16" s="22"/>
+      <c r="D16" s="22"/>
+      <c r="E16" s="22"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="22"/>
+      <c r="H16" s="22"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="22"/>
+      <c r="K16" s="22"/>
+      <c r="L16" s="22"/>
+      <c r="M16" s="22"/>
+      <c r="N16" s="22"/>
+      <c r="O16" s="22"/>
+      <c r="P16" s="22"/>
+      <c r="Q16" s="5"/>
+    </row>
+    <row r="17" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B17" s="6"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="7"/>
+      <c r="J17" s="7"/>
+      <c r="K17" s="7"/>
+      <c r="L17" s="7"/>
+      <c r="M17" s="7"/>
+      <c r="N17" s="7"/>
+      <c r="O17" s="7"/>
+      <c r="P17" s="7"/>
+      <c r="Q17" s="8"/>
+    </row>
+    <row r="20" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B20" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
+      <c r="L20" s="2"/>
+      <c r="M20" s="2"/>
+      <c r="N20" s="2"/>
+      <c r="O20" s="2"/>
+      <c r="P20" s="2"/>
+      <c r="Q20" s="3"/>
+    </row>
+    <row r="21" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B21" s="4"/>
+      <c r="C21" s="22"/>
+      <c r="D21" s="22"/>
+      <c r="E21" s="22"/>
+      <c r="F21" s="22"/>
+      <c r="G21" s="22"/>
+      <c r="H21" s="22"/>
+      <c r="I21" s="22"/>
+      <c r="J21" s="22"/>
+      <c r="K21" s="22"/>
+      <c r="L21" s="22"/>
+      <c r="M21" s="22"/>
+      <c r="N21" s="22"/>
+      <c r="O21" s="22"/>
+      <c r="P21" s="22"/>
+      <c r="Q21" s="5"/>
+    </row>
+    <row r="22" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B22" s="4"/>
+      <c r="C22" s="22"/>
+      <c r="D22" s="22"/>
+      <c r="E22" s="22"/>
+      <c r="F22" s="22"/>
+      <c r="G22" s="22"/>
+      <c r="H22" s="22"/>
+      <c r="I22" s="22"/>
+      <c r="J22" s="22"/>
+      <c r="K22" s="22"/>
+      <c r="L22" s="22"/>
+      <c r="M22" s="22"/>
+      <c r="N22" s="22"/>
+      <c r="O22" s="22"/>
+      <c r="P22" s="22"/>
+      <c r="Q22" s="5"/>
+    </row>
+    <row r="23" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B23" s="4"/>
+      <c r="C23" s="22"/>
+      <c r="D23" s="22"/>
+      <c r="E23" s="22"/>
+      <c r="F23" s="22"/>
+      <c r="G23" s="22"/>
+      <c r="H23" s="22"/>
+      <c r="I23" s="22"/>
+      <c r="J23" s="22"/>
+      <c r="K23" s="22"/>
+      <c r="L23" s="22"/>
+      <c r="M23" s="22"/>
+      <c r="N23" s="22"/>
+      <c r="O23" s="22"/>
+      <c r="P23" s="22"/>
+      <c r="Q23" s="5"/>
+    </row>
+    <row r="24" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B24" s="4"/>
+      <c r="C24" s="22"/>
+      <c r="D24" s="22"/>
+      <c r="E24" s="22"/>
+      <c r="F24" s="22"/>
+      <c r="G24" s="22"/>
+      <c r="H24" s="22"/>
+      <c r="I24" s="22"/>
+      <c r="J24" s="22"/>
+      <c r="K24" s="22"/>
+      <c r="L24" s="22"/>
+      <c r="M24" s="22"/>
+      <c r="N24" s="22"/>
+      <c r="O24" s="22"/>
+      <c r="P24" s="22"/>
+      <c r="Q24" s="5"/>
+    </row>
+    <row r="25" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B25" s="4"/>
+      <c r="C25" s="22"/>
+      <c r="D25" s="22"/>
+      <c r="E25" s="22"/>
+      <c r="F25" s="22"/>
+      <c r="G25" s="22"/>
+      <c r="H25" s="22"/>
+      <c r="I25" s="22"/>
+      <c r="J25" s="22"/>
+      <c r="K25" s="22"/>
+      <c r="L25" s="22"/>
+      <c r="M25" s="22"/>
+      <c r="N25" s="22"/>
+      <c r="O25" s="22"/>
+      <c r="P25" s="22"/>
+      <c r="Q25" s="5"/>
+    </row>
+    <row r="26" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B26" s="4"/>
+      <c r="C26" s="22"/>
+      <c r="D26" s="22"/>
+      <c r="E26" s="22"/>
+      <c r="F26" s="22"/>
+      <c r="G26" s="22"/>
+      <c r="H26" s="22"/>
+      <c r="I26" s="22"/>
+      <c r="J26" s="22"/>
+      <c r="K26" s="22"/>
+      <c r="L26" s="22"/>
+      <c r="M26" s="22"/>
+      <c r="N26" s="22"/>
+      <c r="O26" s="22"/>
+      <c r="P26" s="22"/>
+      <c r="Q26" s="5"/>
+    </row>
+    <row r="27" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B27" s="4"/>
+      <c r="C27" s="22"/>
+      <c r="D27" s="22"/>
+      <c r="E27" s="22"/>
+      <c r="F27" s="22"/>
+      <c r="G27" s="22"/>
+      <c r="H27" s="22"/>
+      <c r="I27" s="22"/>
+      <c r="J27" s="22"/>
+      <c r="K27" s="22"/>
+      <c r="L27" s="22"/>
+      <c r="M27" s="22"/>
+      <c r="N27" s="22"/>
+      <c r="O27" s="22"/>
+      <c r="P27" s="22"/>
+      <c r="Q27" s="5"/>
+    </row>
+    <row r="28" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B28" s="4"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="22"/>
+      <c r="E28" s="22"/>
+      <c r="F28" s="22"/>
+      <c r="G28" s="22"/>
+      <c r="H28" s="22"/>
+      <c r="I28" s="22"/>
+      <c r="J28" s="22"/>
+      <c r="K28" s="22"/>
+      <c r="L28" s="22"/>
+      <c r="M28" s="22"/>
+      <c r="N28" s="22"/>
+      <c r="O28" s="22"/>
+      <c r="P28" s="22"/>
+      <c r="Q28" s="5"/>
+    </row>
+    <row r="29" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B29" s="4"/>
+      <c r="C29" s="22"/>
+      <c r="D29" s="22"/>
+      <c r="E29" s="22"/>
+      <c r="F29" s="22"/>
+      <c r="G29" s="22"/>
+      <c r="H29" s="22"/>
+      <c r="I29" s="22"/>
+      <c r="J29" s="22"/>
+      <c r="K29" s="22"/>
+      <c r="L29" s="22"/>
+      <c r="M29" s="22"/>
+      <c r="N29" s="22"/>
+      <c r="O29" s="22"/>
+      <c r="P29" s="22"/>
+      <c r="Q29" s="5"/>
+    </row>
+    <row r="30" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B30" s="4"/>
+      <c r="C30" s="22"/>
+      <c r="D30" s="22"/>
+      <c r="E30" s="22"/>
+      <c r="F30" s="22"/>
+      <c r="G30" s="22"/>
+      <c r="H30" s="22"/>
+      <c r="I30" s="22"/>
+      <c r="J30" s="22"/>
+      <c r="K30" s="22"/>
+      <c r="L30" s="22"/>
+      <c r="M30" s="22"/>
+      <c r="N30" s="22"/>
+      <c r="O30" s="22"/>
+      <c r="P30" s="22"/>
+      <c r="Q30" s="5"/>
+    </row>
+    <row r="31" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B31" s="4"/>
+      <c r="C31" s="22"/>
+      <c r="D31" s="22"/>
+      <c r="E31" s="22"/>
+      <c r="F31" s="22"/>
+      <c r="G31" s="22"/>
+      <c r="H31" s="22"/>
+      <c r="I31" s="22"/>
+      <c r="J31" s="22"/>
+      <c r="K31" s="22"/>
+      <c r="L31" s="22"/>
+      <c r="M31" s="22"/>
+      <c r="N31" s="22"/>
+      <c r="O31" s="22"/>
+      <c r="P31" s="22"/>
+      <c r="Q31" s="5"/>
+    </row>
+    <row r="32" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B32" s="6"/>
+      <c r="C32" s="7"/>
+      <c r="D32" s="7"/>
+      <c r="E32" s="7"/>
+      <c r="F32" s="7"/>
+      <c r="G32" s="7"/>
+      <c r="H32" s="7"/>
+      <c r="I32" s="7"/>
+      <c r="J32" s="7"/>
+      <c r="K32" s="7"/>
+      <c r="L32" s="7"/>
+      <c r="M32" s="7"/>
+      <c r="N32" s="7"/>
+      <c r="O32" s="7"/>
+      <c r="P32" s="7"/>
+      <c r="Q32" s="8"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B35" s="13"/>
+      <c r="C35" s="13"/>
+      <c r="D35" s="13"/>
+      <c r="E35" s="13"/>
+      <c r="F35" s="13"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="13"/>
+      <c r="B36" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C36" s="15"/>
+      <c r="D36" s="15"/>
+      <c r="E36" s="15"/>
+      <c r="F36" s="16"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="13"/>
+      <c r="B37" s="17"/>
+      <c r="C37" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D37" s="13"/>
+      <c r="E37" s="13"/>
+      <c r="F37" s="18"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="13"/>
+      <c r="B38" s="17"/>
+      <c r="C38" s="13"/>
+      <c r="D38" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E38" s="13"/>
+      <c r="F38" s="18"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="13"/>
+      <c r="B39" s="17"/>
+      <c r="C39" s="13"/>
+      <c r="D39" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E39" s="13"/>
+      <c r="F39" s="18"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="13"/>
+      <c r="B40" s="17"/>
+      <c r="C40" s="13"/>
+      <c r="D40" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="E40" s="13"/>
+      <c r="F40" s="18"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="13"/>
+      <c r="B41" s="17"/>
+      <c r="C41" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D41" s="13"/>
+      <c r="E41" s="13"/>
+      <c r="F41" s="18"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="13"/>
+      <c r="B42" s="17"/>
+      <c r="C42" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D42" s="13"/>
+      <c r="E42" s="13"/>
+      <c r="F42" s="18"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="13"/>
+      <c r="B43" s="17"/>
+      <c r="C43" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D43" s="13"/>
+      <c r="E43" s="13"/>
+      <c r="F43" s="18"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" s="13"/>
+      <c r="B44" s="17"/>
+      <c r="C44" s="13"/>
+      <c r="D44" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="E44" s="13"/>
+      <c r="F44" s="18"/>
+      <c r="G44" t="s">
+        <v>20</v>
+      </c>
+      <c r="H44" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="13"/>
+      <c r="B45" s="17"/>
+      <c r="C45" s="13"/>
+      <c r="D45" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E45" s="13"/>
+      <c r="F45" s="18"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" s="13"/>
+      <c r="B46" s="19"/>
+      <c r="C46" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="D46" s="20"/>
+      <c r="E46" s="20"/>
+      <c r="F46" s="21"/>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B50" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C50" s="2"/>
+      <c r="D50" s="2"/>
+      <c r="E50" s="2"/>
+      <c r="F50" s="2"/>
+      <c r="G50" s="2"/>
+      <c r="H50" s="2"/>
+      <c r="I50" s="3"/>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B51" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C51" s="22"/>
+      <c r="D51" s="22"/>
+      <c r="E51" s="22"/>
+      <c r="F51" s="22"/>
+      <c r="G51" s="22"/>
+      <c r="H51" s="22"/>
+      <c r="I51" s="5"/>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B52" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C52" s="22"/>
+      <c r="D52" s="22"/>
+      <c r="E52" s="22"/>
+      <c r="F52" s="22"/>
+      <c r="G52" s="22"/>
+      <c r="H52" s="22"/>
+      <c r="I52" s="5"/>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B53" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C53" s="22"/>
+      <c r="D53" s="22"/>
+      <c r="E53" s="22"/>
+      <c r="F53" s="22"/>
+      <c r="G53" s="22"/>
+      <c r="H53" s="22"/>
+      <c r="I53" s="5"/>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B54" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C54" s="22"/>
+      <c r="D54" s="22"/>
+      <c r="E54" s="22"/>
+      <c r="F54" s="22"/>
+      <c r="G54" s="22"/>
+      <c r="H54" s="22"/>
+      <c r="I54" s="5"/>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B55" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C55" s="7"/>
+      <c r="D55" s="7"/>
+      <c r="E55" s="7"/>
+      <c r="F55" s="7"/>
+      <c r="G55" s="7"/>
+      <c r="H55" s="7"/>
+      <c r="I55" s="8"/>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C58" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C60" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C62" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C63" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C64" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A67" s="9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B68" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="C68" s="2"/>
+      <c r="D68" s="2"/>
+      <c r="E68" s="2"/>
+      <c r="F68" s="2"/>
+      <c r="G68" s="2"/>
+      <c r="H68" s="2"/>
+      <c r="I68" s="2"/>
+      <c r="J68" s="3"/>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B69" s="4"/>
+      <c r="C69" s="22"/>
+      <c r="D69" s="22"/>
+      <c r="E69" s="22"/>
+      <c r="F69" s="22"/>
+      <c r="G69" s="22"/>
+      <c r="H69" s="22"/>
+      <c r="I69" s="22"/>
+      <c r="J69" s="5"/>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B70" s="4"/>
+      <c r="C70" s="22"/>
+      <c r="D70" s="22"/>
+      <c r="E70" s="22"/>
+      <c r="F70" s="22"/>
+      <c r="G70" s="22"/>
+      <c r="H70" s="22"/>
+      <c r="I70" s="22"/>
+      <c r="J70" s="5"/>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B71" s="4"/>
+      <c r="C71" s="22"/>
+      <c r="D71" s="22"/>
+      <c r="E71" s="22"/>
+      <c r="F71" s="22"/>
+      <c r="G71" s="22"/>
+      <c r="H71" s="22"/>
+      <c r="I71" s="22"/>
+      <c r="J71" s="5"/>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B72" s="4"/>
+      <c r="C72" s="22"/>
+      <c r="D72" s="22"/>
+      <c r="E72" s="22"/>
+      <c r="F72" s="22"/>
+      <c r="G72" s="22"/>
+      <c r="H72" s="22"/>
+      <c r="I72" s="22"/>
+      <c r="J72" s="5"/>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B73" s="4"/>
+      <c r="C73" s="22"/>
+      <c r="D73" s="22"/>
+      <c r="E73" s="22"/>
+      <c r="F73" s="22"/>
+      <c r="G73" s="22"/>
+      <c r="H73" s="22"/>
+      <c r="I73" s="22"/>
+      <c r="J73" s="5"/>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B74" s="4"/>
+      <c r="C74" s="22"/>
+      <c r="D74" s="22"/>
+      <c r="E74" s="22"/>
+      <c r="F74" s="22"/>
+      <c r="G74" s="22"/>
+      <c r="H74" s="22"/>
+      <c r="I74" s="22"/>
+      <c r="J74" s="5"/>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B75" s="6"/>
+      <c r="C75" s="7"/>
+      <c r="D75" s="7"/>
+      <c r="E75" s="7"/>
+      <c r="F75" s="7"/>
+      <c r="G75" s="7"/>
+      <c r="H75" s="7"/>
+      <c r="I75" s="7"/>
+      <c r="J75" s="8"/>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B78" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C78" s="2"/>
+      <c r="D78" s="2"/>
+      <c r="E78" s="2"/>
+      <c r="F78" s="2"/>
+      <c r="G78" s="2"/>
+      <c r="H78" s="2"/>
+      <c r="I78" s="2"/>
+      <c r="J78" s="3"/>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B79" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="C79" s="22"/>
+      <c r="D79" s="22"/>
+      <c r="E79" s="22"/>
+      <c r="F79" s="22"/>
+      <c r="G79" s="22"/>
+      <c r="H79" s="22"/>
+      <c r="I79" s="22"/>
+      <c r="J79" s="5"/>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B80" s="4"/>
+      <c r="C80" s="22"/>
+      <c r="D80" s="22"/>
+      <c r="E80" s="22"/>
+      <c r="F80" s="22"/>
+      <c r="G80" s="22"/>
+      <c r="H80" s="22"/>
+      <c r="I80" s="22"/>
+      <c r="J80" s="5"/>
+    </row>
+    <row r="81" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B81" s="4"/>
+      <c r="C81" s="22"/>
+      <c r="D81" s="22"/>
+      <c r="E81" s="22"/>
+      <c r="F81" s="22"/>
+      <c r="G81" s="22"/>
+      <c r="H81" s="22"/>
+      <c r="I81" s="22"/>
+      <c r="J81" s="5"/>
+    </row>
+    <row r="82" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B82" s="4"/>
+      <c r="C82" s="22"/>
+      <c r="D82" s="22"/>
+      <c r="E82" s="22"/>
+      <c r="F82" s="22"/>
+      <c r="G82" s="22"/>
+      <c r="H82" s="22"/>
+      <c r="I82" s="22"/>
+      <c r="J82" s="5"/>
+    </row>
+    <row r="83" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B83" s="4"/>
+      <c r="C83" s="22"/>
+      <c r="D83" s="22"/>
+      <c r="E83" s="22"/>
+      <c r="F83" s="22"/>
+      <c r="G83" s="22"/>
+      <c r="H83" s="22"/>
+      <c r="I83" s="22"/>
+      <c r="J83" s="5"/>
+    </row>
+    <row r="84" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B84" s="4"/>
+      <c r="C84" s="22"/>
+      <c r="D84" s="22"/>
+      <c r="E84" s="22"/>
+      <c r="F84" s="22"/>
+      <c r="G84" s="22"/>
+      <c r="H84" s="22"/>
+      <c r="I84" s="22"/>
+      <c r="J84" s="5"/>
+    </row>
+    <row r="85" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B85" s="4"/>
+      <c r="C85" s="22"/>
+      <c r="D85" s="22"/>
+      <c r="E85" s="22"/>
+      <c r="F85" s="22"/>
+      <c r="G85" s="22"/>
+      <c r="H85" s="22"/>
+      <c r="I85" s="22"/>
+      <c r="J85" s="5"/>
+    </row>
+    <row r="86" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B86" s="4"/>
+      <c r="C86" s="22"/>
+      <c r="D86" s="22"/>
+      <c r="E86" s="22"/>
+      <c r="F86" s="22"/>
+      <c r="G86" s="22"/>
+      <c r="H86" s="22"/>
+      <c r="I86" s="22"/>
+      <c r="J86" s="5"/>
+    </row>
+    <row r="87" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B87" s="6"/>
+      <c r="C87" s="7"/>
+      <c r="D87" s="7"/>
+      <c r="E87" s="7"/>
+      <c r="F87" s="7"/>
+      <c r="G87" s="7"/>
+      <c r="H87" s="7"/>
+      <c r="I87" s="7"/>
+      <c r="J87" s="8"/>
+    </row>
+    <row r="90" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B90" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C90" s="2"/>
+      <c r="D90" s="2"/>
+      <c r="E90" s="2"/>
+      <c r="F90" s="2"/>
+      <c r="G90" s="2"/>
+      <c r="H90" s="2"/>
+      <c r="I90" s="2"/>
+      <c r="J90" s="3"/>
+    </row>
+    <row r="91" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B91" s="4"/>
+      <c r="C91" s="22"/>
+      <c r="D91" s="22"/>
+      <c r="E91" s="22"/>
+      <c r="F91" s="22"/>
+      <c r="G91" s="22"/>
+      <c r="H91" s="22"/>
+      <c r="I91" s="22"/>
+      <c r="J91" s="5"/>
+    </row>
+    <row r="92" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B92" s="4"/>
+      <c r="C92" s="22"/>
+      <c r="D92" s="22"/>
+      <c r="E92" s="22"/>
+      <c r="F92" s="22"/>
+      <c r="G92" s="22"/>
+      <c r="H92" s="22"/>
+      <c r="I92" s="22"/>
+      <c r="J92" s="5"/>
+    </row>
+    <row r="93" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B93" s="4"/>
+      <c r="C93" s="22"/>
+      <c r="D93" s="22"/>
+      <c r="E93" s="22"/>
+      <c r="F93" s="22"/>
+      <c r="G93" s="22"/>
+      <c r="H93" s="22"/>
+      <c r="I93" s="22"/>
+      <c r="J93" s="5"/>
+    </row>
+    <row r="94" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B94" s="4"/>
+      <c r="C94" s="22"/>
+      <c r="D94" s="22"/>
+      <c r="E94" s="22"/>
+      <c r="F94" s="22"/>
+      <c r="G94" s="22"/>
+      <c r="H94" s="22"/>
+      <c r="I94" s="22"/>
+      <c r="J94" s="5"/>
+    </row>
+    <row r="95" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B95" s="4"/>
+      <c r="C95" s="22"/>
+      <c r="D95" s="22"/>
+      <c r="E95" s="22"/>
+      <c r="F95" s="22"/>
+      <c r="G95" s="22"/>
+      <c r="H95" s="22"/>
+      <c r="I95" s="22"/>
+      <c r="J95" s="5"/>
+    </row>
+    <row r="96" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B96" s="4"/>
+      <c r="C96" s="22"/>
+      <c r="D96" s="22"/>
+      <c r="E96" s="22"/>
+      <c r="F96" s="22"/>
+      <c r="G96" s="22"/>
+      <c r="H96" s="22"/>
+      <c r="I96" s="22"/>
+      <c r="J96" s="5"/>
+    </row>
+    <row r="97" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B97" s="6"/>
+      <c r="C97" s="7"/>
+      <c r="D97" s="7"/>
+      <c r="E97" s="7"/>
+      <c r="F97" s="7"/>
+      <c r="G97" s="7"/>
+      <c r="H97" s="7"/>
+      <c r="I97" s="7"/>
+      <c r="J97" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Create and require (not include) the router class
</commit_message>
<xml_diff>
--- a/me/2.routing.xlsx
+++ b/me/2.routing.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\build-php-mvc-framework\me\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{175E3279-08BC-4718-821E-6A549FD18A15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2786820C-A4E4-4ED0-94D9-F9419649F89C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="central entry point" sheetId="1" r:id="rId1"/>
     <sheet name="Configure URLs" sheetId="2" r:id="rId2"/>
+    <sheet name="CreateAndRequireRouterClass" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="69">
   <si>
     <t>Create a central entry point to the framework: the front controller</t>
   </si>
@@ -267,6 +268,72 @@
   </si>
   <si>
     <t>Remove dấu ? Ở vị trí đầu tiên, mình vẫn nhận được kết quả "product/list?page=1" như vậy</t>
+  </si>
+  <si>
+    <t>Create and require (not include) the router class</t>
+  </si>
+  <si>
+    <t>Router.php</t>
+  </si>
+  <si>
+    <t>build-php-mvc-framework\Core\Router.php</t>
+  </si>
+  <si>
+    <t>/**</t>
+  </si>
+  <si>
+    <t> * Router</t>
+  </si>
+  <si>
+    <t> */</t>
+  </si>
+  <si>
+    <t>class Router</t>
+  </si>
+  <si>
+    <t>{</t>
+  </si>
+  <si>
+    <t>}</t>
+  </si>
+  <si>
+    <t> * Front controller</t>
+  </si>
+  <si>
+    <t> * Routing</t>
+  </si>
+  <si>
+    <t>require '../Core/Router.php';</t>
+  </si>
+  <si>
+    <t>$router = new Router();</t>
+  </si>
+  <si>
+    <t>echo get_class($router);</t>
+  </si>
+  <si>
+    <t>Mọi request ban đầu đều được gửi đến 1 file front controller và mình dùng querystring để lấy request URL hoặc route.</t>
+  </si>
+  <si>
+    <t>Giờ mình sẽ dựa vào URL lấy được để quyết định trỏ đến Controller và action nào</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trong PHP thì ko bắt buộc phải tạo class đối với 1 file riêng nhưng việc dùng class thì có 1 số thuận lợi đó là dễ maintain và việc dùng class giúp mình có thể </t>
+  </si>
+  <si>
+    <t>load class file tự động</t>
+  </si>
+  <si>
+    <t>Dùng require thì PHP sẽ đưa ra lỗi trong trường hợp file ko tồn tại, nếu dùng include thì PHP vẫn tiếp tục xử lý nếu file ko tồn tại</t>
+  </si>
+  <si>
+    <t>Vì dùng require nên khi code hoạt động và ko có error thì có nghĩa là class đã được load vào</t>
+  </si>
+  <si>
+    <t>Check by browser</t>
+  </si>
+  <si>
+    <t>Router là thành phần sẽ lấy request url hay route và từ đó đưa ra xử lý, nó là central part of framework</t>
   </si>
 </sst>
 </file>
@@ -408,6 +475,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -419,8 +488,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1643,6 +1710,302 @@
         </a:fontRef>
       </xdr:style>
     </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>427442</xdr:colOff>
+      <xdr:row>88</xdr:row>
+      <xdr:rowOff>37744</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F14729BE-45DB-C93B-0C18-B43469D2717E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="714375" y="13811250"/>
+          <a:ext cx="9466667" cy="2847619"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="7" name="Straight Arrow Connector 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{10021D71-490C-7AC9-47FF-F4D7B798B0DF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="990600" y="6067425"/>
+          <a:ext cx="647700" cy="2771775"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>123824</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>323849</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>87618</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7C1A235E-ADE7-63D9-6B74-73B6505DCD82}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="781050" y="1076324"/>
+          <a:ext cx="11125199" cy="4202419"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="Straight Arrow Connector 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0C285745-8F10-4682-5F74-55450CB259CF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="676275" y="923925"/>
+          <a:ext cx="1190625" cy="2371725"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="11" name="Straight Arrow Connector 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BC9ABB82-917F-02F7-AB76-7642EC7D820E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="1809750" y="12801600"/>
+          <a:ext cx="6219825" cy="647700"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>91</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>103934</xdr:colOff>
+      <xdr:row>98</xdr:row>
+      <xdr:rowOff>104602</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9410A410-5AE9-6547-4A73-E14C69FE7FBE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="695325" y="17249775"/>
+          <a:ext cx="6723809" cy="1380952"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -2417,8 +2780,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0EE5C4F-42B3-4F42-80A8-CAE45B1514F0}">
   <dimension ref="A2:Q97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="O100" sqref="O100"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35:F46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2450,200 +2813,46 @@
     </row>
     <row r="6" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B6" s="4"/>
-      <c r="C6" s="22"/>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
-      <c r="F6" s="22"/>
-      <c r="G6" s="22"/>
-      <c r="H6" s="22"/>
-      <c r="I6" s="22"/>
-      <c r="J6" s="22"/>
-      <c r="K6" s="22"/>
-      <c r="L6" s="22"/>
-      <c r="M6" s="22"/>
-      <c r="N6" s="22"/>
-      <c r="O6" s="22"/>
-      <c r="P6" s="22"/>
       <c r="Q6" s="5"/>
     </row>
     <row r="7" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B7" s="4"/>
-      <c r="C7" s="22"/>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
-      <c r="F7" s="22"/>
-      <c r="G7" s="22"/>
-      <c r="H7" s="22"/>
-      <c r="I7" s="22"/>
-      <c r="J7" s="22"/>
-      <c r="K7" s="22"/>
-      <c r="L7" s="22"/>
-      <c r="M7" s="22"/>
-      <c r="N7" s="22"/>
-      <c r="O7" s="22"/>
-      <c r="P7" s="22"/>
       <c r="Q7" s="5"/>
     </row>
     <row r="8" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B8" s="4"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="22"/>
-      <c r="E8" s="22"/>
-      <c r="F8" s="22"/>
-      <c r="G8" s="22"/>
-      <c r="H8" s="22"/>
-      <c r="I8" s="22"/>
-      <c r="J8" s="22"/>
-      <c r="K8" s="22"/>
-      <c r="L8" s="22"/>
-      <c r="M8" s="22"/>
-      <c r="N8" s="22"/>
-      <c r="O8" s="22"/>
-      <c r="P8" s="22"/>
       <c r="Q8" s="5"/>
     </row>
     <row r="9" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B9" s="4"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="22"/>
-      <c r="E9" s="22"/>
-      <c r="F9" s="22"/>
-      <c r="G9" s="22"/>
-      <c r="H9" s="22"/>
-      <c r="I9" s="22"/>
-      <c r="J9" s="22"/>
-      <c r="K9" s="22"/>
-      <c r="L9" s="22"/>
-      <c r="M9" s="22"/>
-      <c r="N9" s="22"/>
-      <c r="O9" s="22"/>
-      <c r="P9" s="22"/>
       <c r="Q9" s="5"/>
     </row>
     <row r="10" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B10" s="4"/>
-      <c r="C10" s="22"/>
-      <c r="D10" s="22"/>
-      <c r="E10" s="22"/>
-      <c r="F10" s="22"/>
-      <c r="G10" s="22"/>
-      <c r="H10" s="22"/>
-      <c r="I10" s="22"/>
-      <c r="J10" s="22"/>
-      <c r="K10" s="22"/>
-      <c r="L10" s="22"/>
-      <c r="M10" s="22"/>
-      <c r="N10" s="22"/>
-      <c r="O10" s="22"/>
-      <c r="P10" s="22"/>
       <c r="Q10" s="5"/>
     </row>
     <row r="11" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B11" s="4"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="22"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="22"/>
-      <c r="G11" s="22"/>
-      <c r="H11" s="22"/>
-      <c r="I11" s="22"/>
-      <c r="J11" s="22"/>
-      <c r="K11" s="22"/>
-      <c r="L11" s="22"/>
-      <c r="M11" s="22"/>
-      <c r="N11" s="22"/>
-      <c r="O11" s="22"/>
-      <c r="P11" s="22"/>
       <c r="Q11" s="5"/>
     </row>
     <row r="12" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B12" s="4"/>
-      <c r="C12" s="22"/>
-      <c r="D12" s="22"/>
-      <c r="E12" s="22"/>
-      <c r="F12" s="22"/>
-      <c r="G12" s="22"/>
-      <c r="H12" s="22"/>
-      <c r="I12" s="22"/>
-      <c r="J12" s="22"/>
-      <c r="K12" s="22"/>
-      <c r="L12" s="22"/>
-      <c r="M12" s="22"/>
-      <c r="N12" s="22"/>
-      <c r="O12" s="22"/>
-      <c r="P12" s="22"/>
       <c r="Q12" s="5"/>
     </row>
     <row r="13" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B13" s="4"/>
-      <c r="C13" s="22"/>
-      <c r="D13" s="22"/>
-      <c r="E13" s="22"/>
-      <c r="F13" s="22"/>
-      <c r="G13" s="22"/>
-      <c r="H13" s="22"/>
-      <c r="I13" s="22"/>
-      <c r="J13" s="22"/>
-      <c r="K13" s="22"/>
-      <c r="L13" s="22"/>
-      <c r="M13" s="22"/>
-      <c r="N13" s="22"/>
-      <c r="O13" s="22"/>
-      <c r="P13" s="22"/>
       <c r="Q13" s="5"/>
     </row>
     <row r="14" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B14" s="4"/>
-      <c r="C14" s="22"/>
-      <c r="D14" s="22"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="22"/>
-      <c r="G14" s="22"/>
-      <c r="H14" s="22"/>
-      <c r="I14" s="22"/>
-      <c r="J14" s="22"/>
-      <c r="K14" s="22"/>
-      <c r="L14" s="22"/>
-      <c r="M14" s="22"/>
-      <c r="N14" s="22"/>
-      <c r="O14" s="22"/>
-      <c r="P14" s="22"/>
       <c r="Q14" s="5"/>
     </row>
     <row r="15" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B15" s="4"/>
-      <c r="C15" s="22"/>
-      <c r="D15" s="22"/>
-      <c r="E15" s="22"/>
-      <c r="F15" s="22"/>
-      <c r="G15" s="22"/>
-      <c r="H15" s="22"/>
-      <c r="I15" s="22"/>
-      <c r="J15" s="22"/>
-      <c r="K15" s="22"/>
-      <c r="L15" s="22"/>
-      <c r="M15" s="22"/>
-      <c r="N15" s="22"/>
-      <c r="O15" s="22"/>
-      <c r="P15" s="22"/>
       <c r="Q15" s="5"/>
     </row>
     <row r="16" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B16" s="4"/>
-      <c r="C16" s="22"/>
-      <c r="D16" s="22"/>
-      <c r="E16" s="22"/>
-      <c r="F16" s="22"/>
-      <c r="G16" s="22"/>
-      <c r="H16" s="22"/>
-      <c r="I16" s="22"/>
-      <c r="J16" s="22"/>
-      <c r="K16" s="22"/>
-      <c r="L16" s="22"/>
-      <c r="M16" s="22"/>
-      <c r="N16" s="22"/>
-      <c r="O16" s="22"/>
-      <c r="P16" s="22"/>
       <c r="Q16" s="5"/>
     </row>
     <row r="17" spans="2:17" x14ac:dyDescent="0.25">
@@ -2686,200 +2895,46 @@
     </row>
     <row r="21" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B21" s="4"/>
-      <c r="C21" s="22"/>
-      <c r="D21" s="22"/>
-      <c r="E21" s="22"/>
-      <c r="F21" s="22"/>
-      <c r="G21" s="22"/>
-      <c r="H21" s="22"/>
-      <c r="I21" s="22"/>
-      <c r="J21" s="22"/>
-      <c r="K21" s="22"/>
-      <c r="L21" s="22"/>
-      <c r="M21" s="22"/>
-      <c r="N21" s="22"/>
-      <c r="O21" s="22"/>
-      <c r="P21" s="22"/>
       <c r="Q21" s="5"/>
     </row>
     <row r="22" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B22" s="4"/>
-      <c r="C22" s="22"/>
-      <c r="D22" s="22"/>
-      <c r="E22" s="22"/>
-      <c r="F22" s="22"/>
-      <c r="G22" s="22"/>
-      <c r="H22" s="22"/>
-      <c r="I22" s="22"/>
-      <c r="J22" s="22"/>
-      <c r="K22" s="22"/>
-      <c r="L22" s="22"/>
-      <c r="M22" s="22"/>
-      <c r="N22" s="22"/>
-      <c r="O22" s="22"/>
-      <c r="P22" s="22"/>
       <c r="Q22" s="5"/>
     </row>
     <row r="23" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B23" s="4"/>
-      <c r="C23" s="22"/>
-      <c r="D23" s="22"/>
-      <c r="E23" s="22"/>
-      <c r="F23" s="22"/>
-      <c r="G23" s="22"/>
-      <c r="H23" s="22"/>
-      <c r="I23" s="22"/>
-      <c r="J23" s="22"/>
-      <c r="K23" s="22"/>
-      <c r="L23" s="22"/>
-      <c r="M23" s="22"/>
-      <c r="N23" s="22"/>
-      <c r="O23" s="22"/>
-      <c r="P23" s="22"/>
       <c r="Q23" s="5"/>
     </row>
     <row r="24" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B24" s="4"/>
-      <c r="C24" s="22"/>
-      <c r="D24" s="22"/>
-      <c r="E24" s="22"/>
-      <c r="F24" s="22"/>
-      <c r="G24" s="22"/>
-      <c r="H24" s="22"/>
-      <c r="I24" s="22"/>
-      <c r="J24" s="22"/>
-      <c r="K24" s="22"/>
-      <c r="L24" s="22"/>
-      <c r="M24" s="22"/>
-      <c r="N24" s="22"/>
-      <c r="O24" s="22"/>
-      <c r="P24" s="22"/>
       <c r="Q24" s="5"/>
     </row>
     <row r="25" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B25" s="4"/>
-      <c r="C25" s="22"/>
-      <c r="D25" s="22"/>
-      <c r="E25" s="22"/>
-      <c r="F25" s="22"/>
-      <c r="G25" s="22"/>
-      <c r="H25" s="22"/>
-      <c r="I25" s="22"/>
-      <c r="J25" s="22"/>
-      <c r="K25" s="22"/>
-      <c r="L25" s="22"/>
-      <c r="M25" s="22"/>
-      <c r="N25" s="22"/>
-      <c r="O25" s="22"/>
-      <c r="P25" s="22"/>
       <c r="Q25" s="5"/>
     </row>
     <row r="26" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B26" s="4"/>
-      <c r="C26" s="22"/>
-      <c r="D26" s="22"/>
-      <c r="E26" s="22"/>
-      <c r="F26" s="22"/>
-      <c r="G26" s="22"/>
-      <c r="H26" s="22"/>
-      <c r="I26" s="22"/>
-      <c r="J26" s="22"/>
-      <c r="K26" s="22"/>
-      <c r="L26" s="22"/>
-      <c r="M26" s="22"/>
-      <c r="N26" s="22"/>
-      <c r="O26" s="22"/>
-      <c r="P26" s="22"/>
       <c r="Q26" s="5"/>
     </row>
     <row r="27" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B27" s="4"/>
-      <c r="C27" s="22"/>
-      <c r="D27" s="22"/>
-      <c r="E27" s="22"/>
-      <c r="F27" s="22"/>
-      <c r="G27" s="22"/>
-      <c r="H27" s="22"/>
-      <c r="I27" s="22"/>
-      <c r="J27" s="22"/>
-      <c r="K27" s="22"/>
-      <c r="L27" s="22"/>
-      <c r="M27" s="22"/>
-      <c r="N27" s="22"/>
-      <c r="O27" s="22"/>
-      <c r="P27" s="22"/>
       <c r="Q27" s="5"/>
     </row>
     <row r="28" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B28" s="4"/>
-      <c r="C28" s="22"/>
-      <c r="D28" s="22"/>
-      <c r="E28" s="22"/>
-      <c r="F28" s="22"/>
-      <c r="G28" s="22"/>
-      <c r="H28" s="22"/>
-      <c r="I28" s="22"/>
-      <c r="J28" s="22"/>
-      <c r="K28" s="22"/>
-      <c r="L28" s="22"/>
-      <c r="M28" s="22"/>
-      <c r="N28" s="22"/>
-      <c r="O28" s="22"/>
-      <c r="P28" s="22"/>
       <c r="Q28" s="5"/>
     </row>
     <row r="29" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B29" s="4"/>
-      <c r="C29" s="22"/>
-      <c r="D29" s="22"/>
-      <c r="E29" s="22"/>
-      <c r="F29" s="22"/>
-      <c r="G29" s="22"/>
-      <c r="H29" s="22"/>
-      <c r="I29" s="22"/>
-      <c r="J29" s="22"/>
-      <c r="K29" s="22"/>
-      <c r="L29" s="22"/>
-      <c r="M29" s="22"/>
-      <c r="N29" s="22"/>
-      <c r="O29" s="22"/>
-      <c r="P29" s="22"/>
       <c r="Q29" s="5"/>
     </row>
     <row r="30" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B30" s="4"/>
-      <c r="C30" s="22"/>
-      <c r="D30" s="22"/>
-      <c r="E30" s="22"/>
-      <c r="F30" s="22"/>
-      <c r="G30" s="22"/>
-      <c r="H30" s="22"/>
-      <c r="I30" s="22"/>
-      <c r="J30" s="22"/>
-      <c r="K30" s="22"/>
-      <c r="L30" s="22"/>
-      <c r="M30" s="22"/>
-      <c r="N30" s="22"/>
-      <c r="O30" s="22"/>
-      <c r="P30" s="22"/>
       <c r="Q30" s="5"/>
     </row>
     <row r="31" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B31" s="4"/>
-      <c r="C31" s="22"/>
-      <c r="D31" s="22"/>
-      <c r="E31" s="22"/>
-      <c r="F31" s="22"/>
-      <c r="G31" s="22"/>
-      <c r="H31" s="22"/>
-      <c r="I31" s="22"/>
-      <c r="J31" s="22"/>
-      <c r="K31" s="22"/>
-      <c r="L31" s="22"/>
-      <c r="M31" s="22"/>
-      <c r="N31" s="22"/>
-      <c r="O31" s="22"/>
-      <c r="P31" s="22"/>
       <c r="Q31" s="5"/>
     </row>
     <row r="32" spans="2:17" x14ac:dyDescent="0.25">
@@ -2901,104 +2956,74 @@
       <c r="Q32" s="8"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="12" t="s">
+      <c r="A35" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B35" s="13"/>
-      <c r="C35" s="13"/>
-      <c r="D35" s="13"/>
-      <c r="E35" s="13"/>
-      <c r="F35" s="13"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="13"/>
-      <c r="B36" s="14" t="s">
+      <c r="B36" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C36" s="15"/>
-      <c r="D36" s="15"/>
-      <c r="E36" s="15"/>
-      <c r="F36" s="16"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="3"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="13"/>
-      <c r="B37" s="17"/>
-      <c r="C37" s="13" t="s">
+      <c r="B37" s="4"/>
+      <c r="C37" t="s">
         <v>10</v>
       </c>
-      <c r="D37" s="13"/>
-      <c r="E37" s="13"/>
-      <c r="F37" s="18"/>
+      <c r="F37" s="5"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="13"/>
-      <c r="B38" s="17"/>
-      <c r="C38" s="13"/>
-      <c r="D38" s="13" t="s">
+      <c r="B38" s="4"/>
+      <c r="D38" t="s">
         <v>11</v>
       </c>
-      <c r="E38" s="13"/>
-      <c r="F38" s="18"/>
+      <c r="F38" s="5"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="13"/>
-      <c r="B39" s="17"/>
-      <c r="C39" s="13"/>
-      <c r="D39" s="13" t="s">
+      <c r="B39" s="4"/>
+      <c r="D39" t="s">
         <v>12</v>
       </c>
-      <c r="E39" s="13"/>
-      <c r="F39" s="18"/>
+      <c r="F39" s="5"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="13"/>
-      <c r="B40" s="17"/>
-      <c r="C40" s="13"/>
-      <c r="D40" s="13" t="s">
+      <c r="B40" s="4"/>
+      <c r="D40" t="s">
         <v>13</v>
       </c>
-      <c r="E40" s="13"/>
-      <c r="F40" s="18"/>
+      <c r="F40" s="5"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="13"/>
-      <c r="B41" s="17"/>
-      <c r="C41" s="13" t="s">
+      <c r="B41" s="4"/>
+      <c r="C41" t="s">
         <v>14</v>
       </c>
-      <c r="D41" s="13"/>
-      <c r="E41" s="13"/>
-      <c r="F41" s="18"/>
+      <c r="F41" s="5"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="13"/>
-      <c r="B42" s="17"/>
-      <c r="C42" s="13" t="s">
+      <c r="B42" s="4"/>
+      <c r="C42" t="s">
         <v>15</v>
       </c>
-      <c r="D42" s="13"/>
-      <c r="E42" s="13"/>
-      <c r="F42" s="18"/>
+      <c r="F42" s="5"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" s="13"/>
-      <c r="B43" s="17"/>
-      <c r="C43" s="13" t="s">
+      <c r="B43" s="4"/>
+      <c r="C43" t="s">
         <v>16</v>
       </c>
-      <c r="D43" s="13"/>
-      <c r="E43" s="13"/>
-      <c r="F43" s="18"/>
+      <c r="F43" s="5"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" s="13"/>
-      <c r="B44" s="17"/>
-      <c r="C44" s="13"/>
+      <c r="B44" s="4"/>
       <c r="D44" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="E44" s="13"/>
-      <c r="F44" s="18"/>
+      <c r="F44" s="5"/>
       <c r="G44" t="s">
         <v>20</v>
       </c>
@@ -3007,24 +3032,20 @@
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" s="13"/>
-      <c r="B45" s="17"/>
-      <c r="C45" s="13"/>
-      <c r="D45" s="13" t="s">
+      <c r="B45" s="4"/>
+      <c r="D45" t="s">
         <v>17</v>
       </c>
-      <c r="E45" s="13"/>
-      <c r="F45" s="18"/>
+      <c r="F45" s="5"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" s="13"/>
-      <c r="B46" s="19"/>
-      <c r="C46" s="20" t="s">
+      <c r="B46" s="6"/>
+      <c r="C46" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D46" s="20"/>
-      <c r="E46" s="20"/>
-      <c r="F46" s="21"/>
+      <c r="D46" s="7"/>
+      <c r="E46" s="7"/>
+      <c r="F46" s="8"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
@@ -3047,48 +3068,24 @@
       <c r="B51" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C51" s="22"/>
-      <c r="D51" s="22"/>
-      <c r="E51" s="22"/>
-      <c r="F51" s="22"/>
-      <c r="G51" s="22"/>
-      <c r="H51" s="22"/>
       <c r="I51" s="5"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B52" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C52" s="22"/>
-      <c r="D52" s="22"/>
-      <c r="E52" s="22"/>
-      <c r="F52" s="22"/>
-      <c r="G52" s="22"/>
-      <c r="H52" s="22"/>
       <c r="I52" s="5"/>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B53" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C53" s="22"/>
-      <c r="D53" s="22"/>
-      <c r="E53" s="22"/>
-      <c r="F53" s="22"/>
-      <c r="G53" s="22"/>
-      <c r="H53" s="22"/>
       <c r="I53" s="5"/>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B54" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C54" s="22"/>
-      <c r="D54" s="22"/>
-      <c r="E54" s="22"/>
-      <c r="F54" s="22"/>
-      <c r="G54" s="22"/>
-      <c r="H54" s="22"/>
       <c r="I54" s="5"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
@@ -3149,7 +3146,7 @@
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B68" s="23" t="s">
+      <c r="B68" s="12" t="s">
         <v>44</v>
       </c>
       <c r="C68" s="2"/>
@@ -3163,68 +3160,26 @@
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B69" s="4"/>
-      <c r="C69" s="22"/>
-      <c r="D69" s="22"/>
-      <c r="E69" s="22"/>
-      <c r="F69" s="22"/>
-      <c r="G69" s="22"/>
-      <c r="H69" s="22"/>
-      <c r="I69" s="22"/>
       <c r="J69" s="5"/>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B70" s="4"/>
-      <c r="C70" s="22"/>
-      <c r="D70" s="22"/>
-      <c r="E70" s="22"/>
-      <c r="F70" s="22"/>
-      <c r="G70" s="22"/>
-      <c r="H70" s="22"/>
-      <c r="I70" s="22"/>
       <c r="J70" s="5"/>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B71" s="4"/>
-      <c r="C71" s="22"/>
-      <c r="D71" s="22"/>
-      <c r="E71" s="22"/>
-      <c r="F71" s="22"/>
-      <c r="G71" s="22"/>
-      <c r="H71" s="22"/>
-      <c r="I71" s="22"/>
       <c r="J71" s="5"/>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B72" s="4"/>
-      <c r="C72" s="22"/>
-      <c r="D72" s="22"/>
-      <c r="E72" s="22"/>
-      <c r="F72" s="22"/>
-      <c r="G72" s="22"/>
-      <c r="H72" s="22"/>
-      <c r="I72" s="22"/>
       <c r="J72" s="5"/>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B73" s="4"/>
-      <c r="C73" s="22"/>
-      <c r="D73" s="22"/>
-      <c r="E73" s="22"/>
-      <c r="F73" s="22"/>
-      <c r="G73" s="22"/>
-      <c r="H73" s="22"/>
-      <c r="I73" s="22"/>
       <c r="J73" s="5"/>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B74" s="4"/>
-      <c r="C74" s="22"/>
-      <c r="D74" s="22"/>
-      <c r="E74" s="22"/>
-      <c r="F74" s="22"/>
-      <c r="G74" s="22"/>
-      <c r="H74" s="22"/>
-      <c r="I74" s="22"/>
       <c r="J74" s="5"/>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.25">
@@ -3252,93 +3207,37 @@
       <c r="J78" s="3"/>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B79" s="24" t="s">
+      <c r="B79" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="C79" s="22"/>
-      <c r="D79" s="22"/>
-      <c r="E79" s="22"/>
-      <c r="F79" s="22"/>
-      <c r="G79" s="22"/>
-      <c r="H79" s="22"/>
-      <c r="I79" s="22"/>
       <c r="J79" s="5"/>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B80" s="4"/>
-      <c r="C80" s="22"/>
-      <c r="D80" s="22"/>
-      <c r="E80" s="22"/>
-      <c r="F80" s="22"/>
-      <c r="G80" s="22"/>
-      <c r="H80" s="22"/>
-      <c r="I80" s="22"/>
       <c r="J80" s="5"/>
     </row>
     <row r="81" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B81" s="4"/>
-      <c r="C81" s="22"/>
-      <c r="D81" s="22"/>
-      <c r="E81" s="22"/>
-      <c r="F81" s="22"/>
-      <c r="G81" s="22"/>
-      <c r="H81" s="22"/>
-      <c r="I81" s="22"/>
       <c r="J81" s="5"/>
     </row>
     <row r="82" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B82" s="4"/>
-      <c r="C82" s="22"/>
-      <c r="D82" s="22"/>
-      <c r="E82" s="22"/>
-      <c r="F82" s="22"/>
-      <c r="G82" s="22"/>
-      <c r="H82" s="22"/>
-      <c r="I82" s="22"/>
       <c r="J82" s="5"/>
     </row>
     <row r="83" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B83" s="4"/>
-      <c r="C83" s="22"/>
-      <c r="D83" s="22"/>
-      <c r="E83" s="22"/>
-      <c r="F83" s="22"/>
-      <c r="G83" s="22"/>
-      <c r="H83" s="22"/>
-      <c r="I83" s="22"/>
       <c r="J83" s="5"/>
     </row>
     <row r="84" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B84" s="4"/>
-      <c r="C84" s="22"/>
-      <c r="D84" s="22"/>
-      <c r="E84" s="22"/>
-      <c r="F84" s="22"/>
-      <c r="G84" s="22"/>
-      <c r="H84" s="22"/>
-      <c r="I84" s="22"/>
       <c r="J84" s="5"/>
     </row>
     <row r="85" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B85" s="4"/>
-      <c r="C85" s="22"/>
-      <c r="D85" s="22"/>
-      <c r="E85" s="22"/>
-      <c r="F85" s="22"/>
-      <c r="G85" s="22"/>
-      <c r="H85" s="22"/>
-      <c r="I85" s="22"/>
       <c r="J85" s="5"/>
     </row>
     <row r="86" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B86" s="4"/>
-      <c r="C86" s="22"/>
-      <c r="D86" s="22"/>
-      <c r="E86" s="22"/>
-      <c r="F86" s="22"/>
-      <c r="G86" s="22"/>
-      <c r="H86" s="22"/>
-      <c r="I86" s="22"/>
       <c r="J86" s="5"/>
     </row>
     <row r="87" spans="2:10" x14ac:dyDescent="0.25">
@@ -3367,68 +3266,26 @@
     </row>
     <row r="91" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B91" s="4"/>
-      <c r="C91" s="22"/>
-      <c r="D91" s="22"/>
-      <c r="E91" s="22"/>
-      <c r="F91" s="22"/>
-      <c r="G91" s="22"/>
-      <c r="H91" s="22"/>
-      <c r="I91" s="22"/>
       <c r="J91" s="5"/>
     </row>
     <row r="92" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B92" s="4"/>
-      <c r="C92" s="22"/>
-      <c r="D92" s="22"/>
-      <c r="E92" s="22"/>
-      <c r="F92" s="22"/>
-      <c r="G92" s="22"/>
-      <c r="H92" s="22"/>
-      <c r="I92" s="22"/>
       <c r="J92" s="5"/>
     </row>
     <row r="93" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B93" s="4"/>
-      <c r="C93" s="22"/>
-      <c r="D93" s="22"/>
-      <c r="E93" s="22"/>
-      <c r="F93" s="22"/>
-      <c r="G93" s="22"/>
-      <c r="H93" s="22"/>
-      <c r="I93" s="22"/>
       <c r="J93" s="5"/>
     </row>
     <row r="94" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B94" s="4"/>
-      <c r="C94" s="22"/>
-      <c r="D94" s="22"/>
-      <c r="E94" s="22"/>
-      <c r="F94" s="22"/>
-      <c r="G94" s="22"/>
-      <c r="H94" s="22"/>
-      <c r="I94" s="22"/>
       <c r="J94" s="5"/>
     </row>
     <row r="95" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B95" s="4"/>
-      <c r="C95" s="22"/>
-      <c r="D95" s="22"/>
-      <c r="E95" s="22"/>
-      <c r="F95" s="22"/>
-      <c r="G95" s="22"/>
-      <c r="H95" s="22"/>
-      <c r="I95" s="22"/>
       <c r="J95" s="5"/>
     </row>
     <row r="96" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B96" s="4"/>
-      <c r="C96" s="22"/>
-      <c r="D96" s="22"/>
-      <c r="E96" s="22"/>
-      <c r="F96" s="22"/>
-      <c r="G96" s="22"/>
-      <c r="H96" s="22"/>
-      <c r="I96" s="22"/>
       <c r="J96" s="5"/>
     </row>
     <row r="97" spans="2:10" x14ac:dyDescent="0.25">
@@ -3446,4 +3303,898 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9976F058-B1B7-4D54-8A36-C2B299C50638}">
+  <dimension ref="A2:T91"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="P71" sqref="P71"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="2"/>
+      <c r="R5" s="2"/>
+      <c r="S5" s="2"/>
+      <c r="T5" s="3"/>
+    </row>
+    <row r="6" spans="2:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="4"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="24"/>
+      <c r="I6" s="24"/>
+      <c r="J6" s="24"/>
+      <c r="K6" s="24"/>
+      <c r="L6" s="24"/>
+      <c r="M6" s="24"/>
+      <c r="N6" s="24"/>
+      <c r="O6" s="24"/>
+      <c r="P6" s="24"/>
+      <c r="Q6" s="24"/>
+      <c r="R6" s="24"/>
+      <c r="S6" s="24"/>
+      <c r="T6" s="5"/>
+    </row>
+    <row r="7" spans="2:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="4"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="24"/>
+      <c r="H7" s="24"/>
+      <c r="I7" s="24"/>
+      <c r="J7" s="24"/>
+      <c r="K7" s="24"/>
+      <c r="L7" s="24"/>
+      <c r="M7" s="24"/>
+      <c r="N7" s="24"/>
+      <c r="O7" s="24"/>
+      <c r="P7" s="24"/>
+      <c r="Q7" s="24"/>
+      <c r="R7" s="24"/>
+      <c r="S7" s="24"/>
+      <c r="T7" s="5"/>
+    </row>
+    <row r="8" spans="2:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="4"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="24"/>
+      <c r="I8" s="24"/>
+      <c r="J8" s="24"/>
+      <c r="K8" s="24"/>
+      <c r="L8" s="24"/>
+      <c r="M8" s="24"/>
+      <c r="N8" s="24"/>
+      <c r="O8" s="24"/>
+      <c r="P8" s="24"/>
+      <c r="Q8" s="24"/>
+      <c r="R8" s="24"/>
+      <c r="S8" s="24"/>
+      <c r="T8" s="5"/>
+    </row>
+    <row r="9" spans="2:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="4"/>
+      <c r="C9" s="24"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="24"/>
+      <c r="H9" s="24"/>
+      <c r="I9" s="24"/>
+      <c r="J9" s="24"/>
+      <c r="K9" s="24"/>
+      <c r="L9" s="24"/>
+      <c r="M9" s="24"/>
+      <c r="N9" s="24"/>
+      <c r="O9" s="24"/>
+      <c r="P9" s="24"/>
+      <c r="Q9" s="24"/>
+      <c r="R9" s="24"/>
+      <c r="S9" s="24"/>
+      <c r="T9" s="5"/>
+    </row>
+    <row r="10" spans="2:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="4"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="24"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="24"/>
+      <c r="J10" s="24"/>
+      <c r="K10" s="24"/>
+      <c r="L10" s="24"/>
+      <c r="M10" s="24"/>
+      <c r="N10" s="24"/>
+      <c r="O10" s="24"/>
+      <c r="P10" s="24"/>
+      <c r="Q10" s="24"/>
+      <c r="R10" s="24"/>
+      <c r="S10" s="24"/>
+      <c r="T10" s="5"/>
+    </row>
+    <row r="11" spans="2:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="4"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="24"/>
+      <c r="J11" s="24"/>
+      <c r="K11" s="24"/>
+      <c r="L11" s="24"/>
+      <c r="M11" s="24"/>
+      <c r="N11" s="24"/>
+      <c r="O11" s="24"/>
+      <c r="P11" s="24"/>
+      <c r="Q11" s="24"/>
+      <c r="R11" s="24"/>
+      <c r="S11" s="24"/>
+      <c r="T11" s="5"/>
+    </row>
+    <row r="12" spans="2:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="4"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="24"/>
+      <c r="H12" s="24"/>
+      <c r="I12" s="24"/>
+      <c r="J12" s="24"/>
+      <c r="K12" s="24"/>
+      <c r="L12" s="24"/>
+      <c r="M12" s="24"/>
+      <c r="N12" s="24"/>
+      <c r="O12" s="24"/>
+      <c r="P12" s="24"/>
+      <c r="Q12" s="24"/>
+      <c r="R12" s="24"/>
+      <c r="S12" s="24"/>
+      <c r="T12" s="5"/>
+    </row>
+    <row r="13" spans="2:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="4"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="24"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="24"/>
+      <c r="G13" s="24"/>
+      <c r="H13" s="24"/>
+      <c r="I13" s="24"/>
+      <c r="J13" s="24"/>
+      <c r="K13" s="24"/>
+      <c r="L13" s="24"/>
+      <c r="M13" s="24"/>
+      <c r="N13" s="24"/>
+      <c r="O13" s="24"/>
+      <c r="P13" s="24"/>
+      <c r="Q13" s="24"/>
+      <c r="R13" s="24"/>
+      <c r="S13" s="24"/>
+      <c r="T13" s="5"/>
+    </row>
+    <row r="14" spans="2:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="4"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="24"/>
+      <c r="H14" s="24"/>
+      <c r="I14" s="24"/>
+      <c r="J14" s="24"/>
+      <c r="K14" s="24"/>
+      <c r="L14" s="24"/>
+      <c r="M14" s="24"/>
+      <c r="N14" s="24"/>
+      <c r="O14" s="24"/>
+      <c r="P14" s="24"/>
+      <c r="Q14" s="24"/>
+      <c r="R14" s="24"/>
+      <c r="S14" s="24"/>
+      <c r="T14" s="5"/>
+    </row>
+    <row r="15" spans="2:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="4"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="24"/>
+      <c r="G15" s="24"/>
+      <c r="H15" s="24"/>
+      <c r="I15" s="24"/>
+      <c r="J15" s="24"/>
+      <c r="K15" s="24"/>
+      <c r="L15" s="24"/>
+      <c r="M15" s="24"/>
+      <c r="N15" s="24"/>
+      <c r="O15" s="24"/>
+      <c r="P15" s="24"/>
+      <c r="Q15" s="24"/>
+      <c r="R15" s="24"/>
+      <c r="S15" s="24"/>
+      <c r="T15" s="5"/>
+    </row>
+    <row r="16" spans="2:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="4"/>
+      <c r="C16" s="24"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="24"/>
+      <c r="F16" s="24"/>
+      <c r="G16" s="24"/>
+      <c r="H16" s="24"/>
+      <c r="I16" s="24"/>
+      <c r="J16" s="24"/>
+      <c r="K16" s="24"/>
+      <c r="L16" s="24"/>
+      <c r="M16" s="24"/>
+      <c r="N16" s="24"/>
+      <c r="O16" s="24"/>
+      <c r="P16" s="24"/>
+      <c r="Q16" s="24"/>
+      <c r="R16" s="24"/>
+      <c r="S16" s="24"/>
+      <c r="T16" s="5"/>
+    </row>
+    <row r="17" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="4"/>
+      <c r="C17" s="24"/>
+      <c r="D17" s="24"/>
+      <c r="E17" s="24"/>
+      <c r="F17" s="24"/>
+      <c r="G17" s="24"/>
+      <c r="H17" s="24"/>
+      <c r="I17" s="24"/>
+      <c r="J17" s="24"/>
+      <c r="K17" s="24"/>
+      <c r="L17" s="24"/>
+      <c r="M17" s="24"/>
+      <c r="N17" s="24"/>
+      <c r="O17" s="24"/>
+      <c r="P17" s="24"/>
+      <c r="Q17" s="24"/>
+      <c r="R17" s="24"/>
+      <c r="S17" s="24"/>
+      <c r="T17" s="5"/>
+    </row>
+    <row r="18" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="4"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="24"/>
+      <c r="E18" s="24"/>
+      <c r="F18" s="24"/>
+      <c r="G18" s="24"/>
+      <c r="H18" s="24"/>
+      <c r="I18" s="24"/>
+      <c r="J18" s="24"/>
+      <c r="K18" s="24"/>
+      <c r="L18" s="24"/>
+      <c r="M18" s="24"/>
+      <c r="N18" s="24"/>
+      <c r="O18" s="24"/>
+      <c r="P18" s="24"/>
+      <c r="Q18" s="24"/>
+      <c r="R18" s="24"/>
+      <c r="S18" s="24"/>
+      <c r="T18" s="5"/>
+    </row>
+    <row r="19" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="4"/>
+      <c r="C19" s="24"/>
+      <c r="D19" s="24"/>
+      <c r="E19" s="24"/>
+      <c r="F19" s="24"/>
+      <c r="G19" s="24"/>
+      <c r="H19" s="24"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="24"/>
+      <c r="K19" s="24"/>
+      <c r="L19" s="24"/>
+      <c r="M19" s="24"/>
+      <c r="N19" s="24"/>
+      <c r="O19" s="24"/>
+      <c r="P19" s="24"/>
+      <c r="Q19" s="24"/>
+      <c r="R19" s="24"/>
+      <c r="S19" s="24"/>
+      <c r="T19" s="5"/>
+    </row>
+    <row r="20" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="4"/>
+      <c r="C20" s="24"/>
+      <c r="D20" s="24"/>
+      <c r="E20" s="24"/>
+      <c r="F20" s="24"/>
+      <c r="G20" s="24"/>
+      <c r="H20" s="24"/>
+      <c r="I20" s="24"/>
+      <c r="J20" s="24"/>
+      <c r="K20" s="24"/>
+      <c r="L20" s="24"/>
+      <c r="M20" s="24"/>
+      <c r="N20" s="24"/>
+      <c r="O20" s="24"/>
+      <c r="P20" s="24"/>
+      <c r="Q20" s="24"/>
+      <c r="R20" s="24"/>
+      <c r="S20" s="24"/>
+      <c r="T20" s="5"/>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B21" s="4"/>
+      <c r="C21" s="24"/>
+      <c r="D21" s="24"/>
+      <c r="E21" s="24"/>
+      <c r="F21" s="24"/>
+      <c r="G21" s="24"/>
+      <c r="H21" s="24"/>
+      <c r="I21" s="24"/>
+      <c r="J21" s="24"/>
+      <c r="K21" s="24"/>
+      <c r="L21" s="24"/>
+      <c r="M21" s="24"/>
+      <c r="N21" s="24"/>
+      <c r="O21" s="24"/>
+      <c r="P21" s="24"/>
+      <c r="Q21" s="24"/>
+      <c r="R21" s="24"/>
+      <c r="S21" s="24"/>
+      <c r="T21" s="5"/>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B22" s="4"/>
+      <c r="C22" s="24"/>
+      <c r="D22" s="24"/>
+      <c r="E22" s="24"/>
+      <c r="F22" s="24"/>
+      <c r="G22" s="24"/>
+      <c r="H22" s="24"/>
+      <c r="I22" s="24"/>
+      <c r="J22" s="24"/>
+      <c r="K22" s="24"/>
+      <c r="L22" s="24"/>
+      <c r="M22" s="24"/>
+      <c r="N22" s="24"/>
+      <c r="O22" s="24"/>
+      <c r="P22" s="24"/>
+      <c r="Q22" s="24"/>
+      <c r="R22" s="24"/>
+      <c r="S22" s="24"/>
+      <c r="T22" s="5"/>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B23" s="4"/>
+      <c r="C23" s="24"/>
+      <c r="D23" s="24"/>
+      <c r="E23" s="24"/>
+      <c r="F23" s="24"/>
+      <c r="G23" s="24"/>
+      <c r="H23" s="24"/>
+      <c r="I23" s="24"/>
+      <c r="J23" s="24"/>
+      <c r="K23" s="24"/>
+      <c r="L23" s="24"/>
+      <c r="M23" s="24"/>
+      <c r="N23" s="24"/>
+      <c r="O23" s="24"/>
+      <c r="P23" s="24"/>
+      <c r="Q23" s="24"/>
+      <c r="R23" s="24"/>
+      <c r="S23" s="24"/>
+      <c r="T23" s="5"/>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B24" s="4"/>
+      <c r="C24" s="24"/>
+      <c r="D24" s="24"/>
+      <c r="E24" s="24"/>
+      <c r="F24" s="24"/>
+      <c r="G24" s="24"/>
+      <c r="H24" s="24"/>
+      <c r="I24" s="24"/>
+      <c r="J24" s="24"/>
+      <c r="K24" s="24"/>
+      <c r="L24" s="24"/>
+      <c r="M24" s="24"/>
+      <c r="N24" s="24"/>
+      <c r="O24" s="24"/>
+      <c r="P24" s="24"/>
+      <c r="Q24" s="24"/>
+      <c r="R24" s="24"/>
+      <c r="S24" s="24"/>
+      <c r="T24" s="5"/>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B25" s="4"/>
+      <c r="C25" s="24"/>
+      <c r="D25" s="24"/>
+      <c r="E25" s="24"/>
+      <c r="F25" s="24"/>
+      <c r="G25" s="24"/>
+      <c r="H25" s="24"/>
+      <c r="I25" s="24"/>
+      <c r="J25" s="24"/>
+      <c r="K25" s="24"/>
+      <c r="L25" s="24"/>
+      <c r="M25" s="24"/>
+      <c r="N25" s="24"/>
+      <c r="O25" s="24"/>
+      <c r="P25" s="24"/>
+      <c r="Q25" s="24"/>
+      <c r="R25" s="24"/>
+      <c r="S25" s="24"/>
+      <c r="T25" s="5"/>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B26" s="4"/>
+      <c r="C26" s="24"/>
+      <c r="D26" s="24"/>
+      <c r="E26" s="24"/>
+      <c r="F26" s="24"/>
+      <c r="G26" s="24"/>
+      <c r="H26" s="24"/>
+      <c r="I26" s="24"/>
+      <c r="J26" s="24"/>
+      <c r="K26" s="24"/>
+      <c r="L26" s="24"/>
+      <c r="M26" s="24"/>
+      <c r="N26" s="24"/>
+      <c r="O26" s="24"/>
+      <c r="P26" s="24"/>
+      <c r="Q26" s="24"/>
+      <c r="R26" s="24"/>
+      <c r="S26" s="24"/>
+      <c r="T26" s="5"/>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B27" s="4"/>
+      <c r="C27" s="24"/>
+      <c r="D27" s="24"/>
+      <c r="E27" s="24"/>
+      <c r="F27" s="24"/>
+      <c r="G27" s="24"/>
+      <c r="H27" s="24"/>
+      <c r="I27" s="24"/>
+      <c r="J27" s="24"/>
+      <c r="K27" s="24"/>
+      <c r="L27" s="24"/>
+      <c r="M27" s="24"/>
+      <c r="N27" s="24"/>
+      <c r="O27" s="24"/>
+      <c r="P27" s="24"/>
+      <c r="Q27" s="24"/>
+      <c r="R27" s="24"/>
+      <c r="S27" s="24"/>
+      <c r="T27" s="5"/>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B28" s="4"/>
+      <c r="C28" s="24"/>
+      <c r="D28" s="24"/>
+      <c r="E28" s="24"/>
+      <c r="F28" s="24"/>
+      <c r="G28" s="24"/>
+      <c r="H28" s="24"/>
+      <c r="I28" s="24"/>
+      <c r="J28" s="24"/>
+      <c r="K28" s="24"/>
+      <c r="L28" s="24"/>
+      <c r="M28" s="24"/>
+      <c r="N28" s="24"/>
+      <c r="O28" s="24"/>
+      <c r="P28" s="24"/>
+      <c r="Q28" s="24"/>
+      <c r="R28" s="24"/>
+      <c r="S28" s="24"/>
+      <c r="T28" s="5"/>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B29" s="6"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7"/>
+      <c r="G29" s="7"/>
+      <c r="H29" s="7"/>
+      <c r="I29" s="7"/>
+      <c r="J29" s="7"/>
+      <c r="K29" s="7"/>
+      <c r="L29" s="7"/>
+      <c r="M29" s="7"/>
+      <c r="N29" s="7"/>
+      <c r="O29" s="7"/>
+      <c r="P29" s="7"/>
+      <c r="Q29" s="7"/>
+      <c r="R29" s="7"/>
+      <c r="S29" s="7"/>
+      <c r="T29" s="8"/>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A32" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B32" s="15"/>
+      <c r="C32" s="15"/>
+      <c r="D32" s="15"/>
+      <c r="E32" s="15"/>
+      <c r="F32" s="15"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="15"/>
+      <c r="B33" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C33" s="17"/>
+      <c r="D33" s="17"/>
+      <c r="E33" s="17"/>
+      <c r="F33" s="18"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="15"/>
+      <c r="B34" s="19"/>
+      <c r="C34" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="D34" s="15"/>
+      <c r="E34" s="15"/>
+      <c r="F34" s="20"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="15"/>
+      <c r="B35" s="19"/>
+      <c r="C35" s="15"/>
+      <c r="D35" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="E35" s="15"/>
+      <c r="F35" s="20"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="15"/>
+      <c r="B36" s="19"/>
+      <c r="C36" s="15"/>
+      <c r="D36" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="E36" s="15"/>
+      <c r="F36" s="20"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="15"/>
+      <c r="B37" s="19"/>
+      <c r="C37" s="15"/>
+      <c r="D37" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E37" s="15"/>
+      <c r="F37" s="20"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="15"/>
+      <c r="B38" s="19"/>
+      <c r="C38" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D38" s="15"/>
+      <c r="E38" s="15"/>
+      <c r="F38" s="20"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="15"/>
+      <c r="B39" s="19"/>
+      <c r="C39" s="15"/>
+      <c r="D39" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="E39" s="15"/>
+      <c r="F39" s="20"/>
+      <c r="G39" t="s">
+        <v>20</v>
+      </c>
+      <c r="H39" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="15"/>
+      <c r="B40" s="19"/>
+      <c r="C40" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="D40" s="15"/>
+      <c r="E40" s="15"/>
+      <c r="F40" s="20"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="15"/>
+      <c r="B41" s="19"/>
+      <c r="C41" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D41" s="15"/>
+      <c r="E41" s="15"/>
+      <c r="F41" s="20"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="15"/>
+      <c r="B42" s="19"/>
+      <c r="C42" s="15"/>
+      <c r="D42" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="E42" s="15"/>
+      <c r="F42" s="20"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="15"/>
+      <c r="B43" s="19"/>
+      <c r="C43" s="15"/>
+      <c r="D43" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E43" s="15"/>
+      <c r="F43" s="20"/>
+      <c r="G43" t="s">
+        <v>20</v>
+      </c>
+      <c r="H43" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" s="15"/>
+      <c r="B44" s="21"/>
+      <c r="C44" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="D44" s="22"/>
+      <c r="E44" s="22"/>
+      <c r="F44" s="23"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B48" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C48" s="2"/>
+      <c r="D48" s="3"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B49" s="4"/>
+      <c r="C49" s="24"/>
+      <c r="D49" s="5"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B50" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C50" s="24"/>
+      <c r="D50" s="5"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B51" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C51" s="24"/>
+      <c r="D51" s="5"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B52" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C52" s="24"/>
+      <c r="D52" s="5"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B53" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C53" s="24"/>
+      <c r="D53" s="5"/>
+      <c r="E53" t="s">
+        <v>20</v>
+      </c>
+      <c r="F53" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B54" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C54" s="24"/>
+      <c r="D54" s="5"/>
+      <c r="F54" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B55" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C55" s="7"/>
+      <c r="D55" s="8"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B59" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C59" s="2"/>
+      <c r="D59" s="2"/>
+      <c r="E59" s="3"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B60" s="4"/>
+      <c r="C60" s="24"/>
+      <c r="D60" s="24"/>
+      <c r="E60" s="5"/>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B61" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C61" s="24"/>
+      <c r="D61" s="24"/>
+      <c r="E61" s="5"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B62" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C62" s="24"/>
+      <c r="D62" s="24"/>
+      <c r="E62" s="5"/>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B63" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C63" s="24"/>
+      <c r="D63" s="24"/>
+      <c r="E63" s="5"/>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B64" s="4"/>
+      <c r="C64" s="24"/>
+      <c r="D64" s="24"/>
+      <c r="E64" s="5"/>
+    </row>
+    <row r="65" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B65" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C65" s="24"/>
+      <c r="D65" s="24"/>
+      <c r="E65" s="5"/>
+    </row>
+    <row r="66" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B66" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C66" s="24"/>
+      <c r="D66" s="24"/>
+      <c r="E66" s="5"/>
+    </row>
+    <row r="67" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B67" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C67" s="24"/>
+      <c r="D67" s="24"/>
+      <c r="E67" s="5"/>
+    </row>
+    <row r="68" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B68" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C68" s="24"/>
+      <c r="D68" s="24"/>
+      <c r="E68" s="5"/>
+      <c r="F68" t="s">
+        <v>20</v>
+      </c>
+      <c r="G68" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="69" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B69" s="4"/>
+      <c r="C69" s="24"/>
+      <c r="D69" s="24"/>
+      <c r="E69" s="5"/>
+    </row>
+    <row r="70" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B70" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C70" s="24"/>
+      <c r="D70" s="24"/>
+      <c r="E70" s="5"/>
+    </row>
+    <row r="71" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B71" s="4"/>
+      <c r="C71" s="24"/>
+      <c r="D71" s="24"/>
+      <c r="E71" s="5"/>
+    </row>
+    <row r="72" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B72" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C72" s="7"/>
+      <c r="D72" s="7"/>
+      <c r="E72" s="8"/>
+      <c r="F72" t="s">
+        <v>20</v>
+      </c>
+      <c r="G72" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Create the routing table in the router, and add some routes
</commit_message>
<xml_diff>
--- a/me/2.routing.xlsx
+++ b/me/2.routing.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\build-php-mvc-framework\me\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2786820C-A4E4-4ED0-94D9-F9419649F89C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92C31426-A54B-44B3-B786-328F997C0922}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="central entry point" sheetId="1" r:id="rId1"/>
     <sheet name="Configure URLs" sheetId="2" r:id="rId2"/>
     <sheet name="CreateAndRequireRouterClass" sheetId="3" r:id="rId3"/>
+    <sheet name="routing table in the router" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="106">
   <si>
     <t>Create a central entry point to the framework: the front controller</t>
   </si>
@@ -334,6 +335,117 @@
   </si>
   <si>
     <t>Router là thành phần sẽ lấy request url hay route và từ đó đưa ra xử lý, nó là central part of framework</t>
+  </si>
+  <si>
+    <t>Create the routing table in the router, and add some routes</t>
+  </si>
+  <si>
+    <t>router có nhiệm vụ đưa ra quyết định controller và action nào được thực thi dựa vào route đến từ URL</t>
+  </si>
+  <si>
+    <t>Để làm được điều này thì router có 1 bảng để match các route(lấy được từ URL) đến controller và action và nó được gọi là routing table</t>
+  </si>
+  <si>
+    <t>Mỗi 1 route lấy được từ URL sẽ tương ứng với 1 controller và 1 action bên trong controller đó. Ở đây thì mình ko match route lấy được từ URL đến 1 PHP script cụ thể nào đó mà nó trỏ đến Controller</t>
+  </si>
+  <si>
+    <t>và action trong controller đó</t>
+  </si>
+  <si>
+    <t>    /**</t>
+  </si>
+  <si>
+    <t>     * Associative array of routes (the routing table)</t>
+  </si>
+  <si>
+    <t>     * @var array</t>
+  </si>
+  <si>
+    <t>     */</t>
+  </si>
+  <si>
+    <t>    protected $routes = [];</t>
+  </si>
+  <si>
+    <t>     * Add a route to the routing table</t>
+  </si>
+  <si>
+    <t>     *</t>
+  </si>
+  <si>
+    <t>     * @param string $route  The route URL</t>
+  </si>
+  <si>
+    <t>     * @param array  $params Parameters (controller, action, etc.)</t>
+  </si>
+  <si>
+    <t>     * @return void</t>
+  </si>
+  <si>
+    <t>    public function add($route, $params)</t>
+  </si>
+  <si>
+    <t>    {</t>
+  </si>
+  <si>
+    <t>        $this-&gt;routes[$route] = $params;</t>
+  </si>
+  <si>
+    <t>    }</t>
+  </si>
+  <si>
+    <t>     * Get all the routes from the routing table</t>
+  </si>
+  <si>
+    <t>     * @return array</t>
+  </si>
+  <si>
+    <t>    public function getRoutes()</t>
+  </si>
+  <si>
+    <t>        return $this-&gt;routes;</t>
+  </si>
+  <si>
+    <t>// Add the routes</t>
+  </si>
+  <si>
+    <t>$router-&gt;add('', ['controller' =&gt; 'Home', 'action' =&gt; 'index']);</t>
+  </si>
+  <si>
+    <t>$router-&gt;add('posts', ['controller' =&gt; 'Posts', 'action' =&gt; 'index']);</t>
+  </si>
+  <si>
+    <t>$router-&gt;add('posts/new', ['controller' =&gt; 'Posts', 'action' =&gt; 'new']);</t>
+  </si>
+  <si>
+    <t>// Display the routing table</t>
+  </si>
+  <si>
+    <t>echo '&lt;pre&gt;';</t>
+  </si>
+  <si>
+    <t>var_dump($router-&gt;getRoutes());</t>
+  </si>
+  <si>
+    <t>echo '&lt;/pre&gt;';</t>
+  </si>
+  <si>
+    <t>Đóng vai trò là routing table</t>
+  </si>
+  <si>
+    <t>Add route vào trong routing table</t>
+  </si>
+  <si>
+    <t>params chứa thông tin controller và action</t>
+  </si>
+  <si>
+    <t>Xem thông tin bên trong routing table</t>
+  </si>
+  <si>
+    <t>Home page</t>
+  </si>
+  <si>
+    <t>Check routing table</t>
   </si>
 </sst>
 </file>
@@ -462,7 +574,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -477,17 +589,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2000,6 +2105,611 @@
         <a:xfrm>
           <a:off x="695325" y="17249775"/>
           <a:ext cx="6723809" cy="1380952"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>66676</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>95251</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>352426</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>22129</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D22A81A8-F412-0BA4-CBE8-3A6987C3AF62}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="676276" y="1047751"/>
+          <a:ext cx="11258550" cy="4117878"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>313000</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>85275</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{33606A27-AA67-A40B-79FD-C6376A3E2162}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="685800" y="6391275"/>
+          <a:ext cx="10600000" cy="3600000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="Straight Arrow Connector 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BDC25835-6B8E-194D-8ACE-B7873185EA92}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="1657350" y="5867400"/>
+          <a:ext cx="2324100" cy="923925"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="7" name="Straight Arrow Connector 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{11F0D180-B9DE-B8D7-D670-763964D9BF61}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="5038725" y="5886450"/>
+          <a:ext cx="428625" cy="847725"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="9" name="Straight Arrow Connector 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00BB63DF-DAB8-0BAF-32DB-D7B589B4EDAF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5476875" y="5895975"/>
+          <a:ext cx="2447925" cy="895350"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>93</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>94</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="15" name="Straight Arrow Connector 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{50A736B8-D26D-EE26-9A47-F7E0B8CBA37F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2886075" y="17878425"/>
+          <a:ext cx="2019300" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>93</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>125</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="17" name="Straight Arrow Connector 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B486DAFC-658C-3DC8-FD40-C1961A3E1396}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="1219200" y="17887950"/>
+          <a:ext cx="514350" cy="6010275"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>93</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="21" name="Straight Arrow Connector 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A77668C8-C25D-7046-C80E-75AABF5A9307}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1428750" y="6924675"/>
+          <a:ext cx="666750" cy="10896600"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>125</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="27" name="Straight Arrow Connector 26">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{65D47E2E-FC5E-9519-DB39-14069146555D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="1914525" y="6953250"/>
+          <a:ext cx="2962275" cy="16973550"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>125</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="34" name="Straight Arrow Connector 33">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2108DAAD-9E6B-6343-036E-3913D37BC01F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="3076575" y="6962775"/>
+          <a:ext cx="4867275" cy="16954500"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>137</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>351936</xdr:colOff>
+      <xdr:row>159</xdr:row>
+      <xdr:rowOff>28057</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="40" name="Picture 39">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8C331B69-171D-FAF4-A5F8-5D2EF59B2A76}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="704850" y="26174700"/>
+          <a:ext cx="3914286" cy="4142857"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>110</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>417569</xdr:colOff>
+      <xdr:row>132</xdr:row>
+      <xdr:rowOff>161398</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="41" name="Picture 40">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D1199145-E011-F5D5-6B23-D637A5831878}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6457950" y="21088350"/>
+          <a:ext cx="12247619" cy="4219048"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3309,8 +4019,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9976F058-B1B7-4D54-8A36-C2B299C50638}">
   <dimension ref="A2:T91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="P71" sqref="P71"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32:F44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3355,485 +4065,94 @@
     </row>
     <row r="6" spans="2:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="4"/>
-      <c r="C6" s="24"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="24"/>
-      <c r="H6" s="24"/>
-      <c r="I6" s="24"/>
-      <c r="J6" s="24"/>
-      <c r="K6" s="24"/>
-      <c r="L6" s="24"/>
-      <c r="M6" s="24"/>
-      <c r="N6" s="24"/>
-      <c r="O6" s="24"/>
-      <c r="P6" s="24"/>
-      <c r="Q6" s="24"/>
-      <c r="R6" s="24"/>
-      <c r="S6" s="24"/>
       <c r="T6" s="5"/>
     </row>
     <row r="7" spans="2:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="4"/>
-      <c r="C7" s="24"/>
-      <c r="D7" s="24"/>
-      <c r="E7" s="24"/>
-      <c r="F7" s="24"/>
-      <c r="G7" s="24"/>
-      <c r="H7" s="24"/>
-      <c r="I7" s="24"/>
-      <c r="J7" s="24"/>
-      <c r="K7" s="24"/>
-      <c r="L7" s="24"/>
-      <c r="M7" s="24"/>
-      <c r="N7" s="24"/>
-      <c r="O7" s="24"/>
-      <c r="P7" s="24"/>
-      <c r="Q7" s="24"/>
-      <c r="R7" s="24"/>
-      <c r="S7" s="24"/>
       <c r="T7" s="5"/>
     </row>
     <row r="8" spans="2:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="4"/>
-      <c r="C8" s="24"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="24"/>
-      <c r="F8" s="24"/>
-      <c r="G8" s="24"/>
-      <c r="H8" s="24"/>
-      <c r="I8" s="24"/>
-      <c r="J8" s="24"/>
-      <c r="K8" s="24"/>
-      <c r="L8" s="24"/>
-      <c r="M8" s="24"/>
-      <c r="N8" s="24"/>
-      <c r="O8" s="24"/>
-      <c r="P8" s="24"/>
-      <c r="Q8" s="24"/>
-      <c r="R8" s="24"/>
-      <c r="S8" s="24"/>
       <c r="T8" s="5"/>
     </row>
     <row r="9" spans="2:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="4"/>
-      <c r="C9" s="24"/>
-      <c r="D9" s="24"/>
-      <c r="E9" s="24"/>
-      <c r="F9" s="24"/>
-      <c r="G9" s="24"/>
-      <c r="H9" s="24"/>
-      <c r="I9" s="24"/>
-      <c r="J9" s="24"/>
-      <c r="K9" s="24"/>
-      <c r="L9" s="24"/>
-      <c r="M9" s="24"/>
-      <c r="N9" s="24"/>
-      <c r="O9" s="24"/>
-      <c r="P9" s="24"/>
-      <c r="Q9" s="24"/>
-      <c r="R9" s="24"/>
-      <c r="S9" s="24"/>
       <c r="T9" s="5"/>
     </row>
     <row r="10" spans="2:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="4"/>
-      <c r="C10" s="24"/>
-      <c r="D10" s="24"/>
-      <c r="E10" s="24"/>
-      <c r="F10" s="24"/>
-      <c r="G10" s="24"/>
-      <c r="H10" s="24"/>
-      <c r="I10" s="24"/>
-      <c r="J10" s="24"/>
-      <c r="K10" s="24"/>
-      <c r="L10" s="24"/>
-      <c r="M10" s="24"/>
-      <c r="N10" s="24"/>
-      <c r="O10" s="24"/>
-      <c r="P10" s="24"/>
-      <c r="Q10" s="24"/>
-      <c r="R10" s="24"/>
-      <c r="S10" s="24"/>
       <c r="T10" s="5"/>
     </row>
     <row r="11" spans="2:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="4"/>
-      <c r="C11" s="24"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="24"/>
-      <c r="G11" s="24"/>
-      <c r="H11" s="24"/>
-      <c r="I11" s="24"/>
-      <c r="J11" s="24"/>
-      <c r="K11" s="24"/>
-      <c r="L11" s="24"/>
-      <c r="M11" s="24"/>
-      <c r="N11" s="24"/>
-      <c r="O11" s="24"/>
-      <c r="P11" s="24"/>
-      <c r="Q11" s="24"/>
-      <c r="R11" s="24"/>
-      <c r="S11" s="24"/>
       <c r="T11" s="5"/>
     </row>
     <row r="12" spans="2:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="4"/>
-      <c r="C12" s="24"/>
-      <c r="D12" s="24"/>
-      <c r="E12" s="24"/>
-      <c r="F12" s="24"/>
-      <c r="G12" s="24"/>
-      <c r="H12" s="24"/>
-      <c r="I12" s="24"/>
-      <c r="J12" s="24"/>
-      <c r="K12" s="24"/>
-      <c r="L12" s="24"/>
-      <c r="M12" s="24"/>
-      <c r="N12" s="24"/>
-      <c r="O12" s="24"/>
-      <c r="P12" s="24"/>
-      <c r="Q12" s="24"/>
-      <c r="R12" s="24"/>
-      <c r="S12" s="24"/>
       <c r="T12" s="5"/>
     </row>
     <row r="13" spans="2:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="4"/>
-      <c r="C13" s="24"/>
-      <c r="D13" s="24"/>
-      <c r="E13" s="24"/>
-      <c r="F13" s="24"/>
-      <c r="G13" s="24"/>
-      <c r="H13" s="24"/>
-      <c r="I13" s="24"/>
-      <c r="J13" s="24"/>
-      <c r="K13" s="24"/>
-      <c r="L13" s="24"/>
-      <c r="M13" s="24"/>
-      <c r="N13" s="24"/>
-      <c r="O13" s="24"/>
-      <c r="P13" s="24"/>
-      <c r="Q13" s="24"/>
-      <c r="R13" s="24"/>
-      <c r="S13" s="24"/>
       <c r="T13" s="5"/>
     </row>
     <row r="14" spans="2:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="4"/>
-      <c r="C14" s="24"/>
-      <c r="D14" s="24"/>
-      <c r="E14" s="24"/>
-      <c r="F14" s="24"/>
-      <c r="G14" s="24"/>
-      <c r="H14" s="24"/>
-      <c r="I14" s="24"/>
-      <c r="J14" s="24"/>
-      <c r="K14" s="24"/>
-      <c r="L14" s="24"/>
-      <c r="M14" s="24"/>
-      <c r="N14" s="24"/>
-      <c r="O14" s="24"/>
-      <c r="P14" s="24"/>
-      <c r="Q14" s="24"/>
-      <c r="R14" s="24"/>
-      <c r="S14" s="24"/>
       <c r="T14" s="5"/>
     </row>
     <row r="15" spans="2:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="4"/>
-      <c r="C15" s="24"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="24"/>
-      <c r="F15" s="24"/>
-      <c r="G15" s="24"/>
-      <c r="H15" s="24"/>
-      <c r="I15" s="24"/>
-      <c r="J15" s="24"/>
-      <c r="K15" s="24"/>
-      <c r="L15" s="24"/>
-      <c r="M15" s="24"/>
-      <c r="N15" s="24"/>
-      <c r="O15" s="24"/>
-      <c r="P15" s="24"/>
-      <c r="Q15" s="24"/>
-      <c r="R15" s="24"/>
-      <c r="S15" s="24"/>
       <c r="T15" s="5"/>
     </row>
     <row r="16" spans="2:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="4"/>
-      <c r="C16" s="24"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="24"/>
-      <c r="F16" s="24"/>
-      <c r="G16" s="24"/>
-      <c r="H16" s="24"/>
-      <c r="I16" s="24"/>
-      <c r="J16" s="24"/>
-      <c r="K16" s="24"/>
-      <c r="L16" s="24"/>
-      <c r="M16" s="24"/>
-      <c r="N16" s="24"/>
-      <c r="O16" s="24"/>
-      <c r="P16" s="24"/>
-      <c r="Q16" s="24"/>
-      <c r="R16" s="24"/>
-      <c r="S16" s="24"/>
       <c r="T16" s="5"/>
     </row>
     <row r="17" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="4"/>
-      <c r="C17" s="24"/>
-      <c r="D17" s="24"/>
-      <c r="E17" s="24"/>
-      <c r="F17" s="24"/>
-      <c r="G17" s="24"/>
-      <c r="H17" s="24"/>
-      <c r="I17" s="24"/>
-      <c r="J17" s="24"/>
-      <c r="K17" s="24"/>
-      <c r="L17" s="24"/>
-      <c r="M17" s="24"/>
-      <c r="N17" s="24"/>
-      <c r="O17" s="24"/>
-      <c r="P17" s="24"/>
-      <c r="Q17" s="24"/>
-      <c r="R17" s="24"/>
-      <c r="S17" s="24"/>
       <c r="T17" s="5"/>
     </row>
     <row r="18" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="4"/>
-      <c r="C18" s="24"/>
-      <c r="D18" s="24"/>
-      <c r="E18" s="24"/>
-      <c r="F18" s="24"/>
-      <c r="G18" s="24"/>
-      <c r="H18" s="24"/>
-      <c r="I18" s="24"/>
-      <c r="J18" s="24"/>
-      <c r="K18" s="24"/>
-      <c r="L18" s="24"/>
-      <c r="M18" s="24"/>
-      <c r="N18" s="24"/>
-      <c r="O18" s="24"/>
-      <c r="P18" s="24"/>
-      <c r="Q18" s="24"/>
-      <c r="R18" s="24"/>
-      <c r="S18" s="24"/>
       <c r="T18" s="5"/>
     </row>
     <row r="19" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="4"/>
-      <c r="C19" s="24"/>
-      <c r="D19" s="24"/>
-      <c r="E19" s="24"/>
-      <c r="F19" s="24"/>
-      <c r="G19" s="24"/>
-      <c r="H19" s="24"/>
-      <c r="I19" s="24"/>
-      <c r="J19" s="24"/>
-      <c r="K19" s="24"/>
-      <c r="L19" s="24"/>
-      <c r="M19" s="24"/>
-      <c r="N19" s="24"/>
-      <c r="O19" s="24"/>
-      <c r="P19" s="24"/>
-      <c r="Q19" s="24"/>
-      <c r="R19" s="24"/>
-      <c r="S19" s="24"/>
       <c r="T19" s="5"/>
     </row>
     <row r="20" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="4"/>
-      <c r="C20" s="24"/>
-      <c r="D20" s="24"/>
-      <c r="E20" s="24"/>
-      <c r="F20" s="24"/>
-      <c r="G20" s="24"/>
-      <c r="H20" s="24"/>
-      <c r="I20" s="24"/>
-      <c r="J20" s="24"/>
-      <c r="K20" s="24"/>
-      <c r="L20" s="24"/>
-      <c r="M20" s="24"/>
-      <c r="N20" s="24"/>
-      <c r="O20" s="24"/>
-      <c r="P20" s="24"/>
-      <c r="Q20" s="24"/>
-      <c r="R20" s="24"/>
-      <c r="S20" s="24"/>
       <c r="T20" s="5"/>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B21" s="4"/>
-      <c r="C21" s="24"/>
-      <c r="D21" s="24"/>
-      <c r="E21" s="24"/>
-      <c r="F21" s="24"/>
-      <c r="G21" s="24"/>
-      <c r="H21" s="24"/>
-      <c r="I21" s="24"/>
-      <c r="J21" s="24"/>
-      <c r="K21" s="24"/>
-      <c r="L21" s="24"/>
-      <c r="M21" s="24"/>
-      <c r="N21" s="24"/>
-      <c r="O21" s="24"/>
-      <c r="P21" s="24"/>
-      <c r="Q21" s="24"/>
-      <c r="R21" s="24"/>
-      <c r="S21" s="24"/>
       <c r="T21" s="5"/>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B22" s="4"/>
-      <c r="C22" s="24"/>
-      <c r="D22" s="24"/>
-      <c r="E22" s="24"/>
-      <c r="F22" s="24"/>
-      <c r="G22" s="24"/>
-      <c r="H22" s="24"/>
-      <c r="I22" s="24"/>
-      <c r="J22" s="24"/>
-      <c r="K22" s="24"/>
-      <c r="L22" s="24"/>
-      <c r="M22" s="24"/>
-      <c r="N22" s="24"/>
-      <c r="O22" s="24"/>
-      <c r="P22" s="24"/>
-      <c r="Q22" s="24"/>
-      <c r="R22" s="24"/>
-      <c r="S22" s="24"/>
       <c r="T22" s="5"/>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B23" s="4"/>
-      <c r="C23" s="24"/>
-      <c r="D23" s="24"/>
-      <c r="E23" s="24"/>
-      <c r="F23" s="24"/>
-      <c r="G23" s="24"/>
-      <c r="H23" s="24"/>
-      <c r="I23" s="24"/>
-      <c r="J23" s="24"/>
-      <c r="K23" s="24"/>
-      <c r="L23" s="24"/>
-      <c r="M23" s="24"/>
-      <c r="N23" s="24"/>
-      <c r="O23" s="24"/>
-      <c r="P23" s="24"/>
-      <c r="Q23" s="24"/>
-      <c r="R23" s="24"/>
-      <c r="S23" s="24"/>
       <c r="T23" s="5"/>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B24" s="4"/>
-      <c r="C24" s="24"/>
-      <c r="D24" s="24"/>
-      <c r="E24" s="24"/>
-      <c r="F24" s="24"/>
-      <c r="G24" s="24"/>
-      <c r="H24" s="24"/>
-      <c r="I24" s="24"/>
-      <c r="J24" s="24"/>
-      <c r="K24" s="24"/>
-      <c r="L24" s="24"/>
-      <c r="M24" s="24"/>
-      <c r="N24" s="24"/>
-      <c r="O24" s="24"/>
-      <c r="P24" s="24"/>
-      <c r="Q24" s="24"/>
-      <c r="R24" s="24"/>
-      <c r="S24" s="24"/>
       <c r="T24" s="5"/>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B25" s="4"/>
-      <c r="C25" s="24"/>
-      <c r="D25" s="24"/>
-      <c r="E25" s="24"/>
-      <c r="F25" s="24"/>
-      <c r="G25" s="24"/>
-      <c r="H25" s="24"/>
-      <c r="I25" s="24"/>
-      <c r="J25" s="24"/>
-      <c r="K25" s="24"/>
-      <c r="L25" s="24"/>
-      <c r="M25" s="24"/>
-      <c r="N25" s="24"/>
-      <c r="O25" s="24"/>
-      <c r="P25" s="24"/>
-      <c r="Q25" s="24"/>
-      <c r="R25" s="24"/>
-      <c r="S25" s="24"/>
       <c r="T25" s="5"/>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B26" s="4"/>
-      <c r="C26" s="24"/>
-      <c r="D26" s="24"/>
-      <c r="E26" s="24"/>
-      <c r="F26" s="24"/>
-      <c r="G26" s="24"/>
-      <c r="H26" s="24"/>
-      <c r="I26" s="24"/>
-      <c r="J26" s="24"/>
-      <c r="K26" s="24"/>
-      <c r="L26" s="24"/>
-      <c r="M26" s="24"/>
-      <c r="N26" s="24"/>
-      <c r="O26" s="24"/>
-      <c r="P26" s="24"/>
-      <c r="Q26" s="24"/>
-      <c r="R26" s="24"/>
-      <c r="S26" s="24"/>
       <c r="T26" s="5"/>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B27" s="4"/>
-      <c r="C27" s="24"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="24"/>
-      <c r="F27" s="24"/>
-      <c r="G27" s="24"/>
-      <c r="H27" s="24"/>
-      <c r="I27" s="24"/>
-      <c r="J27" s="24"/>
-      <c r="K27" s="24"/>
-      <c r="L27" s="24"/>
-      <c r="M27" s="24"/>
-      <c r="N27" s="24"/>
-      <c r="O27" s="24"/>
-      <c r="P27" s="24"/>
-      <c r="Q27" s="24"/>
-      <c r="R27" s="24"/>
-      <c r="S27" s="24"/>
       <c r="T27" s="5"/>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B28" s="4"/>
-      <c r="C28" s="24"/>
-      <c r="D28" s="24"/>
-      <c r="E28" s="24"/>
-      <c r="F28" s="24"/>
-      <c r="G28" s="24"/>
-      <c r="H28" s="24"/>
-      <c r="I28" s="24"/>
-      <c r="J28" s="24"/>
-      <c r="K28" s="24"/>
-      <c r="L28" s="24"/>
-      <c r="M28" s="24"/>
-      <c r="N28" s="24"/>
-      <c r="O28" s="24"/>
-      <c r="P28" s="24"/>
-      <c r="Q28" s="24"/>
-      <c r="R28" s="24"/>
-      <c r="S28" s="24"/>
       <c r="T28" s="5"/>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.25">
@@ -3858,84 +4177,60 @@
       <c r="T29" s="8"/>
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A32" s="14" t="s">
+      <c r="A32" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B32" s="15"/>
-      <c r="C32" s="15"/>
-      <c r="D32" s="15"/>
-      <c r="E32" s="15"/>
-      <c r="F32" s="15"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="15"/>
-      <c r="B33" s="16" t="s">
+      <c r="B33" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C33" s="17"/>
-      <c r="D33" s="17"/>
-      <c r="E33" s="17"/>
-      <c r="F33" s="18"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="3"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="15"/>
-      <c r="B34" s="19"/>
-      <c r="C34" s="15" t="s">
+      <c r="B34" s="4"/>
+      <c r="C34" t="s">
         <v>10</v>
       </c>
-      <c r="D34" s="15"/>
-      <c r="E34" s="15"/>
-      <c r="F34" s="20"/>
+      <c r="F34" s="5"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="15"/>
-      <c r="B35" s="19"/>
-      <c r="C35" s="15"/>
-      <c r="D35" s="15" t="s">
+      <c r="B35" s="4"/>
+      <c r="D35" t="s">
         <v>11</v>
       </c>
-      <c r="E35" s="15"/>
-      <c r="F35" s="20"/>
+      <c r="F35" s="5"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="15"/>
-      <c r="B36" s="19"/>
-      <c r="C36" s="15"/>
-      <c r="D36" s="15" t="s">
+      <c r="B36" s="4"/>
+      <c r="D36" t="s">
         <v>12</v>
       </c>
-      <c r="E36" s="15"/>
-      <c r="F36" s="20"/>
+      <c r="F36" s="5"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="15"/>
-      <c r="B37" s="19"/>
-      <c r="C37" s="15"/>
-      <c r="D37" s="15" t="s">
+      <c r="B37" s="4"/>
+      <c r="D37" t="s">
         <v>13</v>
       </c>
-      <c r="E37" s="15"/>
-      <c r="F37" s="20"/>
+      <c r="F37" s="5"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="15"/>
-      <c r="B38" s="19"/>
-      <c r="C38" s="15" t="s">
+      <c r="B38" s="4"/>
+      <c r="C38" t="s">
         <v>14</v>
       </c>
-      <c r="D38" s="15"/>
-      <c r="E38" s="15"/>
-      <c r="F38" s="20"/>
+      <c r="F38" s="5"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="15"/>
-      <c r="B39" s="19"/>
-      <c r="C39" s="15"/>
+      <c r="B39" s="4"/>
       <c r="D39" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="E39" s="15"/>
-      <c r="F39" s="20"/>
+      <c r="F39" s="5"/>
       <c r="G39" t="s">
         <v>20</v>
       </c>
@@ -3944,44 +4239,32 @@
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="15"/>
-      <c r="B40" s="19"/>
-      <c r="C40" s="15" t="s">
+      <c r="B40" s="4"/>
+      <c r="C40" t="s">
         <v>15</v>
       </c>
-      <c r="D40" s="15"/>
-      <c r="E40" s="15"/>
-      <c r="F40" s="20"/>
+      <c r="F40" s="5"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="15"/>
-      <c r="B41" s="19"/>
-      <c r="C41" s="15" t="s">
+      <c r="B41" s="4"/>
+      <c r="C41" t="s">
         <v>16</v>
       </c>
-      <c r="D41" s="15"/>
-      <c r="E41" s="15"/>
-      <c r="F41" s="20"/>
+      <c r="F41" s="5"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="15"/>
-      <c r="B42" s="19"/>
-      <c r="C42" s="15"/>
-      <c r="D42" s="15" t="s">
+      <c r="B42" s="4"/>
+      <c r="D42" t="s">
         <v>26</v>
       </c>
-      <c r="E42" s="15"/>
-      <c r="F42" s="20"/>
+      <c r="F42" s="5"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" s="15"/>
-      <c r="B43" s="19"/>
-      <c r="C43" s="15"/>
+      <c r="B43" s="4"/>
       <c r="D43" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="E43" s="15"/>
-      <c r="F43" s="20"/>
+      <c r="F43" s="5"/>
       <c r="G43" t="s">
         <v>20</v>
       </c>
@@ -3990,14 +4273,13 @@
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" s="15"/>
-      <c r="B44" s="21"/>
-      <c r="C44" s="22" t="s">
+      <c r="B44" s="6"/>
+      <c r="C44" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D44" s="22"/>
-      <c r="E44" s="22"/>
-      <c r="F44" s="23"/>
+      <c r="D44" s="7"/>
+      <c r="E44" s="7"/>
+      <c r="F44" s="8"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
@@ -4013,35 +4295,30 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B49" s="4"/>
-      <c r="C49" s="24"/>
       <c r="D49" s="5"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B50" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C50" s="24"/>
       <c r="D50" s="5"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B51" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C51" s="24"/>
       <c r="D51" s="5"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B52" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C52" s="24"/>
       <c r="D52" s="5"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B53" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C53" s="24"/>
       <c r="D53" s="5"/>
       <c r="E53" t="s">
         <v>20</v>
@@ -4054,7 +4331,6 @@
       <c r="B54" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C54" s="24"/>
       <c r="D54" s="5"/>
       <c r="F54" t="s">
         <v>64</v>
@@ -4082,70 +4358,52 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B60" s="4"/>
-      <c r="C60" s="24"/>
-      <c r="D60" s="24"/>
       <c r="E60" s="5"/>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B61" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C61" s="24"/>
-      <c r="D61" s="24"/>
       <c r="E61" s="5"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B62" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C62" s="24"/>
-      <c r="D62" s="24"/>
       <c r="E62" s="5"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B63" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C63" s="24"/>
-      <c r="D63" s="24"/>
       <c r="E63" s="5"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B64" s="4"/>
-      <c r="C64" s="24"/>
-      <c r="D64" s="24"/>
       <c r="E64" s="5"/>
     </row>
     <row r="65" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B65" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C65" s="24"/>
-      <c r="D65" s="24"/>
       <c r="E65" s="5"/>
     </row>
     <row r="66" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B66" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="C66" s="24"/>
-      <c r="D66" s="24"/>
       <c r="E66" s="5"/>
     </row>
     <row r="67" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B67" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C67" s="24"/>
-      <c r="D67" s="24"/>
       <c r="E67" s="5"/>
     </row>
     <row r="68" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B68" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C68" s="24"/>
-      <c r="D68" s="24"/>
       <c r="E68" s="5"/>
       <c r="F68" t="s">
         <v>20</v>
@@ -4156,22 +4414,16 @@
     </row>
     <row r="69" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B69" s="4"/>
-      <c r="C69" s="24"/>
-      <c r="D69" s="24"/>
       <c r="E69" s="5"/>
     </row>
     <row r="70" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B70" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="C70" s="24"/>
-      <c r="D70" s="24"/>
       <c r="E70" s="5"/>
     </row>
     <row r="71" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B71" s="4"/>
-      <c r="C71" s="24"/>
-      <c r="D71" s="24"/>
       <c r="E71" s="5"/>
     </row>
     <row r="72" spans="2:7" x14ac:dyDescent="0.25">
@@ -4197,4 +4449,2048 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3C2F33E-AFC9-4549-979A-DBAB82CF5E66}">
+  <dimension ref="A2:T160"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
+      <selection activeCell="L142" sqref="L142"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="2"/>
+      <c r="R5" s="2"/>
+      <c r="S5" s="2"/>
+      <c r="T5" s="3"/>
+    </row>
+    <row r="6" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B6" s="4"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="14"/>
+      <c r="M6" s="14"/>
+      <c r="N6" s="14"/>
+      <c r="O6" s="14"/>
+      <c r="P6" s="14"/>
+      <c r="Q6" s="14"/>
+      <c r="R6" s="14"/>
+      <c r="S6" s="14"/>
+      <c r="T6" s="5"/>
+    </row>
+    <row r="7" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B7" s="4"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="14"/>
+      <c r="L7" s="14"/>
+      <c r="M7" s="14"/>
+      <c r="N7" s="14"/>
+      <c r="O7" s="14"/>
+      <c r="P7" s="14"/>
+      <c r="Q7" s="14"/>
+      <c r="R7" s="14"/>
+      <c r="S7" s="14"/>
+      <c r="T7" s="5"/>
+    </row>
+    <row r="8" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B8" s="4"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="14"/>
+      <c r="L8" s="14"/>
+      <c r="M8" s="14"/>
+      <c r="N8" s="14"/>
+      <c r="O8" s="14"/>
+      <c r="P8" s="14"/>
+      <c r="Q8" s="14"/>
+      <c r="R8" s="14"/>
+      <c r="S8" s="14"/>
+      <c r="T8" s="5"/>
+    </row>
+    <row r="9" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B9" s="4"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="14"/>
+      <c r="L9" s="14"/>
+      <c r="M9" s="14"/>
+      <c r="N9" s="14"/>
+      <c r="O9" s="14"/>
+      <c r="P9" s="14"/>
+      <c r="Q9" s="14"/>
+      <c r="R9" s="14"/>
+      <c r="S9" s="14"/>
+      <c r="T9" s="5"/>
+    </row>
+    <row r="10" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B10" s="4"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="14"/>
+      <c r="K10" s="14"/>
+      <c r="L10" s="14"/>
+      <c r="M10" s="14"/>
+      <c r="N10" s="14"/>
+      <c r="O10" s="14"/>
+      <c r="P10" s="14"/>
+      <c r="Q10" s="14"/>
+      <c r="R10" s="14"/>
+      <c r="S10" s="14"/>
+      <c r="T10" s="5"/>
+    </row>
+    <row r="11" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B11" s="4"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="14"/>
+      <c r="K11" s="14"/>
+      <c r="L11" s="14"/>
+      <c r="M11" s="14"/>
+      <c r="N11" s="14"/>
+      <c r="O11" s="14"/>
+      <c r="P11" s="14"/>
+      <c r="Q11" s="14"/>
+      <c r="R11" s="14"/>
+      <c r="S11" s="14"/>
+      <c r="T11" s="5"/>
+    </row>
+    <row r="12" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B12" s="4"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="14"/>
+      <c r="K12" s="14"/>
+      <c r="L12" s="14"/>
+      <c r="M12" s="14"/>
+      <c r="N12" s="14"/>
+      <c r="O12" s="14"/>
+      <c r="P12" s="14"/>
+      <c r="Q12" s="14"/>
+      <c r="R12" s="14"/>
+      <c r="S12" s="14"/>
+      <c r="T12" s="5"/>
+    </row>
+    <row r="13" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B13" s="4"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="14"/>
+      <c r="K13" s="14"/>
+      <c r="L13" s="14"/>
+      <c r="M13" s="14"/>
+      <c r="N13" s="14"/>
+      <c r="O13" s="14"/>
+      <c r="P13" s="14"/>
+      <c r="Q13" s="14"/>
+      <c r="R13" s="14"/>
+      <c r="S13" s="14"/>
+      <c r="T13" s="5"/>
+    </row>
+    <row r="14" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B14" s="4"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="14"/>
+      <c r="K14" s="14"/>
+      <c r="L14" s="14"/>
+      <c r="M14" s="14"/>
+      <c r="N14" s="14"/>
+      <c r="O14" s="14"/>
+      <c r="P14" s="14"/>
+      <c r="Q14" s="14"/>
+      <c r="R14" s="14"/>
+      <c r="S14" s="14"/>
+      <c r="T14" s="5"/>
+    </row>
+    <row r="15" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B15" s="4"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
+      <c r="K15" s="14"/>
+      <c r="L15" s="14"/>
+      <c r="M15" s="14"/>
+      <c r="N15" s="14"/>
+      <c r="O15" s="14"/>
+      <c r="P15" s="14"/>
+      <c r="Q15" s="14"/>
+      <c r="R15" s="14"/>
+      <c r="S15" s="14"/>
+      <c r="T15" s="5"/>
+    </row>
+    <row r="16" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B16" s="4"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="14"/>
+      <c r="K16" s="14"/>
+      <c r="L16" s="14"/>
+      <c r="M16" s="14"/>
+      <c r="N16" s="14"/>
+      <c r="O16" s="14"/>
+      <c r="P16" s="14"/>
+      <c r="Q16" s="14"/>
+      <c r="R16" s="14"/>
+      <c r="S16" s="14"/>
+      <c r="T16" s="5"/>
+    </row>
+    <row r="17" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B17" s="4"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="14"/>
+      <c r="J17" s="14"/>
+      <c r="K17" s="14"/>
+      <c r="L17" s="14"/>
+      <c r="M17" s="14"/>
+      <c r="N17" s="14"/>
+      <c r="O17" s="14"/>
+      <c r="P17" s="14"/>
+      <c r="Q17" s="14"/>
+      <c r="R17" s="14"/>
+      <c r="S17" s="14"/>
+      <c r="T17" s="5"/>
+    </row>
+    <row r="18" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B18" s="4"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="14"/>
+      <c r="J18" s="14"/>
+      <c r="K18" s="14"/>
+      <c r="L18" s="14"/>
+      <c r="M18" s="14"/>
+      <c r="N18" s="14"/>
+      <c r="O18" s="14"/>
+      <c r="P18" s="14"/>
+      <c r="Q18" s="14"/>
+      <c r="R18" s="14"/>
+      <c r="S18" s="14"/>
+      <c r="T18" s="5"/>
+    </row>
+    <row r="19" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B19" s="4"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="14"/>
+      <c r="I19" s="14"/>
+      <c r="J19" s="14"/>
+      <c r="K19" s="14"/>
+      <c r="L19" s="14"/>
+      <c r="M19" s="14"/>
+      <c r="N19" s="14"/>
+      <c r="O19" s="14"/>
+      <c r="P19" s="14"/>
+      <c r="Q19" s="14"/>
+      <c r="R19" s="14"/>
+      <c r="S19" s="14"/>
+      <c r="T19" s="5"/>
+    </row>
+    <row r="20" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B20" s="4"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="14"/>
+      <c r="J20" s="14"/>
+      <c r="K20" s="14"/>
+      <c r="L20" s="14"/>
+      <c r="M20" s="14"/>
+      <c r="N20" s="14"/>
+      <c r="O20" s="14"/>
+      <c r="P20" s="14"/>
+      <c r="Q20" s="14"/>
+      <c r="R20" s="14"/>
+      <c r="S20" s="14"/>
+      <c r="T20" s="5"/>
+    </row>
+    <row r="21" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B21" s="4"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="14"/>
+      <c r="J21" s="14"/>
+      <c r="K21" s="14"/>
+      <c r="L21" s="14"/>
+      <c r="M21" s="14"/>
+      <c r="N21" s="14"/>
+      <c r="O21" s="14"/>
+      <c r="P21" s="14"/>
+      <c r="Q21" s="14"/>
+      <c r="R21" s="14"/>
+      <c r="S21" s="14"/>
+      <c r="T21" s="5"/>
+    </row>
+    <row r="22" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B22" s="4"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="14"/>
+      <c r="I22" s="14"/>
+      <c r="J22" s="14"/>
+      <c r="K22" s="14"/>
+      <c r="L22" s="14"/>
+      <c r="M22" s="14"/>
+      <c r="N22" s="14"/>
+      <c r="O22" s="14"/>
+      <c r="P22" s="14"/>
+      <c r="Q22" s="14"/>
+      <c r="R22" s="14"/>
+      <c r="S22" s="14"/>
+      <c r="T22" s="5"/>
+    </row>
+    <row r="23" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B23" s="4"/>
+      <c r="C23" s="14"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="14"/>
+      <c r="G23" s="14"/>
+      <c r="H23" s="14"/>
+      <c r="I23" s="14"/>
+      <c r="J23" s="14"/>
+      <c r="K23" s="14"/>
+      <c r="L23" s="14"/>
+      <c r="M23" s="14"/>
+      <c r="N23" s="14"/>
+      <c r="O23" s="14"/>
+      <c r="P23" s="14"/>
+      <c r="Q23" s="14"/>
+      <c r="R23" s="14"/>
+      <c r="S23" s="14"/>
+      <c r="T23" s="5"/>
+    </row>
+    <row r="24" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B24" s="4"/>
+      <c r="C24" s="14"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="14"/>
+      <c r="G24" s="14"/>
+      <c r="H24" s="14"/>
+      <c r="I24" s="14"/>
+      <c r="J24" s="14"/>
+      <c r="K24" s="14"/>
+      <c r="L24" s="14"/>
+      <c r="M24" s="14"/>
+      <c r="N24" s="14"/>
+      <c r="O24" s="14"/>
+      <c r="P24" s="14"/>
+      <c r="Q24" s="14"/>
+      <c r="R24" s="14"/>
+      <c r="S24" s="14"/>
+      <c r="T24" s="5"/>
+    </row>
+    <row r="25" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B25" s="4"/>
+      <c r="C25" s="14"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="14"/>
+      <c r="G25" s="14"/>
+      <c r="H25" s="14"/>
+      <c r="I25" s="14"/>
+      <c r="J25" s="14"/>
+      <c r="K25" s="14"/>
+      <c r="L25" s="14"/>
+      <c r="M25" s="14"/>
+      <c r="N25" s="14"/>
+      <c r="O25" s="14"/>
+      <c r="P25" s="14"/>
+      <c r="Q25" s="14"/>
+      <c r="R25" s="14"/>
+      <c r="S25" s="14"/>
+      <c r="T25" s="5"/>
+    </row>
+    <row r="26" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B26" s="4"/>
+      <c r="C26" s="14"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="14"/>
+      <c r="F26" s="14"/>
+      <c r="G26" s="14"/>
+      <c r="H26" s="14"/>
+      <c r="I26" s="14"/>
+      <c r="J26" s="14"/>
+      <c r="K26" s="14"/>
+      <c r="L26" s="14"/>
+      <c r="M26" s="14"/>
+      <c r="N26" s="14"/>
+      <c r="O26" s="14"/>
+      <c r="P26" s="14"/>
+      <c r="Q26" s="14"/>
+      <c r="R26" s="14"/>
+      <c r="S26" s="14"/>
+      <c r="T26" s="5"/>
+    </row>
+    <row r="27" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B27" s="4"/>
+      <c r="C27" s="14"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="14"/>
+      <c r="G27" s="14"/>
+      <c r="H27" s="14"/>
+      <c r="I27" s="14"/>
+      <c r="J27" s="14"/>
+      <c r="K27" s="14"/>
+      <c r="L27" s="14"/>
+      <c r="M27" s="14"/>
+      <c r="N27" s="14"/>
+      <c r="O27" s="14"/>
+      <c r="P27" s="14"/>
+      <c r="Q27" s="14"/>
+      <c r="R27" s="14"/>
+      <c r="S27" s="14"/>
+      <c r="T27" s="5"/>
+    </row>
+    <row r="28" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B28" s="6"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="7"/>
+      <c r="H28" s="7"/>
+      <c r="I28" s="7"/>
+      <c r="J28" s="7"/>
+      <c r="K28" s="7"/>
+      <c r="L28" s="7"/>
+      <c r="M28" s="7"/>
+      <c r="N28" s="7"/>
+      <c r="O28" s="7"/>
+      <c r="P28" s="7"/>
+      <c r="Q28" s="7"/>
+      <c r="R28" s="7"/>
+      <c r="S28" s="7"/>
+      <c r="T28" s="8"/>
+    </row>
+    <row r="31" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B31" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
+      <c r="I31" s="2"/>
+      <c r="J31" s="2"/>
+      <c r="K31" s="2"/>
+      <c r="L31" s="2"/>
+      <c r="M31" s="2"/>
+      <c r="N31" s="2"/>
+      <c r="O31" s="2"/>
+      <c r="P31" s="2"/>
+      <c r="Q31" s="2"/>
+      <c r="R31" s="2"/>
+      <c r="S31" s="2"/>
+      <c r="T31" s="3"/>
+    </row>
+    <row r="32" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B32" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C32" s="14"/>
+      <c r="D32" s="14"/>
+      <c r="E32" s="14"/>
+      <c r="F32" s="14"/>
+      <c r="G32" s="14"/>
+      <c r="H32" s="14"/>
+      <c r="I32" s="14"/>
+      <c r="J32" s="14"/>
+      <c r="K32" s="14"/>
+      <c r="L32" s="14"/>
+      <c r="M32" s="14"/>
+      <c r="N32" s="14"/>
+      <c r="O32" s="14"/>
+      <c r="P32" s="14"/>
+      <c r="Q32" s="14"/>
+      <c r="R32" s="14"/>
+      <c r="S32" s="14"/>
+      <c r="T32" s="5"/>
+    </row>
+    <row r="33" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B33" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C33" s="14"/>
+      <c r="D33" s="14"/>
+      <c r="E33" s="14"/>
+      <c r="F33" s="14"/>
+      <c r="G33" s="14"/>
+      <c r="H33" s="14"/>
+      <c r="I33" s="14"/>
+      <c r="J33" s="14"/>
+      <c r="K33" s="14"/>
+      <c r="L33" s="14"/>
+      <c r="M33" s="14"/>
+      <c r="N33" s="14"/>
+      <c r="O33" s="14"/>
+      <c r="P33" s="14"/>
+      <c r="Q33" s="14"/>
+      <c r="R33" s="14"/>
+      <c r="S33" s="14"/>
+      <c r="T33" s="5"/>
+    </row>
+    <row r="34" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B34" s="4"/>
+      <c r="C34" s="14"/>
+      <c r="D34" s="14"/>
+      <c r="E34" s="14"/>
+      <c r="F34" s="14"/>
+      <c r="G34" s="14"/>
+      <c r="H34" s="14"/>
+      <c r="I34" s="14"/>
+      <c r="J34" s="14"/>
+      <c r="K34" s="14"/>
+      <c r="L34" s="14"/>
+      <c r="M34" s="14"/>
+      <c r="N34" s="14"/>
+      <c r="O34" s="14"/>
+      <c r="P34" s="14"/>
+      <c r="Q34" s="14"/>
+      <c r="R34" s="14"/>
+      <c r="S34" s="14"/>
+      <c r="T34" s="5"/>
+    </row>
+    <row r="35" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B35" s="4"/>
+      <c r="C35" s="14"/>
+      <c r="D35" s="14"/>
+      <c r="E35" s="14"/>
+      <c r="F35" s="14"/>
+      <c r="G35" s="14"/>
+      <c r="H35" s="14"/>
+      <c r="I35" s="14"/>
+      <c r="J35" s="14"/>
+      <c r="K35" s="14"/>
+      <c r="L35" s="14"/>
+      <c r="M35" s="14"/>
+      <c r="N35" s="14"/>
+      <c r="O35" s="14"/>
+      <c r="P35" s="14"/>
+      <c r="Q35" s="14"/>
+      <c r="R35" s="14"/>
+      <c r="S35" s="14"/>
+      <c r="T35" s="5"/>
+    </row>
+    <row r="36" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B36" s="4"/>
+      <c r="C36" s="14"/>
+      <c r="D36" s="14"/>
+      <c r="E36" s="14"/>
+      <c r="F36" s="14"/>
+      <c r="G36" s="14"/>
+      <c r="H36" s="14"/>
+      <c r="I36" s="14"/>
+      <c r="J36" s="14"/>
+      <c r="K36" s="14"/>
+      <c r="L36" s="14"/>
+      <c r="M36" s="14"/>
+      <c r="N36" s="14"/>
+      <c r="O36" s="14"/>
+      <c r="P36" s="14"/>
+      <c r="Q36" s="14"/>
+      <c r="R36" s="14"/>
+      <c r="S36" s="14"/>
+      <c r="T36" s="5"/>
+    </row>
+    <row r="37" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B37" s="4"/>
+      <c r="C37" s="14"/>
+      <c r="D37" s="14"/>
+      <c r="E37" s="14"/>
+      <c r="F37" s="14"/>
+      <c r="G37" s="14"/>
+      <c r="H37" s="14"/>
+      <c r="I37" s="14"/>
+      <c r="J37" s="14"/>
+      <c r="K37" s="14"/>
+      <c r="L37" s="14"/>
+      <c r="M37" s="14"/>
+      <c r="N37" s="14"/>
+      <c r="O37" s="14"/>
+      <c r="P37" s="14"/>
+      <c r="Q37" s="14"/>
+      <c r="R37" s="14"/>
+      <c r="S37" s="14"/>
+      <c r="T37" s="5"/>
+    </row>
+    <row r="38" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B38" s="4"/>
+      <c r="C38" s="14"/>
+      <c r="D38" s="14"/>
+      <c r="E38" s="14"/>
+      <c r="F38" s="14"/>
+      <c r="G38" s="14"/>
+      <c r="H38" s="14"/>
+      <c r="I38" s="14"/>
+      <c r="J38" s="14"/>
+      <c r="K38" s="14"/>
+      <c r="L38" s="14"/>
+      <c r="M38" s="14"/>
+      <c r="N38" s="14"/>
+      <c r="O38" s="14"/>
+      <c r="P38" s="14"/>
+      <c r="Q38" s="14"/>
+      <c r="R38" s="14"/>
+      <c r="S38" s="14"/>
+      <c r="T38" s="5"/>
+    </row>
+    <row r="39" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B39" s="4"/>
+      <c r="C39" s="14"/>
+      <c r="D39" s="14"/>
+      <c r="E39" s="14"/>
+      <c r="F39" s="14"/>
+      <c r="G39" s="14"/>
+      <c r="H39" s="14"/>
+      <c r="I39" s="14"/>
+      <c r="J39" s="14"/>
+      <c r="K39" s="14"/>
+      <c r="L39" s="14"/>
+      <c r="M39" s="14"/>
+      <c r="N39" s="14"/>
+      <c r="O39" s="14"/>
+      <c r="P39" s="14"/>
+      <c r="Q39" s="14"/>
+      <c r="R39" s="14"/>
+      <c r="S39" s="14"/>
+      <c r="T39" s="5"/>
+    </row>
+    <row r="40" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B40" s="4"/>
+      <c r="C40" s="14"/>
+      <c r="D40" s="14"/>
+      <c r="E40" s="14"/>
+      <c r="F40" s="14"/>
+      <c r="G40" s="14"/>
+      <c r="H40" s="14"/>
+      <c r="I40" s="14"/>
+      <c r="J40" s="14"/>
+      <c r="K40" s="14"/>
+      <c r="L40" s="14"/>
+      <c r="M40" s="14"/>
+      <c r="N40" s="14"/>
+      <c r="O40" s="14"/>
+      <c r="P40" s="14"/>
+      <c r="Q40" s="14"/>
+      <c r="R40" s="14"/>
+      <c r="S40" s="14"/>
+      <c r="T40" s="5"/>
+    </row>
+    <row r="41" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B41" s="4"/>
+      <c r="C41" s="14"/>
+      <c r="D41" s="14"/>
+      <c r="E41" s="14"/>
+      <c r="F41" s="14"/>
+      <c r="G41" s="14"/>
+      <c r="H41" s="14"/>
+      <c r="I41" s="14"/>
+      <c r="J41" s="14"/>
+      <c r="K41" s="14"/>
+      <c r="L41" s="14"/>
+      <c r="M41" s="14"/>
+      <c r="N41" s="14"/>
+      <c r="O41" s="14"/>
+      <c r="P41" s="14"/>
+      <c r="Q41" s="14"/>
+      <c r="R41" s="14"/>
+      <c r="S41" s="14"/>
+      <c r="T41" s="5"/>
+    </row>
+    <row r="42" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B42" s="4"/>
+      <c r="C42" s="14"/>
+      <c r="D42" s="14"/>
+      <c r="E42" s="14"/>
+      <c r="F42" s="14"/>
+      <c r="G42" s="14"/>
+      <c r="H42" s="14"/>
+      <c r="I42" s="14"/>
+      <c r="J42" s="14"/>
+      <c r="K42" s="14"/>
+      <c r="L42" s="14"/>
+      <c r="M42" s="14"/>
+      <c r="N42" s="14"/>
+      <c r="O42" s="14"/>
+      <c r="P42" s="14"/>
+      <c r="Q42" s="14"/>
+      <c r="R42" s="14"/>
+      <c r="S42" s="14"/>
+      <c r="T42" s="5"/>
+    </row>
+    <row r="43" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B43" s="4"/>
+      <c r="C43" s="14"/>
+      <c r="D43" s="14"/>
+      <c r="E43" s="14"/>
+      <c r="F43" s="14"/>
+      <c r="G43" s="14"/>
+      <c r="H43" s="14"/>
+      <c r="I43" s="14"/>
+      <c r="J43" s="14"/>
+      <c r="K43" s="14"/>
+      <c r="L43" s="14"/>
+      <c r="M43" s="14"/>
+      <c r="N43" s="14"/>
+      <c r="O43" s="14"/>
+      <c r="P43" s="14"/>
+      <c r="Q43" s="14"/>
+      <c r="R43" s="14"/>
+      <c r="S43" s="14"/>
+      <c r="T43" s="5"/>
+    </row>
+    <row r="44" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B44" s="4"/>
+      <c r="C44" s="14"/>
+      <c r="D44" s="14"/>
+      <c r="E44" s="14"/>
+      <c r="F44" s="14"/>
+      <c r="G44" s="14"/>
+      <c r="H44" s="14"/>
+      <c r="I44" s="14"/>
+      <c r="J44" s="14"/>
+      <c r="K44" s="14"/>
+      <c r="L44" s="14"/>
+      <c r="M44" s="14"/>
+      <c r="N44" s="14"/>
+      <c r="O44" s="14"/>
+      <c r="P44" s="14"/>
+      <c r="Q44" s="14"/>
+      <c r="R44" s="14"/>
+      <c r="S44" s="14"/>
+      <c r="T44" s="5"/>
+    </row>
+    <row r="45" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B45" s="4"/>
+      <c r="C45" s="14"/>
+      <c r="D45" s="14"/>
+      <c r="E45" s="14"/>
+      <c r="F45" s="14"/>
+      <c r="G45" s="14"/>
+      <c r="H45" s="14"/>
+      <c r="I45" s="14"/>
+      <c r="J45" s="14"/>
+      <c r="K45" s="14"/>
+      <c r="L45" s="14"/>
+      <c r="M45" s="14"/>
+      <c r="N45" s="14"/>
+      <c r="O45" s="14"/>
+      <c r="P45" s="14"/>
+      <c r="Q45" s="14"/>
+      <c r="R45" s="14"/>
+      <c r="S45" s="14"/>
+      <c r="T45" s="5"/>
+    </row>
+    <row r="46" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B46" s="4"/>
+      <c r="C46" s="14"/>
+      <c r="D46" s="14"/>
+      <c r="E46" s="14"/>
+      <c r="F46" s="14"/>
+      <c r="G46" s="14"/>
+      <c r="H46" s="14"/>
+      <c r="I46" s="14"/>
+      <c r="J46" s="14"/>
+      <c r="K46" s="14"/>
+      <c r="L46" s="14"/>
+      <c r="M46" s="14"/>
+      <c r="N46" s="14"/>
+      <c r="O46" s="14"/>
+      <c r="P46" s="14"/>
+      <c r="Q46" s="14"/>
+      <c r="R46" s="14"/>
+      <c r="S46" s="14"/>
+      <c r="T46" s="5"/>
+    </row>
+    <row r="47" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B47" s="4"/>
+      <c r="C47" s="14"/>
+      <c r="D47" s="14"/>
+      <c r="E47" s="14"/>
+      <c r="F47" s="14"/>
+      <c r="G47" s="14"/>
+      <c r="H47" s="14"/>
+      <c r="I47" s="14"/>
+      <c r="J47" s="14"/>
+      <c r="K47" s="14"/>
+      <c r="L47" s="14"/>
+      <c r="M47" s="14"/>
+      <c r="N47" s="14"/>
+      <c r="O47" s="14"/>
+      <c r="P47" s="14"/>
+      <c r="Q47" s="14"/>
+      <c r="R47" s="14"/>
+      <c r="S47" s="14"/>
+      <c r="T47" s="5"/>
+    </row>
+    <row r="48" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B48" s="4"/>
+      <c r="C48" s="14"/>
+      <c r="D48" s="14"/>
+      <c r="E48" s="14"/>
+      <c r="F48" s="14"/>
+      <c r="G48" s="14"/>
+      <c r="H48" s="14"/>
+      <c r="I48" s="14"/>
+      <c r="J48" s="14"/>
+      <c r="K48" s="14"/>
+      <c r="L48" s="14"/>
+      <c r="M48" s="14"/>
+      <c r="N48" s="14"/>
+      <c r="O48" s="14"/>
+      <c r="P48" s="14"/>
+      <c r="Q48" s="14"/>
+      <c r="R48" s="14"/>
+      <c r="S48" s="14"/>
+      <c r="T48" s="5"/>
+    </row>
+    <row r="49" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B49" s="4"/>
+      <c r="C49" s="14"/>
+      <c r="D49" s="14"/>
+      <c r="E49" s="14"/>
+      <c r="F49" s="14"/>
+      <c r="G49" s="14"/>
+      <c r="H49" s="14"/>
+      <c r="I49" s="14"/>
+      <c r="J49" s="14"/>
+      <c r="K49" s="14"/>
+      <c r="L49" s="14"/>
+      <c r="M49" s="14"/>
+      <c r="N49" s="14"/>
+      <c r="O49" s="14"/>
+      <c r="P49" s="14"/>
+      <c r="Q49" s="14"/>
+      <c r="R49" s="14"/>
+      <c r="S49" s="14"/>
+      <c r="T49" s="5"/>
+    </row>
+    <row r="50" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B50" s="4"/>
+      <c r="C50" s="14"/>
+      <c r="D50" s="14"/>
+      <c r="E50" s="14"/>
+      <c r="F50" s="14"/>
+      <c r="G50" s="14"/>
+      <c r="H50" s="14"/>
+      <c r="I50" s="14"/>
+      <c r="J50" s="14"/>
+      <c r="K50" s="14"/>
+      <c r="L50" s="14"/>
+      <c r="M50" s="14"/>
+      <c r="N50" s="14"/>
+      <c r="O50" s="14"/>
+      <c r="P50" s="14"/>
+      <c r="Q50" s="14"/>
+      <c r="R50" s="14"/>
+      <c r="S50" s="14"/>
+      <c r="T50" s="5"/>
+    </row>
+    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B51" s="4"/>
+      <c r="C51" s="14"/>
+      <c r="D51" s="14"/>
+      <c r="E51" s="14"/>
+      <c r="F51" s="14"/>
+      <c r="G51" s="14"/>
+      <c r="H51" s="14"/>
+      <c r="I51" s="14"/>
+      <c r="J51" s="14"/>
+      <c r="K51" s="14"/>
+      <c r="L51" s="14"/>
+      <c r="M51" s="14"/>
+      <c r="N51" s="14"/>
+      <c r="O51" s="14"/>
+      <c r="P51" s="14"/>
+      <c r="Q51" s="14"/>
+      <c r="R51" s="14"/>
+      <c r="S51" s="14"/>
+      <c r="T51" s="5"/>
+    </row>
+    <row r="52" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B52" s="4"/>
+      <c r="C52" s="14"/>
+      <c r="D52" s="14"/>
+      <c r="E52" s="14"/>
+      <c r="F52" s="14"/>
+      <c r="G52" s="14"/>
+      <c r="H52" s="14"/>
+      <c r="I52" s="14"/>
+      <c r="J52" s="14"/>
+      <c r="K52" s="14"/>
+      <c r="L52" s="14"/>
+      <c r="M52" s="14"/>
+      <c r="N52" s="14"/>
+      <c r="O52" s="14"/>
+      <c r="P52" s="14"/>
+      <c r="Q52" s="14"/>
+      <c r="R52" s="14"/>
+      <c r="S52" s="14"/>
+      <c r="T52" s="5"/>
+    </row>
+    <row r="53" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B53" s="6"/>
+      <c r="C53" s="7"/>
+      <c r="D53" s="7"/>
+      <c r="E53" s="7"/>
+      <c r="F53" s="7"/>
+      <c r="G53" s="7"/>
+      <c r="H53" s="7"/>
+      <c r="I53" s="7"/>
+      <c r="J53" s="7"/>
+      <c r="K53" s="7"/>
+      <c r="L53" s="7"/>
+      <c r="M53" s="7"/>
+      <c r="N53" s="7"/>
+      <c r="O53" s="7"/>
+      <c r="P53" s="7"/>
+      <c r="Q53" s="7"/>
+      <c r="R53" s="7"/>
+      <c r="S53" s="7"/>
+      <c r="T53" s="8"/>
+    </row>
+    <row r="56" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A56" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="57" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B57" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C57" s="2"/>
+      <c r="D57" s="2"/>
+      <c r="E57" s="2"/>
+      <c r="F57" s="3"/>
+    </row>
+    <row r="58" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B58" s="4"/>
+      <c r="C58" t="s">
+        <v>10</v>
+      </c>
+      <c r="F58" s="5"/>
+    </row>
+    <row r="59" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B59" s="4"/>
+      <c r="D59" t="s">
+        <v>11</v>
+      </c>
+      <c r="F59" s="5"/>
+    </row>
+    <row r="60" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B60" s="4"/>
+      <c r="D60" t="s">
+        <v>12</v>
+      </c>
+      <c r="F60" s="5"/>
+    </row>
+    <row r="61" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B61" s="4"/>
+      <c r="D61" t="s">
+        <v>13</v>
+      </c>
+      <c r="F61" s="5"/>
+    </row>
+    <row r="62" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B62" s="4"/>
+      <c r="C62" t="s">
+        <v>14</v>
+      </c>
+      <c r="F62" s="5"/>
+    </row>
+    <row r="63" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B63" s="4"/>
+      <c r="D63" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="F63" s="5"/>
+      <c r="G63" t="s">
+        <v>20</v>
+      </c>
+      <c r="H63" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="64" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B64" s="4"/>
+      <c r="C64" t="s">
+        <v>15</v>
+      </c>
+      <c r="F64" s="5"/>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B65" s="4"/>
+      <c r="C65" t="s">
+        <v>16</v>
+      </c>
+      <c r="F65" s="5"/>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B66" s="4"/>
+      <c r="D66" t="s">
+        <v>26</v>
+      </c>
+      <c r="F66" s="5"/>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B67" s="4"/>
+      <c r="D67" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="F67" s="5"/>
+      <c r="G67" t="s">
+        <v>20</v>
+      </c>
+      <c r="H67" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B68" s="6"/>
+      <c r="C68" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D68" s="7"/>
+      <c r="E68" s="7"/>
+      <c r="F68" s="8"/>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B72" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C72" s="2"/>
+      <c r="D72" s="2"/>
+      <c r="E72" s="2"/>
+      <c r="F72" s="2"/>
+      <c r="G72" s="2"/>
+      <c r="H72" s="3"/>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B73" s="4"/>
+      <c r="C73" s="14"/>
+      <c r="D73" s="14"/>
+      <c r="E73" s="14"/>
+      <c r="F73" s="14"/>
+      <c r="G73" s="14"/>
+      <c r="H73" s="5"/>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B74" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C74" s="14"/>
+      <c r="D74" s="14"/>
+      <c r="E74" s="14"/>
+      <c r="F74" s="14"/>
+      <c r="G74" s="14"/>
+      <c r="H74" s="5"/>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B75" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C75" s="14"/>
+      <c r="D75" s="14"/>
+      <c r="E75" s="14"/>
+      <c r="F75" s="14"/>
+      <c r="G75" s="14"/>
+      <c r="H75" s="5"/>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B76" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C76" s="14"/>
+      <c r="D76" s="14"/>
+      <c r="E76" s="14"/>
+      <c r="F76" s="14"/>
+      <c r="G76" s="14"/>
+      <c r="H76" s="5"/>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B77" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C77" s="14"/>
+      <c r="D77" s="14"/>
+      <c r="E77" s="14"/>
+      <c r="F77" s="14"/>
+      <c r="G77" s="14"/>
+      <c r="H77" s="5"/>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B78" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C78" s="14"/>
+      <c r="D78" s="14"/>
+      <c r="E78" s="14"/>
+      <c r="F78" s="14"/>
+      <c r="G78" s="14"/>
+      <c r="H78" s="5"/>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B79" s="4"/>
+      <c r="C79" s="14"/>
+      <c r="D79" s="14"/>
+      <c r="E79" s="14"/>
+      <c r="F79" s="14"/>
+      <c r="G79" s="14"/>
+      <c r="H79" s="5"/>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B80" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="C80" s="14"/>
+      <c r="D80" s="14"/>
+      <c r="E80" s="14"/>
+      <c r="F80" s="14"/>
+      <c r="G80" s="14"/>
+      <c r="H80" s="5"/>
+    </row>
+    <row r="81" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B81" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="C81" s="14"/>
+      <c r="D81" s="14"/>
+      <c r="E81" s="14"/>
+      <c r="F81" s="14"/>
+      <c r="G81" s="14"/>
+      <c r="H81" s="5"/>
+    </row>
+    <row r="82" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B82" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="C82" s="14"/>
+      <c r="D82" s="14"/>
+      <c r="E82" s="14"/>
+      <c r="F82" s="14"/>
+      <c r="G82" s="14"/>
+      <c r="H82" s="5"/>
+    </row>
+    <row r="83" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B83" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="C83" s="14"/>
+      <c r="D83" s="14"/>
+      <c r="E83" s="14"/>
+      <c r="F83" s="14"/>
+      <c r="G83" s="14"/>
+      <c r="H83" s="5"/>
+    </row>
+    <row r="84" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B84" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="C84" s="14"/>
+      <c r="D84" s="14"/>
+      <c r="E84" s="14"/>
+      <c r="F84" s="14"/>
+      <c r="G84" s="14"/>
+      <c r="H84" s="5"/>
+      <c r="I84" t="s">
+        <v>20</v>
+      </c>
+      <c r="J84" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="85" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B85" s="15"/>
+      <c r="C85" s="14"/>
+      <c r="D85" s="14"/>
+      <c r="E85" s="14"/>
+      <c r="F85" s="14"/>
+      <c r="G85" s="14"/>
+      <c r="H85" s="5"/>
+    </row>
+    <row r="86" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B86" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="C86" s="14"/>
+      <c r="D86" s="14"/>
+      <c r="E86" s="14"/>
+      <c r="F86" s="14"/>
+      <c r="G86" s="14"/>
+      <c r="H86" s="5"/>
+    </row>
+    <row r="87" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B87" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="C87" s="14"/>
+      <c r="D87" s="14"/>
+      <c r="E87" s="14"/>
+      <c r="F87" s="14"/>
+      <c r="G87" s="14"/>
+      <c r="H87" s="5"/>
+    </row>
+    <row r="88" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B88" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="C88" s="14"/>
+      <c r="D88" s="14"/>
+      <c r="E88" s="14"/>
+      <c r="F88" s="14"/>
+      <c r="G88" s="14"/>
+      <c r="H88" s="5"/>
+    </row>
+    <row r="89" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B89" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="C89" s="14"/>
+      <c r="D89" s="14"/>
+      <c r="E89" s="14"/>
+      <c r="F89" s="14"/>
+      <c r="G89" s="14"/>
+      <c r="H89" s="5"/>
+    </row>
+    <row r="90" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B90" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C90" s="14"/>
+      <c r="D90" s="14"/>
+      <c r="E90" s="14"/>
+      <c r="F90" s="14"/>
+      <c r="G90" s="14"/>
+      <c r="H90" s="5"/>
+    </row>
+    <row r="91" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B91" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="C91" s="14"/>
+      <c r="D91" s="14"/>
+      <c r="E91" s="14"/>
+      <c r="F91" s="14"/>
+      <c r="G91" s="14"/>
+      <c r="H91" s="5"/>
+    </row>
+    <row r="92" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B92" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="C92" s="14"/>
+      <c r="D92" s="14"/>
+      <c r="E92" s="14"/>
+      <c r="F92" s="14"/>
+      <c r="G92" s="14"/>
+      <c r="H92" s="5"/>
+    </row>
+    <row r="93" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B93" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="C93" s="14"/>
+      <c r="D93" s="14"/>
+      <c r="E93" s="14"/>
+      <c r="F93" s="14"/>
+      <c r="G93" s="14"/>
+      <c r="H93" s="5"/>
+    </row>
+    <row r="94" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B94" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="C94" s="14"/>
+      <c r="D94" s="14"/>
+      <c r="E94" s="14"/>
+      <c r="F94" s="14"/>
+      <c r="G94" s="14"/>
+      <c r="H94" s="5"/>
+      <c r="I94" t="s">
+        <v>20</v>
+      </c>
+      <c r="J94" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="95" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B95" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="C95" s="14"/>
+      <c r="D95" s="14"/>
+      <c r="E95" s="14"/>
+      <c r="F95" s="14"/>
+      <c r="G95" s="14"/>
+      <c r="H95" s="5"/>
+      <c r="J95" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="96" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B96" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="C96" s="14"/>
+      <c r="D96" s="14"/>
+      <c r="E96" s="14"/>
+      <c r="F96" s="14"/>
+      <c r="G96" s="14"/>
+      <c r="H96" s="5"/>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B97" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="C97" s="14"/>
+      <c r="D97" s="14"/>
+      <c r="E97" s="14"/>
+      <c r="F97" s="14"/>
+      <c r="G97" s="14"/>
+      <c r="H97" s="5"/>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B98" s="15"/>
+      <c r="C98" s="14"/>
+      <c r="D98" s="14"/>
+      <c r="E98" s="14"/>
+      <c r="F98" s="14"/>
+      <c r="G98" s="14"/>
+      <c r="H98" s="5"/>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B99" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="C99" s="14"/>
+      <c r="D99" s="14"/>
+      <c r="E99" s="14"/>
+      <c r="F99" s="14"/>
+      <c r="G99" s="14"/>
+      <c r="H99" s="5"/>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B100" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="C100" s="14"/>
+      <c r="D100" s="14"/>
+      <c r="E100" s="14"/>
+      <c r="F100" s="14"/>
+      <c r="G100" s="14"/>
+      <c r="H100" s="5"/>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B101" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="C101" s="14"/>
+      <c r="D101" s="14"/>
+      <c r="E101" s="14"/>
+      <c r="F101" s="14"/>
+      <c r="G101" s="14"/>
+      <c r="H101" s="5"/>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B102" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="C102" s="14"/>
+      <c r="D102" s="14"/>
+      <c r="E102" s="14"/>
+      <c r="F102" s="14"/>
+      <c r="G102" s="14"/>
+      <c r="H102" s="5"/>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B103" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="C103" s="14"/>
+      <c r="D103" s="14"/>
+      <c r="E103" s="14"/>
+      <c r="F103" s="14"/>
+      <c r="G103" s="14"/>
+      <c r="H103" s="5"/>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B104" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="C104" s="14"/>
+      <c r="D104" s="14"/>
+      <c r="E104" s="14"/>
+      <c r="F104" s="14"/>
+      <c r="G104" s="14"/>
+      <c r="H104" s="5"/>
+      <c r="I104" t="s">
+        <v>20</v>
+      </c>
+      <c r="J104" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B105" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="C105" s="14"/>
+      <c r="D105" s="14"/>
+      <c r="E105" s="14"/>
+      <c r="F105" s="14"/>
+      <c r="G105" s="14"/>
+      <c r="H105" s="5"/>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B106" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="C106" s="14"/>
+      <c r="D106" s="14"/>
+      <c r="E106" s="14"/>
+      <c r="F106" s="14"/>
+      <c r="G106" s="14"/>
+      <c r="H106" s="5"/>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B107" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="C107" s="14"/>
+      <c r="D107" s="14"/>
+      <c r="E107" s="14"/>
+      <c r="F107" s="14"/>
+      <c r="G107" s="14"/>
+      <c r="H107" s="5"/>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B108" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C108" s="7"/>
+      <c r="D108" s="7"/>
+      <c r="E108" s="7"/>
+      <c r="F108" s="7"/>
+      <c r="G108" s="7"/>
+      <c r="H108" s="8"/>
+    </row>
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B112" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C112" s="2"/>
+      <c r="D112" s="2"/>
+      <c r="E112" s="2"/>
+      <c r="F112" s="2"/>
+      <c r="G112" s="2"/>
+      <c r="H112" s="3"/>
+    </row>
+    <row r="113" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B113" s="4"/>
+      <c r="C113" s="14"/>
+      <c r="D113" s="14"/>
+      <c r="E113" s="14"/>
+      <c r="F113" s="14"/>
+      <c r="G113" s="14"/>
+      <c r="H113" s="5"/>
+    </row>
+    <row r="114" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B114" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C114" s="14"/>
+      <c r="D114" s="14"/>
+      <c r="E114" s="14"/>
+      <c r="F114" s="14"/>
+      <c r="G114" s="14"/>
+      <c r="H114" s="5"/>
+    </row>
+    <row r="115" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B115" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C115" s="14"/>
+      <c r="D115" s="14"/>
+      <c r="E115" s="14"/>
+      <c r="F115" s="14"/>
+      <c r="G115" s="14"/>
+      <c r="H115" s="5"/>
+    </row>
+    <row r="116" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B116" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C116" s="14"/>
+      <c r="D116" s="14"/>
+      <c r="E116" s="14"/>
+      <c r="F116" s="14"/>
+      <c r="G116" s="14"/>
+      <c r="H116" s="5"/>
+    </row>
+    <row r="117" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B117" s="4"/>
+      <c r="C117" s="14"/>
+      <c r="D117" s="14"/>
+      <c r="E117" s="14"/>
+      <c r="F117" s="14"/>
+      <c r="G117" s="14"/>
+      <c r="H117" s="5"/>
+    </row>
+    <row r="118" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B118" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C118" s="14"/>
+      <c r="D118" s="14"/>
+      <c r="E118" s="14"/>
+      <c r="F118" s="14"/>
+      <c r="G118" s="14"/>
+      <c r="H118" s="5"/>
+    </row>
+    <row r="119" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B119" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C119" s="14"/>
+      <c r="D119" s="14"/>
+      <c r="E119" s="14"/>
+      <c r="F119" s="14"/>
+      <c r="G119" s="14"/>
+      <c r="H119" s="5"/>
+    </row>
+    <row r="120" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B120" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C120" s="14"/>
+      <c r="D120" s="14"/>
+      <c r="E120" s="14"/>
+      <c r="F120" s="14"/>
+      <c r="G120" s="14"/>
+      <c r="H120" s="5"/>
+    </row>
+    <row r="121" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B121" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C121" s="14"/>
+      <c r="D121" s="14"/>
+      <c r="E121" s="14"/>
+      <c r="F121" s="14"/>
+      <c r="G121" s="14"/>
+      <c r="H121" s="5"/>
+    </row>
+    <row r="122" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B122" s="4"/>
+      <c r="C122" s="14"/>
+      <c r="D122" s="14"/>
+      <c r="E122" s="14"/>
+      <c r="F122" s="14"/>
+      <c r="G122" s="14"/>
+      <c r="H122" s="5"/>
+    </row>
+    <row r="123" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B123" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C123" s="14"/>
+      <c r="D123" s="14"/>
+      <c r="E123" s="14"/>
+      <c r="F123" s="14"/>
+      <c r="G123" s="14"/>
+      <c r="H123" s="5"/>
+    </row>
+    <row r="124" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B124" s="4"/>
+      <c r="C124" s="14"/>
+      <c r="D124" s="14"/>
+      <c r="E124" s="14"/>
+      <c r="F124" s="14"/>
+      <c r="G124" s="14"/>
+      <c r="H124" s="5"/>
+    </row>
+    <row r="125" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B125" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="C125" s="14"/>
+      <c r="D125" s="14"/>
+      <c r="E125" s="14"/>
+      <c r="F125" s="14"/>
+      <c r="G125" s="14"/>
+      <c r="H125" s="5"/>
+    </row>
+    <row r="126" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B126" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="C126" s="14"/>
+      <c r="D126" s="14"/>
+      <c r="E126" s="14"/>
+      <c r="F126" s="14"/>
+      <c r="G126" s="14"/>
+      <c r="H126" s="5"/>
+      <c r="I126" t="s">
+        <v>20</v>
+      </c>
+      <c r="J126" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="127" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B127" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="C127" s="14"/>
+      <c r="D127" s="14"/>
+      <c r="E127" s="14"/>
+      <c r="F127" s="14"/>
+      <c r="G127" s="14"/>
+      <c r="H127" s="5"/>
+    </row>
+    <row r="128" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B128" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="C128" s="14"/>
+      <c r="D128" s="14"/>
+      <c r="E128" s="14"/>
+      <c r="F128" s="14"/>
+      <c r="G128" s="14"/>
+      <c r="H128" s="5"/>
+    </row>
+    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B129" s="15"/>
+      <c r="C129" s="14"/>
+      <c r="D129" s="14"/>
+      <c r="E129" s="14"/>
+      <c r="F129" s="14"/>
+      <c r="G129" s="14"/>
+      <c r="H129" s="5"/>
+    </row>
+    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B130" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="C130" s="14"/>
+      <c r="D130" s="14"/>
+      <c r="E130" s="14"/>
+      <c r="F130" s="14"/>
+      <c r="G130" s="14"/>
+      <c r="H130" s="5"/>
+    </row>
+    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B131" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="C131" s="14"/>
+      <c r="D131" s="14"/>
+      <c r="E131" s="14"/>
+      <c r="F131" s="14"/>
+      <c r="G131" s="14"/>
+      <c r="H131" s="5"/>
+    </row>
+    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B132" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="C132" s="14"/>
+      <c r="D132" s="14"/>
+      <c r="E132" s="14"/>
+      <c r="F132" s="14"/>
+      <c r="G132" s="14"/>
+      <c r="H132" s="5"/>
+    </row>
+    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B133" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="C133" s="7"/>
+      <c r="D133" s="7"/>
+      <c r="E133" s="7"/>
+      <c r="F133" s="7"/>
+      <c r="G133" s="7"/>
+      <c r="H133" s="8"/>
+    </row>
+    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A136" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B136" s="2"/>
+      <c r="C136" s="2"/>
+      <c r="D136" s="2"/>
+      <c r="E136" s="2"/>
+      <c r="F136" s="2"/>
+      <c r="G136" s="2"/>
+      <c r="H136" s="3"/>
+    </row>
+    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A137" s="4"/>
+      <c r="B137" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="C137" s="14"/>
+      <c r="D137" s="14"/>
+      <c r="E137" s="14"/>
+      <c r="F137" s="14"/>
+      <c r="G137" s="14"/>
+      <c r="H137" s="5"/>
+    </row>
+    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A138" s="4"/>
+      <c r="B138" s="14"/>
+      <c r="C138" s="14"/>
+      <c r="D138" s="14"/>
+      <c r="E138" s="14"/>
+      <c r="F138" s="14"/>
+      <c r="G138" s="14"/>
+      <c r="H138" s="5"/>
+    </row>
+    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A139" s="4"/>
+      <c r="B139" s="14"/>
+      <c r="C139" s="14"/>
+      <c r="D139" s="14"/>
+      <c r="E139" s="14"/>
+      <c r="F139" s="14"/>
+      <c r="G139" s="14"/>
+      <c r="H139" s="5"/>
+    </row>
+    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A140" s="4"/>
+      <c r="B140" s="14"/>
+      <c r="C140" s="14"/>
+      <c r="D140" s="14"/>
+      <c r="E140" s="14"/>
+      <c r="F140" s="14"/>
+      <c r="G140" s="14"/>
+      <c r="H140" s="5"/>
+    </row>
+    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A141" s="4"/>
+      <c r="B141" s="14"/>
+      <c r="C141" s="14"/>
+      <c r="D141" s="14"/>
+      <c r="E141" s="14"/>
+      <c r="F141" s="14"/>
+      <c r="G141" s="14"/>
+      <c r="H141" s="5"/>
+    </row>
+    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A142" s="4"/>
+      <c r="B142" s="14"/>
+      <c r="C142" s="14"/>
+      <c r="D142" s="14"/>
+      <c r="E142" s="14"/>
+      <c r="F142" s="14"/>
+      <c r="G142" s="14"/>
+      <c r="H142" s="5"/>
+    </row>
+    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A143" s="4"/>
+      <c r="B143" s="14"/>
+      <c r="C143" s="14"/>
+      <c r="D143" s="14"/>
+      <c r="E143" s="14"/>
+      <c r="F143" s="14"/>
+      <c r="G143" s="14"/>
+      <c r="H143" s="5"/>
+    </row>
+    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A144" s="4"/>
+      <c r="B144" s="14"/>
+      <c r="C144" s="14"/>
+      <c r="D144" s="14"/>
+      <c r="E144" s="14"/>
+      <c r="F144" s="14"/>
+      <c r="G144" s="14"/>
+      <c r="H144" s="5"/>
+    </row>
+    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A145" s="4"/>
+      <c r="B145" s="14"/>
+      <c r="C145" s="14"/>
+      <c r="D145" s="14"/>
+      <c r="E145" s="14"/>
+      <c r="F145" s="14"/>
+      <c r="G145" s="14"/>
+      <c r="H145" s="5"/>
+    </row>
+    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A146" s="4"/>
+      <c r="B146" s="14"/>
+      <c r="C146" s="14"/>
+      <c r="D146" s="14"/>
+      <c r="E146" s="14"/>
+      <c r="F146" s="14"/>
+      <c r="G146" s="14"/>
+      <c r="H146" s="5"/>
+    </row>
+    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A147" s="4"/>
+      <c r="B147" s="14"/>
+      <c r="C147" s="14"/>
+      <c r="D147" s="14"/>
+      <c r="E147" s="14"/>
+      <c r="F147" s="14"/>
+      <c r="G147" s="14"/>
+      <c r="H147" s="5"/>
+    </row>
+    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A148" s="4"/>
+      <c r="B148" s="14"/>
+      <c r="C148" s="14"/>
+      <c r="D148" s="14"/>
+      <c r="E148" s="14"/>
+      <c r="F148" s="14"/>
+      <c r="G148" s="14"/>
+      <c r="H148" s="5"/>
+    </row>
+    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A149" s="4"/>
+      <c r="B149" s="14"/>
+      <c r="C149" s="14"/>
+      <c r="D149" s="14"/>
+      <c r="E149" s="14"/>
+      <c r="F149" s="14"/>
+      <c r="G149" s="14"/>
+      <c r="H149" s="5"/>
+    </row>
+    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A150" s="4"/>
+      <c r="B150" s="14"/>
+      <c r="C150" s="14"/>
+      <c r="D150" s="14"/>
+      <c r="E150" s="14"/>
+      <c r="F150" s="14"/>
+      <c r="G150" s="14"/>
+      <c r="H150" s="5"/>
+    </row>
+    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A151" s="4"/>
+      <c r="B151" s="14"/>
+      <c r="C151" s="14"/>
+      <c r="D151" s="14"/>
+      <c r="E151" s="14"/>
+      <c r="F151" s="14"/>
+      <c r="G151" s="14"/>
+      <c r="H151" s="5"/>
+    </row>
+    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A152" s="4"/>
+      <c r="B152" s="14"/>
+      <c r="C152" s="14"/>
+      <c r="D152" s="14"/>
+      <c r="E152" s="14"/>
+      <c r="F152" s="14"/>
+      <c r="G152" s="14"/>
+      <c r="H152" s="5"/>
+    </row>
+    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A153" s="4"/>
+      <c r="B153" s="14"/>
+      <c r="C153" s="14"/>
+      <c r="D153" s="14"/>
+      <c r="E153" s="14"/>
+      <c r="F153" s="14"/>
+      <c r="G153" s="14"/>
+      <c r="H153" s="5"/>
+    </row>
+    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A154" s="4"/>
+      <c r="B154" s="14"/>
+      <c r="C154" s="14"/>
+      <c r="D154" s="14"/>
+      <c r="E154" s="14"/>
+      <c r="F154" s="14"/>
+      <c r="G154" s="14"/>
+      <c r="H154" s="5"/>
+    </row>
+    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A155" s="4"/>
+      <c r="B155" s="14"/>
+      <c r="C155" s="14"/>
+      <c r="D155" s="14"/>
+      <c r="E155" s="14"/>
+      <c r="F155" s="14"/>
+      <c r="G155" s="14"/>
+      <c r="H155" s="5"/>
+    </row>
+    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A156" s="4"/>
+      <c r="B156" s="14"/>
+      <c r="C156" s="14"/>
+      <c r="D156" s="14"/>
+      <c r="E156" s="14"/>
+      <c r="F156" s="14"/>
+      <c r="G156" s="14"/>
+      <c r="H156" s="5"/>
+    </row>
+    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A157" s="4"/>
+      <c r="B157" s="14"/>
+      <c r="C157" s="14"/>
+      <c r="D157" s="14"/>
+      <c r="E157" s="14"/>
+      <c r="F157" s="14"/>
+      <c r="G157" s="14"/>
+      <c r="H157" s="5"/>
+    </row>
+    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A158" s="4"/>
+      <c r="B158" s="14"/>
+      <c r="C158" s="14"/>
+      <c r="D158" s="14"/>
+      <c r="E158" s="14"/>
+      <c r="F158" s="14"/>
+      <c r="G158" s="14"/>
+      <c r="H158" s="5"/>
+    </row>
+    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A159" s="4"/>
+      <c r="B159" s="14"/>
+      <c r="C159" s="14"/>
+      <c r="D159" s="14"/>
+      <c r="E159" s="14"/>
+      <c r="F159" s="14"/>
+      <c r="G159" s="14"/>
+      <c r="H159" s="5"/>
+    </row>
+    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A160" s="6"/>
+      <c r="B160" s="7"/>
+      <c r="C160" s="7"/>
+      <c r="D160" s="7"/>
+      <c r="E160" s="7"/>
+      <c r="F160" s="7"/>
+      <c r="G160" s="7"/>
+      <c r="H160" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Match the requested route to the list of routes in the routing table
</commit_message>
<xml_diff>
--- a/me/2.routing.xlsx
+++ b/me/2.routing.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\build-php-mvc-framework\me\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92C31426-A54B-44B3-B786-328F997C0922}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F6E0B84-E0D8-41ED-8DA6-0D2C9E01DFAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="central entry point" sheetId="1" r:id="rId1"/>
     <sheet name="Configure URLs" sheetId="2" r:id="rId2"/>
     <sheet name="CreateAndRequireRouterClass" sheetId="3" r:id="rId3"/>
     <sheet name="routing table in the router" sheetId="4" r:id="rId4"/>
+    <sheet name="MatchRequestedRouteToRoutingTbl" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="137">
   <si>
     <t>Create a central entry point to the framework: the front controller</t>
   </si>
@@ -446,6 +447,99 @@
   </si>
   <si>
     <t>Check routing table</t>
+  </si>
+  <si>
+    <t>Match the requested route to the list of routes in the routing table</t>
+  </si>
+  <si>
+    <t>router có nhiệm vụ matching route(lấy từ url) với controler và action bằng cách dùng routing table</t>
+  </si>
+  <si>
+    <t>Từ route lấy từ url mình tiến hành tìm trong routing table nếu matching thì mình có được controller và action</t>
+  </si>
+  <si>
+    <t>     * Parameters from the matched route</t>
+  </si>
+  <si>
+    <t>    protected $params = [];</t>
+  </si>
+  <si>
+    <t>     * Match the route to the routes in the routing table, setting the $params</t>
+  </si>
+  <si>
+    <t>     * property if a route is found.</t>
+  </si>
+  <si>
+    <t>     * @param string $url The route URL</t>
+  </si>
+  <si>
+    <t>     * @return boolean  true if a match found, false otherwise</t>
+  </si>
+  <si>
+    <t>    public function match($url)</t>
+  </si>
+  <si>
+    <t>        foreach ($this-&gt;routes as $route =&gt; $params) {</t>
+  </si>
+  <si>
+    <t>            if ($url == $route) {</t>
+  </si>
+  <si>
+    <t>                $this-&gt;params = $params;</t>
+  </si>
+  <si>
+    <t>                return true;</t>
+  </si>
+  <si>
+    <t>            }</t>
+  </si>
+  <si>
+    <t>        }</t>
+  </si>
+  <si>
+    <t>        return false;</t>
+  </si>
+  <si>
+    <t>     * Get the currently matched parameters</t>
+  </si>
+  <si>
+    <t>    public function getParams()</t>
+  </si>
+  <si>
+    <t>        return $this-&gt;params;</t>
+  </si>
+  <si>
+    <t>// Match the requested route</t>
+  </si>
+  <si>
+    <t>$url = $_SERVER['QUERY_STRING'];</t>
+  </si>
+  <si>
+    <t>if ($router-&gt;match($url)) {</t>
+  </si>
+  <si>
+    <t>    echo '&lt;pre&gt;';</t>
+  </si>
+  <si>
+    <t>    var_dump($router-&gt;getParams());</t>
+  </si>
+  <si>
+    <t>    echo '&lt;/pre&gt;';</t>
+  </si>
+  <si>
+    <t>} else {</t>
+  </si>
+  <si>
+    <t>    echo "No route found for URL '$url'";</t>
+  </si>
+  <si>
+    <t>http://localhost/</t>
+  </si>
+  <si>
+    <t>http://localhost/posts</t>
+  </si>
+  <si>
+    <t>http://localhost/posts/new</t>
   </si>
 </sst>
 </file>
@@ -589,10 +683,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2716,6 +2810,496 @@
         </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>133351</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>114301</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>342901</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>143969</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FAA40CD0-5136-C26D-6E5A-8C6CDC0486B8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="742951" y="1447801"/>
+          <a:ext cx="11182350" cy="3839668"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>428625</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="Straight Arrow Connector 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{20F134BC-EA2A-1345-2BCC-39C92E3F63EC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1647825" y="1495425"/>
+          <a:ext cx="352425" cy="1905000"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="7" name="Straight Arrow Connector 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{229B40BC-008A-5502-3A36-A706D496F57F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2495550" y="3524250"/>
+          <a:ext cx="1876425" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>134</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>512946</xdr:colOff>
+      <xdr:row>148</xdr:row>
+      <xdr:rowOff>161580</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4C1D2105-650D-9858-745C-0CEA4ABB0A3D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5133975" y="25593675"/>
+          <a:ext cx="11228571" cy="2761905"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>153</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>113923</xdr:colOff>
+      <xdr:row>162</xdr:row>
+      <xdr:rowOff>95035</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4A5C14E9-613C-A06A-28C9-9B132A3D828A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="752475" y="29232225"/>
+          <a:ext cx="3019048" cy="1723810"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>166</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>313837</xdr:colOff>
+      <xdr:row>175</xdr:row>
+      <xdr:rowOff>28368</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{75A0ED33-6D46-B08F-961D-833D79957FB4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="676275" y="31708725"/>
+          <a:ext cx="3904762" cy="1657143"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>179</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>75817</xdr:colOff>
+      <xdr:row>187</xdr:row>
+      <xdr:rowOff>161719</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Picture 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4C5F1188-3E98-AB4F-F625-0B4F7434DED3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="666750" y="34137600"/>
+          <a:ext cx="3066667" cy="1647619"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>135</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>152</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="17" name="Straight Arrow Connector 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EEE9B00F-1EE9-3353-30E1-5FFC0D6793E5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="828675" y="25841325"/>
+          <a:ext cx="657225" cy="3162300"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>136</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>165</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="20" name="Straight Arrow Connector 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FB76BC67-0C05-3C83-254E-56DCFADDCE9F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="762000" y="26069925"/>
+          <a:ext cx="800100" cy="5429250"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>137</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>178</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="24" name="Straight Arrow Connector 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E361BE96-C378-6B16-0549-6441CE5CC671}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="828675" y="26279475"/>
+          <a:ext cx="1019175" cy="7677150"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -4455,8 +5039,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3C2F33E-AFC9-4549-979A-DBAB82CF5E66}">
   <dimension ref="A2:T160"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
-      <selection activeCell="L142" sqref="L142"/>
+    <sheetView topLeftCell="A139" workbookViewId="0">
+      <selection activeCell="G63" sqref="G63:H67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4491,464 +5075,90 @@
     </row>
     <row r="6" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B6" s="4"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="14"/>
-      <c r="L6" s="14"/>
-      <c r="M6" s="14"/>
-      <c r="N6" s="14"/>
-      <c r="O6" s="14"/>
-      <c r="P6" s="14"/>
-      <c r="Q6" s="14"/>
-      <c r="R6" s="14"/>
-      <c r="S6" s="14"/>
       <c r="T6" s="5"/>
     </row>
     <row r="7" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B7" s="4"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="14"/>
-      <c r="K7" s="14"/>
-      <c r="L7" s="14"/>
-      <c r="M7" s="14"/>
-      <c r="N7" s="14"/>
-      <c r="O7" s="14"/>
-      <c r="P7" s="14"/>
-      <c r="Q7" s="14"/>
-      <c r="R7" s="14"/>
-      <c r="S7" s="14"/>
       <c r="T7" s="5"/>
     </row>
     <row r="8" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B8" s="4"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
-      <c r="K8" s="14"/>
-      <c r="L8" s="14"/>
-      <c r="M8" s="14"/>
-      <c r="N8" s="14"/>
-      <c r="O8" s="14"/>
-      <c r="P8" s="14"/>
-      <c r="Q8" s="14"/>
-      <c r="R8" s="14"/>
-      <c r="S8" s="14"/>
       <c r="T8" s="5"/>
     </row>
     <row r="9" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B9" s="4"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="14"/>
-      <c r="K9" s="14"/>
-      <c r="L9" s="14"/>
-      <c r="M9" s="14"/>
-      <c r="N9" s="14"/>
-      <c r="O9" s="14"/>
-      <c r="P9" s="14"/>
-      <c r="Q9" s="14"/>
-      <c r="R9" s="14"/>
-      <c r="S9" s="14"/>
       <c r="T9" s="5"/>
     </row>
     <row r="10" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B10" s="4"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
-      <c r="K10" s="14"/>
-      <c r="L10" s="14"/>
-      <c r="M10" s="14"/>
-      <c r="N10" s="14"/>
-      <c r="O10" s="14"/>
-      <c r="P10" s="14"/>
-      <c r="Q10" s="14"/>
-      <c r="R10" s="14"/>
-      <c r="S10" s="14"/>
       <c r="T10" s="5"/>
     </row>
     <row r="11" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B11" s="4"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="14"/>
-      <c r="K11" s="14"/>
-      <c r="L11" s="14"/>
-      <c r="M11" s="14"/>
-      <c r="N11" s="14"/>
-      <c r="O11" s="14"/>
-      <c r="P11" s="14"/>
-      <c r="Q11" s="14"/>
-      <c r="R11" s="14"/>
-      <c r="S11" s="14"/>
       <c r="T11" s="5"/>
     </row>
     <row r="12" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B12" s="4"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
-      <c r="K12" s="14"/>
-      <c r="L12" s="14"/>
-      <c r="M12" s="14"/>
-      <c r="N12" s="14"/>
-      <c r="O12" s="14"/>
-      <c r="P12" s="14"/>
-      <c r="Q12" s="14"/>
-      <c r="R12" s="14"/>
-      <c r="S12" s="14"/>
       <c r="T12" s="5"/>
     </row>
     <row r="13" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B13" s="4"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14"/>
-      <c r="K13" s="14"/>
-      <c r="L13" s="14"/>
-      <c r="M13" s="14"/>
-      <c r="N13" s="14"/>
-      <c r="O13" s="14"/>
-      <c r="P13" s="14"/>
-      <c r="Q13" s="14"/>
-      <c r="R13" s="14"/>
-      <c r="S13" s="14"/>
       <c r="T13" s="5"/>
     </row>
     <row r="14" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B14" s="4"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="14"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="14"/>
-      <c r="K14" s="14"/>
-      <c r="L14" s="14"/>
-      <c r="M14" s="14"/>
-      <c r="N14" s="14"/>
-      <c r="O14" s="14"/>
-      <c r="P14" s="14"/>
-      <c r="Q14" s="14"/>
-      <c r="R14" s="14"/>
-      <c r="S14" s="14"/>
       <c r="T14" s="5"/>
     </row>
     <row r="15" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B15" s="4"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
-      <c r="K15" s="14"/>
-      <c r="L15" s="14"/>
-      <c r="M15" s="14"/>
-      <c r="N15" s="14"/>
-      <c r="O15" s="14"/>
-      <c r="P15" s="14"/>
-      <c r="Q15" s="14"/>
-      <c r="R15" s="14"/>
-      <c r="S15" s="14"/>
       <c r="T15" s="5"/>
     </row>
     <row r="16" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B16" s="4"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="14"/>
-      <c r="I16" s="14"/>
-      <c r="J16" s="14"/>
-      <c r="K16" s="14"/>
-      <c r="L16" s="14"/>
-      <c r="M16" s="14"/>
-      <c r="N16" s="14"/>
-      <c r="O16" s="14"/>
-      <c r="P16" s="14"/>
-      <c r="Q16" s="14"/>
-      <c r="R16" s="14"/>
-      <c r="S16" s="14"/>
       <c r="T16" s="5"/>
     </row>
     <row r="17" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B17" s="4"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="14"/>
-      <c r="I17" s="14"/>
-      <c r="J17" s="14"/>
-      <c r="K17" s="14"/>
-      <c r="L17" s="14"/>
-      <c r="M17" s="14"/>
-      <c r="N17" s="14"/>
-      <c r="O17" s="14"/>
-      <c r="P17" s="14"/>
-      <c r="Q17" s="14"/>
-      <c r="R17" s="14"/>
-      <c r="S17" s="14"/>
       <c r="T17" s="5"/>
     </row>
     <row r="18" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B18" s="4"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
-      <c r="H18" s="14"/>
-      <c r="I18" s="14"/>
-      <c r="J18" s="14"/>
-      <c r="K18" s="14"/>
-      <c r="L18" s="14"/>
-      <c r="M18" s="14"/>
-      <c r="N18" s="14"/>
-      <c r="O18" s="14"/>
-      <c r="P18" s="14"/>
-      <c r="Q18" s="14"/>
-      <c r="R18" s="14"/>
-      <c r="S18" s="14"/>
       <c r="T18" s="5"/>
     </row>
     <row r="19" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B19" s="4"/>
-      <c r="C19" s="14"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="14"/>
-      <c r="I19" s="14"/>
-      <c r="J19" s="14"/>
-      <c r="K19" s="14"/>
-      <c r="L19" s="14"/>
-      <c r="M19" s="14"/>
-      <c r="N19" s="14"/>
-      <c r="O19" s="14"/>
-      <c r="P19" s="14"/>
-      <c r="Q19" s="14"/>
-      <c r="R19" s="14"/>
-      <c r="S19" s="14"/>
       <c r="T19" s="5"/>
     </row>
     <row r="20" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B20" s="4"/>
-      <c r="C20" s="14"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
-      <c r="G20" s="14"/>
-      <c r="H20" s="14"/>
-      <c r="I20" s="14"/>
-      <c r="J20" s="14"/>
-      <c r="K20" s="14"/>
-      <c r="L20" s="14"/>
-      <c r="M20" s="14"/>
-      <c r="N20" s="14"/>
-      <c r="O20" s="14"/>
-      <c r="P20" s="14"/>
-      <c r="Q20" s="14"/>
-      <c r="R20" s="14"/>
-      <c r="S20" s="14"/>
       <c r="T20" s="5"/>
     </row>
     <row r="21" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B21" s="4"/>
-      <c r="C21" s="14"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="14"/>
-      <c r="H21" s="14"/>
-      <c r="I21" s="14"/>
-      <c r="J21" s="14"/>
-      <c r="K21" s="14"/>
-      <c r="L21" s="14"/>
-      <c r="M21" s="14"/>
-      <c r="N21" s="14"/>
-      <c r="O21" s="14"/>
-      <c r="P21" s="14"/>
-      <c r="Q21" s="14"/>
-      <c r="R21" s="14"/>
-      <c r="S21" s="14"/>
       <c r="T21" s="5"/>
     </row>
     <row r="22" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B22" s="4"/>
-      <c r="C22" s="14"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="14"/>
-      <c r="G22" s="14"/>
-      <c r="H22" s="14"/>
-      <c r="I22" s="14"/>
-      <c r="J22" s="14"/>
-      <c r="K22" s="14"/>
-      <c r="L22" s="14"/>
-      <c r="M22" s="14"/>
-      <c r="N22" s="14"/>
-      <c r="O22" s="14"/>
-      <c r="P22" s="14"/>
-      <c r="Q22" s="14"/>
-      <c r="R22" s="14"/>
-      <c r="S22" s="14"/>
       <c r="T22" s="5"/>
     </row>
     <row r="23" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B23" s="4"/>
-      <c r="C23" s="14"/>
-      <c r="D23" s="14"/>
-      <c r="E23" s="14"/>
-      <c r="F23" s="14"/>
-      <c r="G23" s="14"/>
-      <c r="H23" s="14"/>
-      <c r="I23" s="14"/>
-      <c r="J23" s="14"/>
-      <c r="K23" s="14"/>
-      <c r="L23" s="14"/>
-      <c r="M23" s="14"/>
-      <c r="N23" s="14"/>
-      <c r="O23" s="14"/>
-      <c r="P23" s="14"/>
-      <c r="Q23" s="14"/>
-      <c r="R23" s="14"/>
-      <c r="S23" s="14"/>
       <c r="T23" s="5"/>
     </row>
     <row r="24" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B24" s="4"/>
-      <c r="C24" s="14"/>
-      <c r="D24" s="14"/>
-      <c r="E24" s="14"/>
-      <c r="F24" s="14"/>
-      <c r="G24" s="14"/>
-      <c r="H24" s="14"/>
-      <c r="I24" s="14"/>
-      <c r="J24" s="14"/>
-      <c r="K24" s="14"/>
-      <c r="L24" s="14"/>
-      <c r="M24" s="14"/>
-      <c r="N24" s="14"/>
-      <c r="O24" s="14"/>
-      <c r="P24" s="14"/>
-      <c r="Q24" s="14"/>
-      <c r="R24" s="14"/>
-      <c r="S24" s="14"/>
       <c r="T24" s="5"/>
     </row>
     <row r="25" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B25" s="4"/>
-      <c r="C25" s="14"/>
-      <c r="D25" s="14"/>
-      <c r="E25" s="14"/>
-      <c r="F25" s="14"/>
-      <c r="G25" s="14"/>
-      <c r="H25" s="14"/>
-      <c r="I25" s="14"/>
-      <c r="J25" s="14"/>
-      <c r="K25" s="14"/>
-      <c r="L25" s="14"/>
-      <c r="M25" s="14"/>
-      <c r="N25" s="14"/>
-      <c r="O25" s="14"/>
-      <c r="P25" s="14"/>
-      <c r="Q25" s="14"/>
-      <c r="R25" s="14"/>
-      <c r="S25" s="14"/>
       <c r="T25" s="5"/>
     </row>
     <row r="26" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B26" s="4"/>
-      <c r="C26" s="14"/>
-      <c r="D26" s="14"/>
-      <c r="E26" s="14"/>
-      <c r="F26" s="14"/>
-      <c r="G26" s="14"/>
-      <c r="H26" s="14"/>
-      <c r="I26" s="14"/>
-      <c r="J26" s="14"/>
-      <c r="K26" s="14"/>
-      <c r="L26" s="14"/>
-      <c r="M26" s="14"/>
-      <c r="N26" s="14"/>
-      <c r="O26" s="14"/>
-      <c r="P26" s="14"/>
-      <c r="Q26" s="14"/>
-      <c r="R26" s="14"/>
-      <c r="S26" s="14"/>
       <c r="T26" s="5"/>
     </row>
     <row r="27" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B27" s="4"/>
-      <c r="C27" s="14"/>
-      <c r="D27" s="14"/>
-      <c r="E27" s="14"/>
-      <c r="F27" s="14"/>
-      <c r="G27" s="14"/>
-      <c r="H27" s="14"/>
-      <c r="I27" s="14"/>
-      <c r="J27" s="14"/>
-      <c r="K27" s="14"/>
-      <c r="L27" s="14"/>
-      <c r="M27" s="14"/>
-      <c r="N27" s="14"/>
-      <c r="O27" s="14"/>
-      <c r="P27" s="14"/>
-      <c r="Q27" s="14"/>
-      <c r="R27" s="14"/>
-      <c r="S27" s="14"/>
       <c r="T27" s="5"/>
     </row>
     <row r="28" spans="2:20" x14ac:dyDescent="0.25">
@@ -4999,445 +5209,88 @@
       <c r="B32" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="C32" s="14"/>
-      <c r="D32" s="14"/>
-      <c r="E32" s="14"/>
-      <c r="F32" s="14"/>
-      <c r="G32" s="14"/>
-      <c r="H32" s="14"/>
-      <c r="I32" s="14"/>
-      <c r="J32" s="14"/>
-      <c r="K32" s="14"/>
-      <c r="L32" s="14"/>
-      <c r="M32" s="14"/>
-      <c r="N32" s="14"/>
-      <c r="O32" s="14"/>
-      <c r="P32" s="14"/>
-      <c r="Q32" s="14"/>
-      <c r="R32" s="14"/>
-      <c r="S32" s="14"/>
       <c r="T32" s="5"/>
     </row>
     <row r="33" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B33" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="C33" s="14"/>
-      <c r="D33" s="14"/>
-      <c r="E33" s="14"/>
-      <c r="F33" s="14"/>
-      <c r="G33" s="14"/>
-      <c r="H33" s="14"/>
-      <c r="I33" s="14"/>
-      <c r="J33" s="14"/>
-      <c r="K33" s="14"/>
-      <c r="L33" s="14"/>
-      <c r="M33" s="14"/>
-      <c r="N33" s="14"/>
-      <c r="O33" s="14"/>
-      <c r="P33" s="14"/>
-      <c r="Q33" s="14"/>
-      <c r="R33" s="14"/>
-      <c r="S33" s="14"/>
       <c r="T33" s="5"/>
     </row>
     <row r="34" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B34" s="4"/>
-      <c r="C34" s="14"/>
-      <c r="D34" s="14"/>
-      <c r="E34" s="14"/>
-      <c r="F34" s="14"/>
-      <c r="G34" s="14"/>
-      <c r="H34" s="14"/>
-      <c r="I34" s="14"/>
-      <c r="J34" s="14"/>
-      <c r="K34" s="14"/>
-      <c r="L34" s="14"/>
-      <c r="M34" s="14"/>
-      <c r="N34" s="14"/>
-      <c r="O34" s="14"/>
-      <c r="P34" s="14"/>
-      <c r="Q34" s="14"/>
-      <c r="R34" s="14"/>
-      <c r="S34" s="14"/>
       <c r="T34" s="5"/>
     </row>
     <row r="35" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B35" s="4"/>
-      <c r="C35" s="14"/>
-      <c r="D35" s="14"/>
-      <c r="E35" s="14"/>
-      <c r="F35" s="14"/>
-      <c r="G35" s="14"/>
-      <c r="H35" s="14"/>
-      <c r="I35" s="14"/>
-      <c r="J35" s="14"/>
-      <c r="K35" s="14"/>
-      <c r="L35" s="14"/>
-      <c r="M35" s="14"/>
-      <c r="N35" s="14"/>
-      <c r="O35" s="14"/>
-      <c r="P35" s="14"/>
-      <c r="Q35" s="14"/>
-      <c r="R35" s="14"/>
-      <c r="S35" s="14"/>
       <c r="T35" s="5"/>
     </row>
     <row r="36" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B36" s="4"/>
-      <c r="C36" s="14"/>
-      <c r="D36" s="14"/>
-      <c r="E36" s="14"/>
-      <c r="F36" s="14"/>
-      <c r="G36" s="14"/>
-      <c r="H36" s="14"/>
-      <c r="I36" s="14"/>
-      <c r="J36" s="14"/>
-      <c r="K36" s="14"/>
-      <c r="L36" s="14"/>
-      <c r="M36" s="14"/>
-      <c r="N36" s="14"/>
-      <c r="O36" s="14"/>
-      <c r="P36" s="14"/>
-      <c r="Q36" s="14"/>
-      <c r="R36" s="14"/>
-      <c r="S36" s="14"/>
       <c r="T36" s="5"/>
     </row>
     <row r="37" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B37" s="4"/>
-      <c r="C37" s="14"/>
-      <c r="D37" s="14"/>
-      <c r="E37" s="14"/>
-      <c r="F37" s="14"/>
-      <c r="G37" s="14"/>
-      <c r="H37" s="14"/>
-      <c r="I37" s="14"/>
-      <c r="J37" s="14"/>
-      <c r="K37" s="14"/>
-      <c r="L37" s="14"/>
-      <c r="M37" s="14"/>
-      <c r="N37" s="14"/>
-      <c r="O37" s="14"/>
-      <c r="P37" s="14"/>
-      <c r="Q37" s="14"/>
-      <c r="R37" s="14"/>
-      <c r="S37" s="14"/>
       <c r="T37" s="5"/>
     </row>
     <row r="38" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B38" s="4"/>
-      <c r="C38" s="14"/>
-      <c r="D38" s="14"/>
-      <c r="E38" s="14"/>
-      <c r="F38" s="14"/>
-      <c r="G38" s="14"/>
-      <c r="H38" s="14"/>
-      <c r="I38" s="14"/>
-      <c r="J38" s="14"/>
-      <c r="K38" s="14"/>
-      <c r="L38" s="14"/>
-      <c r="M38" s="14"/>
-      <c r="N38" s="14"/>
-      <c r="O38" s="14"/>
-      <c r="P38" s="14"/>
-      <c r="Q38" s="14"/>
-      <c r="R38" s="14"/>
-      <c r="S38" s="14"/>
       <c r="T38" s="5"/>
     </row>
     <row r="39" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B39" s="4"/>
-      <c r="C39" s="14"/>
-      <c r="D39" s="14"/>
-      <c r="E39" s="14"/>
-      <c r="F39" s="14"/>
-      <c r="G39" s="14"/>
-      <c r="H39" s="14"/>
-      <c r="I39" s="14"/>
-      <c r="J39" s="14"/>
-      <c r="K39" s="14"/>
-      <c r="L39" s="14"/>
-      <c r="M39" s="14"/>
-      <c r="N39" s="14"/>
-      <c r="O39" s="14"/>
-      <c r="P39" s="14"/>
-      <c r="Q39" s="14"/>
-      <c r="R39" s="14"/>
-      <c r="S39" s="14"/>
       <c r="T39" s="5"/>
     </row>
     <row r="40" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B40" s="4"/>
-      <c r="C40" s="14"/>
-      <c r="D40" s="14"/>
-      <c r="E40" s="14"/>
-      <c r="F40" s="14"/>
-      <c r="G40" s="14"/>
-      <c r="H40" s="14"/>
-      <c r="I40" s="14"/>
-      <c r="J40" s="14"/>
-      <c r="K40" s="14"/>
-      <c r="L40" s="14"/>
-      <c r="M40" s="14"/>
-      <c r="N40" s="14"/>
-      <c r="O40" s="14"/>
-      <c r="P40" s="14"/>
-      <c r="Q40" s="14"/>
-      <c r="R40" s="14"/>
-      <c r="S40" s="14"/>
       <c r="T40" s="5"/>
     </row>
     <row r="41" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B41" s="4"/>
-      <c r="C41" s="14"/>
-      <c r="D41" s="14"/>
-      <c r="E41" s="14"/>
-      <c r="F41" s="14"/>
-      <c r="G41" s="14"/>
-      <c r="H41" s="14"/>
-      <c r="I41" s="14"/>
-      <c r="J41" s="14"/>
-      <c r="K41" s="14"/>
-      <c r="L41" s="14"/>
-      <c r="M41" s="14"/>
-      <c r="N41" s="14"/>
-      <c r="O41" s="14"/>
-      <c r="P41" s="14"/>
-      <c r="Q41" s="14"/>
-      <c r="R41" s="14"/>
-      <c r="S41" s="14"/>
       <c r="T41" s="5"/>
     </row>
     <row r="42" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B42" s="4"/>
-      <c r="C42" s="14"/>
-      <c r="D42" s="14"/>
-      <c r="E42" s="14"/>
-      <c r="F42" s="14"/>
-      <c r="G42" s="14"/>
-      <c r="H42" s="14"/>
-      <c r="I42" s="14"/>
-      <c r="J42" s="14"/>
-      <c r="K42" s="14"/>
-      <c r="L42" s="14"/>
-      <c r="M42" s="14"/>
-      <c r="N42" s="14"/>
-      <c r="O42" s="14"/>
-      <c r="P42" s="14"/>
-      <c r="Q42" s="14"/>
-      <c r="R42" s="14"/>
-      <c r="S42" s="14"/>
       <c r="T42" s="5"/>
     </row>
     <row r="43" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B43" s="4"/>
-      <c r="C43" s="14"/>
-      <c r="D43" s="14"/>
-      <c r="E43" s="14"/>
-      <c r="F43" s="14"/>
-      <c r="G43" s="14"/>
-      <c r="H43" s="14"/>
-      <c r="I43" s="14"/>
-      <c r="J43" s="14"/>
-      <c r="K43" s="14"/>
-      <c r="L43" s="14"/>
-      <c r="M43" s="14"/>
-      <c r="N43" s="14"/>
-      <c r="O43" s="14"/>
-      <c r="P43" s="14"/>
-      <c r="Q43" s="14"/>
-      <c r="R43" s="14"/>
-      <c r="S43" s="14"/>
       <c r="T43" s="5"/>
     </row>
     <row r="44" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B44" s="4"/>
-      <c r="C44" s="14"/>
-      <c r="D44" s="14"/>
-      <c r="E44" s="14"/>
-      <c r="F44" s="14"/>
-      <c r="G44" s="14"/>
-      <c r="H44" s="14"/>
-      <c r="I44" s="14"/>
-      <c r="J44" s="14"/>
-      <c r="K44" s="14"/>
-      <c r="L44" s="14"/>
-      <c r="M44" s="14"/>
-      <c r="N44" s="14"/>
-      <c r="O44" s="14"/>
-      <c r="P44" s="14"/>
-      <c r="Q44" s="14"/>
-      <c r="R44" s="14"/>
-      <c r="S44" s="14"/>
       <c r="T44" s="5"/>
     </row>
     <row r="45" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B45" s="4"/>
-      <c r="C45" s="14"/>
-      <c r="D45" s="14"/>
-      <c r="E45" s="14"/>
-      <c r="F45" s="14"/>
-      <c r="G45" s="14"/>
-      <c r="H45" s="14"/>
-      <c r="I45" s="14"/>
-      <c r="J45" s="14"/>
-      <c r="K45" s="14"/>
-      <c r="L45" s="14"/>
-      <c r="M45" s="14"/>
-      <c r="N45" s="14"/>
-      <c r="O45" s="14"/>
-      <c r="P45" s="14"/>
-      <c r="Q45" s="14"/>
-      <c r="R45" s="14"/>
-      <c r="S45" s="14"/>
       <c r="T45" s="5"/>
     </row>
     <row r="46" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B46" s="4"/>
-      <c r="C46" s="14"/>
-      <c r="D46" s="14"/>
-      <c r="E46" s="14"/>
-      <c r="F46" s="14"/>
-      <c r="G46" s="14"/>
-      <c r="H46" s="14"/>
-      <c r="I46" s="14"/>
-      <c r="J46" s="14"/>
-      <c r="K46" s="14"/>
-      <c r="L46" s="14"/>
-      <c r="M46" s="14"/>
-      <c r="N46" s="14"/>
-      <c r="O46" s="14"/>
-      <c r="P46" s="14"/>
-      <c r="Q46" s="14"/>
-      <c r="R46" s="14"/>
-      <c r="S46" s="14"/>
       <c r="T46" s="5"/>
     </row>
     <row r="47" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B47" s="4"/>
-      <c r="C47" s="14"/>
-      <c r="D47" s="14"/>
-      <c r="E47" s="14"/>
-      <c r="F47" s="14"/>
-      <c r="G47" s="14"/>
-      <c r="H47" s="14"/>
-      <c r="I47" s="14"/>
-      <c r="J47" s="14"/>
-      <c r="K47" s="14"/>
-      <c r="L47" s="14"/>
-      <c r="M47" s="14"/>
-      <c r="N47" s="14"/>
-      <c r="O47" s="14"/>
-      <c r="P47" s="14"/>
-      <c r="Q47" s="14"/>
-      <c r="R47" s="14"/>
-      <c r="S47" s="14"/>
       <c r="T47" s="5"/>
     </row>
     <row r="48" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B48" s="4"/>
-      <c r="C48" s="14"/>
-      <c r="D48" s="14"/>
-      <c r="E48" s="14"/>
-      <c r="F48" s="14"/>
-      <c r="G48" s="14"/>
-      <c r="H48" s="14"/>
-      <c r="I48" s="14"/>
-      <c r="J48" s="14"/>
-      <c r="K48" s="14"/>
-      <c r="L48" s="14"/>
-      <c r="M48" s="14"/>
-      <c r="N48" s="14"/>
-      <c r="O48" s="14"/>
-      <c r="P48" s="14"/>
-      <c r="Q48" s="14"/>
-      <c r="R48" s="14"/>
-      <c r="S48" s="14"/>
       <c r="T48" s="5"/>
     </row>
     <row r="49" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B49" s="4"/>
-      <c r="C49" s="14"/>
-      <c r="D49" s="14"/>
-      <c r="E49" s="14"/>
-      <c r="F49" s="14"/>
-      <c r="G49" s="14"/>
-      <c r="H49" s="14"/>
-      <c r="I49" s="14"/>
-      <c r="J49" s="14"/>
-      <c r="K49" s="14"/>
-      <c r="L49" s="14"/>
-      <c r="M49" s="14"/>
-      <c r="N49" s="14"/>
-      <c r="O49" s="14"/>
-      <c r="P49" s="14"/>
-      <c r="Q49" s="14"/>
-      <c r="R49" s="14"/>
-      <c r="S49" s="14"/>
       <c r="T49" s="5"/>
     </row>
     <row r="50" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B50" s="4"/>
-      <c r="C50" s="14"/>
-      <c r="D50" s="14"/>
-      <c r="E50" s="14"/>
-      <c r="F50" s="14"/>
-      <c r="G50" s="14"/>
-      <c r="H50" s="14"/>
-      <c r="I50" s="14"/>
-      <c r="J50" s="14"/>
-      <c r="K50" s="14"/>
-      <c r="L50" s="14"/>
-      <c r="M50" s="14"/>
-      <c r="N50" s="14"/>
-      <c r="O50" s="14"/>
-      <c r="P50" s="14"/>
-      <c r="Q50" s="14"/>
-      <c r="R50" s="14"/>
-      <c r="S50" s="14"/>
       <c r="T50" s="5"/>
     </row>
     <row r="51" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B51" s="4"/>
-      <c r="C51" s="14"/>
-      <c r="D51" s="14"/>
-      <c r="E51" s="14"/>
-      <c r="F51" s="14"/>
-      <c r="G51" s="14"/>
-      <c r="H51" s="14"/>
-      <c r="I51" s="14"/>
-      <c r="J51" s="14"/>
-      <c r="K51" s="14"/>
-      <c r="L51" s="14"/>
-      <c r="M51" s="14"/>
-      <c r="N51" s="14"/>
-      <c r="O51" s="14"/>
-      <c r="P51" s="14"/>
-      <c r="Q51" s="14"/>
-      <c r="R51" s="14"/>
-      <c r="S51" s="14"/>
       <c r="T51" s="5"/>
     </row>
     <row r="52" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B52" s="4"/>
-      <c r="C52" s="14"/>
-      <c r="D52" s="14"/>
-      <c r="E52" s="14"/>
-      <c r="F52" s="14"/>
-      <c r="G52" s="14"/>
-      <c r="H52" s="14"/>
-      <c r="I52" s="14"/>
-      <c r="J52" s="14"/>
-      <c r="K52" s="14"/>
-      <c r="L52" s="14"/>
-      <c r="M52" s="14"/>
-      <c r="N52" s="14"/>
-      <c r="O52" s="14"/>
-      <c r="P52" s="14"/>
-      <c r="Q52" s="14"/>
-      <c r="R52" s="14"/>
-      <c r="S52" s="14"/>
       <c r="T52" s="5"/>
     </row>
     <row r="53" spans="1:20" x14ac:dyDescent="0.25">
@@ -5584,130 +5437,70 @@
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B73" s="4"/>
-      <c r="C73" s="14"/>
-      <c r="D73" s="14"/>
-      <c r="E73" s="14"/>
-      <c r="F73" s="14"/>
-      <c r="G73" s="14"/>
       <c r="H73" s="5"/>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B74" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C74" s="14"/>
-      <c r="D74" s="14"/>
-      <c r="E74" s="14"/>
-      <c r="F74" s="14"/>
-      <c r="G74" s="14"/>
       <c r="H74" s="5"/>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B75" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C75" s="14"/>
-      <c r="D75" s="14"/>
-      <c r="E75" s="14"/>
-      <c r="F75" s="14"/>
-      <c r="G75" s="14"/>
       <c r="H75" s="5"/>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B76" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C76" s="14"/>
-      <c r="D76" s="14"/>
-      <c r="E76" s="14"/>
-      <c r="F76" s="14"/>
-      <c r="G76" s="14"/>
       <c r="H76" s="5"/>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B77" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C77" s="14"/>
-      <c r="D77" s="14"/>
-      <c r="E77" s="14"/>
-      <c r="F77" s="14"/>
-      <c r="G77" s="14"/>
       <c r="H77" s="5"/>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B78" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C78" s="14"/>
-      <c r="D78" s="14"/>
-      <c r="E78" s="14"/>
-      <c r="F78" s="14"/>
-      <c r="G78" s="14"/>
       <c r="H78" s="5"/>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B79" s="4"/>
-      <c r="C79" s="14"/>
-      <c r="D79" s="14"/>
-      <c r="E79" s="14"/>
-      <c r="F79" s="14"/>
-      <c r="G79" s="14"/>
       <c r="H79" s="5"/>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B80" s="15" t="s">
+      <c r="B80" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="C80" s="14"/>
-      <c r="D80" s="14"/>
-      <c r="E80" s="14"/>
-      <c r="F80" s="14"/>
-      <c r="G80" s="14"/>
       <c r="H80" s="5"/>
     </row>
     <row r="81" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B81" s="15" t="s">
+      <c r="B81" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="C81" s="14"/>
-      <c r="D81" s="14"/>
-      <c r="E81" s="14"/>
-      <c r="F81" s="14"/>
-      <c r="G81" s="14"/>
       <c r="H81" s="5"/>
     </row>
     <row r="82" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B82" s="15" t="s">
+      <c r="B82" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="C82" s="14"/>
-      <c r="D82" s="14"/>
-      <c r="E82" s="14"/>
-      <c r="F82" s="14"/>
-      <c r="G82" s="14"/>
       <c r="H82" s="5"/>
     </row>
     <row r="83" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B83" s="15" t="s">
+      <c r="B83" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="C83" s="14"/>
-      <c r="D83" s="14"/>
-      <c r="E83" s="14"/>
-      <c r="F83" s="14"/>
-      <c r="G83" s="14"/>
       <c r="H83" s="5"/>
     </row>
     <row r="84" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B84" s="15" t="s">
+      <c r="B84" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="C84" s="14"/>
-      <c r="D84" s="14"/>
-      <c r="E84" s="14"/>
-      <c r="F84" s="14"/>
-      <c r="G84" s="14"/>
       <c r="H84" s="5"/>
       <c r="I84" t="s">
         <v>20</v>
@@ -5717,111 +5510,61 @@
       </c>
     </row>
     <row r="85" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B85" s="15"/>
-      <c r="C85" s="14"/>
-      <c r="D85" s="14"/>
-      <c r="E85" s="14"/>
-      <c r="F85" s="14"/>
-      <c r="G85" s="14"/>
+      <c r="B85" s="14"/>
       <c r="H85" s="5"/>
     </row>
     <row r="86" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B86" s="15" t="s">
+      <c r="B86" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="C86" s="14"/>
-      <c r="D86" s="14"/>
-      <c r="E86" s="14"/>
-      <c r="F86" s="14"/>
-      <c r="G86" s="14"/>
       <c r="H86" s="5"/>
     </row>
     <row r="87" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B87" s="15" t="s">
+      <c r="B87" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="C87" s="14"/>
-      <c r="D87" s="14"/>
-      <c r="E87" s="14"/>
-      <c r="F87" s="14"/>
-      <c r="G87" s="14"/>
       <c r="H87" s="5"/>
     </row>
     <row r="88" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B88" s="15" t="s">
+      <c r="B88" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="C88" s="14"/>
-      <c r="D88" s="14"/>
-      <c r="E88" s="14"/>
-      <c r="F88" s="14"/>
-      <c r="G88" s="14"/>
       <c r="H88" s="5"/>
     </row>
     <row r="89" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B89" s="15" t="s">
+      <c r="B89" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="C89" s="14"/>
-      <c r="D89" s="14"/>
-      <c r="E89" s="14"/>
-      <c r="F89" s="14"/>
-      <c r="G89" s="14"/>
       <c r="H89" s="5"/>
     </row>
     <row r="90" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B90" s="15" t="s">
+      <c r="B90" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="C90" s="14"/>
-      <c r="D90" s="14"/>
-      <c r="E90" s="14"/>
-      <c r="F90" s="14"/>
-      <c r="G90" s="14"/>
       <c r="H90" s="5"/>
     </row>
     <row r="91" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B91" s="15" t="s">
+      <c r="B91" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="C91" s="14"/>
-      <c r="D91" s="14"/>
-      <c r="E91" s="14"/>
-      <c r="F91" s="14"/>
-      <c r="G91" s="14"/>
       <c r="H91" s="5"/>
     </row>
     <row r="92" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B92" s="15" t="s">
+      <c r="B92" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="C92" s="14"/>
-      <c r="D92" s="14"/>
-      <c r="E92" s="14"/>
-      <c r="F92" s="14"/>
-      <c r="G92" s="14"/>
       <c r="H92" s="5"/>
     </row>
     <row r="93" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B93" s="15" t="s">
+      <c r="B93" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="C93" s="14"/>
-      <c r="D93" s="14"/>
-      <c r="E93" s="14"/>
-      <c r="F93" s="14"/>
-      <c r="G93" s="14"/>
       <c r="H93" s="5"/>
     </row>
     <row r="94" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B94" s="15" t="s">
+      <c r="B94" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="C94" s="14"/>
-      <c r="D94" s="14"/>
-      <c r="E94" s="14"/>
-      <c r="F94" s="14"/>
-      <c r="G94" s="14"/>
       <c r="H94" s="5"/>
       <c r="I94" t="s">
         <v>20</v>
@@ -5831,114 +5574,64 @@
       </c>
     </row>
     <row r="95" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B95" s="15" t="s">
+      <c r="B95" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="C95" s="14"/>
-      <c r="D95" s="14"/>
-      <c r="E95" s="14"/>
-      <c r="F95" s="14"/>
-      <c r="G95" s="14"/>
       <c r="H95" s="5"/>
       <c r="J95" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="96" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B96" s="15" t="s">
+      <c r="B96" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="C96" s="14"/>
-      <c r="D96" s="14"/>
-      <c r="E96" s="14"/>
-      <c r="F96" s="14"/>
-      <c r="G96" s="14"/>
       <c r="H96" s="5"/>
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B97" s="15" t="s">
+      <c r="B97" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="C97" s="14"/>
-      <c r="D97" s="14"/>
-      <c r="E97" s="14"/>
-      <c r="F97" s="14"/>
-      <c r="G97" s="14"/>
       <c r="H97" s="5"/>
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B98" s="15"/>
-      <c r="C98" s="14"/>
-      <c r="D98" s="14"/>
-      <c r="E98" s="14"/>
-      <c r="F98" s="14"/>
-      <c r="G98" s="14"/>
+      <c r="B98" s="14"/>
       <c r="H98" s="5"/>
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B99" s="15" t="s">
+      <c r="B99" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="C99" s="14"/>
-      <c r="D99" s="14"/>
-      <c r="E99" s="14"/>
-      <c r="F99" s="14"/>
-      <c r="G99" s="14"/>
       <c r="H99" s="5"/>
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B100" s="15" t="s">
+      <c r="B100" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="C100" s="14"/>
-      <c r="D100" s="14"/>
-      <c r="E100" s="14"/>
-      <c r="F100" s="14"/>
-      <c r="G100" s="14"/>
       <c r="H100" s="5"/>
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B101" s="15" t="s">
+      <c r="B101" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="C101" s="14"/>
-      <c r="D101" s="14"/>
-      <c r="E101" s="14"/>
-      <c r="F101" s="14"/>
-      <c r="G101" s="14"/>
       <c r="H101" s="5"/>
     </row>
     <row r="102" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B102" s="15" t="s">
+      <c r="B102" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="C102" s="14"/>
-      <c r="D102" s="14"/>
-      <c r="E102" s="14"/>
-      <c r="F102" s="14"/>
-      <c r="G102" s="14"/>
       <c r="H102" s="5"/>
     </row>
     <row r="103" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B103" s="15" t="s">
+      <c r="B103" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="C103" s="14"/>
-      <c r="D103" s="14"/>
-      <c r="E103" s="14"/>
-      <c r="F103" s="14"/>
-      <c r="G103" s="14"/>
       <c r="H103" s="5"/>
     </row>
     <row r="104" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B104" s="15" t="s">
+      <c r="B104" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="C104" s="14"/>
-      <c r="D104" s="14"/>
-      <c r="E104" s="14"/>
-      <c r="F104" s="14"/>
-      <c r="G104" s="14"/>
       <c r="H104" s="5"/>
       <c r="I104" t="s">
         <v>20</v>
@@ -5948,36 +5641,21 @@
       </c>
     </row>
     <row r="105" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B105" s="15" t="s">
+      <c r="B105" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="C105" s="14"/>
-      <c r="D105" s="14"/>
-      <c r="E105" s="14"/>
-      <c r="F105" s="14"/>
-      <c r="G105" s="14"/>
       <c r="H105" s="5"/>
     </row>
     <row r="106" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B106" s="15" t="s">
+      <c r="B106" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="C106" s="14"/>
-      <c r="D106" s="14"/>
-      <c r="E106" s="14"/>
-      <c r="F106" s="14"/>
-      <c r="G106" s="14"/>
       <c r="H106" s="5"/>
     </row>
     <row r="107" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B107" s="15" t="s">
+      <c r="B107" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="C107" s="14"/>
-      <c r="D107" s="14"/>
-      <c r="E107" s="14"/>
-      <c r="F107" s="14"/>
-      <c r="G107" s="14"/>
       <c r="H107" s="5"/>
     </row>
     <row r="108" spans="1:10" x14ac:dyDescent="0.25">
@@ -6009,148 +5687,78 @@
     </row>
     <row r="113" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B113" s="4"/>
-      <c r="C113" s="14"/>
-      <c r="D113" s="14"/>
-      <c r="E113" s="14"/>
-      <c r="F113" s="14"/>
-      <c r="G113" s="14"/>
       <c r="H113" s="5"/>
     </row>
     <row r="114" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B114" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C114" s="14"/>
-      <c r="D114" s="14"/>
-      <c r="E114" s="14"/>
-      <c r="F114" s="14"/>
-      <c r="G114" s="14"/>
       <c r="H114" s="5"/>
     </row>
     <row r="115" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B115" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C115" s="14"/>
-      <c r="D115" s="14"/>
-      <c r="E115" s="14"/>
-      <c r="F115" s="14"/>
-      <c r="G115" s="14"/>
       <c r="H115" s="5"/>
     </row>
     <row r="116" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B116" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C116" s="14"/>
-      <c r="D116" s="14"/>
-      <c r="E116" s="14"/>
-      <c r="F116" s="14"/>
-      <c r="G116" s="14"/>
       <c r="H116" s="5"/>
     </row>
     <row r="117" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B117" s="4"/>
-      <c r="C117" s="14"/>
-      <c r="D117" s="14"/>
-      <c r="E117" s="14"/>
-      <c r="F117" s="14"/>
-      <c r="G117" s="14"/>
       <c r="H117" s="5"/>
     </row>
     <row r="118" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B118" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C118" s="14"/>
-      <c r="D118" s="14"/>
-      <c r="E118" s="14"/>
-      <c r="F118" s="14"/>
-      <c r="G118" s="14"/>
       <c r="H118" s="5"/>
     </row>
     <row r="119" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B119" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="C119" s="14"/>
-      <c r="D119" s="14"/>
-      <c r="E119" s="14"/>
-      <c r="F119" s="14"/>
-      <c r="G119" s="14"/>
       <c r="H119" s="5"/>
     </row>
     <row r="120" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B120" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C120" s="14"/>
-      <c r="D120" s="14"/>
-      <c r="E120" s="14"/>
-      <c r="F120" s="14"/>
-      <c r="G120" s="14"/>
       <c r="H120" s="5"/>
     </row>
     <row r="121" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B121" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C121" s="14"/>
-      <c r="D121" s="14"/>
-      <c r="E121" s="14"/>
-      <c r="F121" s="14"/>
-      <c r="G121" s="14"/>
       <c r="H121" s="5"/>
     </row>
     <row r="122" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B122" s="4"/>
-      <c r="C122" s="14"/>
-      <c r="D122" s="14"/>
-      <c r="E122" s="14"/>
-      <c r="F122" s="14"/>
-      <c r="G122" s="14"/>
       <c r="H122" s="5"/>
     </row>
     <row r="123" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B123" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="C123" s="14"/>
-      <c r="D123" s="14"/>
-      <c r="E123" s="14"/>
-      <c r="F123" s="14"/>
-      <c r="G123" s="14"/>
       <c r="H123" s="5"/>
     </row>
     <row r="124" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B124" s="4"/>
-      <c r="C124" s="14"/>
-      <c r="D124" s="14"/>
-      <c r="E124" s="14"/>
-      <c r="F124" s="14"/>
-      <c r="G124" s="14"/>
       <c r="H124" s="5"/>
     </row>
     <row r="125" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B125" s="15" t="s">
+      <c r="B125" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="C125" s="14"/>
-      <c r="D125" s="14"/>
-      <c r="E125" s="14"/>
-      <c r="F125" s="14"/>
-      <c r="G125" s="14"/>
       <c r="H125" s="5"/>
     </row>
     <row r="126" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B126" s="15" t="s">
+      <c r="B126" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="C126" s="14"/>
-      <c r="D126" s="14"/>
-      <c r="E126" s="14"/>
-      <c r="F126" s="14"/>
-      <c r="G126" s="14"/>
       <c r="H126" s="5"/>
       <c r="I126" t="s">
         <v>20</v>
@@ -6160,71 +5768,41 @@
       </c>
     </row>
     <row r="127" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B127" s="15" t="s">
+      <c r="B127" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="C127" s="14"/>
-      <c r="D127" s="14"/>
-      <c r="E127" s="14"/>
-      <c r="F127" s="14"/>
-      <c r="G127" s="14"/>
       <c r="H127" s="5"/>
     </row>
     <row r="128" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B128" s="15" t="s">
+      <c r="B128" s="14" t="s">
         <v>95</v>
       </c>
-      <c r="C128" s="14"/>
-      <c r="D128" s="14"/>
-      <c r="E128" s="14"/>
-      <c r="F128" s="14"/>
-      <c r="G128" s="14"/>
       <c r="H128" s="5"/>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B129" s="15"/>
-      <c r="C129" s="14"/>
-      <c r="D129" s="14"/>
-      <c r="E129" s="14"/>
-      <c r="F129" s="14"/>
-      <c r="G129" s="14"/>
+      <c r="B129" s="14"/>
       <c r="H129" s="5"/>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B130" s="15" t="s">
+      <c r="B130" s="14" t="s">
         <v>96</v>
       </c>
-      <c r="C130" s="14"/>
-      <c r="D130" s="14"/>
-      <c r="E130" s="14"/>
-      <c r="F130" s="14"/>
-      <c r="G130" s="14"/>
       <c r="H130" s="5"/>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B131" s="15" t="s">
+      <c r="B131" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="C131" s="14"/>
-      <c r="D131" s="14"/>
-      <c r="E131" s="14"/>
-      <c r="F131" s="14"/>
-      <c r="G131" s="14"/>
       <c r="H131" s="5"/>
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B132" s="15" t="s">
+      <c r="B132" s="14" t="s">
         <v>98</v>
       </c>
-      <c r="C132" s="14"/>
-      <c r="D132" s="14"/>
-      <c r="E132" s="14"/>
-      <c r="F132" s="14"/>
-      <c r="G132" s="14"/>
       <c r="H132" s="5"/>
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B133" s="16" t="s">
+      <c r="B133" s="15" t="s">
         <v>99</v>
       </c>
       <c r="C133" s="7"/>
@@ -6235,7 +5813,7 @@
       <c r="H133" s="8"/>
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A136" s="17" t="s">
+      <c r="A136" s="16" t="s">
         <v>23</v>
       </c>
       <c r="B136" s="2"/>
@@ -6248,234 +5826,97 @@
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A137" s="4"/>
-      <c r="B137" s="14" t="s">
+      <c r="B137" t="s">
         <v>105</v>
       </c>
-      <c r="C137" s="14"/>
-      <c r="D137" s="14"/>
-      <c r="E137" s="14"/>
-      <c r="F137" s="14"/>
-      <c r="G137" s="14"/>
       <c r="H137" s="5"/>
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A138" s="4"/>
-      <c r="B138" s="14"/>
-      <c r="C138" s="14"/>
-      <c r="D138" s="14"/>
-      <c r="E138" s="14"/>
-      <c r="F138" s="14"/>
-      <c r="G138" s="14"/>
       <c r="H138" s="5"/>
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A139" s="4"/>
-      <c r="B139" s="14"/>
-      <c r="C139" s="14"/>
-      <c r="D139" s="14"/>
-      <c r="E139" s="14"/>
-      <c r="F139" s="14"/>
-      <c r="G139" s="14"/>
       <c r="H139" s="5"/>
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A140" s="4"/>
-      <c r="B140" s="14"/>
-      <c r="C140" s="14"/>
-      <c r="D140" s="14"/>
-      <c r="E140" s="14"/>
-      <c r="F140" s="14"/>
-      <c r="G140" s="14"/>
       <c r="H140" s="5"/>
     </row>
     <row r="141" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A141" s="4"/>
-      <c r="B141" s="14"/>
-      <c r="C141" s="14"/>
-      <c r="D141" s="14"/>
-      <c r="E141" s="14"/>
-      <c r="F141" s="14"/>
-      <c r="G141" s="14"/>
       <c r="H141" s="5"/>
     </row>
     <row r="142" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A142" s="4"/>
-      <c r="B142" s="14"/>
-      <c r="C142" s="14"/>
-      <c r="D142" s="14"/>
-      <c r="E142" s="14"/>
-      <c r="F142" s="14"/>
-      <c r="G142" s="14"/>
       <c r="H142" s="5"/>
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A143" s="4"/>
-      <c r="B143" s="14"/>
-      <c r="C143" s="14"/>
-      <c r="D143" s="14"/>
-      <c r="E143" s="14"/>
-      <c r="F143" s="14"/>
-      <c r="G143" s="14"/>
       <c r="H143" s="5"/>
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A144" s="4"/>
-      <c r="B144" s="14"/>
-      <c r="C144" s="14"/>
-      <c r="D144" s="14"/>
-      <c r="E144" s="14"/>
-      <c r="F144" s="14"/>
-      <c r="G144" s="14"/>
       <c r="H144" s="5"/>
     </row>
     <row r="145" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A145" s="4"/>
-      <c r="B145" s="14"/>
-      <c r="C145" s="14"/>
-      <c r="D145" s="14"/>
-      <c r="E145" s="14"/>
-      <c r="F145" s="14"/>
-      <c r="G145" s="14"/>
       <c r="H145" s="5"/>
     </row>
     <row r="146" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A146" s="4"/>
-      <c r="B146" s="14"/>
-      <c r="C146" s="14"/>
-      <c r="D146" s="14"/>
-      <c r="E146" s="14"/>
-      <c r="F146" s="14"/>
-      <c r="G146" s="14"/>
       <c r="H146" s="5"/>
     </row>
     <row r="147" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A147" s="4"/>
-      <c r="B147" s="14"/>
-      <c r="C147" s="14"/>
-      <c r="D147" s="14"/>
-      <c r="E147" s="14"/>
-      <c r="F147" s="14"/>
-      <c r="G147" s="14"/>
       <c r="H147" s="5"/>
     </row>
     <row r="148" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A148" s="4"/>
-      <c r="B148" s="14"/>
-      <c r="C148" s="14"/>
-      <c r="D148" s="14"/>
-      <c r="E148" s="14"/>
-      <c r="F148" s="14"/>
-      <c r="G148" s="14"/>
       <c r="H148" s="5"/>
     </row>
     <row r="149" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A149" s="4"/>
-      <c r="B149" s="14"/>
-      <c r="C149" s="14"/>
-      <c r="D149" s="14"/>
-      <c r="E149" s="14"/>
-      <c r="F149" s="14"/>
-      <c r="G149" s="14"/>
       <c r="H149" s="5"/>
     </row>
     <row r="150" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A150" s="4"/>
-      <c r="B150" s="14"/>
-      <c r="C150" s="14"/>
-      <c r="D150" s="14"/>
-      <c r="E150" s="14"/>
-      <c r="F150" s="14"/>
-      <c r="G150" s="14"/>
       <c r="H150" s="5"/>
     </row>
     <row r="151" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A151" s="4"/>
-      <c r="B151" s="14"/>
-      <c r="C151" s="14"/>
-      <c r="D151" s="14"/>
-      <c r="E151" s="14"/>
-      <c r="F151" s="14"/>
-      <c r="G151" s="14"/>
       <c r="H151" s="5"/>
     </row>
     <row r="152" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A152" s="4"/>
-      <c r="B152" s="14"/>
-      <c r="C152" s="14"/>
-      <c r="D152" s="14"/>
-      <c r="E152" s="14"/>
-      <c r="F152" s="14"/>
-      <c r="G152" s="14"/>
       <c r="H152" s="5"/>
     </row>
     <row r="153" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A153" s="4"/>
-      <c r="B153" s="14"/>
-      <c r="C153" s="14"/>
-      <c r="D153" s="14"/>
-      <c r="E153" s="14"/>
-      <c r="F153" s="14"/>
-      <c r="G153" s="14"/>
       <c r="H153" s="5"/>
     </row>
     <row r="154" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A154" s="4"/>
-      <c r="B154" s="14"/>
-      <c r="C154" s="14"/>
-      <c r="D154" s="14"/>
-      <c r="E154" s="14"/>
-      <c r="F154" s="14"/>
-      <c r="G154" s="14"/>
       <c r="H154" s="5"/>
     </row>
     <row r="155" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A155" s="4"/>
-      <c r="B155" s="14"/>
-      <c r="C155" s="14"/>
-      <c r="D155" s="14"/>
-      <c r="E155" s="14"/>
-      <c r="F155" s="14"/>
-      <c r="G155" s="14"/>
       <c r="H155" s="5"/>
     </row>
     <row r="156" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A156" s="4"/>
-      <c r="B156" s="14"/>
-      <c r="C156" s="14"/>
-      <c r="D156" s="14"/>
-      <c r="E156" s="14"/>
-      <c r="F156" s="14"/>
-      <c r="G156" s="14"/>
       <c r="H156" s="5"/>
     </row>
     <row r="157" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A157" s="4"/>
-      <c r="B157" s="14"/>
-      <c r="C157" s="14"/>
-      <c r="D157" s="14"/>
-      <c r="E157" s="14"/>
-      <c r="F157" s="14"/>
-      <c r="G157" s="14"/>
       <c r="H157" s="5"/>
     </row>
     <row r="158" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A158" s="4"/>
-      <c r="B158" s="14"/>
-      <c r="C158" s="14"/>
-      <c r="D158" s="14"/>
-      <c r="E158" s="14"/>
-      <c r="F158" s="14"/>
-      <c r="G158" s="14"/>
       <c r="H158" s="5"/>
     </row>
     <row r="159" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A159" s="4"/>
-      <c r="B159" s="14"/>
-      <c r="C159" s="14"/>
-      <c r="D159" s="14"/>
-      <c r="E159" s="14"/>
-      <c r="F159" s="14"/>
-      <c r="G159" s="14"/>
       <c r="H159" s="5"/>
     </row>
     <row r="160" spans="1:8" x14ac:dyDescent="0.25">
@@ -6493,4 +5934,2062 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AE241D4-197C-4BF6-874B-4B7E9956690B}">
+  <dimension ref="A2:T188"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A167" workbookViewId="0">
+      <selection activeCell="P182" sqref="P182"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="5" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="2"/>
+      <c r="R5" s="2"/>
+      <c r="S5" s="2"/>
+      <c r="T5" s="3"/>
+    </row>
+    <row r="6" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B6" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="17"/>
+      <c r="J6" s="17"/>
+      <c r="K6" s="17"/>
+      <c r="L6" s="17"/>
+      <c r="M6" s="17"/>
+      <c r="N6" s="17"/>
+      <c r="O6" s="17"/>
+      <c r="P6" s="17"/>
+      <c r="Q6" s="17"/>
+      <c r="R6" s="17"/>
+      <c r="S6" s="17"/>
+      <c r="T6" s="5"/>
+    </row>
+    <row r="7" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B7" s="4"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="17"/>
+      <c r="I7" s="17"/>
+      <c r="J7" s="17"/>
+      <c r="K7" s="17"/>
+      <c r="L7" s="17"/>
+      <c r="M7" s="17"/>
+      <c r="N7" s="17"/>
+      <c r="O7" s="17"/>
+      <c r="P7" s="17"/>
+      <c r="Q7" s="17"/>
+      <c r="R7" s="17"/>
+      <c r="S7" s="17"/>
+      <c r="T7" s="5"/>
+    </row>
+    <row r="8" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B8" s="4"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="17"/>
+      <c r="J8" s="17"/>
+      <c r="K8" s="17"/>
+      <c r="L8" s="17"/>
+      <c r="M8" s="17"/>
+      <c r="N8" s="17"/>
+      <c r="O8" s="17"/>
+      <c r="P8" s="17"/>
+      <c r="Q8" s="17"/>
+      <c r="R8" s="17"/>
+      <c r="S8" s="17"/>
+      <c r="T8" s="5"/>
+    </row>
+    <row r="9" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B9" s="4"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="17"/>
+      <c r="J9" s="17"/>
+      <c r="K9" s="17"/>
+      <c r="L9" s="17"/>
+      <c r="M9" s="17"/>
+      <c r="N9" s="17"/>
+      <c r="O9" s="17"/>
+      <c r="P9" s="17"/>
+      <c r="Q9" s="17"/>
+      <c r="R9" s="17"/>
+      <c r="S9" s="17"/>
+      <c r="T9" s="5"/>
+    </row>
+    <row r="10" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B10" s="4"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="17"/>
+      <c r="K10" s="17"/>
+      <c r="L10" s="17"/>
+      <c r="M10" s="17"/>
+      <c r="N10" s="17"/>
+      <c r="O10" s="17"/>
+      <c r="P10" s="17"/>
+      <c r="Q10" s="17"/>
+      <c r="R10" s="17"/>
+      <c r="S10" s="17"/>
+      <c r="T10" s="5"/>
+    </row>
+    <row r="11" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B11" s="4"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="17"/>
+      <c r="I11" s="17"/>
+      <c r="J11" s="17"/>
+      <c r="K11" s="17"/>
+      <c r="L11" s="17"/>
+      <c r="M11" s="17"/>
+      <c r="N11" s="17"/>
+      <c r="O11" s="17"/>
+      <c r="P11" s="17"/>
+      <c r="Q11" s="17"/>
+      <c r="R11" s="17"/>
+      <c r="S11" s="17"/>
+      <c r="T11" s="5"/>
+    </row>
+    <row r="12" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B12" s="4"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="17"/>
+      <c r="I12" s="17"/>
+      <c r="J12" s="17"/>
+      <c r="K12" s="17"/>
+      <c r="L12" s="17"/>
+      <c r="M12" s="17"/>
+      <c r="N12" s="17"/>
+      <c r="O12" s="17"/>
+      <c r="P12" s="17"/>
+      <c r="Q12" s="17"/>
+      <c r="R12" s="17"/>
+      <c r="S12" s="17"/>
+      <c r="T12" s="5"/>
+    </row>
+    <row r="13" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B13" s="4"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="17"/>
+      <c r="H13" s="17"/>
+      <c r="I13" s="17"/>
+      <c r="J13" s="17"/>
+      <c r="K13" s="17"/>
+      <c r="L13" s="17"/>
+      <c r="M13" s="17"/>
+      <c r="N13" s="17"/>
+      <c r="O13" s="17"/>
+      <c r="P13" s="17"/>
+      <c r="Q13" s="17"/>
+      <c r="R13" s="17"/>
+      <c r="S13" s="17"/>
+      <c r="T13" s="5"/>
+    </row>
+    <row r="14" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B14" s="4"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="17"/>
+      <c r="I14" s="17"/>
+      <c r="J14" s="17"/>
+      <c r="K14" s="17"/>
+      <c r="L14" s="17"/>
+      <c r="M14" s="17"/>
+      <c r="N14" s="17"/>
+      <c r="O14" s="17"/>
+      <c r="P14" s="17"/>
+      <c r="Q14" s="17"/>
+      <c r="R14" s="17"/>
+      <c r="S14" s="17"/>
+      <c r="T14" s="5"/>
+    </row>
+    <row r="15" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B15" s="4"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="17"/>
+      <c r="J15" s="17"/>
+      <c r="K15" s="17"/>
+      <c r="L15" s="17"/>
+      <c r="M15" s="17"/>
+      <c r="N15" s="17"/>
+      <c r="O15" s="17"/>
+      <c r="P15" s="17"/>
+      <c r="Q15" s="17"/>
+      <c r="R15" s="17"/>
+      <c r="S15" s="17"/>
+      <c r="T15" s="5"/>
+    </row>
+    <row r="16" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B16" s="4"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="17"/>
+      <c r="I16" s="17"/>
+      <c r="J16" s="17"/>
+      <c r="K16" s="17"/>
+      <c r="L16" s="17"/>
+      <c r="M16" s="17"/>
+      <c r="N16" s="17"/>
+      <c r="O16" s="17"/>
+      <c r="P16" s="17"/>
+      <c r="Q16" s="17"/>
+      <c r="R16" s="17"/>
+      <c r="S16" s="17"/>
+      <c r="T16" s="5"/>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B17" s="4"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="17"/>
+      <c r="H17" s="17"/>
+      <c r="I17" s="17"/>
+      <c r="J17" s="17"/>
+      <c r="K17" s="17"/>
+      <c r="L17" s="17"/>
+      <c r="M17" s="17"/>
+      <c r="N17" s="17"/>
+      <c r="O17" s="17"/>
+      <c r="P17" s="17"/>
+      <c r="Q17" s="17"/>
+      <c r="R17" s="17"/>
+      <c r="S17" s="17"/>
+      <c r="T17" s="5"/>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B18" s="4"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="17"/>
+      <c r="G18" s="17"/>
+      <c r="H18" s="17"/>
+      <c r="I18" s="17"/>
+      <c r="J18" s="17"/>
+      <c r="K18" s="17"/>
+      <c r="L18" s="17"/>
+      <c r="M18" s="17"/>
+      <c r="N18" s="17"/>
+      <c r="O18" s="17"/>
+      <c r="P18" s="17"/>
+      <c r="Q18" s="17"/>
+      <c r="R18" s="17"/>
+      <c r="S18" s="17"/>
+      <c r="T18" s="5"/>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B19" s="4"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="17"/>
+      <c r="F19" s="17"/>
+      <c r="G19" s="17"/>
+      <c r="H19" s="17"/>
+      <c r="I19" s="17"/>
+      <c r="J19" s="17"/>
+      <c r="K19" s="17"/>
+      <c r="L19" s="17"/>
+      <c r="M19" s="17"/>
+      <c r="N19" s="17"/>
+      <c r="O19" s="17"/>
+      <c r="P19" s="17"/>
+      <c r="Q19" s="17"/>
+      <c r="R19" s="17"/>
+      <c r="S19" s="17"/>
+      <c r="T19" s="5"/>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B20" s="4"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="17"/>
+      <c r="G20" s="17"/>
+      <c r="H20" s="17"/>
+      <c r="I20" s="17"/>
+      <c r="J20" s="17"/>
+      <c r="K20" s="17"/>
+      <c r="L20" s="17"/>
+      <c r="M20" s="17"/>
+      <c r="N20" s="17"/>
+      <c r="O20" s="17"/>
+      <c r="P20" s="17"/>
+      <c r="Q20" s="17"/>
+      <c r="R20" s="17"/>
+      <c r="S20" s="17"/>
+      <c r="T20" s="5"/>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B21" s="4"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="17"/>
+      <c r="G21" s="17"/>
+      <c r="H21" s="17"/>
+      <c r="I21" s="17"/>
+      <c r="J21" s="17"/>
+      <c r="K21" s="17"/>
+      <c r="L21" s="17"/>
+      <c r="M21" s="17"/>
+      <c r="N21" s="17"/>
+      <c r="O21" s="17"/>
+      <c r="P21" s="17"/>
+      <c r="Q21" s="17"/>
+      <c r="R21" s="17"/>
+      <c r="S21" s="17"/>
+      <c r="T21" s="5"/>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B22" s="4"/>
+      <c r="C22" s="17"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="17"/>
+      <c r="G22" s="17"/>
+      <c r="H22" s="17"/>
+      <c r="I22" s="17"/>
+      <c r="J22" s="17"/>
+      <c r="K22" s="17"/>
+      <c r="L22" s="17"/>
+      <c r="M22" s="17"/>
+      <c r="N22" s="17"/>
+      <c r="O22" s="17"/>
+      <c r="P22" s="17"/>
+      <c r="Q22" s="17"/>
+      <c r="R22" s="17"/>
+      <c r="S22" s="17"/>
+      <c r="T22" s="5"/>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B23" s="4"/>
+      <c r="C23" s="17"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="17"/>
+      <c r="G23" s="17"/>
+      <c r="H23" s="17"/>
+      <c r="I23" s="17"/>
+      <c r="J23" s="17"/>
+      <c r="K23" s="17"/>
+      <c r="L23" s="17"/>
+      <c r="M23" s="17"/>
+      <c r="N23" s="17"/>
+      <c r="O23" s="17"/>
+      <c r="P23" s="17"/>
+      <c r="Q23" s="17"/>
+      <c r="R23" s="17"/>
+      <c r="S23" s="17"/>
+      <c r="T23" s="5"/>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B24" s="4"/>
+      <c r="C24" s="17"/>
+      <c r="D24" s="17"/>
+      <c r="E24" s="17"/>
+      <c r="F24" s="17"/>
+      <c r="G24" s="17"/>
+      <c r="H24" s="17"/>
+      <c r="I24" s="17"/>
+      <c r="J24" s="17"/>
+      <c r="K24" s="17"/>
+      <c r="L24" s="17"/>
+      <c r="M24" s="17"/>
+      <c r="N24" s="17"/>
+      <c r="O24" s="17"/>
+      <c r="P24" s="17"/>
+      <c r="Q24" s="17"/>
+      <c r="R24" s="17"/>
+      <c r="S24" s="17"/>
+      <c r="T24" s="5"/>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B25" s="4"/>
+      <c r="C25" s="17"/>
+      <c r="D25" s="17"/>
+      <c r="E25" s="17"/>
+      <c r="F25" s="17"/>
+      <c r="G25" s="17"/>
+      <c r="H25" s="17"/>
+      <c r="I25" s="17"/>
+      <c r="J25" s="17"/>
+      <c r="K25" s="17"/>
+      <c r="L25" s="17"/>
+      <c r="M25" s="17"/>
+      <c r="N25" s="17"/>
+      <c r="O25" s="17"/>
+      <c r="P25" s="17"/>
+      <c r="Q25" s="17"/>
+      <c r="R25" s="17"/>
+      <c r="S25" s="17"/>
+      <c r="T25" s="5"/>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B26" s="4"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="17"/>
+      <c r="E26" s="17"/>
+      <c r="F26" s="17"/>
+      <c r="G26" s="17"/>
+      <c r="H26" s="17"/>
+      <c r="I26" s="17"/>
+      <c r="J26" s="17"/>
+      <c r="K26" s="17"/>
+      <c r="L26" s="17"/>
+      <c r="M26" s="17"/>
+      <c r="N26" s="17"/>
+      <c r="O26" s="17"/>
+      <c r="P26" s="17"/>
+      <c r="Q26" s="17"/>
+      <c r="R26" s="17"/>
+      <c r="S26" s="17"/>
+      <c r="T26" s="5"/>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B27" s="6"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="7"/>
+      <c r="H27" s="7"/>
+      <c r="I27" s="7"/>
+      <c r="J27" s="7"/>
+      <c r="K27" s="7"/>
+      <c r="L27" s="7"/>
+      <c r="M27" s="7"/>
+      <c r="N27" s="7"/>
+      <c r="O27" s="7"/>
+      <c r="P27" s="7"/>
+      <c r="Q27" s="7"/>
+      <c r="R27" s="7"/>
+      <c r="S27" s="7"/>
+      <c r="T27" s="8"/>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A30" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B31" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="3"/>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B32" s="4"/>
+      <c r="C32" t="s">
+        <v>10</v>
+      </c>
+      <c r="F32" s="5"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B33" s="4"/>
+      <c r="D33" t="s">
+        <v>11</v>
+      </c>
+      <c r="F33" s="5"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B34" s="4"/>
+      <c r="D34" t="s">
+        <v>12</v>
+      </c>
+      <c r="F34" s="5"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B35" s="4"/>
+      <c r="D35" t="s">
+        <v>13</v>
+      </c>
+      <c r="F35" s="5"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B36" s="4"/>
+      <c r="C36" t="s">
+        <v>14</v>
+      </c>
+      <c r="F36" s="5"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B37" s="4"/>
+      <c r="D37" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="F37" s="5"/>
+      <c r="G37" t="s">
+        <v>20</v>
+      </c>
+      <c r="H37" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B38" s="4"/>
+      <c r="C38" t="s">
+        <v>15</v>
+      </c>
+      <c r="F38" s="5"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B39" s="4"/>
+      <c r="C39" t="s">
+        <v>16</v>
+      </c>
+      <c r="F39" s="5"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B40" s="4"/>
+      <c r="D40" t="s">
+        <v>26</v>
+      </c>
+      <c r="F40" s="5"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B41" s="4"/>
+      <c r="D41" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="F41" s="5"/>
+      <c r="G41" t="s">
+        <v>20</v>
+      </c>
+      <c r="H41" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B42" s="6"/>
+      <c r="C42" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D42" s="7"/>
+      <c r="E42" s="7"/>
+      <c r="F42" s="8"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B46" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C46" s="2"/>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
+      <c r="F46" s="2"/>
+      <c r="G46" s="2"/>
+      <c r="H46" s="2"/>
+      <c r="I46" s="3"/>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B47" s="4"/>
+      <c r="C47" s="17"/>
+      <c r="D47" s="17"/>
+      <c r="E47" s="17"/>
+      <c r="F47" s="17"/>
+      <c r="G47" s="17"/>
+      <c r="H47" s="17"/>
+      <c r="I47" s="5"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B48" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C48" s="17"/>
+      <c r="D48" s="17"/>
+      <c r="E48" s="17"/>
+      <c r="F48" s="17"/>
+      <c r="G48" s="17"/>
+      <c r="H48" s="17"/>
+      <c r="I48" s="5"/>
+    </row>
+    <row r="49" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B49" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C49" s="17"/>
+      <c r="D49" s="17"/>
+      <c r="E49" s="17"/>
+      <c r="F49" s="17"/>
+      <c r="G49" s="17"/>
+      <c r="H49" s="17"/>
+      <c r="I49" s="5"/>
+    </row>
+    <row r="50" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B50" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C50" s="17"/>
+      <c r="D50" s="17"/>
+      <c r="E50" s="17"/>
+      <c r="F50" s="17"/>
+      <c r="G50" s="17"/>
+      <c r="H50" s="17"/>
+      <c r="I50" s="5"/>
+    </row>
+    <row r="51" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B51" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C51" s="17"/>
+      <c r="D51" s="17"/>
+      <c r="E51" s="17"/>
+      <c r="F51" s="17"/>
+      <c r="G51" s="17"/>
+      <c r="H51" s="17"/>
+      <c r="I51" s="5"/>
+    </row>
+    <row r="52" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B52" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C52" s="17"/>
+      <c r="D52" s="17"/>
+      <c r="E52" s="17"/>
+      <c r="F52" s="17"/>
+      <c r="G52" s="17"/>
+      <c r="H52" s="17"/>
+      <c r="I52" s="5"/>
+    </row>
+    <row r="53" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B53" s="4"/>
+      <c r="C53" s="17"/>
+      <c r="D53" s="17"/>
+      <c r="E53" s="17"/>
+      <c r="F53" s="17"/>
+      <c r="G53" s="17"/>
+      <c r="H53" s="17"/>
+      <c r="I53" s="5"/>
+    </row>
+    <row r="54" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B54" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="C54" s="17"/>
+      <c r="D54" s="17"/>
+      <c r="E54" s="17"/>
+      <c r="F54" s="17"/>
+      <c r="G54" s="17"/>
+      <c r="H54" s="17"/>
+      <c r="I54" s="5"/>
+    </row>
+    <row r="55" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B55" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="C55" s="17"/>
+      <c r="D55" s="17"/>
+      <c r="E55" s="17"/>
+      <c r="F55" s="17"/>
+      <c r="G55" s="17"/>
+      <c r="H55" s="17"/>
+      <c r="I55" s="5"/>
+    </row>
+    <row r="56" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B56" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="C56" s="17"/>
+      <c r="D56" s="17"/>
+      <c r="E56" s="17"/>
+      <c r="F56" s="17"/>
+      <c r="G56" s="17"/>
+      <c r="H56" s="17"/>
+      <c r="I56" s="5"/>
+    </row>
+    <row r="57" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B57" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="C57" s="17"/>
+      <c r="D57" s="17"/>
+      <c r="E57" s="17"/>
+      <c r="F57" s="17"/>
+      <c r="G57" s="17"/>
+      <c r="H57" s="17"/>
+      <c r="I57" s="5"/>
+    </row>
+    <row r="58" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B58" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="C58" s="17"/>
+      <c r="D58" s="17"/>
+      <c r="E58" s="17"/>
+      <c r="F58" s="17"/>
+      <c r="G58" s="17"/>
+      <c r="H58" s="17"/>
+      <c r="I58" s="5"/>
+    </row>
+    <row r="59" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B59" s="4"/>
+      <c r="C59" s="17"/>
+      <c r="D59" s="17"/>
+      <c r="E59" s="17"/>
+      <c r="F59" s="17"/>
+      <c r="G59" s="17"/>
+      <c r="H59" s="17"/>
+      <c r="I59" s="5"/>
+    </row>
+    <row r="60" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B60" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C60" s="17"/>
+      <c r="D60" s="17"/>
+      <c r="E60" s="17"/>
+      <c r="F60" s="17"/>
+      <c r="G60" s="17"/>
+      <c r="H60" s="17"/>
+      <c r="I60" s="5"/>
+    </row>
+    <row r="61" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B61" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C61" s="17"/>
+      <c r="D61" s="17"/>
+      <c r="E61" s="17"/>
+      <c r="F61" s="17"/>
+      <c r="G61" s="17"/>
+      <c r="H61" s="17"/>
+      <c r="I61" s="5"/>
+    </row>
+    <row r="62" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B62" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C62" s="17"/>
+      <c r="D62" s="17"/>
+      <c r="E62" s="17"/>
+      <c r="F62" s="17"/>
+      <c r="G62" s="17"/>
+      <c r="H62" s="17"/>
+      <c r="I62" s="5"/>
+    </row>
+    <row r="63" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B63" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C63" s="17"/>
+      <c r="D63" s="17"/>
+      <c r="E63" s="17"/>
+      <c r="F63" s="17"/>
+      <c r="G63" s="17"/>
+      <c r="H63" s="17"/>
+      <c r="I63" s="5"/>
+    </row>
+    <row r="64" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B64" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="C64" s="17"/>
+      <c r="D64" s="17"/>
+      <c r="E64" s="17"/>
+      <c r="F64" s="17"/>
+      <c r="G64" s="17"/>
+      <c r="H64" s="17"/>
+      <c r="I64" s="5"/>
+    </row>
+    <row r="65" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B65" s="4"/>
+      <c r="C65" s="17"/>
+      <c r="D65" s="17"/>
+      <c r="E65" s="17"/>
+      <c r="F65" s="17"/>
+      <c r="G65" s="17"/>
+      <c r="H65" s="17"/>
+      <c r="I65" s="5"/>
+    </row>
+    <row r="66" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B66" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C66" s="17"/>
+      <c r="D66" s="17"/>
+      <c r="E66" s="17"/>
+      <c r="F66" s="17"/>
+      <c r="G66" s="17"/>
+      <c r="H66" s="17"/>
+      <c r="I66" s="5"/>
+    </row>
+    <row r="67" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B67" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C67" s="17"/>
+      <c r="D67" s="17"/>
+      <c r="E67" s="17"/>
+      <c r="F67" s="17"/>
+      <c r="G67" s="17"/>
+      <c r="H67" s="17"/>
+      <c r="I67" s="5"/>
+    </row>
+    <row r="68" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B68" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C68" s="17"/>
+      <c r="D68" s="17"/>
+      <c r="E68" s="17"/>
+      <c r="F68" s="17"/>
+      <c r="G68" s="17"/>
+      <c r="H68" s="17"/>
+      <c r="I68" s="5"/>
+    </row>
+    <row r="69" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B69" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C69" s="17"/>
+      <c r="D69" s="17"/>
+      <c r="E69" s="17"/>
+      <c r="F69" s="17"/>
+      <c r="G69" s="17"/>
+      <c r="H69" s="17"/>
+      <c r="I69" s="5"/>
+    </row>
+    <row r="70" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B70" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C70" s="17"/>
+      <c r="D70" s="17"/>
+      <c r="E70" s="17"/>
+      <c r="F70" s="17"/>
+      <c r="G70" s="17"/>
+      <c r="H70" s="17"/>
+      <c r="I70" s="5"/>
+    </row>
+    <row r="71" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B71" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C71" s="17"/>
+      <c r="D71" s="17"/>
+      <c r="E71" s="17"/>
+      <c r="F71" s="17"/>
+      <c r="G71" s="17"/>
+      <c r="H71" s="17"/>
+      <c r="I71" s="5"/>
+    </row>
+    <row r="72" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B72" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C72" s="17"/>
+      <c r="D72" s="17"/>
+      <c r="E72" s="17"/>
+      <c r="F72" s="17"/>
+      <c r="G72" s="17"/>
+      <c r="H72" s="17"/>
+      <c r="I72" s="5"/>
+    </row>
+    <row r="73" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B73" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C73" s="17"/>
+      <c r="D73" s="17"/>
+      <c r="E73" s="17"/>
+      <c r="F73" s="17"/>
+      <c r="G73" s="17"/>
+      <c r="H73" s="17"/>
+      <c r="I73" s="5"/>
+    </row>
+    <row r="74" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B74" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C74" s="17"/>
+      <c r="D74" s="17"/>
+      <c r="E74" s="17"/>
+      <c r="F74" s="17"/>
+      <c r="G74" s="17"/>
+      <c r="H74" s="17"/>
+      <c r="I74" s="5"/>
+    </row>
+    <row r="75" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B75" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C75" s="17"/>
+      <c r="D75" s="17"/>
+      <c r="E75" s="17"/>
+      <c r="F75" s="17"/>
+      <c r="G75" s="17"/>
+      <c r="H75" s="17"/>
+      <c r="I75" s="5"/>
+    </row>
+    <row r="76" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B76" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C76" s="17"/>
+      <c r="D76" s="17"/>
+      <c r="E76" s="17"/>
+      <c r="F76" s="17"/>
+      <c r="G76" s="17"/>
+      <c r="H76" s="17"/>
+      <c r="I76" s="5"/>
+    </row>
+    <row r="77" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B77" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C77" s="17"/>
+      <c r="D77" s="17"/>
+      <c r="E77" s="17"/>
+      <c r="F77" s="17"/>
+      <c r="G77" s="17"/>
+      <c r="H77" s="17"/>
+      <c r="I77" s="5"/>
+    </row>
+    <row r="78" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B78" s="4"/>
+      <c r="C78" s="17"/>
+      <c r="D78" s="17"/>
+      <c r="E78" s="17"/>
+      <c r="F78" s="17"/>
+      <c r="G78" s="17"/>
+      <c r="H78" s="17"/>
+      <c r="I78" s="5"/>
+    </row>
+    <row r="79" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B79" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C79" s="17"/>
+      <c r="D79" s="17"/>
+      <c r="E79" s="17"/>
+      <c r="F79" s="17"/>
+      <c r="G79" s="17"/>
+      <c r="H79" s="17"/>
+      <c r="I79" s="5"/>
+    </row>
+    <row r="80" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B80" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C80" s="17"/>
+      <c r="D80" s="17"/>
+      <c r="E80" s="17"/>
+      <c r="F80" s="17"/>
+      <c r="G80" s="17"/>
+      <c r="H80" s="17"/>
+      <c r="I80" s="5"/>
+    </row>
+    <row r="81" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B81" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C81" s="17"/>
+      <c r="D81" s="17"/>
+      <c r="E81" s="17"/>
+      <c r="F81" s="17"/>
+      <c r="G81" s="17"/>
+      <c r="H81" s="17"/>
+      <c r="I81" s="5"/>
+    </row>
+    <row r="82" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B82" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C82" s="17"/>
+      <c r="D82" s="17"/>
+      <c r="E82" s="17"/>
+      <c r="F82" s="17"/>
+      <c r="G82" s="17"/>
+      <c r="H82" s="17"/>
+      <c r="I82" s="5"/>
+    </row>
+    <row r="83" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B83" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C83" s="17"/>
+      <c r="D83" s="17"/>
+      <c r="E83" s="17"/>
+      <c r="F83" s="17"/>
+      <c r="G83" s="17"/>
+      <c r="H83" s="17"/>
+      <c r="I83" s="5"/>
+    </row>
+    <row r="84" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B84" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C84" s="17"/>
+      <c r="D84" s="17"/>
+      <c r="E84" s="17"/>
+      <c r="F84" s="17"/>
+      <c r="G84" s="17"/>
+      <c r="H84" s="17"/>
+      <c r="I84" s="5"/>
+    </row>
+    <row r="85" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B85" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C85" s="17"/>
+      <c r="D85" s="17"/>
+      <c r="E85" s="17"/>
+      <c r="F85" s="17"/>
+      <c r="G85" s="17"/>
+      <c r="H85" s="17"/>
+      <c r="I85" s="5"/>
+    </row>
+    <row r="86" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B86" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C86" s="17"/>
+      <c r="D86" s="17"/>
+      <c r="E86" s="17"/>
+      <c r="F86" s="17"/>
+      <c r="G86" s="17"/>
+      <c r="H86" s="17"/>
+      <c r="I86" s="5"/>
+    </row>
+    <row r="87" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B87" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C87" s="17"/>
+      <c r="D87" s="17"/>
+      <c r="E87" s="17"/>
+      <c r="F87" s="17"/>
+      <c r="G87" s="17"/>
+      <c r="H87" s="17"/>
+      <c r="I87" s="5"/>
+    </row>
+    <row r="88" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B88" s="4"/>
+      <c r="C88" s="17"/>
+      <c r="D88" s="17"/>
+      <c r="E88" s="17"/>
+      <c r="F88" s="17"/>
+      <c r="G88" s="17"/>
+      <c r="H88" s="17"/>
+      <c r="I88" s="5"/>
+    </row>
+    <row r="89" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B89" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="C89" s="17"/>
+      <c r="D89" s="17"/>
+      <c r="E89" s="17"/>
+      <c r="F89" s="17"/>
+      <c r="G89" s="17"/>
+      <c r="H89" s="17"/>
+      <c r="I89" s="5"/>
+    </row>
+    <row r="90" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B90" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="C90" s="17"/>
+      <c r="D90" s="17"/>
+      <c r="E90" s="17"/>
+      <c r="F90" s="17"/>
+      <c r="G90" s="17"/>
+      <c r="H90" s="17"/>
+      <c r="I90" s="5"/>
+    </row>
+    <row r="91" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B91" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="C91" s="17"/>
+      <c r="D91" s="17"/>
+      <c r="E91" s="17"/>
+      <c r="F91" s="17"/>
+      <c r="G91" s="17"/>
+      <c r="H91" s="17"/>
+      <c r="I91" s="5"/>
+    </row>
+    <row r="92" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B92" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="C92" s="17"/>
+      <c r="D92" s="17"/>
+      <c r="E92" s="17"/>
+      <c r="F92" s="17"/>
+      <c r="G92" s="17"/>
+      <c r="H92" s="17"/>
+      <c r="I92" s="5"/>
+    </row>
+    <row r="93" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B93" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="C93" s="17"/>
+      <c r="D93" s="17"/>
+      <c r="E93" s="17"/>
+      <c r="F93" s="17"/>
+      <c r="G93" s="17"/>
+      <c r="H93" s="17"/>
+      <c r="I93" s="5"/>
+    </row>
+    <row r="94" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B94" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="C94" s="17"/>
+      <c r="D94" s="17"/>
+      <c r="E94" s="17"/>
+      <c r="F94" s="17"/>
+      <c r="G94" s="17"/>
+      <c r="H94" s="17"/>
+      <c r="I94" s="5"/>
+    </row>
+    <row r="95" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B95" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="C95" s="17"/>
+      <c r="D95" s="17"/>
+      <c r="E95" s="17"/>
+      <c r="F95" s="17"/>
+      <c r="G95" s="17"/>
+      <c r="H95" s="17"/>
+      <c r="I95" s="5"/>
+    </row>
+    <row r="96" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B96" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="C96" s="17"/>
+      <c r="D96" s="17"/>
+      <c r="E96" s="17"/>
+      <c r="F96" s="17"/>
+      <c r="G96" s="17"/>
+      <c r="H96" s="17"/>
+      <c r="I96" s="5"/>
+    </row>
+    <row r="97" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B97" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="C97" s="17"/>
+      <c r="D97" s="17"/>
+      <c r="E97" s="17"/>
+      <c r="F97" s="17"/>
+      <c r="G97" s="17"/>
+      <c r="H97" s="17"/>
+      <c r="I97" s="5"/>
+    </row>
+    <row r="98" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B98" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="C98" s="17"/>
+      <c r="D98" s="17"/>
+      <c r="E98" s="17"/>
+      <c r="F98" s="17"/>
+      <c r="G98" s="17"/>
+      <c r="H98" s="17"/>
+      <c r="I98" s="5"/>
+    </row>
+    <row r="99" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B99" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="C99" s="17"/>
+      <c r="D99" s="17"/>
+      <c r="E99" s="17"/>
+      <c r="F99" s="17"/>
+      <c r="G99" s="17"/>
+      <c r="H99" s="17"/>
+      <c r="I99" s="5"/>
+    </row>
+    <row r="100" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B100" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="C100" s="17"/>
+      <c r="D100" s="17"/>
+      <c r="E100" s="17"/>
+      <c r="F100" s="17"/>
+      <c r="G100" s="17"/>
+      <c r="H100" s="17"/>
+      <c r="I100" s="5"/>
+    </row>
+    <row r="101" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B101" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="C101" s="17"/>
+      <c r="D101" s="17"/>
+      <c r="E101" s="17"/>
+      <c r="F101" s="17"/>
+      <c r="G101" s="17"/>
+      <c r="H101" s="17"/>
+      <c r="I101" s="5"/>
+    </row>
+    <row r="102" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B102" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="C102" s="17"/>
+      <c r="D102" s="17"/>
+      <c r="E102" s="17"/>
+      <c r="F102" s="17"/>
+      <c r="G102" s="17"/>
+      <c r="H102" s="17"/>
+      <c r="I102" s="5"/>
+    </row>
+    <row r="103" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B103" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="C103" s="17"/>
+      <c r="D103" s="17"/>
+      <c r="E103" s="17"/>
+      <c r="F103" s="17"/>
+      <c r="G103" s="17"/>
+      <c r="H103" s="17"/>
+      <c r="I103" s="5"/>
+    </row>
+    <row r="104" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B104" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="C104" s="17"/>
+      <c r="D104" s="17"/>
+      <c r="E104" s="17"/>
+      <c r="F104" s="17"/>
+      <c r="G104" s="17"/>
+      <c r="H104" s="17"/>
+      <c r="I104" s="5"/>
+    </row>
+    <row r="105" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B105" s="14"/>
+      <c r="C105" s="17"/>
+      <c r="D105" s="17"/>
+      <c r="E105" s="17"/>
+      <c r="F105" s="17"/>
+      <c r="G105" s="17"/>
+      <c r="H105" s="17"/>
+      <c r="I105" s="5"/>
+    </row>
+    <row r="106" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B106" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="C106" s="17"/>
+      <c r="D106" s="17"/>
+      <c r="E106" s="17"/>
+      <c r="F106" s="17"/>
+      <c r="G106" s="17"/>
+      <c r="H106" s="17"/>
+      <c r="I106" s="5"/>
+    </row>
+    <row r="107" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B107" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="C107" s="17"/>
+      <c r="D107" s="17"/>
+      <c r="E107" s="17"/>
+      <c r="F107" s="17"/>
+      <c r="G107" s="17"/>
+      <c r="H107" s="17"/>
+      <c r="I107" s="5"/>
+    </row>
+    <row r="108" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B108" s="14"/>
+      <c r="C108" s="17"/>
+      <c r="D108" s="17"/>
+      <c r="E108" s="17"/>
+      <c r="F108" s="17"/>
+      <c r="G108" s="17"/>
+      <c r="H108" s="17"/>
+      <c r="I108" s="5"/>
+    </row>
+    <row r="109" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B109" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="C109" s="17"/>
+      <c r="D109" s="17"/>
+      <c r="E109" s="17"/>
+      <c r="F109" s="17"/>
+      <c r="G109" s="17"/>
+      <c r="H109" s="17"/>
+      <c r="I109" s="5"/>
+    </row>
+    <row r="110" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B110" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="C110" s="17"/>
+      <c r="D110" s="17"/>
+      <c r="E110" s="17"/>
+      <c r="F110" s="17"/>
+      <c r="G110" s="17"/>
+      <c r="H110" s="17"/>
+      <c r="I110" s="5"/>
+    </row>
+    <row r="111" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B111" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="C111" s="17"/>
+      <c r="D111" s="17"/>
+      <c r="E111" s="17"/>
+      <c r="F111" s="17"/>
+      <c r="G111" s="17"/>
+      <c r="H111" s="17"/>
+      <c r="I111" s="5"/>
+    </row>
+    <row r="112" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B112" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="C112" s="17"/>
+      <c r="D112" s="17"/>
+      <c r="E112" s="17"/>
+      <c r="F112" s="17"/>
+      <c r="G112" s="17"/>
+      <c r="H112" s="17"/>
+      <c r="I112" s="5"/>
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B113" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="C113" s="17"/>
+      <c r="D113" s="17"/>
+      <c r="E113" s="17"/>
+      <c r="F113" s="17"/>
+      <c r="G113" s="17"/>
+      <c r="H113" s="17"/>
+      <c r="I113" s="5"/>
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B114" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="C114" s="17"/>
+      <c r="D114" s="17"/>
+      <c r="E114" s="17"/>
+      <c r="F114" s="17"/>
+      <c r="G114" s="17"/>
+      <c r="H114" s="17"/>
+      <c r="I114" s="5"/>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B115" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="C115" s="17"/>
+      <c r="D115" s="17"/>
+      <c r="E115" s="17"/>
+      <c r="F115" s="17"/>
+      <c r="G115" s="17"/>
+      <c r="H115" s="17"/>
+      <c r="I115" s="5"/>
+    </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B116" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="C116" s="17"/>
+      <c r="D116" s="17"/>
+      <c r="E116" s="17"/>
+      <c r="F116" s="17"/>
+      <c r="G116" s="17"/>
+      <c r="H116" s="17"/>
+      <c r="I116" s="5"/>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B117" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="C117" s="17"/>
+      <c r="D117" s="17"/>
+      <c r="E117" s="17"/>
+      <c r="F117" s="17"/>
+      <c r="G117" s="17"/>
+      <c r="H117" s="17"/>
+      <c r="I117" s="5"/>
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B118" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="C118" s="7"/>
+      <c r="D118" s="7"/>
+      <c r="E118" s="7"/>
+      <c r="F118" s="7"/>
+      <c r="G118" s="7"/>
+      <c r="H118" s="7"/>
+      <c r="I118" s="8"/>
+    </row>
+    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B122" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C122" s="2"/>
+      <c r="D122" s="2"/>
+      <c r="E122" s="2"/>
+      <c r="F122" s="2"/>
+      <c r="G122" s="2"/>
+      <c r="H122" s="3"/>
+    </row>
+    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B123" s="4"/>
+      <c r="C123" s="17"/>
+      <c r="D123" s="17"/>
+      <c r="E123" s="17"/>
+      <c r="F123" s="17"/>
+      <c r="G123" s="17"/>
+      <c r="H123" s="5"/>
+    </row>
+    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B124" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C124" s="17"/>
+      <c r="D124" s="17"/>
+      <c r="E124" s="17"/>
+      <c r="F124" s="17"/>
+      <c r="G124" s="17"/>
+      <c r="H124" s="5"/>
+    </row>
+    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B125" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C125" s="17"/>
+      <c r="D125" s="17"/>
+      <c r="E125" s="17"/>
+      <c r="F125" s="17"/>
+      <c r="G125" s="17"/>
+      <c r="H125" s="5"/>
+    </row>
+    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B126" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C126" s="17"/>
+      <c r="D126" s="17"/>
+      <c r="E126" s="17"/>
+      <c r="F126" s="17"/>
+      <c r="G126" s="17"/>
+      <c r="H126" s="5"/>
+    </row>
+    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B127" s="4"/>
+      <c r="C127" s="17"/>
+      <c r="D127" s="17"/>
+      <c r="E127" s="17"/>
+      <c r="F127" s="17"/>
+      <c r="G127" s="17"/>
+      <c r="H127" s="5"/>
+    </row>
+    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B128" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C128" s="17"/>
+      <c r="D128" s="17"/>
+      <c r="E128" s="17"/>
+      <c r="F128" s="17"/>
+      <c r="G128" s="17"/>
+      <c r="H128" s="5"/>
+    </row>
+    <row r="129" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B129" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C129" s="17"/>
+      <c r="D129" s="17"/>
+      <c r="E129" s="17"/>
+      <c r="F129" s="17"/>
+      <c r="G129" s="17"/>
+      <c r="H129" s="5"/>
+    </row>
+    <row r="130" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B130" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C130" s="17"/>
+      <c r="D130" s="17"/>
+      <c r="E130" s="17"/>
+      <c r="F130" s="17"/>
+      <c r="G130" s="17"/>
+      <c r="H130" s="5"/>
+    </row>
+    <row r="131" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B131" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C131" s="17"/>
+      <c r="D131" s="17"/>
+      <c r="E131" s="17"/>
+      <c r="F131" s="17"/>
+      <c r="G131" s="17"/>
+      <c r="H131" s="5"/>
+    </row>
+    <row r="132" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B132" s="4"/>
+      <c r="C132" s="17"/>
+      <c r="D132" s="17"/>
+      <c r="E132" s="17"/>
+      <c r="F132" s="17"/>
+      <c r="G132" s="17"/>
+      <c r="H132" s="5"/>
+    </row>
+    <row r="133" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B133" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C133" s="17"/>
+      <c r="D133" s="17"/>
+      <c r="E133" s="17"/>
+      <c r="F133" s="17"/>
+      <c r="G133" s="17"/>
+      <c r="H133" s="5"/>
+    </row>
+    <row r="134" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B134" s="4"/>
+      <c r="C134" s="17"/>
+      <c r="D134" s="17"/>
+      <c r="E134" s="17"/>
+      <c r="F134" s="17"/>
+      <c r="G134" s="17"/>
+      <c r="H134" s="5"/>
+    </row>
+    <row r="135" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B135" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C135" s="17"/>
+      <c r="D135" s="17"/>
+      <c r="E135" s="17"/>
+      <c r="F135" s="17"/>
+      <c r="G135" s="17"/>
+      <c r="H135" s="5"/>
+    </row>
+    <row r="136" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B136" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="C136" s="17"/>
+      <c r="D136" s="17"/>
+      <c r="E136" s="17"/>
+      <c r="F136" s="17"/>
+      <c r="G136" s="17"/>
+      <c r="H136" s="5"/>
+    </row>
+    <row r="137" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B137" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C137" s="17"/>
+      <c r="D137" s="17"/>
+      <c r="E137" s="17"/>
+      <c r="F137" s="17"/>
+      <c r="G137" s="17"/>
+      <c r="H137" s="5"/>
+    </row>
+    <row r="138" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B138" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C138" s="17"/>
+      <c r="D138" s="17"/>
+      <c r="E138" s="17"/>
+      <c r="F138" s="17"/>
+      <c r="G138" s="17"/>
+      <c r="H138" s="5"/>
+    </row>
+    <row r="139" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B139" s="4"/>
+      <c r="C139" s="17"/>
+      <c r="D139" s="17"/>
+      <c r="E139" s="17"/>
+      <c r="F139" s="17"/>
+      <c r="G139" s="17"/>
+      <c r="H139" s="5"/>
+    </row>
+    <row r="140" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B140" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="C140" s="17"/>
+      <c r="D140" s="17"/>
+      <c r="E140" s="17"/>
+      <c r="F140" s="17"/>
+      <c r="G140" s="17"/>
+      <c r="H140" s="5"/>
+    </row>
+    <row r="141" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B141" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="C141" s="17"/>
+      <c r="D141" s="17"/>
+      <c r="E141" s="17"/>
+      <c r="F141" s="17"/>
+      <c r="G141" s="17"/>
+      <c r="H141" s="5"/>
+    </row>
+    <row r="142" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B142" s="14"/>
+      <c r="C142" s="17"/>
+      <c r="D142" s="17"/>
+      <c r="E142" s="17"/>
+      <c r="F142" s="17"/>
+      <c r="G142" s="17"/>
+      <c r="H142" s="5"/>
+    </row>
+    <row r="143" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B143" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="C143" s="17"/>
+      <c r="D143" s="17"/>
+      <c r="E143" s="17"/>
+      <c r="F143" s="17"/>
+      <c r="G143" s="17"/>
+      <c r="H143" s="5"/>
+    </row>
+    <row r="144" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B144" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="C144" s="17"/>
+      <c r="D144" s="17"/>
+      <c r="E144" s="17"/>
+      <c r="F144" s="17"/>
+      <c r="G144" s="17"/>
+      <c r="H144" s="5"/>
+    </row>
+    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B145" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="C145" s="17"/>
+      <c r="D145" s="17"/>
+      <c r="E145" s="17"/>
+      <c r="F145" s="17"/>
+      <c r="G145" s="17"/>
+      <c r="H145" s="5"/>
+    </row>
+    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B146" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="C146" s="17"/>
+      <c r="D146" s="17"/>
+      <c r="E146" s="17"/>
+      <c r="F146" s="17"/>
+      <c r="G146" s="17"/>
+      <c r="H146" s="5"/>
+    </row>
+    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B147" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="C147" s="17"/>
+      <c r="D147" s="17"/>
+      <c r="E147" s="17"/>
+      <c r="F147" s="17"/>
+      <c r="G147" s="17"/>
+      <c r="H147" s="5"/>
+    </row>
+    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B148" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="C148" s="17"/>
+      <c r="D148" s="17"/>
+      <c r="E148" s="17"/>
+      <c r="F148" s="17"/>
+      <c r="G148" s="17"/>
+      <c r="H148" s="5"/>
+    </row>
+    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B149" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="C149" s="7"/>
+      <c r="D149" s="7"/>
+      <c r="E149" s="7"/>
+      <c r="F149" s="7"/>
+      <c r="G149" s="7"/>
+      <c r="H149" s="8"/>
+    </row>
+    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A152" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B153" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="C153" s="2"/>
+      <c r="D153" s="2"/>
+      <c r="E153" s="2"/>
+      <c r="F153" s="2"/>
+      <c r="G153" s="3"/>
+    </row>
+    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B154" s="4"/>
+      <c r="C154" s="17"/>
+      <c r="D154" s="17"/>
+      <c r="E154" s="17"/>
+      <c r="F154" s="17"/>
+      <c r="G154" s="5"/>
+    </row>
+    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B155" s="4"/>
+      <c r="C155" s="17"/>
+      <c r="D155" s="17"/>
+      <c r="E155" s="17"/>
+      <c r="F155" s="17"/>
+      <c r="G155" s="5"/>
+    </row>
+    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B156" s="4"/>
+      <c r="C156" s="17"/>
+      <c r="D156" s="17"/>
+      <c r="E156" s="17"/>
+      <c r="F156" s="17"/>
+      <c r="G156" s="5"/>
+    </row>
+    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B157" s="4"/>
+      <c r="C157" s="17"/>
+      <c r="D157" s="17"/>
+      <c r="E157" s="17"/>
+      <c r="F157" s="17"/>
+      <c r="G157" s="5"/>
+    </row>
+    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B158" s="4"/>
+      <c r="C158" s="17"/>
+      <c r="D158" s="17"/>
+      <c r="E158" s="17"/>
+      <c r="F158" s="17"/>
+      <c r="G158" s="5"/>
+    </row>
+    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B159" s="4"/>
+      <c r="C159" s="17"/>
+      <c r="D159" s="17"/>
+      <c r="E159" s="17"/>
+      <c r="F159" s="17"/>
+      <c r="G159" s="5"/>
+    </row>
+    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B160" s="4"/>
+      <c r="C160" s="17"/>
+      <c r="D160" s="17"/>
+      <c r="E160" s="17"/>
+      <c r="F160" s="17"/>
+      <c r="G160" s="5"/>
+    </row>
+    <row r="161" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B161" s="4"/>
+      <c r="C161" s="17"/>
+      <c r="D161" s="17"/>
+      <c r="E161" s="17"/>
+      <c r="F161" s="17"/>
+      <c r="G161" s="5"/>
+    </row>
+    <row r="162" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B162" s="4"/>
+      <c r="C162" s="17"/>
+      <c r="D162" s="17"/>
+      <c r="E162" s="17"/>
+      <c r="F162" s="17"/>
+      <c r="G162" s="5"/>
+    </row>
+    <row r="163" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B163" s="6"/>
+      <c r="C163" s="7"/>
+      <c r="D163" s="7"/>
+      <c r="E163" s="7"/>
+      <c r="F163" s="7"/>
+      <c r="G163" s="8"/>
+    </row>
+    <row r="166" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B166" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="C166" s="2"/>
+      <c r="D166" s="2"/>
+      <c r="E166" s="2"/>
+      <c r="F166" s="2"/>
+      <c r="G166" s="2"/>
+      <c r="H166" s="3"/>
+    </row>
+    <row r="167" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B167" s="4"/>
+      <c r="C167" s="17"/>
+      <c r="D167" s="17"/>
+      <c r="E167" s="17"/>
+      <c r="F167" s="17"/>
+      <c r="G167" s="17"/>
+      <c r="H167" s="5"/>
+    </row>
+    <row r="168" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B168" s="4"/>
+      <c r="C168" s="17"/>
+      <c r="D168" s="17"/>
+      <c r="E168" s="17"/>
+      <c r="F168" s="17"/>
+      <c r="G168" s="17"/>
+      <c r="H168" s="5"/>
+    </row>
+    <row r="169" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B169" s="4"/>
+      <c r="C169" s="17"/>
+      <c r="D169" s="17"/>
+      <c r="E169" s="17"/>
+      <c r="F169" s="17"/>
+      <c r="G169" s="17"/>
+      <c r="H169" s="5"/>
+    </row>
+    <row r="170" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B170" s="4"/>
+      <c r="C170" s="17"/>
+      <c r="D170" s="17"/>
+      <c r="E170" s="17"/>
+      <c r="F170" s="17"/>
+      <c r="G170" s="17"/>
+      <c r="H170" s="5"/>
+    </row>
+    <row r="171" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B171" s="4"/>
+      <c r="C171" s="17"/>
+      <c r="D171" s="17"/>
+      <c r="E171" s="17"/>
+      <c r="F171" s="17"/>
+      <c r="G171" s="17"/>
+      <c r="H171" s="5"/>
+    </row>
+    <row r="172" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B172" s="4"/>
+      <c r="C172" s="17"/>
+      <c r="D172" s="17"/>
+      <c r="E172" s="17"/>
+      <c r="F172" s="17"/>
+      <c r="G172" s="17"/>
+      <c r="H172" s="5"/>
+    </row>
+    <row r="173" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B173" s="4"/>
+      <c r="C173" s="17"/>
+      <c r="D173" s="17"/>
+      <c r="E173" s="17"/>
+      <c r="F173" s="17"/>
+      <c r="G173" s="17"/>
+      <c r="H173" s="5"/>
+    </row>
+    <row r="174" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B174" s="4"/>
+      <c r="C174" s="17"/>
+      <c r="D174" s="17"/>
+      <c r="E174" s="17"/>
+      <c r="F174" s="17"/>
+      <c r="G174" s="17"/>
+      <c r="H174" s="5"/>
+    </row>
+    <row r="175" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B175" s="4"/>
+      <c r="C175" s="17"/>
+      <c r="D175" s="17"/>
+      <c r="E175" s="17"/>
+      <c r="F175" s="17"/>
+      <c r="G175" s="17"/>
+      <c r="H175" s="5"/>
+    </row>
+    <row r="176" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B176" s="6"/>
+      <c r="C176" s="7"/>
+      <c r="D176" s="7"/>
+      <c r="E176" s="7"/>
+      <c r="F176" s="7"/>
+      <c r="G176" s="7"/>
+      <c r="H176" s="8"/>
+    </row>
+    <row r="179" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B179" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="C179" s="2"/>
+      <c r="D179" s="2"/>
+      <c r="E179" s="2"/>
+      <c r="F179" s="2"/>
+      <c r="G179" s="3"/>
+    </row>
+    <row r="180" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B180" s="4"/>
+      <c r="C180" s="17"/>
+      <c r="D180" s="17"/>
+      <c r="E180" s="17"/>
+      <c r="F180" s="17"/>
+      <c r="G180" s="5"/>
+    </row>
+    <row r="181" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B181" s="4"/>
+      <c r="C181" s="17"/>
+      <c r="D181" s="17"/>
+      <c r="E181" s="17"/>
+      <c r="F181" s="17"/>
+      <c r="G181" s="5"/>
+    </row>
+    <row r="182" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B182" s="4"/>
+      <c r="C182" s="17"/>
+      <c r="D182" s="17"/>
+      <c r="E182" s="17"/>
+      <c r="F182" s="17"/>
+      <c r="G182" s="5"/>
+    </row>
+    <row r="183" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B183" s="4"/>
+      <c r="C183" s="17"/>
+      <c r="D183" s="17"/>
+      <c r="E183" s="17"/>
+      <c r="F183" s="17"/>
+      <c r="G183" s="5"/>
+    </row>
+    <row r="184" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B184" s="4"/>
+      <c r="C184" s="17"/>
+      <c r="D184" s="17"/>
+      <c r="E184" s="17"/>
+      <c r="F184" s="17"/>
+      <c r="G184" s="5"/>
+    </row>
+    <row r="185" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B185" s="4"/>
+      <c r="C185" s="17"/>
+      <c r="D185" s="17"/>
+      <c r="E185" s="17"/>
+      <c r="F185" s="17"/>
+      <c r="G185" s="5"/>
+    </row>
+    <row r="186" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B186" s="4"/>
+      <c r="C186" s="17"/>
+      <c r="D186" s="17"/>
+      <c r="E186" s="17"/>
+      <c r="F186" s="17"/>
+      <c r="G186" s="5"/>
+    </row>
+    <row r="187" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B187" s="4"/>
+      <c r="C187" s="17"/>
+      <c r="D187" s="17"/>
+      <c r="E187" s="17"/>
+      <c r="F187" s="17"/>
+      <c r="G187" s="5"/>
+    </row>
+    <row r="188" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B188" s="6"/>
+      <c r="C188" s="7"/>
+      <c r="D188" s="7"/>
+      <c r="E188" s="7"/>
+      <c r="F188" s="7"/>
+      <c r="G188" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Introduction to advanced routing using route variables
</commit_message>
<xml_diff>
--- a/me/2.routing.xlsx
+++ b/me/2.routing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\build-php-mvc-framework\me\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F6E0B84-E0D8-41ED-8DA6-0D2C9E01DFAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7340DDF7-771D-4B12-9661-DA3F3E964300}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="central entry point" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="CreateAndRequireRouterClass" sheetId="3" r:id="rId3"/>
     <sheet name="routing table in the router" sheetId="4" r:id="rId4"/>
     <sheet name="MatchRequestedRouteToRoutingTbl" sheetId="5" r:id="rId5"/>
+    <sheet name="routing using route variables" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="143">
   <si>
     <t>Create a central entry point to the framework: the front controller</t>
   </si>
@@ -540,6 +541,24 @@
   </si>
   <si>
     <t>http://localhost/posts/new</t>
+  </si>
+  <si>
+    <t>Introduction to advanced routing using route variables</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Routing table của mình hiện tại có dạng single route bởi chỉ thực hiện so sánh chuỗi đơn thuần của giá trị route lấy được từ url với route trong routing table. Nếu như thế thì mình phải có rất  nhiều </t>
+  </si>
+  <si>
+    <t>route và url trong ứng dụng của mình điều đó sẽ làm cho routing table trở lên rất lớn.</t>
+  </si>
+  <si>
+    <t>Nhưng mình có thể dễ dàng nhận thấy rằng rất nhiều route có dạng pattern giống nhau đó là phần đầu tiên của url hay route đó là controller, phần thứ 2 đó là action</t>
+  </si>
+  <si>
+    <t>Do đó mình có thể define pattern hay variable part của route mà sẽ map parameter với route(Controller hay action). Điều này giúp cho routing table của mình sẽ trở lên đơn giản hơn nhiều. Mình chỉ</t>
+  </si>
+  <si>
+    <t>cần 1 route nhưng có thể cover tất cả các url</t>
   </si>
 </sst>
 </file>
@@ -3305,6 +3324,523 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>60761</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F3166C2C-25EB-6619-855C-9069401F347A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="723900" y="1219200"/>
+          <a:ext cx="11363325" cy="3413561"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>152401</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>476251</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>69721</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4B6E0C68-377F-8CC6-DBCD-848B5BA211A7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="762001" y="5448300"/>
+          <a:ext cx="11296650" cy="3384421"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="Straight Arrow Connector 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A03E361D-36C3-897F-7AF4-3D994317A0A2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="5353050" y="1323975"/>
+          <a:ext cx="2933700" cy="1495425"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="7" name="Straight Arrow Connector 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8C789BBB-7936-A84A-EAD1-8401984AE21A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8296275" y="1323975"/>
+          <a:ext cx="657225" cy="1485900"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="9" name="Straight Arrow Connector 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8AB69EB7-92EA-7FF0-D1A0-D1D54BE3F023}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="6372225" y="1295400"/>
+          <a:ext cx="3571875" cy="1533525"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="11" name="Straight Arrow Connector 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1BC0B916-D3C0-89AD-EE0A-12BF49D12FDE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9944100" y="1276350"/>
+          <a:ext cx="657225" cy="1514475"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="14" name="Straight Arrow Connector 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{51BA6E27-491B-CFF6-B63B-7C98FB70A047}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="5219700" y="5524500"/>
+          <a:ext cx="190500" cy="2200275"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="16" name="Straight Arrow Connector 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F216CE11-EA02-E53D-CB42-4861D940CC77}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5410200" y="5505450"/>
+          <a:ext cx="1714500" cy="2219325"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="19" name="Straight Arrow Connector 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FE241EDA-E325-5AF6-03F0-A48B0ADFCCE7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6657975" y="5495925"/>
+          <a:ext cx="2181225" cy="1485900"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="21" name="Straight Arrow Connector 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B4A141D7-61D7-4B0C-C5F6-7DECC1D80145}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7248525" y="5495925"/>
+          <a:ext cx="3181350" cy="1514475"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -5940,7 +6476,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AE241D4-197C-4BF6-874B-4B7E9956690B}">
   <dimension ref="A2:T188"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A167" workbookViewId="0">
+    <sheetView topLeftCell="A167" workbookViewId="0">
       <selection activeCell="P182" sqref="P182"/>
     </sheetView>
   </sheetViews>
@@ -5978,6 +6514,1038 @@
       <c r="B6" s="4" t="s">
         <v>108</v>
       </c>
+      <c r="T6" s="5"/>
+    </row>
+    <row r="7" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B7" s="4"/>
+      <c r="T7" s="5"/>
+    </row>
+    <row r="8" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B8" s="4"/>
+      <c r="T8" s="5"/>
+    </row>
+    <row r="9" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B9" s="4"/>
+      <c r="T9" s="5"/>
+    </row>
+    <row r="10" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B10" s="4"/>
+      <c r="T10" s="5"/>
+    </row>
+    <row r="11" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B11" s="4"/>
+      <c r="T11" s="5"/>
+    </row>
+    <row r="12" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B12" s="4"/>
+      <c r="T12" s="5"/>
+    </row>
+    <row r="13" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B13" s="4"/>
+      <c r="T13" s="5"/>
+    </row>
+    <row r="14" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B14" s="4"/>
+      <c r="T14" s="5"/>
+    </row>
+    <row r="15" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B15" s="4"/>
+      <c r="T15" s="5"/>
+    </row>
+    <row r="16" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B16" s="4"/>
+      <c r="T16" s="5"/>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B17" s="4"/>
+      <c r="T17" s="5"/>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B18" s="4"/>
+      <c r="T18" s="5"/>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B19" s="4"/>
+      <c r="T19" s="5"/>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B20" s="4"/>
+      <c r="T20" s="5"/>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B21" s="4"/>
+      <c r="T21" s="5"/>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B22" s="4"/>
+      <c r="T22" s="5"/>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B23" s="4"/>
+      <c r="T23" s="5"/>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B24" s="4"/>
+      <c r="T24" s="5"/>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B25" s="4"/>
+      <c r="T25" s="5"/>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B26" s="4"/>
+      <c r="T26" s="5"/>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B27" s="6"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="7"/>
+      <c r="H27" s="7"/>
+      <c r="I27" s="7"/>
+      <c r="J27" s="7"/>
+      <c r="K27" s="7"/>
+      <c r="L27" s="7"/>
+      <c r="M27" s="7"/>
+      <c r="N27" s="7"/>
+      <c r="O27" s="7"/>
+      <c r="P27" s="7"/>
+      <c r="Q27" s="7"/>
+      <c r="R27" s="7"/>
+      <c r="S27" s="7"/>
+      <c r="T27" s="8"/>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A30" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B31" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="3"/>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B32" s="4"/>
+      <c r="C32" t="s">
+        <v>10</v>
+      </c>
+      <c r="F32" s="5"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B33" s="4"/>
+      <c r="D33" t="s">
+        <v>11</v>
+      </c>
+      <c r="F33" s="5"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B34" s="4"/>
+      <c r="D34" t="s">
+        <v>12</v>
+      </c>
+      <c r="F34" s="5"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B35" s="4"/>
+      <c r="D35" t="s">
+        <v>13</v>
+      </c>
+      <c r="F35" s="5"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B36" s="4"/>
+      <c r="C36" t="s">
+        <v>14</v>
+      </c>
+      <c r="F36" s="5"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B37" s="4"/>
+      <c r="D37" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="F37" s="5"/>
+      <c r="G37" t="s">
+        <v>20</v>
+      </c>
+      <c r="H37" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B38" s="4"/>
+      <c r="C38" t="s">
+        <v>15</v>
+      </c>
+      <c r="F38" s="5"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B39" s="4"/>
+      <c r="C39" t="s">
+        <v>16</v>
+      </c>
+      <c r="F39" s="5"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B40" s="4"/>
+      <c r="D40" t="s">
+        <v>26</v>
+      </c>
+      <c r="F40" s="5"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B41" s="4"/>
+      <c r="D41" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="F41" s="5"/>
+      <c r="G41" t="s">
+        <v>20</v>
+      </c>
+      <c r="H41" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B42" s="6"/>
+      <c r="C42" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D42" s="7"/>
+      <c r="E42" s="7"/>
+      <c r="F42" s="8"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B46" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C46" s="2"/>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
+      <c r="F46" s="2"/>
+      <c r="G46" s="2"/>
+      <c r="H46" s="2"/>
+      <c r="I46" s="3"/>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B47" s="4"/>
+      <c r="I47" s="5"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B48" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="I48" s="5"/>
+    </row>
+    <row r="49" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B49" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="I49" s="5"/>
+    </row>
+    <row r="50" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B50" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="I50" s="5"/>
+    </row>
+    <row r="51" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B51" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="I51" s="5"/>
+    </row>
+    <row r="52" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B52" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="I52" s="5"/>
+    </row>
+    <row r="53" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B53" s="4"/>
+      <c r="I53" s="5"/>
+    </row>
+    <row r="54" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B54" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="I54" s="5"/>
+    </row>
+    <row r="55" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B55" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="I55" s="5"/>
+    </row>
+    <row r="56" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B56" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="I56" s="5"/>
+    </row>
+    <row r="57" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B57" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="I57" s="5"/>
+    </row>
+    <row r="58" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B58" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="I58" s="5"/>
+    </row>
+    <row r="59" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B59" s="4"/>
+      <c r="I59" s="5"/>
+    </row>
+    <row r="60" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B60" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="I60" s="5"/>
+    </row>
+    <row r="61" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B61" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="I61" s="5"/>
+    </row>
+    <row r="62" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B62" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="I62" s="5"/>
+    </row>
+    <row r="63" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B63" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="I63" s="5"/>
+    </row>
+    <row r="64" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B64" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="I64" s="5"/>
+    </row>
+    <row r="65" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B65" s="4"/>
+      <c r="I65" s="5"/>
+    </row>
+    <row r="66" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B66" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="I66" s="5"/>
+    </row>
+    <row r="67" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B67" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="I67" s="5"/>
+    </row>
+    <row r="68" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B68" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="I68" s="5"/>
+    </row>
+    <row r="69" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B69" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="I69" s="5"/>
+    </row>
+    <row r="70" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B70" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="I70" s="5"/>
+    </row>
+    <row r="71" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B71" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="I71" s="5"/>
+    </row>
+    <row r="72" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B72" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="I72" s="5"/>
+    </row>
+    <row r="73" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B73" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="I73" s="5"/>
+    </row>
+    <row r="74" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B74" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="I74" s="5"/>
+    </row>
+    <row r="75" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B75" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="I75" s="5"/>
+    </row>
+    <row r="76" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B76" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="I76" s="5"/>
+    </row>
+    <row r="77" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B77" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="I77" s="5"/>
+    </row>
+    <row r="78" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B78" s="4"/>
+      <c r="I78" s="5"/>
+    </row>
+    <row r="79" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B79" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="I79" s="5"/>
+    </row>
+    <row r="80" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B80" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="I80" s="5"/>
+    </row>
+    <row r="81" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B81" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="I81" s="5"/>
+    </row>
+    <row r="82" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B82" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="I82" s="5"/>
+    </row>
+    <row r="83" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B83" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="I83" s="5"/>
+    </row>
+    <row r="84" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B84" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="I84" s="5"/>
+    </row>
+    <row r="85" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B85" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="I85" s="5"/>
+    </row>
+    <row r="86" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B86" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="I86" s="5"/>
+    </row>
+    <row r="87" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B87" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="I87" s="5"/>
+    </row>
+    <row r="88" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B88" s="4"/>
+      <c r="I88" s="5"/>
+    </row>
+    <row r="89" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B89" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="I89" s="5"/>
+    </row>
+    <row r="90" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B90" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="I90" s="5"/>
+    </row>
+    <row r="91" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B91" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="I91" s="5"/>
+    </row>
+    <row r="92" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B92" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="I92" s="5"/>
+    </row>
+    <row r="93" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B93" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="I93" s="5"/>
+    </row>
+    <row r="94" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B94" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="I94" s="5"/>
+    </row>
+    <row r="95" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B95" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="I95" s="5"/>
+    </row>
+    <row r="96" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B96" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="I96" s="5"/>
+    </row>
+    <row r="97" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B97" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="I97" s="5"/>
+    </row>
+    <row r="98" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B98" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="I98" s="5"/>
+    </row>
+    <row r="99" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B99" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="I99" s="5"/>
+    </row>
+    <row r="100" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B100" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="I100" s="5"/>
+    </row>
+    <row r="101" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B101" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="I101" s="5"/>
+    </row>
+    <row r="102" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B102" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="I102" s="5"/>
+    </row>
+    <row r="103" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B103" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="I103" s="5"/>
+    </row>
+    <row r="104" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B104" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="I104" s="5"/>
+    </row>
+    <row r="105" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B105" s="14"/>
+      <c r="I105" s="5"/>
+    </row>
+    <row r="106" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B106" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="I106" s="5"/>
+    </row>
+    <row r="107" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B107" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="I107" s="5"/>
+    </row>
+    <row r="108" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B108" s="14"/>
+      <c r="I108" s="5"/>
+    </row>
+    <row r="109" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B109" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="I109" s="5"/>
+    </row>
+    <row r="110" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B110" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="I110" s="5"/>
+    </row>
+    <row r="111" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B111" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="I111" s="5"/>
+    </row>
+    <row r="112" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B112" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="I112" s="5"/>
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B113" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="I113" s="5"/>
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B114" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="I114" s="5"/>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B115" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="I115" s="5"/>
+    </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B116" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="I116" s="5"/>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B117" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="I117" s="5"/>
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B118" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="C118" s="7"/>
+      <c r="D118" s="7"/>
+      <c r="E118" s="7"/>
+      <c r="F118" s="7"/>
+      <c r="G118" s="7"/>
+      <c r="H118" s="7"/>
+      <c r="I118" s="8"/>
+    </row>
+    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B122" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C122" s="2"/>
+      <c r="D122" s="2"/>
+      <c r="E122" s="2"/>
+      <c r="F122" s="2"/>
+      <c r="G122" s="2"/>
+      <c r="H122" s="3"/>
+    </row>
+    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B123" s="4"/>
+      <c r="H123" s="5"/>
+    </row>
+    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B124" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H124" s="5"/>
+    </row>
+    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B125" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="H125" s="5"/>
+    </row>
+    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B126" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="H126" s="5"/>
+    </row>
+    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B127" s="4"/>
+      <c r="H127" s="5"/>
+    </row>
+    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B128" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H128" s="5"/>
+    </row>
+    <row r="129" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B129" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="H129" s="5"/>
+    </row>
+    <row r="130" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B130" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="H130" s="5"/>
+    </row>
+    <row r="131" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B131" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="H131" s="5"/>
+    </row>
+    <row r="132" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B132" s="4"/>
+      <c r="H132" s="5"/>
+    </row>
+    <row r="133" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B133" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="H133" s="5"/>
+    </row>
+    <row r="134" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B134" s="4"/>
+      <c r="H134" s="5"/>
+    </row>
+    <row r="135" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B135" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="H135" s="5"/>
+    </row>
+    <row r="136" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B136" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="H136" s="5"/>
+    </row>
+    <row r="137" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B137" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="H137" s="5"/>
+    </row>
+    <row r="138" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B138" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="H138" s="5"/>
+    </row>
+    <row r="139" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B139" s="4"/>
+      <c r="H139" s="5"/>
+    </row>
+    <row r="140" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B140" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="H140" s="5"/>
+    </row>
+    <row r="141" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B141" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="H141" s="5"/>
+    </row>
+    <row r="142" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B142" s="14"/>
+      <c r="H142" s="5"/>
+    </row>
+    <row r="143" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B143" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="H143" s="5"/>
+    </row>
+    <row r="144" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B144" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="H144" s="5"/>
+    </row>
+    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B145" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="H145" s="5"/>
+    </row>
+    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B146" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="H146" s="5"/>
+    </row>
+    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B147" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="H147" s="5"/>
+    </row>
+    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B148" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="H148" s="5"/>
+    </row>
+    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B149" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="C149" s="7"/>
+      <c r="D149" s="7"/>
+      <c r="E149" s="7"/>
+      <c r="F149" s="7"/>
+      <c r="G149" s="7"/>
+      <c r="H149" s="8"/>
+    </row>
+    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A152" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B153" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="C153" s="2"/>
+      <c r="D153" s="2"/>
+      <c r="E153" s="2"/>
+      <c r="F153" s="2"/>
+      <c r="G153" s="3"/>
+    </row>
+    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B154" s="4"/>
+      <c r="G154" s="5"/>
+    </row>
+    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B155" s="4"/>
+      <c r="G155" s="5"/>
+    </row>
+    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B156" s="4"/>
+      <c r="G156" s="5"/>
+    </row>
+    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B157" s="4"/>
+      <c r="G157" s="5"/>
+    </row>
+    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B158" s="4"/>
+      <c r="G158" s="5"/>
+    </row>
+    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B159" s="4"/>
+      <c r="G159" s="5"/>
+    </row>
+    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B160" s="4"/>
+      <c r="G160" s="5"/>
+    </row>
+    <row r="161" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B161" s="4"/>
+      <c r="G161" s="5"/>
+    </row>
+    <row r="162" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B162" s="4"/>
+      <c r="G162" s="5"/>
+    </row>
+    <row r="163" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B163" s="6"/>
+      <c r="C163" s="7"/>
+      <c r="D163" s="7"/>
+      <c r="E163" s="7"/>
+      <c r="F163" s="7"/>
+      <c r="G163" s="8"/>
+    </row>
+    <row r="166" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B166" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="C166" s="2"/>
+      <c r="D166" s="2"/>
+      <c r="E166" s="2"/>
+      <c r="F166" s="2"/>
+      <c r="G166" s="2"/>
+      <c r="H166" s="3"/>
+    </row>
+    <row r="167" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B167" s="4"/>
+      <c r="H167" s="5"/>
+    </row>
+    <row r="168" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B168" s="4"/>
+      <c r="H168" s="5"/>
+    </row>
+    <row r="169" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B169" s="4"/>
+      <c r="H169" s="5"/>
+    </row>
+    <row r="170" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B170" s="4"/>
+      <c r="H170" s="5"/>
+    </row>
+    <row r="171" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B171" s="4"/>
+      <c r="H171" s="5"/>
+    </row>
+    <row r="172" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B172" s="4"/>
+      <c r="H172" s="5"/>
+    </row>
+    <row r="173" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B173" s="4"/>
+      <c r="H173" s="5"/>
+    </row>
+    <row r="174" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B174" s="4"/>
+      <c r="H174" s="5"/>
+    </row>
+    <row r="175" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B175" s="4"/>
+      <c r="H175" s="5"/>
+    </row>
+    <row r="176" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B176" s="6"/>
+      <c r="C176" s="7"/>
+      <c r="D176" s="7"/>
+      <c r="E176" s="7"/>
+      <c r="F176" s="7"/>
+      <c r="G176" s="7"/>
+      <c r="H176" s="8"/>
+    </row>
+    <row r="179" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B179" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="C179" s="2"/>
+      <c r="D179" s="2"/>
+      <c r="E179" s="2"/>
+      <c r="F179" s="2"/>
+      <c r="G179" s="3"/>
+    </row>
+    <row r="180" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B180" s="4"/>
+      <c r="G180" s="5"/>
+    </row>
+    <row r="181" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B181" s="4"/>
+      <c r="G181" s="5"/>
+    </row>
+    <row r="182" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B182" s="4"/>
+      <c r="G182" s="5"/>
+    </row>
+    <row r="183" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B183" s="4"/>
+      <c r="G183" s="5"/>
+    </row>
+    <row r="184" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B184" s="4"/>
+      <c r="G184" s="5"/>
+    </row>
+    <row r="185" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B185" s="4"/>
+      <c r="G185" s="5"/>
+    </row>
+    <row r="186" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B186" s="4"/>
+      <c r="G186" s="5"/>
+    </row>
+    <row r="187" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B187" s="4"/>
+      <c r="G187" s="5"/>
+    </row>
+    <row r="188" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B188" s="6"/>
+      <c r="C188" s="7"/>
+      <c r="D188" s="7"/>
+      <c r="E188" s="7"/>
+      <c r="F188" s="7"/>
+      <c r="G188" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E01E8A2C-EBC4-4512-8867-F476D8E6BF62}">
+  <dimension ref="B2:T49"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="5" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="2"/>
+      <c r="R5" s="2"/>
+      <c r="S5" s="2"/>
+      <c r="T5" s="3"/>
+    </row>
+    <row r="6" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B6" s="4" t="s">
+        <v>139</v>
+      </c>
       <c r="C6" s="17"/>
       <c r="D6" s="17"/>
       <c r="E6" s="17"/>
@@ -5998,7 +7566,9 @@
       <c r="T6" s="5"/>
     </row>
     <row r="7" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B7" s="4"/>
+      <c r="B7" s="4" t="s">
+        <v>140</v>
+      </c>
       <c r="C7" s="17"/>
       <c r="D7" s="17"/>
       <c r="E7" s="17"/>
@@ -6207,7 +7777,7 @@
       <c r="S16" s="17"/>
       <c r="T16" s="5"/>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B17" s="4"/>
       <c r="C17" s="17"/>
       <c r="D17" s="17"/>
@@ -6228,7 +7798,7 @@
       <c r="S17" s="17"/>
       <c r="T17" s="5"/>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B18" s="4"/>
       <c r="C18" s="17"/>
       <c r="D18" s="17"/>
@@ -6249,7 +7819,7 @@
       <c r="S18" s="17"/>
       <c r="T18" s="5"/>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B19" s="4"/>
       <c r="C19" s="17"/>
       <c r="D19" s="17"/>
@@ -6270,7 +7840,7 @@
       <c r="S19" s="17"/>
       <c r="T19" s="5"/>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B20" s="4"/>
       <c r="C20" s="17"/>
       <c r="D20" s="17"/>
@@ -6291,7 +7861,7 @@
       <c r="S20" s="17"/>
       <c r="T20" s="5"/>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B21" s="4"/>
       <c r="C21" s="17"/>
       <c r="D21" s="17"/>
@@ -6312,7 +7882,7 @@
       <c r="S21" s="17"/>
       <c r="T21" s="5"/>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B22" s="4"/>
       <c r="C22" s="17"/>
       <c r="D22" s="17"/>
@@ -6333,7 +7903,7 @@
       <c r="S22" s="17"/>
       <c r="T22" s="5"/>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B23" s="4"/>
       <c r="C23" s="17"/>
       <c r="D23" s="17"/>
@@ -6354,7 +7924,7 @@
       <c r="S23" s="17"/>
       <c r="T23" s="5"/>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B24" s="4"/>
       <c r="C24" s="17"/>
       <c r="D24" s="17"/>
@@ -6375,7 +7945,7 @@
       <c r="S24" s="17"/>
       <c r="T24" s="5"/>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B25" s="4"/>
       <c r="C25" s="17"/>
       <c r="D25" s="17"/>
@@ -6396,171 +7966,410 @@
       <c r="S25" s="17"/>
       <c r="T25" s="5"/>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B26" s="4"/>
-      <c r="C26" s="17"/>
-      <c r="D26" s="17"/>
-      <c r="E26" s="17"/>
-      <c r="F26" s="17"/>
-      <c r="G26" s="17"/>
-      <c r="H26" s="17"/>
-      <c r="I26" s="17"/>
-      <c r="J26" s="17"/>
-      <c r="K26" s="17"/>
-      <c r="L26" s="17"/>
-      <c r="M26" s="17"/>
-      <c r="N26" s="17"/>
-      <c r="O26" s="17"/>
-      <c r="P26" s="17"/>
-      <c r="Q26" s="17"/>
-      <c r="R26" s="17"/>
-      <c r="S26" s="17"/>
-      <c r="T26" s="5"/>
-    </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B27" s="6"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="7"/>
-      <c r="E27" s="7"/>
-      <c r="F27" s="7"/>
-      <c r="G27" s="7"/>
-      <c r="H27" s="7"/>
-      <c r="I27" s="7"/>
-      <c r="J27" s="7"/>
-      <c r="K27" s="7"/>
-      <c r="L27" s="7"/>
-      <c r="M27" s="7"/>
-      <c r="N27" s="7"/>
-      <c r="O27" s="7"/>
-      <c r="P27" s="7"/>
-      <c r="Q27" s="7"/>
-      <c r="R27" s="7"/>
-      <c r="S27" s="7"/>
-      <c r="T27" s="8"/>
-    </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A30" s="9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B31" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="3"/>
-    </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B26" s="6"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7"/>
+      <c r="H26" s="7"/>
+      <c r="I26" s="7"/>
+      <c r="J26" s="7"/>
+      <c r="K26" s="7"/>
+      <c r="L26" s="7"/>
+      <c r="M26" s="7"/>
+      <c r="N26" s="7"/>
+      <c r="O26" s="7"/>
+      <c r="P26" s="7"/>
+      <c r="Q26" s="7"/>
+      <c r="R26" s="7"/>
+      <c r="S26" s="7"/>
+      <c r="T26" s="8"/>
+    </row>
+    <row r="29" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B29" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="2"/>
+      <c r="L29" s="2"/>
+      <c r="M29" s="2"/>
+      <c r="N29" s="2"/>
+      <c r="O29" s="2"/>
+      <c r="P29" s="2"/>
+      <c r="Q29" s="2"/>
+      <c r="R29" s="2"/>
+      <c r="S29" s="2"/>
+      <c r="T29" s="3"/>
+    </row>
+    <row r="30" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B30" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="C30" s="17"/>
+      <c r="D30" s="17"/>
+      <c r="E30" s="17"/>
+      <c r="F30" s="17"/>
+      <c r="G30" s="17"/>
+      <c r="H30" s="17"/>
+      <c r="I30" s="17"/>
+      <c r="J30" s="17"/>
+      <c r="K30" s="17"/>
+      <c r="L30" s="17"/>
+      <c r="M30" s="17"/>
+      <c r="N30" s="17"/>
+      <c r="O30" s="17"/>
+      <c r="P30" s="17"/>
+      <c r="Q30" s="17"/>
+      <c r="R30" s="17"/>
+      <c r="S30" s="17"/>
+      <c r="T30" s="5"/>
+    </row>
+    <row r="31" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B31" s="4"/>
+      <c r="C31" s="17"/>
+      <c r="D31" s="17"/>
+      <c r="E31" s="17"/>
+      <c r="F31" s="17"/>
+      <c r="G31" s="17"/>
+      <c r="H31" s="17"/>
+      <c r="I31" s="17"/>
+      <c r="J31" s="17"/>
+      <c r="K31" s="17"/>
+      <c r="L31" s="17"/>
+      <c r="M31" s="17"/>
+      <c r="N31" s="17"/>
+      <c r="O31" s="17"/>
+      <c r="P31" s="17"/>
+      <c r="Q31" s="17"/>
+      <c r="R31" s="17"/>
+      <c r="S31" s="17"/>
+      <c r="T31" s="5"/>
+    </row>
+    <row r="32" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B32" s="4"/>
-      <c r="C32" t="s">
-        <v>10</v>
-      </c>
-      <c r="F32" s="5"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C32" s="17"/>
+      <c r="D32" s="17"/>
+      <c r="E32" s="17"/>
+      <c r="F32" s="17"/>
+      <c r="G32" s="17"/>
+      <c r="H32" s="17"/>
+      <c r="I32" s="17"/>
+      <c r="J32" s="17"/>
+      <c r="K32" s="17"/>
+      <c r="L32" s="17"/>
+      <c r="M32" s="17"/>
+      <c r="N32" s="17"/>
+      <c r="O32" s="17"/>
+      <c r="P32" s="17"/>
+      <c r="Q32" s="17"/>
+      <c r="R32" s="17"/>
+      <c r="S32" s="17"/>
+      <c r="T32" s="5"/>
+    </row>
+    <row r="33" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B33" s="4"/>
-      <c r="D33" t="s">
-        <v>11</v>
-      </c>
-      <c r="F33" s="5"/>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C33" s="17"/>
+      <c r="D33" s="17"/>
+      <c r="E33" s="17"/>
+      <c r="F33" s="17"/>
+      <c r="G33" s="17"/>
+      <c r="H33" s="17"/>
+      <c r="I33" s="17"/>
+      <c r="J33" s="17"/>
+      <c r="K33" s="17"/>
+      <c r="L33" s="17"/>
+      <c r="M33" s="17"/>
+      <c r="N33" s="17"/>
+      <c r="O33" s="17"/>
+      <c r="P33" s="17"/>
+      <c r="Q33" s="17"/>
+      <c r="R33" s="17"/>
+      <c r="S33" s="17"/>
+      <c r="T33" s="5"/>
+    </row>
+    <row r="34" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B34" s="4"/>
-      <c r="D34" t="s">
-        <v>12</v>
-      </c>
-      <c r="F34" s="5"/>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C34" s="17"/>
+      <c r="D34" s="17"/>
+      <c r="E34" s="17"/>
+      <c r="F34" s="17"/>
+      <c r="G34" s="17"/>
+      <c r="H34" s="17"/>
+      <c r="I34" s="17"/>
+      <c r="J34" s="17"/>
+      <c r="K34" s="17"/>
+      <c r="L34" s="17"/>
+      <c r="M34" s="17"/>
+      <c r="N34" s="17"/>
+      <c r="O34" s="17"/>
+      <c r="P34" s="17"/>
+      <c r="Q34" s="17"/>
+      <c r="R34" s="17"/>
+      <c r="S34" s="17"/>
+      <c r="T34" s="5"/>
+    </row>
+    <row r="35" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B35" s="4"/>
-      <c r="D35" t="s">
-        <v>13</v>
-      </c>
-      <c r="F35" s="5"/>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C35" s="17"/>
+      <c r="D35" s="17"/>
+      <c r="E35" s="17"/>
+      <c r="F35" s="17"/>
+      <c r="G35" s="17"/>
+      <c r="H35" s="17"/>
+      <c r="I35" s="17"/>
+      <c r="J35" s="17"/>
+      <c r="K35" s="17"/>
+      <c r="L35" s="17"/>
+      <c r="M35" s="17"/>
+      <c r="N35" s="17"/>
+      <c r="O35" s="17"/>
+      <c r="P35" s="17"/>
+      <c r="Q35" s="17"/>
+      <c r="R35" s="17"/>
+      <c r="S35" s="17"/>
+      <c r="T35" s="5"/>
+    </row>
+    <row r="36" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B36" s="4"/>
-      <c r="C36" t="s">
-        <v>14</v>
-      </c>
-      <c r="F36" s="5"/>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C36" s="17"/>
+      <c r="D36" s="17"/>
+      <c r="E36" s="17"/>
+      <c r="F36" s="17"/>
+      <c r="G36" s="17"/>
+      <c r="H36" s="17"/>
+      <c r="I36" s="17"/>
+      <c r="J36" s="17"/>
+      <c r="K36" s="17"/>
+      <c r="L36" s="17"/>
+      <c r="M36" s="17"/>
+      <c r="N36" s="17"/>
+      <c r="O36" s="17"/>
+      <c r="P36" s="17"/>
+      <c r="Q36" s="17"/>
+      <c r="R36" s="17"/>
+      <c r="S36" s="17"/>
+      <c r="T36" s="5"/>
+    </row>
+    <row r="37" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B37" s="4"/>
-      <c r="D37" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="F37" s="5"/>
-      <c r="G37" t="s">
-        <v>20</v>
-      </c>
-      <c r="H37" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C37" s="17"/>
+      <c r="D37" s="17"/>
+      <c r="E37" s="17"/>
+      <c r="F37" s="17"/>
+      <c r="G37" s="17"/>
+      <c r="H37" s="17"/>
+      <c r="I37" s="17"/>
+      <c r="J37" s="17"/>
+      <c r="K37" s="17"/>
+      <c r="L37" s="17"/>
+      <c r="M37" s="17"/>
+      <c r="N37" s="17"/>
+      <c r="O37" s="17"/>
+      <c r="P37" s="17"/>
+      <c r="Q37" s="17"/>
+      <c r="R37" s="17"/>
+      <c r="S37" s="17"/>
+      <c r="T37" s="5"/>
+    </row>
+    <row r="38" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B38" s="4"/>
-      <c r="C38" t="s">
-        <v>15</v>
-      </c>
-      <c r="F38" s="5"/>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C38" s="17"/>
+      <c r="D38" s="17"/>
+      <c r="E38" s="17"/>
+      <c r="F38" s="17"/>
+      <c r="G38" s="17"/>
+      <c r="H38" s="17"/>
+      <c r="I38" s="17"/>
+      <c r="J38" s="17"/>
+      <c r="K38" s="17"/>
+      <c r="L38" s="17"/>
+      <c r="M38" s="17"/>
+      <c r="N38" s="17"/>
+      <c r="O38" s="17"/>
+      <c r="P38" s="17"/>
+      <c r="Q38" s="17"/>
+      <c r="R38" s="17"/>
+      <c r="S38" s="17"/>
+      <c r="T38" s="5"/>
+    </row>
+    <row r="39" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B39" s="4"/>
-      <c r="C39" t="s">
-        <v>16</v>
-      </c>
-      <c r="F39" s="5"/>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C39" s="17"/>
+      <c r="D39" s="17"/>
+      <c r="E39" s="17"/>
+      <c r="F39" s="17"/>
+      <c r="G39" s="17"/>
+      <c r="H39" s="17"/>
+      <c r="I39" s="17"/>
+      <c r="J39" s="17"/>
+      <c r="K39" s="17"/>
+      <c r="L39" s="17"/>
+      <c r="M39" s="17"/>
+      <c r="N39" s="17"/>
+      <c r="O39" s="17"/>
+      <c r="P39" s="17"/>
+      <c r="Q39" s="17"/>
+      <c r="R39" s="17"/>
+      <c r="S39" s="17"/>
+      <c r="T39" s="5"/>
+    </row>
+    <row r="40" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B40" s="4"/>
-      <c r="D40" t="s">
-        <v>26</v>
-      </c>
-      <c r="F40" s="5"/>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C40" s="17"/>
+      <c r="D40" s="17"/>
+      <c r="E40" s="17"/>
+      <c r="F40" s="17"/>
+      <c r="G40" s="17"/>
+      <c r="H40" s="17"/>
+      <c r="I40" s="17"/>
+      <c r="J40" s="17"/>
+      <c r="K40" s="17"/>
+      <c r="L40" s="17"/>
+      <c r="M40" s="17"/>
+      <c r="N40" s="17"/>
+      <c r="O40" s="17"/>
+      <c r="P40" s="17"/>
+      <c r="Q40" s="17"/>
+      <c r="R40" s="17"/>
+      <c r="S40" s="17"/>
+      <c r="T40" s="5"/>
+    </row>
+    <row r="41" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B41" s="4"/>
-      <c r="D41" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="F41" s="5"/>
-      <c r="G41" t="s">
-        <v>20</v>
-      </c>
-      <c r="H41" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B42" s="6"/>
-      <c r="C42" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="D42" s="7"/>
-      <c r="E42" s="7"/>
-      <c r="F42" s="8"/>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B46" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C46" s="2"/>
-      <c r="D46" s="2"/>
-      <c r="E46" s="2"/>
-      <c r="F46" s="2"/>
-      <c r="G46" s="2"/>
-      <c r="H46" s="2"/>
-      <c r="I46" s="3"/>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C41" s="17"/>
+      <c r="D41" s="17"/>
+      <c r="E41" s="17"/>
+      <c r="F41" s="17"/>
+      <c r="G41" s="17"/>
+      <c r="H41" s="17"/>
+      <c r="I41" s="17"/>
+      <c r="J41" s="17"/>
+      <c r="K41" s="17"/>
+      <c r="L41" s="17"/>
+      <c r="M41" s="17"/>
+      <c r="N41" s="17"/>
+      <c r="O41" s="17"/>
+      <c r="P41" s="17"/>
+      <c r="Q41" s="17"/>
+      <c r="R41" s="17"/>
+      <c r="S41" s="17"/>
+      <c r="T41" s="5"/>
+    </row>
+    <row r="42" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B42" s="4"/>
+      <c r="C42" s="17"/>
+      <c r="D42" s="17"/>
+      <c r="E42" s="17"/>
+      <c r="F42" s="17"/>
+      <c r="G42" s="17"/>
+      <c r="H42" s="17"/>
+      <c r="I42" s="17"/>
+      <c r="J42" s="17"/>
+      <c r="K42" s="17"/>
+      <c r="L42" s="17"/>
+      <c r="M42" s="17"/>
+      <c r="N42" s="17"/>
+      <c r="O42" s="17"/>
+      <c r="P42" s="17"/>
+      <c r="Q42" s="17"/>
+      <c r="R42" s="17"/>
+      <c r="S42" s="17"/>
+      <c r="T42" s="5"/>
+    </row>
+    <row r="43" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B43" s="4"/>
+      <c r="C43" s="17"/>
+      <c r="D43" s="17"/>
+      <c r="E43" s="17"/>
+      <c r="F43" s="17"/>
+      <c r="G43" s="17"/>
+      <c r="H43" s="17"/>
+      <c r="I43" s="17"/>
+      <c r="J43" s="17"/>
+      <c r="K43" s="17"/>
+      <c r="L43" s="17"/>
+      <c r="M43" s="17"/>
+      <c r="N43" s="17"/>
+      <c r="O43" s="17"/>
+      <c r="P43" s="17"/>
+      <c r="Q43" s="17"/>
+      <c r="R43" s="17"/>
+      <c r="S43" s="17"/>
+      <c r="T43" s="5"/>
+    </row>
+    <row r="44" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B44" s="4"/>
+      <c r="C44" s="17"/>
+      <c r="D44" s="17"/>
+      <c r="E44" s="17"/>
+      <c r="F44" s="17"/>
+      <c r="G44" s="17"/>
+      <c r="H44" s="17"/>
+      <c r="I44" s="17"/>
+      <c r="J44" s="17"/>
+      <c r="K44" s="17"/>
+      <c r="L44" s="17"/>
+      <c r="M44" s="17"/>
+      <c r="N44" s="17"/>
+      <c r="O44" s="17"/>
+      <c r="P44" s="17"/>
+      <c r="Q44" s="17"/>
+      <c r="R44" s="17"/>
+      <c r="S44" s="17"/>
+      <c r="T44" s="5"/>
+    </row>
+    <row r="45" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B45" s="4"/>
+      <c r="C45" s="17"/>
+      <c r="D45" s="17"/>
+      <c r="E45" s="17"/>
+      <c r="F45" s="17"/>
+      <c r="G45" s="17"/>
+      <c r="H45" s="17"/>
+      <c r="I45" s="17"/>
+      <c r="J45" s="17"/>
+      <c r="K45" s="17"/>
+      <c r="L45" s="17"/>
+      <c r="M45" s="17"/>
+      <c r="N45" s="17"/>
+      <c r="O45" s="17"/>
+      <c r="P45" s="17"/>
+      <c r="Q45" s="17"/>
+      <c r="R45" s="17"/>
+      <c r="S45" s="17"/>
+      <c r="T45" s="5"/>
+    </row>
+    <row r="46" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B46" s="4"/>
+      <c r="C46" s="17"/>
+      <c r="D46" s="17"/>
+      <c r="E46" s="17"/>
+      <c r="F46" s="17"/>
+      <c r="G46" s="17"/>
+      <c r="H46" s="17"/>
+      <c r="I46" s="17"/>
+      <c r="J46" s="17"/>
+      <c r="K46" s="17"/>
+      <c r="L46" s="17"/>
+      <c r="M46" s="17"/>
+      <c r="N46" s="17"/>
+      <c r="O46" s="17"/>
+      <c r="P46" s="17"/>
+      <c r="Q46" s="17"/>
+      <c r="R46" s="17"/>
+      <c r="S46" s="17"/>
+      <c r="T46" s="5"/>
+    </row>
+    <row r="47" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B47" s="4"/>
       <c r="C47" s="17"/>
       <c r="D47" s="17"/>
@@ -6568,1428 +8377,63 @@
       <c r="F47" s="17"/>
       <c r="G47" s="17"/>
       <c r="H47" s="17"/>
-      <c r="I47" s="5"/>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B48" s="4" t="s">
-        <v>50</v>
-      </c>
+      <c r="I47" s="17"/>
+      <c r="J47" s="17"/>
+      <c r="K47" s="17"/>
+      <c r="L47" s="17"/>
+      <c r="M47" s="17"/>
+      <c r="N47" s="17"/>
+      <c r="O47" s="17"/>
+      <c r="P47" s="17"/>
+      <c r="Q47" s="17"/>
+      <c r="R47" s="17"/>
+      <c r="S47" s="17"/>
+      <c r="T47" s="5"/>
+    </row>
+    <row r="48" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B48" s="4"/>
       <c r="C48" s="17"/>
       <c r="D48" s="17"/>
       <c r="E48" s="17"/>
       <c r="F48" s="17"/>
       <c r="G48" s="17"/>
       <c r="H48" s="17"/>
-      <c r="I48" s="5"/>
-    </row>
-    <row r="49" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B49" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C49" s="17"/>
-      <c r="D49" s="17"/>
-      <c r="E49" s="17"/>
-      <c r="F49" s="17"/>
-      <c r="G49" s="17"/>
-      <c r="H49" s="17"/>
-      <c r="I49" s="5"/>
-    </row>
-    <row r="50" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B50" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="C50" s="17"/>
-      <c r="D50" s="17"/>
-      <c r="E50" s="17"/>
-      <c r="F50" s="17"/>
-      <c r="G50" s="17"/>
-      <c r="H50" s="17"/>
-      <c r="I50" s="5"/>
-    </row>
-    <row r="51" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B51" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C51" s="17"/>
-      <c r="D51" s="17"/>
-      <c r="E51" s="17"/>
-      <c r="F51" s="17"/>
-      <c r="G51" s="17"/>
-      <c r="H51" s="17"/>
-      <c r="I51" s="5"/>
-    </row>
-    <row r="52" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B52" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="C52" s="17"/>
-      <c r="D52" s="17"/>
-      <c r="E52" s="17"/>
-      <c r="F52" s="17"/>
-      <c r="G52" s="17"/>
-      <c r="H52" s="17"/>
-      <c r="I52" s="5"/>
-    </row>
-    <row r="53" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B53" s="4"/>
-      <c r="C53" s="17"/>
-      <c r="D53" s="17"/>
-      <c r="E53" s="17"/>
-      <c r="F53" s="17"/>
-      <c r="G53" s="17"/>
-      <c r="H53" s="17"/>
-      <c r="I53" s="5"/>
-    </row>
-    <row r="54" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B54" s="14" t="s">
-        <v>74</v>
-      </c>
-      <c r="C54" s="17"/>
-      <c r="D54" s="17"/>
-      <c r="E54" s="17"/>
-      <c r="F54" s="17"/>
-      <c r="G54" s="17"/>
-      <c r="H54" s="17"/>
-      <c r="I54" s="5"/>
-    </row>
-    <row r="55" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B55" s="14" t="s">
-        <v>75</v>
-      </c>
-      <c r="C55" s="17"/>
-      <c r="D55" s="17"/>
-      <c r="E55" s="17"/>
-      <c r="F55" s="17"/>
-      <c r="G55" s="17"/>
-      <c r="H55" s="17"/>
-      <c r="I55" s="5"/>
-    </row>
-    <row r="56" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B56" s="14" t="s">
-        <v>76</v>
-      </c>
-      <c r="C56" s="17"/>
-      <c r="D56" s="17"/>
-      <c r="E56" s="17"/>
-      <c r="F56" s="17"/>
-      <c r="G56" s="17"/>
-      <c r="H56" s="17"/>
-      <c r="I56" s="5"/>
-    </row>
-    <row r="57" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B57" s="14" t="s">
-        <v>77</v>
-      </c>
-      <c r="C57" s="17"/>
-      <c r="D57" s="17"/>
-      <c r="E57" s="17"/>
-      <c r="F57" s="17"/>
-      <c r="G57" s="17"/>
-      <c r="H57" s="17"/>
-      <c r="I57" s="5"/>
-    </row>
-    <row r="58" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B58" s="14" t="s">
-        <v>78</v>
-      </c>
-      <c r="C58" s="17"/>
-      <c r="D58" s="17"/>
-      <c r="E58" s="17"/>
-      <c r="F58" s="17"/>
-      <c r="G58" s="17"/>
-      <c r="H58" s="17"/>
-      <c r="I58" s="5"/>
-    </row>
-    <row r="59" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B59" s="4"/>
-      <c r="C59" s="17"/>
-      <c r="D59" s="17"/>
-      <c r="E59" s="17"/>
-      <c r="F59" s="17"/>
-      <c r="G59" s="17"/>
-      <c r="H59" s="17"/>
-      <c r="I59" s="5"/>
-    </row>
-    <row r="60" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B60" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="C60" s="17"/>
-      <c r="D60" s="17"/>
-      <c r="E60" s="17"/>
-      <c r="F60" s="17"/>
-      <c r="G60" s="17"/>
-      <c r="H60" s="17"/>
-      <c r="I60" s="5"/>
-    </row>
-    <row r="61" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B61" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="C61" s="17"/>
-      <c r="D61" s="17"/>
-      <c r="E61" s="17"/>
-      <c r="F61" s="17"/>
-      <c r="G61" s="17"/>
-      <c r="H61" s="17"/>
-      <c r="I61" s="5"/>
-    </row>
-    <row r="62" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B62" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="C62" s="17"/>
-      <c r="D62" s="17"/>
-      <c r="E62" s="17"/>
-      <c r="F62" s="17"/>
-      <c r="G62" s="17"/>
-      <c r="H62" s="17"/>
-      <c r="I62" s="5"/>
-    </row>
-    <row r="63" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B63" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="C63" s="17"/>
-      <c r="D63" s="17"/>
-      <c r="E63" s="17"/>
-      <c r="F63" s="17"/>
-      <c r="G63" s="17"/>
-      <c r="H63" s="17"/>
-      <c r="I63" s="5"/>
-    </row>
-    <row r="64" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B64" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="C64" s="17"/>
-      <c r="D64" s="17"/>
-      <c r="E64" s="17"/>
-      <c r="F64" s="17"/>
-      <c r="G64" s="17"/>
-      <c r="H64" s="17"/>
-      <c r="I64" s="5"/>
-    </row>
-    <row r="65" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B65" s="4"/>
-      <c r="C65" s="17"/>
-      <c r="D65" s="17"/>
-      <c r="E65" s="17"/>
-      <c r="F65" s="17"/>
-      <c r="G65" s="17"/>
-      <c r="H65" s="17"/>
-      <c r="I65" s="5"/>
-    </row>
-    <row r="66" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B66" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="C66" s="17"/>
-      <c r="D66" s="17"/>
-      <c r="E66" s="17"/>
-      <c r="F66" s="17"/>
-      <c r="G66" s="17"/>
-      <c r="H66" s="17"/>
-      <c r="I66" s="5"/>
-    </row>
-    <row r="67" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B67" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="C67" s="17"/>
-      <c r="D67" s="17"/>
-      <c r="E67" s="17"/>
-      <c r="F67" s="17"/>
-      <c r="G67" s="17"/>
-      <c r="H67" s="17"/>
-      <c r="I67" s="5"/>
-    </row>
-    <row r="68" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B68" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="C68" s="17"/>
-      <c r="D68" s="17"/>
-      <c r="E68" s="17"/>
-      <c r="F68" s="17"/>
-      <c r="G68" s="17"/>
-      <c r="H68" s="17"/>
-      <c r="I68" s="5"/>
-    </row>
-    <row r="69" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B69" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="C69" s="17"/>
-      <c r="D69" s="17"/>
-      <c r="E69" s="17"/>
-      <c r="F69" s="17"/>
-      <c r="G69" s="17"/>
-      <c r="H69" s="17"/>
-      <c r="I69" s="5"/>
-    </row>
-    <row r="70" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B70" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="C70" s="17"/>
-      <c r="D70" s="17"/>
-      <c r="E70" s="17"/>
-      <c r="F70" s="17"/>
-      <c r="G70" s="17"/>
-      <c r="H70" s="17"/>
-      <c r="I70" s="5"/>
-    </row>
-    <row r="71" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B71" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="C71" s="17"/>
-      <c r="D71" s="17"/>
-      <c r="E71" s="17"/>
-      <c r="F71" s="17"/>
-      <c r="G71" s="17"/>
-      <c r="H71" s="17"/>
-      <c r="I71" s="5"/>
-    </row>
-    <row r="72" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B72" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="C72" s="17"/>
-      <c r="D72" s="17"/>
-      <c r="E72" s="17"/>
-      <c r="F72" s="17"/>
-      <c r="G72" s="17"/>
-      <c r="H72" s="17"/>
-      <c r="I72" s="5"/>
-    </row>
-    <row r="73" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B73" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="C73" s="17"/>
-      <c r="D73" s="17"/>
-      <c r="E73" s="17"/>
-      <c r="F73" s="17"/>
-      <c r="G73" s="17"/>
-      <c r="H73" s="17"/>
-      <c r="I73" s="5"/>
-    </row>
-    <row r="74" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B74" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="C74" s="17"/>
-      <c r="D74" s="17"/>
-      <c r="E74" s="17"/>
-      <c r="F74" s="17"/>
-      <c r="G74" s="17"/>
-      <c r="H74" s="17"/>
-      <c r="I74" s="5"/>
-    </row>
-    <row r="75" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B75" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="C75" s="17"/>
-      <c r="D75" s="17"/>
-      <c r="E75" s="17"/>
-      <c r="F75" s="17"/>
-      <c r="G75" s="17"/>
-      <c r="H75" s="17"/>
-      <c r="I75" s="5"/>
-    </row>
-    <row r="76" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B76" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="C76" s="17"/>
-      <c r="D76" s="17"/>
-      <c r="E76" s="17"/>
-      <c r="F76" s="17"/>
-      <c r="G76" s="17"/>
-      <c r="H76" s="17"/>
-      <c r="I76" s="5"/>
-    </row>
-    <row r="77" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B77" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="C77" s="17"/>
-      <c r="D77" s="17"/>
-      <c r="E77" s="17"/>
-      <c r="F77" s="17"/>
-      <c r="G77" s="17"/>
-      <c r="H77" s="17"/>
-      <c r="I77" s="5"/>
-    </row>
-    <row r="78" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B78" s="4"/>
-      <c r="C78" s="17"/>
-      <c r="D78" s="17"/>
-      <c r="E78" s="17"/>
-      <c r="F78" s="17"/>
-      <c r="G78" s="17"/>
-      <c r="H78" s="17"/>
-      <c r="I78" s="5"/>
-    </row>
-    <row r="79" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B79" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="C79" s="17"/>
-      <c r="D79" s="17"/>
-      <c r="E79" s="17"/>
-      <c r="F79" s="17"/>
-      <c r="G79" s="17"/>
-      <c r="H79" s="17"/>
-      <c r="I79" s="5"/>
-    </row>
-    <row r="80" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B80" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="C80" s="17"/>
-      <c r="D80" s="17"/>
-      <c r="E80" s="17"/>
-      <c r="F80" s="17"/>
-      <c r="G80" s="17"/>
-      <c r="H80" s="17"/>
-      <c r="I80" s="5"/>
-    </row>
-    <row r="81" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B81" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="C81" s="17"/>
-      <c r="D81" s="17"/>
-      <c r="E81" s="17"/>
-      <c r="F81" s="17"/>
-      <c r="G81" s="17"/>
-      <c r="H81" s="17"/>
-      <c r="I81" s="5"/>
-    </row>
-    <row r="82" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B82" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="C82" s="17"/>
-      <c r="D82" s="17"/>
-      <c r="E82" s="17"/>
-      <c r="F82" s="17"/>
-      <c r="G82" s="17"/>
-      <c r="H82" s="17"/>
-      <c r="I82" s="5"/>
-    </row>
-    <row r="83" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B83" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="C83" s="17"/>
-      <c r="D83" s="17"/>
-      <c r="E83" s="17"/>
-      <c r="F83" s="17"/>
-      <c r="G83" s="17"/>
-      <c r="H83" s="17"/>
-      <c r="I83" s="5"/>
-    </row>
-    <row r="84" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B84" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="C84" s="17"/>
-      <c r="D84" s="17"/>
-      <c r="E84" s="17"/>
-      <c r="F84" s="17"/>
-      <c r="G84" s="17"/>
-      <c r="H84" s="17"/>
-      <c r="I84" s="5"/>
-    </row>
-    <row r="85" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B85" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="C85" s="17"/>
-      <c r="D85" s="17"/>
-      <c r="E85" s="17"/>
-      <c r="F85" s="17"/>
-      <c r="G85" s="17"/>
-      <c r="H85" s="17"/>
-      <c r="I85" s="5"/>
-    </row>
-    <row r="86" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B86" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="C86" s="17"/>
-      <c r="D86" s="17"/>
-      <c r="E86" s="17"/>
-      <c r="F86" s="17"/>
-      <c r="G86" s="17"/>
-      <c r="H86" s="17"/>
-      <c r="I86" s="5"/>
-    </row>
-    <row r="87" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B87" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="C87" s="17"/>
-      <c r="D87" s="17"/>
-      <c r="E87" s="17"/>
-      <c r="F87" s="17"/>
-      <c r="G87" s="17"/>
-      <c r="H87" s="17"/>
-      <c r="I87" s="5"/>
-    </row>
-    <row r="88" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B88" s="4"/>
-      <c r="C88" s="17"/>
-      <c r="D88" s="17"/>
-      <c r="E88" s="17"/>
-      <c r="F88" s="17"/>
-      <c r="G88" s="17"/>
-      <c r="H88" s="17"/>
-      <c r="I88" s="5"/>
-    </row>
-    <row r="89" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B89" s="14" t="s">
-        <v>74</v>
-      </c>
-      <c r="C89" s="17"/>
-      <c r="D89" s="17"/>
-      <c r="E89" s="17"/>
-      <c r="F89" s="17"/>
-      <c r="G89" s="17"/>
-      <c r="H89" s="17"/>
-      <c r="I89" s="5"/>
-    </row>
-    <row r="90" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B90" s="14" t="s">
-        <v>111</v>
-      </c>
-      <c r="C90" s="17"/>
-      <c r="D90" s="17"/>
-      <c r="E90" s="17"/>
-      <c r="F90" s="17"/>
-      <c r="G90" s="17"/>
-      <c r="H90" s="17"/>
-      <c r="I90" s="5"/>
-    </row>
-    <row r="91" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B91" s="14" t="s">
-        <v>112</v>
-      </c>
-      <c r="C91" s="17"/>
-      <c r="D91" s="17"/>
-      <c r="E91" s="17"/>
-      <c r="F91" s="17"/>
-      <c r="G91" s="17"/>
-      <c r="H91" s="17"/>
-      <c r="I91" s="5"/>
-    </row>
-    <row r="92" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B92" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="C92" s="17"/>
-      <c r="D92" s="17"/>
-      <c r="E92" s="17"/>
-      <c r="F92" s="17"/>
-      <c r="G92" s="17"/>
-      <c r="H92" s="17"/>
-      <c r="I92" s="5"/>
-    </row>
-    <row r="93" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B93" s="14" t="s">
-        <v>113</v>
-      </c>
-      <c r="C93" s="17"/>
-      <c r="D93" s="17"/>
-      <c r="E93" s="17"/>
-      <c r="F93" s="17"/>
-      <c r="G93" s="17"/>
-      <c r="H93" s="17"/>
-      <c r="I93" s="5"/>
-    </row>
-    <row r="94" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B94" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="C94" s="17"/>
-      <c r="D94" s="17"/>
-      <c r="E94" s="17"/>
-      <c r="F94" s="17"/>
-      <c r="G94" s="17"/>
-      <c r="H94" s="17"/>
-      <c r="I94" s="5"/>
-    </row>
-    <row r="95" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B95" s="14" t="s">
-        <v>114</v>
-      </c>
-      <c r="C95" s="17"/>
-      <c r="D95" s="17"/>
-      <c r="E95" s="17"/>
-      <c r="F95" s="17"/>
-      <c r="G95" s="17"/>
-      <c r="H95" s="17"/>
-      <c r="I95" s="5"/>
-    </row>
-    <row r="96" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B96" s="14" t="s">
-        <v>77</v>
-      </c>
-      <c r="C96" s="17"/>
-      <c r="D96" s="17"/>
-      <c r="E96" s="17"/>
-      <c r="F96" s="17"/>
-      <c r="G96" s="17"/>
-      <c r="H96" s="17"/>
-      <c r="I96" s="5"/>
-    </row>
-    <row r="97" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B97" s="14" t="s">
-        <v>115</v>
-      </c>
-      <c r="C97" s="17"/>
-      <c r="D97" s="17"/>
-      <c r="E97" s="17"/>
-      <c r="F97" s="17"/>
-      <c r="G97" s="17"/>
-      <c r="H97" s="17"/>
-      <c r="I97" s="5"/>
-    </row>
-    <row r="98" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B98" s="14" t="s">
-        <v>85</v>
-      </c>
-      <c r="C98" s="17"/>
-      <c r="D98" s="17"/>
-      <c r="E98" s="17"/>
-      <c r="F98" s="17"/>
-      <c r="G98" s="17"/>
-      <c r="H98" s="17"/>
-      <c r="I98" s="5"/>
-    </row>
-    <row r="99" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B99" s="14" t="s">
-        <v>116</v>
-      </c>
-      <c r="C99" s="17"/>
-      <c r="D99" s="17"/>
-      <c r="E99" s="17"/>
-      <c r="F99" s="17"/>
-      <c r="G99" s="17"/>
-      <c r="H99" s="17"/>
-      <c r="I99" s="5"/>
-    </row>
-    <row r="100" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B100" s="14" t="s">
-        <v>117</v>
-      </c>
-      <c r="C100" s="17"/>
-      <c r="D100" s="17"/>
-      <c r="E100" s="17"/>
-      <c r="F100" s="17"/>
-      <c r="G100" s="17"/>
-      <c r="H100" s="17"/>
-      <c r="I100" s="5"/>
-    </row>
-    <row r="101" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B101" s="14" t="s">
-        <v>118</v>
-      </c>
-      <c r="C101" s="17"/>
-      <c r="D101" s="17"/>
-      <c r="E101" s="17"/>
-      <c r="F101" s="17"/>
-      <c r="G101" s="17"/>
-      <c r="H101" s="17"/>
-      <c r="I101" s="5"/>
-    </row>
-    <row r="102" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B102" s="14" t="s">
-        <v>119</v>
-      </c>
-      <c r="C102" s="17"/>
-      <c r="D102" s="17"/>
-      <c r="E102" s="17"/>
-      <c r="F102" s="17"/>
-      <c r="G102" s="17"/>
-      <c r="H102" s="17"/>
-      <c r="I102" s="5"/>
-    </row>
-    <row r="103" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B103" s="14" t="s">
-        <v>120</v>
-      </c>
-      <c r="C103" s="17"/>
-      <c r="D103" s="17"/>
-      <c r="E103" s="17"/>
-      <c r="F103" s="17"/>
-      <c r="G103" s="17"/>
-      <c r="H103" s="17"/>
-      <c r="I103" s="5"/>
-    </row>
-    <row r="104" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B104" s="14" t="s">
-        <v>121</v>
-      </c>
-      <c r="C104" s="17"/>
-      <c r="D104" s="17"/>
-      <c r="E104" s="17"/>
-      <c r="F104" s="17"/>
-      <c r="G104" s="17"/>
-      <c r="H104" s="17"/>
-      <c r="I104" s="5"/>
-    </row>
-    <row r="105" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B105" s="14"/>
-      <c r="C105" s="17"/>
-      <c r="D105" s="17"/>
-      <c r="E105" s="17"/>
-      <c r="F105" s="17"/>
-      <c r="G105" s="17"/>
-      <c r="H105" s="17"/>
-      <c r="I105" s="5"/>
-    </row>
-    <row r="106" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B106" s="14" t="s">
-        <v>122</v>
-      </c>
-      <c r="C106" s="17"/>
-      <c r="D106" s="17"/>
-      <c r="E106" s="17"/>
-      <c r="F106" s="17"/>
-      <c r="G106" s="17"/>
-      <c r="H106" s="17"/>
-      <c r="I106" s="5"/>
-    </row>
-    <row r="107" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B107" s="14" t="s">
-        <v>87</v>
-      </c>
-      <c r="C107" s="17"/>
-      <c r="D107" s="17"/>
-      <c r="E107" s="17"/>
-      <c r="F107" s="17"/>
-      <c r="G107" s="17"/>
-      <c r="H107" s="17"/>
-      <c r="I107" s="5"/>
-    </row>
-    <row r="108" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B108" s="14"/>
-      <c r="C108" s="17"/>
-      <c r="D108" s="17"/>
-      <c r="E108" s="17"/>
-      <c r="F108" s="17"/>
-      <c r="G108" s="17"/>
-      <c r="H108" s="17"/>
-      <c r="I108" s="5"/>
-    </row>
-    <row r="109" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B109" s="14" t="s">
-        <v>74</v>
-      </c>
-      <c r="C109" s="17"/>
-      <c r="D109" s="17"/>
-      <c r="E109" s="17"/>
-      <c r="F109" s="17"/>
-      <c r="G109" s="17"/>
-      <c r="H109" s="17"/>
-      <c r="I109" s="5"/>
-    </row>
-    <row r="110" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B110" s="14" t="s">
-        <v>123</v>
-      </c>
-      <c r="C110" s="17"/>
-      <c r="D110" s="17"/>
-      <c r="E110" s="17"/>
-      <c r="F110" s="17"/>
-      <c r="G110" s="17"/>
-      <c r="H110" s="17"/>
-      <c r="I110" s="5"/>
-    </row>
-    <row r="111" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B111" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="C111" s="17"/>
-      <c r="D111" s="17"/>
-      <c r="E111" s="17"/>
-      <c r="F111" s="17"/>
-      <c r="G111" s="17"/>
-      <c r="H111" s="17"/>
-      <c r="I111" s="5"/>
-    </row>
-    <row r="112" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B112" s="14" t="s">
-        <v>89</v>
-      </c>
-      <c r="C112" s="17"/>
-      <c r="D112" s="17"/>
-      <c r="E112" s="17"/>
-      <c r="F112" s="17"/>
-      <c r="G112" s="17"/>
-      <c r="H112" s="17"/>
-      <c r="I112" s="5"/>
-    </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B113" s="14" t="s">
-        <v>77</v>
-      </c>
-      <c r="C113" s="17"/>
-      <c r="D113" s="17"/>
-      <c r="E113" s="17"/>
-      <c r="F113" s="17"/>
-      <c r="G113" s="17"/>
-      <c r="H113" s="17"/>
-      <c r="I113" s="5"/>
-    </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B114" s="14" t="s">
-        <v>124</v>
-      </c>
-      <c r="C114" s="17"/>
-      <c r="D114" s="17"/>
-      <c r="E114" s="17"/>
-      <c r="F114" s="17"/>
-      <c r="G114" s="17"/>
-      <c r="H114" s="17"/>
-      <c r="I114" s="5"/>
-    </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B115" s="14" t="s">
-        <v>85</v>
-      </c>
-      <c r="C115" s="17"/>
-      <c r="D115" s="17"/>
-      <c r="E115" s="17"/>
-      <c r="F115" s="17"/>
-      <c r="G115" s="17"/>
-      <c r="H115" s="17"/>
-      <c r="I115" s="5"/>
-    </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B116" s="14" t="s">
-        <v>125</v>
-      </c>
-      <c r="C116" s="17"/>
-      <c r="D116" s="17"/>
-      <c r="E116" s="17"/>
-      <c r="F116" s="17"/>
-      <c r="G116" s="17"/>
-      <c r="H116" s="17"/>
-      <c r="I116" s="5"/>
-    </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B117" s="14" t="s">
-        <v>87</v>
-      </c>
-      <c r="C117" s="17"/>
-      <c r="D117" s="17"/>
-      <c r="E117" s="17"/>
-      <c r="F117" s="17"/>
-      <c r="G117" s="17"/>
-      <c r="H117" s="17"/>
-      <c r="I117" s="5"/>
-    </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B118" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="C118" s="7"/>
-      <c r="D118" s="7"/>
-      <c r="E118" s="7"/>
-      <c r="F118" s="7"/>
-      <c r="G118" s="7"/>
-      <c r="H118" s="7"/>
-      <c r="I118" s="8"/>
-    </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A121" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B122" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C122" s="2"/>
-      <c r="D122" s="2"/>
-      <c r="E122" s="2"/>
-      <c r="F122" s="2"/>
-      <c r="G122" s="2"/>
-      <c r="H122" s="3"/>
-    </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B123" s="4"/>
-      <c r="C123" s="17"/>
-      <c r="D123" s="17"/>
-      <c r="E123" s="17"/>
-      <c r="F123" s="17"/>
-      <c r="G123" s="17"/>
-      <c r="H123" s="5"/>
-    </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B124" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="C124" s="17"/>
-      <c r="D124" s="17"/>
-      <c r="E124" s="17"/>
-      <c r="F124" s="17"/>
-      <c r="G124" s="17"/>
-      <c r="H124" s="5"/>
-    </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B125" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C125" s="17"/>
-      <c r="D125" s="17"/>
-      <c r="E125" s="17"/>
-      <c r="F125" s="17"/>
-      <c r="G125" s="17"/>
-      <c r="H125" s="5"/>
-    </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B126" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="C126" s="17"/>
-      <c r="D126" s="17"/>
-      <c r="E126" s="17"/>
-      <c r="F126" s="17"/>
-      <c r="G126" s="17"/>
-      <c r="H126" s="5"/>
-    </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B127" s="4"/>
-      <c r="C127" s="17"/>
-      <c r="D127" s="17"/>
-      <c r="E127" s="17"/>
-      <c r="F127" s="17"/>
-      <c r="G127" s="17"/>
-      <c r="H127" s="5"/>
-    </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B128" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="C128" s="17"/>
-      <c r="D128" s="17"/>
-      <c r="E128" s="17"/>
-      <c r="F128" s="17"/>
-      <c r="G128" s="17"/>
-      <c r="H128" s="5"/>
-    </row>
-    <row r="129" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B129" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C129" s="17"/>
-      <c r="D129" s="17"/>
-      <c r="E129" s="17"/>
-      <c r="F129" s="17"/>
-      <c r="G129" s="17"/>
-      <c r="H129" s="5"/>
-    </row>
-    <row r="130" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B130" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="C130" s="17"/>
-      <c r="D130" s="17"/>
-      <c r="E130" s="17"/>
-      <c r="F130" s="17"/>
-      <c r="G130" s="17"/>
-      <c r="H130" s="5"/>
-    </row>
-    <row r="131" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B131" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="C131" s="17"/>
-      <c r="D131" s="17"/>
-      <c r="E131" s="17"/>
-      <c r="F131" s="17"/>
-      <c r="G131" s="17"/>
-      <c r="H131" s="5"/>
-    </row>
-    <row r="132" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B132" s="4"/>
-      <c r="C132" s="17"/>
-      <c r="D132" s="17"/>
-      <c r="E132" s="17"/>
-      <c r="F132" s="17"/>
-      <c r="G132" s="17"/>
-      <c r="H132" s="5"/>
-    </row>
-    <row r="133" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B133" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C133" s="17"/>
-      <c r="D133" s="17"/>
-      <c r="E133" s="17"/>
-      <c r="F133" s="17"/>
-      <c r="G133" s="17"/>
-      <c r="H133" s="5"/>
-    </row>
-    <row r="134" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B134" s="4"/>
-      <c r="C134" s="17"/>
-      <c r="D134" s="17"/>
-      <c r="E134" s="17"/>
-      <c r="F134" s="17"/>
-      <c r="G134" s="17"/>
-      <c r="H134" s="5"/>
-    </row>
-    <row r="135" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B135" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="C135" s="17"/>
-      <c r="D135" s="17"/>
-      <c r="E135" s="17"/>
-      <c r="F135" s="17"/>
-      <c r="G135" s="17"/>
-      <c r="H135" s="5"/>
-    </row>
-    <row r="136" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B136" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="C136" s="17"/>
-      <c r="D136" s="17"/>
-      <c r="E136" s="17"/>
-      <c r="F136" s="17"/>
-      <c r="G136" s="17"/>
-      <c r="H136" s="5"/>
-    </row>
-    <row r="137" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B137" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="C137" s="17"/>
-      <c r="D137" s="17"/>
-      <c r="E137" s="17"/>
-      <c r="F137" s="17"/>
-      <c r="G137" s="17"/>
-      <c r="H137" s="5"/>
-    </row>
-    <row r="138" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B138" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="C138" s="17"/>
-      <c r="D138" s="17"/>
-      <c r="E138" s="17"/>
-      <c r="F138" s="17"/>
-      <c r="G138" s="17"/>
-      <c r="H138" s="5"/>
-    </row>
-    <row r="139" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B139" s="4"/>
-      <c r="C139" s="17"/>
-      <c r="D139" s="17"/>
-      <c r="E139" s="17"/>
-      <c r="F139" s="17"/>
-      <c r="G139" s="17"/>
-      <c r="H139" s="5"/>
-    </row>
-    <row r="140" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B140" s="14" t="s">
-        <v>126</v>
-      </c>
-      <c r="C140" s="17"/>
-      <c r="D140" s="17"/>
-      <c r="E140" s="17"/>
-      <c r="F140" s="17"/>
-      <c r="G140" s="17"/>
-      <c r="H140" s="5"/>
-    </row>
-    <row r="141" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B141" s="14" t="s">
-        <v>127</v>
-      </c>
-      <c r="C141" s="17"/>
-      <c r="D141" s="17"/>
-      <c r="E141" s="17"/>
-      <c r="F141" s="17"/>
-      <c r="G141" s="17"/>
-      <c r="H141" s="5"/>
-    </row>
-    <row r="142" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B142" s="14"/>
-      <c r="C142" s="17"/>
-      <c r="D142" s="17"/>
-      <c r="E142" s="17"/>
-      <c r="F142" s="17"/>
-      <c r="G142" s="17"/>
-      <c r="H142" s="5"/>
-    </row>
-    <row r="143" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B143" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="C143" s="17"/>
-      <c r="D143" s="17"/>
-      <c r="E143" s="17"/>
-      <c r="F143" s="17"/>
-      <c r="G143" s="17"/>
-      <c r="H143" s="5"/>
-    </row>
-    <row r="144" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B144" s="14" t="s">
-        <v>129</v>
-      </c>
-      <c r="C144" s="17"/>
-      <c r="D144" s="17"/>
-      <c r="E144" s="17"/>
-      <c r="F144" s="17"/>
-      <c r="G144" s="17"/>
-      <c r="H144" s="5"/>
-    </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B145" s="14" t="s">
-        <v>130</v>
-      </c>
-      <c r="C145" s="17"/>
-      <c r="D145" s="17"/>
-      <c r="E145" s="17"/>
-      <c r="F145" s="17"/>
-      <c r="G145" s="17"/>
-      <c r="H145" s="5"/>
-    </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B146" s="14" t="s">
-        <v>131</v>
-      </c>
-      <c r="C146" s="17"/>
-      <c r="D146" s="17"/>
-      <c r="E146" s="17"/>
-      <c r="F146" s="17"/>
-      <c r="G146" s="17"/>
-      <c r="H146" s="5"/>
-    </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B147" s="14" t="s">
-        <v>132</v>
-      </c>
-      <c r="C147" s="17"/>
-      <c r="D147" s="17"/>
-      <c r="E147" s="17"/>
-      <c r="F147" s="17"/>
-      <c r="G147" s="17"/>
-      <c r="H147" s="5"/>
-    </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B148" s="14" t="s">
-        <v>133</v>
-      </c>
-      <c r="C148" s="17"/>
-      <c r="D148" s="17"/>
-      <c r="E148" s="17"/>
-      <c r="F148" s="17"/>
-      <c r="G148" s="17"/>
-      <c r="H148" s="5"/>
-    </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B149" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="C149" s="7"/>
-      <c r="D149" s="7"/>
-      <c r="E149" s="7"/>
-      <c r="F149" s="7"/>
-      <c r="G149" s="7"/>
-      <c r="H149" s="8"/>
-    </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A152" s="9" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B153" s="12" t="s">
-        <v>134</v>
-      </c>
-      <c r="C153" s="2"/>
-      <c r="D153" s="2"/>
-      <c r="E153" s="2"/>
-      <c r="F153" s="2"/>
-      <c r="G153" s="3"/>
-    </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B154" s="4"/>
-      <c r="C154" s="17"/>
-      <c r="D154" s="17"/>
-      <c r="E154" s="17"/>
-      <c r="F154" s="17"/>
-      <c r="G154" s="5"/>
-    </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B155" s="4"/>
-      <c r="C155" s="17"/>
-      <c r="D155" s="17"/>
-      <c r="E155" s="17"/>
-      <c r="F155" s="17"/>
-      <c r="G155" s="5"/>
-    </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B156" s="4"/>
-      <c r="C156" s="17"/>
-      <c r="D156" s="17"/>
-      <c r="E156" s="17"/>
-      <c r="F156" s="17"/>
-      <c r="G156" s="5"/>
-    </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B157" s="4"/>
-      <c r="C157" s="17"/>
-      <c r="D157" s="17"/>
-      <c r="E157" s="17"/>
-      <c r="F157" s="17"/>
-      <c r="G157" s="5"/>
-    </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B158" s="4"/>
-      <c r="C158" s="17"/>
-      <c r="D158" s="17"/>
-      <c r="E158" s="17"/>
-      <c r="F158" s="17"/>
-      <c r="G158" s="5"/>
-    </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B159" s="4"/>
-      <c r="C159" s="17"/>
-      <c r="D159" s="17"/>
-      <c r="E159" s="17"/>
-      <c r="F159" s="17"/>
-      <c r="G159" s="5"/>
-    </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B160" s="4"/>
-      <c r="C160" s="17"/>
-      <c r="D160" s="17"/>
-      <c r="E160" s="17"/>
-      <c r="F160" s="17"/>
-      <c r="G160" s="5"/>
-    </row>
-    <row r="161" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B161" s="4"/>
-      <c r="C161" s="17"/>
-      <c r="D161" s="17"/>
-      <c r="E161" s="17"/>
-      <c r="F161" s="17"/>
-      <c r="G161" s="5"/>
-    </row>
-    <row r="162" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B162" s="4"/>
-      <c r="C162" s="17"/>
-      <c r="D162" s="17"/>
-      <c r="E162" s="17"/>
-      <c r="F162" s="17"/>
-      <c r="G162" s="5"/>
-    </row>
-    <row r="163" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B163" s="6"/>
-      <c r="C163" s="7"/>
-      <c r="D163" s="7"/>
-      <c r="E163" s="7"/>
-      <c r="F163" s="7"/>
-      <c r="G163" s="8"/>
-    </row>
-    <row r="166" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B166" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="C166" s="2"/>
-      <c r="D166" s="2"/>
-      <c r="E166" s="2"/>
-      <c r="F166" s="2"/>
-      <c r="G166" s="2"/>
-      <c r="H166" s="3"/>
-    </row>
-    <row r="167" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B167" s="4"/>
-      <c r="C167" s="17"/>
-      <c r="D167" s="17"/>
-      <c r="E167" s="17"/>
-      <c r="F167" s="17"/>
-      <c r="G167" s="17"/>
-      <c r="H167" s="5"/>
-    </row>
-    <row r="168" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B168" s="4"/>
-      <c r="C168" s="17"/>
-      <c r="D168" s="17"/>
-      <c r="E168" s="17"/>
-      <c r="F168" s="17"/>
-      <c r="G168" s="17"/>
-      <c r="H168" s="5"/>
-    </row>
-    <row r="169" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B169" s="4"/>
-      <c r="C169" s="17"/>
-      <c r="D169" s="17"/>
-      <c r="E169" s="17"/>
-      <c r="F169" s="17"/>
-      <c r="G169" s="17"/>
-      <c r="H169" s="5"/>
-    </row>
-    <row r="170" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B170" s="4"/>
-      <c r="C170" s="17"/>
-      <c r="D170" s="17"/>
-      <c r="E170" s="17"/>
-      <c r="F170" s="17"/>
-      <c r="G170" s="17"/>
-      <c r="H170" s="5"/>
-    </row>
-    <row r="171" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B171" s="4"/>
-      <c r="C171" s="17"/>
-      <c r="D171" s="17"/>
-      <c r="E171" s="17"/>
-      <c r="F171" s="17"/>
-      <c r="G171" s="17"/>
-      <c r="H171" s="5"/>
-    </row>
-    <row r="172" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B172" s="4"/>
-      <c r="C172" s="17"/>
-      <c r="D172" s="17"/>
-      <c r="E172" s="17"/>
-      <c r="F172" s="17"/>
-      <c r="G172" s="17"/>
-      <c r="H172" s="5"/>
-    </row>
-    <row r="173" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B173" s="4"/>
-      <c r="C173" s="17"/>
-      <c r="D173" s="17"/>
-      <c r="E173" s="17"/>
-      <c r="F173" s="17"/>
-      <c r="G173" s="17"/>
-      <c r="H173" s="5"/>
-    </row>
-    <row r="174" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B174" s="4"/>
-      <c r="C174" s="17"/>
-      <c r="D174" s="17"/>
-      <c r="E174" s="17"/>
-      <c r="F174" s="17"/>
-      <c r="G174" s="17"/>
-      <c r="H174" s="5"/>
-    </row>
-    <row r="175" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B175" s="4"/>
-      <c r="C175" s="17"/>
-      <c r="D175" s="17"/>
-      <c r="E175" s="17"/>
-      <c r="F175" s="17"/>
-      <c r="G175" s="17"/>
-      <c r="H175" s="5"/>
-    </row>
-    <row r="176" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B176" s="6"/>
-      <c r="C176" s="7"/>
-      <c r="D176" s="7"/>
-      <c r="E176" s="7"/>
-      <c r="F176" s="7"/>
-      <c r="G176" s="7"/>
-      <c r="H176" s="8"/>
-    </row>
-    <row r="179" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B179" s="12" t="s">
-        <v>136</v>
-      </c>
-      <c r="C179" s="2"/>
-      <c r="D179" s="2"/>
-      <c r="E179" s="2"/>
-      <c r="F179" s="2"/>
-      <c r="G179" s="3"/>
-    </row>
-    <row r="180" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B180" s="4"/>
-      <c r="C180" s="17"/>
-      <c r="D180" s="17"/>
-      <c r="E180" s="17"/>
-      <c r="F180" s="17"/>
-      <c r="G180" s="5"/>
-    </row>
-    <row r="181" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B181" s="4"/>
-      <c r="C181" s="17"/>
-      <c r="D181" s="17"/>
-      <c r="E181" s="17"/>
-      <c r="F181" s="17"/>
-      <c r="G181" s="5"/>
-    </row>
-    <row r="182" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B182" s="4"/>
-      <c r="C182" s="17"/>
-      <c r="D182" s="17"/>
-      <c r="E182" s="17"/>
-      <c r="F182" s="17"/>
-      <c r="G182" s="5"/>
-    </row>
-    <row r="183" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B183" s="4"/>
-      <c r="C183" s="17"/>
-      <c r="D183" s="17"/>
-      <c r="E183" s="17"/>
-      <c r="F183" s="17"/>
-      <c r="G183" s="5"/>
-    </row>
-    <row r="184" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B184" s="4"/>
-      <c r="C184" s="17"/>
-      <c r="D184" s="17"/>
-      <c r="E184" s="17"/>
-      <c r="F184" s="17"/>
-      <c r="G184" s="5"/>
-    </row>
-    <row r="185" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B185" s="4"/>
-      <c r="C185" s="17"/>
-      <c r="D185" s="17"/>
-      <c r="E185" s="17"/>
-      <c r="F185" s="17"/>
-      <c r="G185" s="5"/>
-    </row>
-    <row r="186" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B186" s="4"/>
-      <c r="C186" s="17"/>
-      <c r="D186" s="17"/>
-      <c r="E186" s="17"/>
-      <c r="F186" s="17"/>
-      <c r="G186" s="5"/>
-    </row>
-    <row r="187" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B187" s="4"/>
-      <c r="C187" s="17"/>
-      <c r="D187" s="17"/>
-      <c r="E187" s="17"/>
-      <c r="F187" s="17"/>
-      <c r="G187" s="5"/>
-    </row>
-    <row r="188" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B188" s="6"/>
-      <c r="C188" s="7"/>
-      <c r="D188" s="7"/>
-      <c r="E188" s="7"/>
-      <c r="F188" s="7"/>
-      <c r="G188" s="8"/>
+      <c r="I48" s="17"/>
+      <c r="J48" s="17"/>
+      <c r="K48" s="17"/>
+      <c r="L48" s="17"/>
+      <c r="M48" s="17"/>
+      <c r="N48" s="17"/>
+      <c r="O48" s="17"/>
+      <c r="P48" s="17"/>
+      <c r="Q48" s="17"/>
+      <c r="R48" s="17"/>
+      <c r="S48" s="17"/>
+      <c r="T48" s="5"/>
+    </row>
+    <row r="49" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B49" s="6"/>
+      <c r="C49" s="7"/>
+      <c r="D49" s="7"/>
+      <c r="E49" s="7"/>
+      <c r="F49" s="7"/>
+      <c r="G49" s="7"/>
+      <c r="H49" s="7"/>
+      <c r="I49" s="7"/>
+      <c r="J49" s="7"/>
+      <c r="K49" s="7"/>
+      <c r="L49" s="7"/>
+      <c r="M49" s="7"/>
+      <c r="N49" s="7"/>
+      <c r="O49" s="7"/>
+      <c r="P49" s="7"/>
+      <c r="Q49" s="7"/>
+      <c r="R49" s="7"/>
+      <c r="S49" s="7"/>
+      <c r="T49" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Get the controller and action from a URL with a fixed structure
</commit_message>
<xml_diff>
--- a/me/2.routing.xlsx
+++ b/me/2.routing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\build-php-mvc-framework\me\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7340DDF7-771D-4B12-9661-DA3F3E964300}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E69B6B92-DD93-4189-AF61-9C1F94832527}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="5" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="central entry point" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="routing table in the router" sheetId="4" r:id="rId4"/>
     <sheet name="MatchRequestedRouteToRoutingTbl" sheetId="5" r:id="rId5"/>
     <sheet name="routing using route variables" sheetId="6" r:id="rId6"/>
+    <sheet name="Get the controller and action" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="157">
   <si>
     <t>Create a central entry point to the framework: the front controller</t>
   </si>
@@ -559,6 +560,48 @@
   </si>
   <si>
     <t>cần 1 route nhưng có thể cover tất cả các url</t>
+  </si>
+  <si>
+    <t>Get the controller and action from a URL with a fixed structure</t>
+  </si>
+  <si>
+    <t>Thấy rằng tất cả các url đều có dạng đó là phần thứ nhất của url là controller và phần thứ 2 là action</t>
+  </si>
+  <si>
+    <t>        // Match to the fixed URL format /controller/action</t>
+  </si>
+  <si>
+    <t>        $reg_exp = "/^(?P&lt;controller&gt;[a-z-]+)\/(?P&lt;action&gt;[a-z-]+)$/";</t>
+  </si>
+  <si>
+    <t>        if (preg_match($reg_exp, $url, $matches)) {</t>
+  </si>
+  <si>
+    <t>            // Get named capture group values</t>
+  </si>
+  <si>
+    <t>            $params = [];</t>
+  </si>
+  <si>
+    <t>            foreach ($matches as $key =&gt; $match) {</t>
+  </si>
+  <si>
+    <t>                if (is_string($key)) {</t>
+  </si>
+  <si>
+    <t>                    $params[$key] = $match;</t>
+  </si>
+  <si>
+    <t>                }</t>
+  </si>
+  <si>
+    <t>            $this-&gt;params = $params;</t>
+  </si>
+  <si>
+    <t>            return true;</t>
+  </si>
+  <si>
+    <t>Sử dụng regular expression mình dùng preg_match</t>
   </si>
 </sst>
 </file>
@@ -687,7 +730,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -705,6 +748,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -3836,6 +3880,249 @@
         </a:fontRef>
       </xdr:style>
     </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>447102</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>123626</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3C5A1D9D-1B25-8EFB-EFAA-C62A2C9993D2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="742950" y="1390650"/>
+          <a:ext cx="4580952" cy="1590476"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="Straight Arrow Connector 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6EE4E676-0C68-CBC2-F185-812DA62663C1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="3552825" y="914400"/>
+          <a:ext cx="1009650" cy="609600"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="6" name="Straight Arrow Connector 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{91BA5CAD-BC51-F1C3-2C96-90598727F484}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="4676775" y="923925"/>
+          <a:ext cx="1390650" cy="581025"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>82</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>474711</xdr:colOff>
+      <xdr:row>102</xdr:row>
+      <xdr:rowOff>75720</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{60D5C753-9601-DBBB-D6CD-DC79664EF80E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5838825" y="15668625"/>
+          <a:ext cx="12314286" cy="3838095"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>118</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>399552</xdr:colOff>
+      <xdr:row>127</xdr:row>
+      <xdr:rowOff>66464</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{84E278BF-718F-6D17-F1C9-5D3241232154}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="685800" y="22574250"/>
+          <a:ext cx="3980952" cy="1685714"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -6476,8 +6763,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AE241D4-197C-4BF6-874B-4B7E9956690B}">
   <dimension ref="A2:T188"/>
   <sheetViews>
-    <sheetView topLeftCell="A167" workbookViewId="0">
-      <selection activeCell="P182" sqref="P182"/>
+    <sheetView topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30:H42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7508,7 +7795,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E01E8A2C-EBC4-4512-8867-F476D8E6BF62}">
   <dimension ref="B2:T49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
@@ -7546,424 +7833,84 @@
       <c r="B6" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="17"/>
-      <c r="I6" s="17"/>
-      <c r="J6" s="17"/>
-      <c r="K6" s="17"/>
-      <c r="L6" s="17"/>
-      <c r="M6" s="17"/>
-      <c r="N6" s="17"/>
-      <c r="O6" s="17"/>
-      <c r="P6" s="17"/>
-      <c r="Q6" s="17"/>
-      <c r="R6" s="17"/>
-      <c r="S6" s="17"/>
       <c r="T6" s="5"/>
     </row>
     <row r="7" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="C7" s="17"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
-      <c r="H7" s="17"/>
-      <c r="I7" s="17"/>
-      <c r="J7" s="17"/>
-      <c r="K7" s="17"/>
-      <c r="L7" s="17"/>
-      <c r="M7" s="17"/>
-      <c r="N7" s="17"/>
-      <c r="O7" s="17"/>
-      <c r="P7" s="17"/>
-      <c r="Q7" s="17"/>
-      <c r="R7" s="17"/>
-      <c r="S7" s="17"/>
       <c r="T7" s="5"/>
     </row>
     <row r="8" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B8" s="4"/>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="17"/>
-      <c r="H8" s="17"/>
-      <c r="I8" s="17"/>
-      <c r="J8" s="17"/>
-      <c r="K8" s="17"/>
-      <c r="L8" s="17"/>
-      <c r="M8" s="17"/>
-      <c r="N8" s="17"/>
-      <c r="O8" s="17"/>
-      <c r="P8" s="17"/>
-      <c r="Q8" s="17"/>
-      <c r="R8" s="17"/>
-      <c r="S8" s="17"/>
       <c r="T8" s="5"/>
     </row>
     <row r="9" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B9" s="4"/>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="17"/>
-      <c r="H9" s="17"/>
-      <c r="I9" s="17"/>
-      <c r="J9" s="17"/>
-      <c r="K9" s="17"/>
-      <c r="L9" s="17"/>
-      <c r="M9" s="17"/>
-      <c r="N9" s="17"/>
-      <c r="O9" s="17"/>
-      <c r="P9" s="17"/>
-      <c r="Q9" s="17"/>
-      <c r="R9" s="17"/>
-      <c r="S9" s="17"/>
       <c r="T9" s="5"/>
     </row>
     <row r="10" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B10" s="4"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="17"/>
-      <c r="H10" s="17"/>
-      <c r="I10" s="17"/>
-      <c r="J10" s="17"/>
-      <c r="K10" s="17"/>
-      <c r="L10" s="17"/>
-      <c r="M10" s="17"/>
-      <c r="N10" s="17"/>
-      <c r="O10" s="17"/>
-      <c r="P10" s="17"/>
-      <c r="Q10" s="17"/>
-      <c r="R10" s="17"/>
-      <c r="S10" s="17"/>
       <c r="T10" s="5"/>
     </row>
     <row r="11" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B11" s="4"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="17"/>
-      <c r="H11" s="17"/>
-      <c r="I11" s="17"/>
-      <c r="J11" s="17"/>
-      <c r="K11" s="17"/>
-      <c r="L11" s="17"/>
-      <c r="M11" s="17"/>
-      <c r="N11" s="17"/>
-      <c r="O11" s="17"/>
-      <c r="P11" s="17"/>
-      <c r="Q11" s="17"/>
-      <c r="R11" s="17"/>
-      <c r="S11" s="17"/>
       <c r="T11" s="5"/>
     </row>
     <row r="12" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B12" s="4"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="17"/>
-      <c r="H12" s="17"/>
-      <c r="I12" s="17"/>
-      <c r="J12" s="17"/>
-      <c r="K12" s="17"/>
-      <c r="L12" s="17"/>
-      <c r="M12" s="17"/>
-      <c r="N12" s="17"/>
-      <c r="O12" s="17"/>
-      <c r="P12" s="17"/>
-      <c r="Q12" s="17"/>
-      <c r="R12" s="17"/>
-      <c r="S12" s="17"/>
       <c r="T12" s="5"/>
     </row>
     <row r="13" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B13" s="4"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="17"/>
-      <c r="G13" s="17"/>
-      <c r="H13" s="17"/>
-      <c r="I13" s="17"/>
-      <c r="J13" s="17"/>
-      <c r="K13" s="17"/>
-      <c r="L13" s="17"/>
-      <c r="M13" s="17"/>
-      <c r="N13" s="17"/>
-      <c r="O13" s="17"/>
-      <c r="P13" s="17"/>
-      <c r="Q13" s="17"/>
-      <c r="R13" s="17"/>
-      <c r="S13" s="17"/>
       <c r="T13" s="5"/>
     </row>
     <row r="14" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B14" s="4"/>
-      <c r="C14" s="17"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="17"/>
-      <c r="H14" s="17"/>
-      <c r="I14" s="17"/>
-      <c r="J14" s="17"/>
-      <c r="K14" s="17"/>
-      <c r="L14" s="17"/>
-      <c r="M14" s="17"/>
-      <c r="N14" s="17"/>
-      <c r="O14" s="17"/>
-      <c r="P14" s="17"/>
-      <c r="Q14" s="17"/>
-      <c r="R14" s="17"/>
-      <c r="S14" s="17"/>
       <c r="T14" s="5"/>
     </row>
     <row r="15" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B15" s="4"/>
-      <c r="C15" s="17"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="17"/>
-      <c r="H15" s="17"/>
-      <c r="I15" s="17"/>
-      <c r="J15" s="17"/>
-      <c r="K15" s="17"/>
-      <c r="L15" s="17"/>
-      <c r="M15" s="17"/>
-      <c r="N15" s="17"/>
-      <c r="O15" s="17"/>
-      <c r="P15" s="17"/>
-      <c r="Q15" s="17"/>
-      <c r="R15" s="17"/>
-      <c r="S15" s="17"/>
       <c r="T15" s="5"/>
     </row>
     <row r="16" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B16" s="4"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="17"/>
-      <c r="H16" s="17"/>
-      <c r="I16" s="17"/>
-      <c r="J16" s="17"/>
-      <c r="K16" s="17"/>
-      <c r="L16" s="17"/>
-      <c r="M16" s="17"/>
-      <c r="N16" s="17"/>
-      <c r="O16" s="17"/>
-      <c r="P16" s="17"/>
-      <c r="Q16" s="17"/>
-      <c r="R16" s="17"/>
-      <c r="S16" s="17"/>
       <c r="T16" s="5"/>
     </row>
     <row r="17" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B17" s="4"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="17"/>
-      <c r="H17" s="17"/>
-      <c r="I17" s="17"/>
-      <c r="J17" s="17"/>
-      <c r="K17" s="17"/>
-      <c r="L17" s="17"/>
-      <c r="M17" s="17"/>
-      <c r="N17" s="17"/>
-      <c r="O17" s="17"/>
-      <c r="P17" s="17"/>
-      <c r="Q17" s="17"/>
-      <c r="R17" s="17"/>
-      <c r="S17" s="17"/>
       <c r="T17" s="5"/>
     </row>
     <row r="18" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B18" s="4"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="17"/>
-      <c r="G18" s="17"/>
-      <c r="H18" s="17"/>
-      <c r="I18" s="17"/>
-      <c r="J18" s="17"/>
-      <c r="K18" s="17"/>
-      <c r="L18" s="17"/>
-      <c r="M18" s="17"/>
-      <c r="N18" s="17"/>
-      <c r="O18" s="17"/>
-      <c r="P18" s="17"/>
-      <c r="Q18" s="17"/>
-      <c r="R18" s="17"/>
-      <c r="S18" s="17"/>
       <c r="T18" s="5"/>
     </row>
     <row r="19" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B19" s="4"/>
-      <c r="C19" s="17"/>
-      <c r="D19" s="17"/>
-      <c r="E19" s="17"/>
-      <c r="F19" s="17"/>
-      <c r="G19" s="17"/>
-      <c r="H19" s="17"/>
-      <c r="I19" s="17"/>
-      <c r="J19" s="17"/>
-      <c r="K19" s="17"/>
-      <c r="L19" s="17"/>
-      <c r="M19" s="17"/>
-      <c r="N19" s="17"/>
-      <c r="O19" s="17"/>
-      <c r="P19" s="17"/>
-      <c r="Q19" s="17"/>
-      <c r="R19" s="17"/>
-      <c r="S19" s="17"/>
       <c r="T19" s="5"/>
     </row>
     <row r="20" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B20" s="4"/>
-      <c r="C20" s="17"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="17"/>
-      <c r="F20" s="17"/>
-      <c r="G20" s="17"/>
-      <c r="H20" s="17"/>
-      <c r="I20" s="17"/>
-      <c r="J20" s="17"/>
-      <c r="K20" s="17"/>
-      <c r="L20" s="17"/>
-      <c r="M20" s="17"/>
-      <c r="N20" s="17"/>
-      <c r="O20" s="17"/>
-      <c r="P20" s="17"/>
-      <c r="Q20" s="17"/>
-      <c r="R20" s="17"/>
-      <c r="S20" s="17"/>
       <c r="T20" s="5"/>
     </row>
     <row r="21" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B21" s="4"/>
-      <c r="C21" s="17"/>
-      <c r="D21" s="17"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="17"/>
-      <c r="G21" s="17"/>
-      <c r="H21" s="17"/>
-      <c r="I21" s="17"/>
-      <c r="J21" s="17"/>
-      <c r="K21" s="17"/>
-      <c r="L21" s="17"/>
-      <c r="M21" s="17"/>
-      <c r="N21" s="17"/>
-      <c r="O21" s="17"/>
-      <c r="P21" s="17"/>
-      <c r="Q21" s="17"/>
-      <c r="R21" s="17"/>
-      <c r="S21" s="17"/>
       <c r="T21" s="5"/>
     </row>
     <row r="22" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B22" s="4"/>
-      <c r="C22" s="17"/>
-      <c r="D22" s="17"/>
-      <c r="E22" s="17"/>
-      <c r="F22" s="17"/>
-      <c r="G22" s="17"/>
-      <c r="H22" s="17"/>
-      <c r="I22" s="17"/>
-      <c r="J22" s="17"/>
-      <c r="K22" s="17"/>
-      <c r="L22" s="17"/>
-      <c r="M22" s="17"/>
-      <c r="N22" s="17"/>
-      <c r="O22" s="17"/>
-      <c r="P22" s="17"/>
-      <c r="Q22" s="17"/>
-      <c r="R22" s="17"/>
-      <c r="S22" s="17"/>
       <c r="T22" s="5"/>
     </row>
     <row r="23" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B23" s="4"/>
-      <c r="C23" s="17"/>
-      <c r="D23" s="17"/>
-      <c r="E23" s="17"/>
-      <c r="F23" s="17"/>
-      <c r="G23" s="17"/>
-      <c r="H23" s="17"/>
-      <c r="I23" s="17"/>
-      <c r="J23" s="17"/>
-      <c r="K23" s="17"/>
-      <c r="L23" s="17"/>
-      <c r="M23" s="17"/>
-      <c r="N23" s="17"/>
-      <c r="O23" s="17"/>
-      <c r="P23" s="17"/>
-      <c r="Q23" s="17"/>
-      <c r="R23" s="17"/>
-      <c r="S23" s="17"/>
       <c r="T23" s="5"/>
     </row>
     <row r="24" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B24" s="4"/>
-      <c r="C24" s="17"/>
-      <c r="D24" s="17"/>
-      <c r="E24" s="17"/>
-      <c r="F24" s="17"/>
-      <c r="G24" s="17"/>
-      <c r="H24" s="17"/>
-      <c r="I24" s="17"/>
-      <c r="J24" s="17"/>
-      <c r="K24" s="17"/>
-      <c r="L24" s="17"/>
-      <c r="M24" s="17"/>
-      <c r="N24" s="17"/>
-      <c r="O24" s="17"/>
-      <c r="P24" s="17"/>
-      <c r="Q24" s="17"/>
-      <c r="R24" s="17"/>
-      <c r="S24" s="17"/>
       <c r="T24" s="5"/>
     </row>
     <row r="25" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B25" s="4"/>
-      <c r="C25" s="17"/>
-      <c r="D25" s="17"/>
-      <c r="E25" s="17"/>
-      <c r="F25" s="17"/>
-      <c r="G25" s="17"/>
-      <c r="H25" s="17"/>
-      <c r="I25" s="17"/>
-      <c r="J25" s="17"/>
-      <c r="K25" s="17"/>
-      <c r="L25" s="17"/>
-      <c r="M25" s="17"/>
-      <c r="N25" s="17"/>
-      <c r="O25" s="17"/>
-      <c r="P25" s="17"/>
-      <c r="Q25" s="17"/>
-      <c r="R25" s="17"/>
-      <c r="S25" s="17"/>
       <c r="T25" s="5"/>
     </row>
     <row r="26" spans="2:20" x14ac:dyDescent="0.25">
@@ -8014,401 +7961,78 @@
       <c r="B30" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="C30" s="17"/>
-      <c r="D30" s="17"/>
-      <c r="E30" s="17"/>
-      <c r="F30" s="17"/>
-      <c r="G30" s="17"/>
-      <c r="H30" s="17"/>
-      <c r="I30" s="17"/>
-      <c r="J30" s="17"/>
-      <c r="K30" s="17"/>
-      <c r="L30" s="17"/>
-      <c r="M30" s="17"/>
-      <c r="N30" s="17"/>
-      <c r="O30" s="17"/>
-      <c r="P30" s="17"/>
-      <c r="Q30" s="17"/>
-      <c r="R30" s="17"/>
-      <c r="S30" s="17"/>
       <c r="T30" s="5"/>
     </row>
     <row r="31" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B31" s="4"/>
-      <c r="C31" s="17"/>
-      <c r="D31" s="17"/>
-      <c r="E31" s="17"/>
-      <c r="F31" s="17"/>
-      <c r="G31" s="17"/>
-      <c r="H31" s="17"/>
-      <c r="I31" s="17"/>
-      <c r="J31" s="17"/>
-      <c r="K31" s="17"/>
-      <c r="L31" s="17"/>
-      <c r="M31" s="17"/>
-      <c r="N31" s="17"/>
-      <c r="O31" s="17"/>
-      <c r="P31" s="17"/>
-      <c r="Q31" s="17"/>
-      <c r="R31" s="17"/>
-      <c r="S31" s="17"/>
       <c r="T31" s="5"/>
     </row>
     <row r="32" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B32" s="4"/>
-      <c r="C32" s="17"/>
-      <c r="D32" s="17"/>
-      <c r="E32" s="17"/>
-      <c r="F32" s="17"/>
-      <c r="G32" s="17"/>
-      <c r="H32" s="17"/>
-      <c r="I32" s="17"/>
-      <c r="J32" s="17"/>
-      <c r="K32" s="17"/>
-      <c r="L32" s="17"/>
-      <c r="M32" s="17"/>
-      <c r="N32" s="17"/>
-      <c r="O32" s="17"/>
-      <c r="P32" s="17"/>
-      <c r="Q32" s="17"/>
-      <c r="R32" s="17"/>
-      <c r="S32" s="17"/>
       <c r="T32" s="5"/>
     </row>
     <row r="33" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B33" s="4"/>
-      <c r="C33" s="17"/>
-      <c r="D33" s="17"/>
-      <c r="E33" s="17"/>
-      <c r="F33" s="17"/>
-      <c r="G33" s="17"/>
-      <c r="H33" s="17"/>
-      <c r="I33" s="17"/>
-      <c r="J33" s="17"/>
-      <c r="K33" s="17"/>
-      <c r="L33" s="17"/>
-      <c r="M33" s="17"/>
-      <c r="N33" s="17"/>
-      <c r="O33" s="17"/>
-      <c r="P33" s="17"/>
-      <c r="Q33" s="17"/>
-      <c r="R33" s="17"/>
-      <c r="S33" s="17"/>
       <c r="T33" s="5"/>
     </row>
     <row r="34" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B34" s="4"/>
-      <c r="C34" s="17"/>
-      <c r="D34" s="17"/>
-      <c r="E34" s="17"/>
-      <c r="F34" s="17"/>
-      <c r="G34" s="17"/>
-      <c r="H34" s="17"/>
-      <c r="I34" s="17"/>
-      <c r="J34" s="17"/>
-      <c r="K34" s="17"/>
-      <c r="L34" s="17"/>
-      <c r="M34" s="17"/>
-      <c r="N34" s="17"/>
-      <c r="O34" s="17"/>
-      <c r="P34" s="17"/>
-      <c r="Q34" s="17"/>
-      <c r="R34" s="17"/>
-      <c r="S34" s="17"/>
       <c r="T34" s="5"/>
     </row>
     <row r="35" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B35" s="4"/>
-      <c r="C35" s="17"/>
-      <c r="D35" s="17"/>
-      <c r="E35" s="17"/>
-      <c r="F35" s="17"/>
-      <c r="G35" s="17"/>
-      <c r="H35" s="17"/>
-      <c r="I35" s="17"/>
-      <c r="J35" s="17"/>
-      <c r="K35" s="17"/>
-      <c r="L35" s="17"/>
-      <c r="M35" s="17"/>
-      <c r="N35" s="17"/>
-      <c r="O35" s="17"/>
-      <c r="P35" s="17"/>
-      <c r="Q35" s="17"/>
-      <c r="R35" s="17"/>
-      <c r="S35" s="17"/>
       <c r="T35" s="5"/>
     </row>
     <row r="36" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B36" s="4"/>
-      <c r="C36" s="17"/>
-      <c r="D36" s="17"/>
-      <c r="E36" s="17"/>
-      <c r="F36" s="17"/>
-      <c r="G36" s="17"/>
-      <c r="H36" s="17"/>
-      <c r="I36" s="17"/>
-      <c r="J36" s="17"/>
-      <c r="K36" s="17"/>
-      <c r="L36" s="17"/>
-      <c r="M36" s="17"/>
-      <c r="N36" s="17"/>
-      <c r="O36" s="17"/>
-      <c r="P36" s="17"/>
-      <c r="Q36" s="17"/>
-      <c r="R36" s="17"/>
-      <c r="S36" s="17"/>
       <c r="T36" s="5"/>
     </row>
     <row r="37" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B37" s="4"/>
-      <c r="C37" s="17"/>
-      <c r="D37" s="17"/>
-      <c r="E37" s="17"/>
-      <c r="F37" s="17"/>
-      <c r="G37" s="17"/>
-      <c r="H37" s="17"/>
-      <c r="I37" s="17"/>
-      <c r="J37" s="17"/>
-      <c r="K37" s="17"/>
-      <c r="L37" s="17"/>
-      <c r="M37" s="17"/>
-      <c r="N37" s="17"/>
-      <c r="O37" s="17"/>
-      <c r="P37" s="17"/>
-      <c r="Q37" s="17"/>
-      <c r="R37" s="17"/>
-      <c r="S37" s="17"/>
       <c r="T37" s="5"/>
     </row>
     <row r="38" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B38" s="4"/>
-      <c r="C38" s="17"/>
-      <c r="D38" s="17"/>
-      <c r="E38" s="17"/>
-      <c r="F38" s="17"/>
-      <c r="G38" s="17"/>
-      <c r="H38" s="17"/>
-      <c r="I38" s="17"/>
-      <c r="J38" s="17"/>
-      <c r="K38" s="17"/>
-      <c r="L38" s="17"/>
-      <c r="M38" s="17"/>
-      <c r="N38" s="17"/>
-      <c r="O38" s="17"/>
-      <c r="P38" s="17"/>
-      <c r="Q38" s="17"/>
-      <c r="R38" s="17"/>
-      <c r="S38" s="17"/>
       <c r="T38" s="5"/>
     </row>
     <row r="39" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B39" s="4"/>
-      <c r="C39" s="17"/>
-      <c r="D39" s="17"/>
-      <c r="E39" s="17"/>
-      <c r="F39" s="17"/>
-      <c r="G39" s="17"/>
-      <c r="H39" s="17"/>
-      <c r="I39" s="17"/>
-      <c r="J39" s="17"/>
-      <c r="K39" s="17"/>
-      <c r="L39" s="17"/>
-      <c r="M39" s="17"/>
-      <c r="N39" s="17"/>
-      <c r="O39" s="17"/>
-      <c r="P39" s="17"/>
-      <c r="Q39" s="17"/>
-      <c r="R39" s="17"/>
-      <c r="S39" s="17"/>
       <c r="T39" s="5"/>
     </row>
     <row r="40" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B40" s="4"/>
-      <c r="C40" s="17"/>
-      <c r="D40" s="17"/>
-      <c r="E40" s="17"/>
-      <c r="F40" s="17"/>
-      <c r="G40" s="17"/>
-      <c r="H40" s="17"/>
-      <c r="I40" s="17"/>
-      <c r="J40" s="17"/>
-      <c r="K40" s="17"/>
-      <c r="L40" s="17"/>
-      <c r="M40" s="17"/>
-      <c r="N40" s="17"/>
-      <c r="O40" s="17"/>
-      <c r="P40" s="17"/>
-      <c r="Q40" s="17"/>
-      <c r="R40" s="17"/>
-      <c r="S40" s="17"/>
       <c r="T40" s="5"/>
     </row>
     <row r="41" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B41" s="4"/>
-      <c r="C41" s="17"/>
-      <c r="D41" s="17"/>
-      <c r="E41" s="17"/>
-      <c r="F41" s="17"/>
-      <c r="G41" s="17"/>
-      <c r="H41" s="17"/>
-      <c r="I41" s="17"/>
-      <c r="J41" s="17"/>
-      <c r="K41" s="17"/>
-      <c r="L41" s="17"/>
-      <c r="M41" s="17"/>
-      <c r="N41" s="17"/>
-      <c r="O41" s="17"/>
-      <c r="P41" s="17"/>
-      <c r="Q41" s="17"/>
-      <c r="R41" s="17"/>
-      <c r="S41" s="17"/>
       <c r="T41" s="5"/>
     </row>
     <row r="42" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B42" s="4"/>
-      <c r="C42" s="17"/>
-      <c r="D42" s="17"/>
-      <c r="E42" s="17"/>
-      <c r="F42" s="17"/>
-      <c r="G42" s="17"/>
-      <c r="H42" s="17"/>
-      <c r="I42" s="17"/>
-      <c r="J42" s="17"/>
-      <c r="K42" s="17"/>
-      <c r="L42" s="17"/>
-      <c r="M42" s="17"/>
-      <c r="N42" s="17"/>
-      <c r="O42" s="17"/>
-      <c r="P42" s="17"/>
-      <c r="Q42" s="17"/>
-      <c r="R42" s="17"/>
-      <c r="S42" s="17"/>
       <c r="T42" s="5"/>
     </row>
     <row r="43" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B43" s="4"/>
-      <c r="C43" s="17"/>
-      <c r="D43" s="17"/>
-      <c r="E43" s="17"/>
-      <c r="F43" s="17"/>
-      <c r="G43" s="17"/>
-      <c r="H43" s="17"/>
-      <c r="I43" s="17"/>
-      <c r="J43" s="17"/>
-      <c r="K43" s="17"/>
-      <c r="L43" s="17"/>
-      <c r="M43" s="17"/>
-      <c r="N43" s="17"/>
-      <c r="O43" s="17"/>
-      <c r="P43" s="17"/>
-      <c r="Q43" s="17"/>
-      <c r="R43" s="17"/>
-      <c r="S43" s="17"/>
       <c r="T43" s="5"/>
     </row>
     <row r="44" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B44" s="4"/>
-      <c r="C44" s="17"/>
-      <c r="D44" s="17"/>
-      <c r="E44" s="17"/>
-      <c r="F44" s="17"/>
-      <c r="G44" s="17"/>
-      <c r="H44" s="17"/>
-      <c r="I44" s="17"/>
-      <c r="J44" s="17"/>
-      <c r="K44" s="17"/>
-      <c r="L44" s="17"/>
-      <c r="M44" s="17"/>
-      <c r="N44" s="17"/>
-      <c r="O44" s="17"/>
-      <c r="P44" s="17"/>
-      <c r="Q44" s="17"/>
-      <c r="R44" s="17"/>
-      <c r="S44" s="17"/>
       <c r="T44" s="5"/>
     </row>
     <row r="45" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B45" s="4"/>
-      <c r="C45" s="17"/>
-      <c r="D45" s="17"/>
-      <c r="E45" s="17"/>
-      <c r="F45" s="17"/>
-      <c r="G45" s="17"/>
-      <c r="H45" s="17"/>
-      <c r="I45" s="17"/>
-      <c r="J45" s="17"/>
-      <c r="K45" s="17"/>
-      <c r="L45" s="17"/>
-      <c r="M45" s="17"/>
-      <c r="N45" s="17"/>
-      <c r="O45" s="17"/>
-      <c r="P45" s="17"/>
-      <c r="Q45" s="17"/>
-      <c r="R45" s="17"/>
-      <c r="S45" s="17"/>
       <c r="T45" s="5"/>
     </row>
     <row r="46" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B46" s="4"/>
-      <c r="C46" s="17"/>
-      <c r="D46" s="17"/>
-      <c r="E46" s="17"/>
-      <c r="F46" s="17"/>
-      <c r="G46" s="17"/>
-      <c r="H46" s="17"/>
-      <c r="I46" s="17"/>
-      <c r="J46" s="17"/>
-      <c r="K46" s="17"/>
-      <c r="L46" s="17"/>
-      <c r="M46" s="17"/>
-      <c r="N46" s="17"/>
-      <c r="O46" s="17"/>
-      <c r="P46" s="17"/>
-      <c r="Q46" s="17"/>
-      <c r="R46" s="17"/>
-      <c r="S46" s="17"/>
       <c r="T46" s="5"/>
     </row>
     <row r="47" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B47" s="4"/>
-      <c r="C47" s="17"/>
-      <c r="D47" s="17"/>
-      <c r="E47" s="17"/>
-      <c r="F47" s="17"/>
-      <c r="G47" s="17"/>
-      <c r="H47" s="17"/>
-      <c r="I47" s="17"/>
-      <c r="J47" s="17"/>
-      <c r="K47" s="17"/>
-      <c r="L47" s="17"/>
-      <c r="M47" s="17"/>
-      <c r="N47" s="17"/>
-      <c r="O47" s="17"/>
-      <c r="P47" s="17"/>
-      <c r="Q47" s="17"/>
-      <c r="R47" s="17"/>
-      <c r="S47" s="17"/>
       <c r="T47" s="5"/>
     </row>
     <row r="48" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B48" s="4"/>
-      <c r="C48" s="17"/>
-      <c r="D48" s="17"/>
-      <c r="E48" s="17"/>
-      <c r="F48" s="17"/>
-      <c r="G48" s="17"/>
-      <c r="H48" s="17"/>
-      <c r="I48" s="17"/>
-      <c r="J48" s="17"/>
-      <c r="K48" s="17"/>
-      <c r="L48" s="17"/>
-      <c r="M48" s="17"/>
-      <c r="N48" s="17"/>
-      <c r="O48" s="17"/>
-      <c r="P48" s="17"/>
-      <c r="Q48" s="17"/>
-      <c r="R48" s="17"/>
-      <c r="S48" s="17"/>
       <c r="T48" s="5"/>
     </row>
     <row r="49" spans="2:20" x14ac:dyDescent="0.25">
@@ -8436,4 +8060,1235 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FB1A8BA-22E8-4830-91FD-4FDCEA0E8662}">
+  <dimension ref="A2:K118"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
+      <selection activeCell="L126" sqref="L126"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="3"/>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B6" s="4"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="18"/>
+      <c r="K6" s="5"/>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B7" s="4"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="18"/>
+      <c r="J7" s="18"/>
+      <c r="K7" s="5"/>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B8" s="4"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="18"/>
+      <c r="I8" s="18"/>
+      <c r="J8" s="18"/>
+      <c r="K8" s="5"/>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B9" s="4"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="18"/>
+      <c r="J9" s="18"/>
+      <c r="K9" s="5"/>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B10" s="4"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="18"/>
+      <c r="J10" s="18"/>
+      <c r="K10" s="5"/>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B11" s="4"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="18"/>
+      <c r="I11" s="18"/>
+      <c r="J11" s="18"/>
+      <c r="K11" s="5"/>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B12" s="4"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="18"/>
+      <c r="I12" s="18"/>
+      <c r="J12" s="18"/>
+      <c r="K12" s="5"/>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B13" s="4"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
+      <c r="H13" s="18"/>
+      <c r="I13" s="18"/>
+      <c r="J13" s="18"/>
+      <c r="K13" s="5"/>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B14" s="6"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="8"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B18" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="3"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B19" s="4"/>
+      <c r="C19" t="s">
+        <v>10</v>
+      </c>
+      <c r="F19" s="5"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B20" s="4"/>
+      <c r="D20" t="s">
+        <v>11</v>
+      </c>
+      <c r="F20" s="5"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B21" s="4"/>
+      <c r="D21" t="s">
+        <v>12</v>
+      </c>
+      <c r="F21" s="5"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B22" s="4"/>
+      <c r="D22" t="s">
+        <v>13</v>
+      </c>
+      <c r="F22" s="5"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B23" s="4"/>
+      <c r="C23" t="s">
+        <v>14</v>
+      </c>
+      <c r="F23" s="5"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B24" s="4"/>
+      <c r="D24" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="F24" s="5"/>
+      <c r="G24" t="s">
+        <v>20</v>
+      </c>
+      <c r="H24" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B25" s="4"/>
+      <c r="C25" t="s">
+        <v>15</v>
+      </c>
+      <c r="F25" s="5"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B26" s="4"/>
+      <c r="C26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F26" s="5"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B27" s="4"/>
+      <c r="D27" t="s">
+        <v>26</v>
+      </c>
+      <c r="F27" s="5"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B28" s="4"/>
+      <c r="D28" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="F28" s="5"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B29" s="6"/>
+      <c r="C29" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="8"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B33" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
+      <c r="I33" s="3"/>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B34" s="4"/>
+      <c r="C34" s="18"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="18"/>
+      <c r="G34" s="18"/>
+      <c r="H34" s="18"/>
+      <c r="I34" s="5"/>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B35" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C35" s="18"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="18"/>
+      <c r="F35" s="18"/>
+      <c r="G35" s="18"/>
+      <c r="H35" s="18"/>
+      <c r="I35" s="5"/>
+    </row>
+    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B36" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C36" s="18"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="18"/>
+      <c r="G36" s="18"/>
+      <c r="H36" s="18"/>
+      <c r="I36" s="5"/>
+    </row>
+    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B37" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C37" s="18"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="18"/>
+      <c r="F37" s="18"/>
+      <c r="G37" s="18"/>
+      <c r="H37" s="18"/>
+      <c r="I37" s="5"/>
+    </row>
+    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B38" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C38" s="18"/>
+      <c r="D38" s="18"/>
+      <c r="E38" s="18"/>
+      <c r="F38" s="18"/>
+      <c r="G38" s="18"/>
+      <c r="H38" s="18"/>
+      <c r="I38" s="5"/>
+    </row>
+    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B39" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C39" s="18"/>
+      <c r="D39" s="18"/>
+      <c r="E39" s="18"/>
+      <c r="F39" s="18"/>
+      <c r="G39" s="18"/>
+      <c r="H39" s="18"/>
+      <c r="I39" s="5"/>
+    </row>
+    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B40" s="4"/>
+      <c r="C40" s="18"/>
+      <c r="D40" s="18"/>
+      <c r="E40" s="18"/>
+      <c r="F40" s="18"/>
+      <c r="G40" s="18"/>
+      <c r="H40" s="18"/>
+      <c r="I40" s="5"/>
+    </row>
+    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B41" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C41" s="18"/>
+      <c r="D41" s="18"/>
+      <c r="E41" s="18"/>
+      <c r="F41" s="18"/>
+      <c r="G41" s="18"/>
+      <c r="H41" s="18"/>
+      <c r="I41" s="5"/>
+    </row>
+    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B42" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C42" s="18"/>
+      <c r="D42" s="18"/>
+      <c r="E42" s="18"/>
+      <c r="F42" s="18"/>
+      <c r="G42" s="18"/>
+      <c r="H42" s="18"/>
+      <c r="I42" s="5"/>
+    </row>
+    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B43" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C43" s="18"/>
+      <c r="D43" s="18"/>
+      <c r="E43" s="18"/>
+      <c r="F43" s="18"/>
+      <c r="G43" s="18"/>
+      <c r="H43" s="18"/>
+      <c r="I43" s="5"/>
+    </row>
+    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B44" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C44" s="18"/>
+      <c r="D44" s="18"/>
+      <c r="E44" s="18"/>
+      <c r="F44" s="18"/>
+      <c r="G44" s="18"/>
+      <c r="H44" s="18"/>
+      <c r="I44" s="5"/>
+    </row>
+    <row r="45" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B45" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C45" s="18"/>
+      <c r="D45" s="18"/>
+      <c r="E45" s="18"/>
+      <c r="F45" s="18"/>
+      <c r="G45" s="18"/>
+      <c r="H45" s="18"/>
+      <c r="I45" s="5"/>
+    </row>
+    <row r="46" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B46" s="4"/>
+      <c r="C46" s="18"/>
+      <c r="D46" s="18"/>
+      <c r="E46" s="18"/>
+      <c r="F46" s="18"/>
+      <c r="G46" s="18"/>
+      <c r="H46" s="18"/>
+      <c r="I46" s="5"/>
+    </row>
+    <row r="47" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B47" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C47" s="18"/>
+      <c r="D47" s="18"/>
+      <c r="E47" s="18"/>
+      <c r="F47" s="18"/>
+      <c r="G47" s="18"/>
+      <c r="H47" s="18"/>
+      <c r="I47" s="5"/>
+    </row>
+    <row r="48" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B48" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C48" s="18"/>
+      <c r="D48" s="18"/>
+      <c r="E48" s="18"/>
+      <c r="F48" s="18"/>
+      <c r="G48" s="18"/>
+      <c r="H48" s="18"/>
+      <c r="I48" s="5"/>
+    </row>
+    <row r="49" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B49" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C49" s="18"/>
+      <c r="D49" s="18"/>
+      <c r="E49" s="18"/>
+      <c r="F49" s="18"/>
+      <c r="G49" s="18"/>
+      <c r="H49" s="18"/>
+      <c r="I49" s="5"/>
+    </row>
+    <row r="50" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B50" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C50" s="18"/>
+      <c r="D50" s="18"/>
+      <c r="E50" s="18"/>
+      <c r="F50" s="18"/>
+      <c r="G50" s="18"/>
+      <c r="H50" s="18"/>
+      <c r="I50" s="5"/>
+    </row>
+    <row r="51" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B51" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="C51" s="18"/>
+      <c r="D51" s="18"/>
+      <c r="E51" s="18"/>
+      <c r="F51" s="18"/>
+      <c r="G51" s="18"/>
+      <c r="H51" s="18"/>
+      <c r="I51" s="5"/>
+    </row>
+    <row r="52" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B52" s="4"/>
+      <c r="C52" s="18"/>
+      <c r="D52" s="18"/>
+      <c r="E52" s="18"/>
+      <c r="F52" s="18"/>
+      <c r="G52" s="18"/>
+      <c r="H52" s="18"/>
+      <c r="I52" s="5"/>
+    </row>
+    <row r="53" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B53" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C53" s="18"/>
+      <c r="D53" s="18"/>
+      <c r="E53" s="18"/>
+      <c r="F53" s="18"/>
+      <c r="G53" s="18"/>
+      <c r="H53" s="18"/>
+      <c r="I53" s="5"/>
+    </row>
+    <row r="54" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B54" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C54" s="18"/>
+      <c r="D54" s="18"/>
+      <c r="E54" s="18"/>
+      <c r="F54" s="18"/>
+      <c r="G54" s="18"/>
+      <c r="H54" s="18"/>
+      <c r="I54" s="5"/>
+    </row>
+    <row r="55" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B55" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C55" s="18"/>
+      <c r="D55" s="18"/>
+      <c r="E55" s="18"/>
+      <c r="F55" s="18"/>
+      <c r="G55" s="18"/>
+      <c r="H55" s="18"/>
+      <c r="I55" s="5"/>
+    </row>
+    <row r="56" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B56" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C56" s="18"/>
+      <c r="D56" s="18"/>
+      <c r="E56" s="18"/>
+      <c r="F56" s="18"/>
+      <c r="G56" s="18"/>
+      <c r="H56" s="18"/>
+      <c r="I56" s="5"/>
+    </row>
+    <row r="57" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B57" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C57" s="18"/>
+      <c r="D57" s="18"/>
+      <c r="E57" s="18"/>
+      <c r="F57" s="18"/>
+      <c r="G57" s="18"/>
+      <c r="H57" s="18"/>
+      <c r="I57" s="5"/>
+    </row>
+    <row r="58" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B58" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C58" s="18"/>
+      <c r="D58" s="18"/>
+      <c r="E58" s="18"/>
+      <c r="F58" s="18"/>
+      <c r="G58" s="18"/>
+      <c r="H58" s="18"/>
+      <c r="I58" s="5"/>
+    </row>
+    <row r="59" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B59" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C59" s="18"/>
+      <c r="D59" s="18"/>
+      <c r="E59" s="18"/>
+      <c r="F59" s="18"/>
+      <c r="G59" s="18"/>
+      <c r="H59" s="18"/>
+      <c r="I59" s="5"/>
+    </row>
+    <row r="60" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B60" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C60" s="18"/>
+      <c r="D60" s="18"/>
+      <c r="E60" s="18"/>
+      <c r="F60" s="18"/>
+      <c r="G60" s="18"/>
+      <c r="H60" s="18"/>
+      <c r="I60" s="5"/>
+    </row>
+    <row r="61" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B61" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C61" s="18"/>
+      <c r="D61" s="18"/>
+      <c r="E61" s="18"/>
+      <c r="F61" s="18"/>
+      <c r="G61" s="18"/>
+      <c r="H61" s="18"/>
+      <c r="I61" s="5"/>
+    </row>
+    <row r="62" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B62" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C62" s="18"/>
+      <c r="D62" s="18"/>
+      <c r="E62" s="18"/>
+      <c r="F62" s="18"/>
+      <c r="G62" s="18"/>
+      <c r="H62" s="18"/>
+      <c r="I62" s="5"/>
+    </row>
+    <row r="63" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B63" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C63" s="18"/>
+      <c r="D63" s="18"/>
+      <c r="E63" s="18"/>
+      <c r="F63" s="18"/>
+      <c r="G63" s="18"/>
+      <c r="H63" s="18"/>
+      <c r="I63" s="5"/>
+    </row>
+    <row r="64" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B64" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C64" s="18"/>
+      <c r="D64" s="18"/>
+      <c r="E64" s="18"/>
+      <c r="F64" s="18"/>
+      <c r="G64" s="18"/>
+      <c r="H64" s="18"/>
+      <c r="I64" s="5"/>
+    </row>
+    <row r="65" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B65" s="4"/>
+      <c r="C65" s="18"/>
+      <c r="D65" s="18"/>
+      <c r="E65" s="18"/>
+      <c r="F65" s="18"/>
+      <c r="G65" s="18"/>
+      <c r="H65" s="18"/>
+      <c r="I65" s="5"/>
+    </row>
+    <row r="66" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B66" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C66" s="18"/>
+      <c r="D66" s="18"/>
+      <c r="E66" s="18"/>
+      <c r="F66" s="18"/>
+      <c r="G66" s="18"/>
+      <c r="H66" s="18"/>
+      <c r="I66" s="5"/>
+    </row>
+    <row r="67" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B67" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C67" s="18"/>
+      <c r="D67" s="18"/>
+      <c r="E67" s="18"/>
+      <c r="F67" s="18"/>
+      <c r="G67" s="18"/>
+      <c r="H67" s="18"/>
+      <c r="I67" s="5"/>
+    </row>
+    <row r="68" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B68" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C68" s="18"/>
+      <c r="D68" s="18"/>
+      <c r="E68" s="18"/>
+      <c r="F68" s="18"/>
+      <c r="G68" s="18"/>
+      <c r="H68" s="18"/>
+      <c r="I68" s="5"/>
+    </row>
+    <row r="69" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B69" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C69" s="18"/>
+      <c r="D69" s="18"/>
+      <c r="E69" s="18"/>
+      <c r="F69" s="18"/>
+      <c r="G69" s="18"/>
+      <c r="H69" s="18"/>
+      <c r="I69" s="5"/>
+    </row>
+    <row r="70" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B70" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C70" s="18"/>
+      <c r="D70" s="18"/>
+      <c r="E70" s="18"/>
+      <c r="F70" s="18"/>
+      <c r="G70" s="18"/>
+      <c r="H70" s="18"/>
+      <c r="I70" s="5"/>
+    </row>
+    <row r="71" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B71" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C71" s="18"/>
+      <c r="D71" s="18"/>
+      <c r="E71" s="18"/>
+      <c r="F71" s="18"/>
+      <c r="G71" s="18"/>
+      <c r="H71" s="18"/>
+      <c r="I71" s="5"/>
+    </row>
+    <row r="72" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B72" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C72" s="18"/>
+      <c r="D72" s="18"/>
+      <c r="E72" s="18"/>
+      <c r="F72" s="18"/>
+      <c r="G72" s="18"/>
+      <c r="H72" s="18"/>
+      <c r="I72" s="5"/>
+    </row>
+    <row r="73" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B73" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C73" s="18"/>
+      <c r="D73" s="18"/>
+      <c r="E73" s="18"/>
+      <c r="F73" s="18"/>
+      <c r="G73" s="18"/>
+      <c r="H73" s="18"/>
+      <c r="I73" s="5"/>
+    </row>
+    <row r="74" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B74" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C74" s="18"/>
+      <c r="D74" s="18"/>
+      <c r="E74" s="18"/>
+      <c r="F74" s="18"/>
+      <c r="G74" s="18"/>
+      <c r="H74" s="18"/>
+      <c r="I74" s="5"/>
+    </row>
+    <row r="75" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B75" s="4"/>
+      <c r="C75" s="18"/>
+      <c r="D75" s="18"/>
+      <c r="E75" s="18"/>
+      <c r="F75" s="18"/>
+      <c r="G75" s="18"/>
+      <c r="H75" s="18"/>
+      <c r="I75" s="5"/>
+    </row>
+    <row r="76" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B76" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C76" s="18"/>
+      <c r="D76" s="18"/>
+      <c r="E76" s="18"/>
+      <c r="F76" s="18"/>
+      <c r="G76" s="18"/>
+      <c r="H76" s="18"/>
+      <c r="I76" s="5"/>
+    </row>
+    <row r="77" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B77" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="C77" s="18"/>
+      <c r="D77" s="18"/>
+      <c r="E77" s="18"/>
+      <c r="F77" s="18"/>
+      <c r="G77" s="18"/>
+      <c r="H77" s="18"/>
+      <c r="I77" s="5"/>
+    </row>
+    <row r="78" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B78" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="C78" s="18"/>
+      <c r="D78" s="18"/>
+      <c r="E78" s="18"/>
+      <c r="F78" s="18"/>
+      <c r="G78" s="18"/>
+      <c r="H78" s="18"/>
+      <c r="I78" s="5"/>
+    </row>
+    <row r="79" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B79" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C79" s="18"/>
+      <c r="D79" s="18"/>
+      <c r="E79" s="18"/>
+      <c r="F79" s="18"/>
+      <c r="G79" s="18"/>
+      <c r="H79" s="18"/>
+      <c r="I79" s="5"/>
+    </row>
+    <row r="80" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B80" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="C80" s="18"/>
+      <c r="D80" s="18"/>
+      <c r="E80" s="18"/>
+      <c r="F80" s="18"/>
+      <c r="G80" s="18"/>
+      <c r="H80" s="18"/>
+      <c r="I80" s="5"/>
+    </row>
+    <row r="81" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B81" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C81" s="18"/>
+      <c r="D81" s="18"/>
+      <c r="E81" s="18"/>
+      <c r="F81" s="18"/>
+      <c r="G81" s="18"/>
+      <c r="H81" s="18"/>
+      <c r="I81" s="5"/>
+    </row>
+    <row r="82" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B82" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="C82" s="18"/>
+      <c r="D82" s="18"/>
+      <c r="E82" s="18"/>
+      <c r="F82" s="18"/>
+      <c r="G82" s="18"/>
+      <c r="H82" s="18"/>
+      <c r="I82" s="5"/>
+    </row>
+    <row r="83" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B83" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C83" s="18"/>
+      <c r="D83" s="18"/>
+      <c r="E83" s="18"/>
+      <c r="F83" s="18"/>
+      <c r="G83" s="18"/>
+      <c r="H83" s="18"/>
+      <c r="I83" s="5"/>
+    </row>
+    <row r="84" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B84" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C84" s="18"/>
+      <c r="D84" s="18"/>
+      <c r="E84" s="18"/>
+      <c r="F84" s="18"/>
+      <c r="G84" s="18"/>
+      <c r="H84" s="18"/>
+      <c r="I84" s="5"/>
+    </row>
+    <row r="85" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B85" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C85" s="18"/>
+      <c r="D85" s="18"/>
+      <c r="E85" s="18"/>
+      <c r="F85" s="18"/>
+      <c r="G85" s="18"/>
+      <c r="H85" s="18"/>
+      <c r="I85" s="5"/>
+    </row>
+    <row r="86" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B86" s="14" t="s">
+        <v>145</v>
+      </c>
+      <c r="C86" s="18"/>
+      <c r="D86" s="18"/>
+      <c r="E86" s="18"/>
+      <c r="F86" s="18"/>
+      <c r="G86" s="18"/>
+      <c r="H86" s="18"/>
+      <c r="I86" s="5"/>
+    </row>
+    <row r="87" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B87" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="C87" s="18"/>
+      <c r="D87" s="18"/>
+      <c r="E87" s="18"/>
+      <c r="F87" s="18"/>
+      <c r="G87" s="18"/>
+      <c r="H87" s="18"/>
+      <c r="I87" s="5"/>
+    </row>
+    <row r="88" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B88" s="14"/>
+      <c r="C88" s="18"/>
+      <c r="D88" s="18"/>
+      <c r="E88" s="18"/>
+      <c r="F88" s="18"/>
+      <c r="G88" s="18"/>
+      <c r="H88" s="18"/>
+      <c r="I88" s="5"/>
+    </row>
+    <row r="89" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B89" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="C89" s="18"/>
+      <c r="D89" s="18"/>
+      <c r="E89" s="18"/>
+      <c r="F89" s="18"/>
+      <c r="G89" s="18"/>
+      <c r="H89" s="18"/>
+      <c r="I89" s="5"/>
+    </row>
+    <row r="90" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B90" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="C90" s="18"/>
+      <c r="D90" s="18"/>
+      <c r="E90" s="18"/>
+      <c r="F90" s="18"/>
+      <c r="G90" s="18"/>
+      <c r="H90" s="18"/>
+      <c r="I90" s="5"/>
+    </row>
+    <row r="91" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B91" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="C91" s="18"/>
+      <c r="D91" s="18"/>
+      <c r="E91" s="18"/>
+      <c r="F91" s="18"/>
+      <c r="G91" s="18"/>
+      <c r="H91" s="18"/>
+      <c r="I91" s="5"/>
+    </row>
+    <row r="92" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B92" s="14"/>
+      <c r="C92" s="18"/>
+      <c r="D92" s="18"/>
+      <c r="E92" s="18"/>
+      <c r="F92" s="18"/>
+      <c r="G92" s="18"/>
+      <c r="H92" s="18"/>
+      <c r="I92" s="5"/>
+    </row>
+    <row r="93" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B93" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="C93" s="18"/>
+      <c r="D93" s="18"/>
+      <c r="E93" s="18"/>
+      <c r="F93" s="18"/>
+      <c r="G93" s="18"/>
+      <c r="H93" s="18"/>
+      <c r="I93" s="5"/>
+    </row>
+    <row r="94" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B94" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="C94" s="18"/>
+      <c r="D94" s="18"/>
+      <c r="E94" s="18"/>
+      <c r="F94" s="18"/>
+      <c r="G94" s="18"/>
+      <c r="H94" s="18"/>
+      <c r="I94" s="5"/>
+    </row>
+    <row r="95" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B95" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="C95" s="18"/>
+      <c r="D95" s="18"/>
+      <c r="E95" s="18"/>
+      <c r="F95" s="18"/>
+      <c r="G95" s="18"/>
+      <c r="H95" s="18"/>
+      <c r="I95" s="5"/>
+    </row>
+    <row r="96" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B96" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="C96" s="18"/>
+      <c r="D96" s="18"/>
+      <c r="E96" s="18"/>
+      <c r="F96" s="18"/>
+      <c r="G96" s="18"/>
+      <c r="H96" s="18"/>
+      <c r="I96" s="5"/>
+    </row>
+    <row r="97" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B97" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="C97" s="18"/>
+      <c r="D97" s="18"/>
+      <c r="E97" s="18"/>
+      <c r="F97" s="18"/>
+      <c r="G97" s="18"/>
+      <c r="H97" s="18"/>
+      <c r="I97" s="5"/>
+    </row>
+    <row r="98" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B98" s="14"/>
+      <c r="C98" s="18"/>
+      <c r="D98" s="18"/>
+      <c r="E98" s="18"/>
+      <c r="F98" s="18"/>
+      <c r="G98" s="18"/>
+      <c r="H98" s="18"/>
+      <c r="I98" s="5"/>
+    </row>
+    <row r="99" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B99" s="14" t="s">
+        <v>154</v>
+      </c>
+      <c r="C99" s="18"/>
+      <c r="D99" s="18"/>
+      <c r="E99" s="18"/>
+      <c r="F99" s="18"/>
+      <c r="G99" s="18"/>
+      <c r="H99" s="18"/>
+      <c r="I99" s="5"/>
+    </row>
+    <row r="100" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B100" s="14" t="s">
+        <v>155</v>
+      </c>
+      <c r="C100" s="18"/>
+      <c r="D100" s="18"/>
+      <c r="E100" s="18"/>
+      <c r="F100" s="18"/>
+      <c r="G100" s="18"/>
+      <c r="H100" s="18"/>
+      <c r="I100" s="5"/>
+    </row>
+    <row r="101" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B101" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="C101" s="18"/>
+      <c r="D101" s="18"/>
+      <c r="E101" s="18"/>
+      <c r="F101" s="18"/>
+      <c r="G101" s="18"/>
+      <c r="H101" s="18"/>
+      <c r="I101" s="5"/>
+    </row>
+    <row r="102" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B102" s="4"/>
+      <c r="C102" s="18"/>
+      <c r="D102" s="18"/>
+      <c r="E102" s="18"/>
+      <c r="F102" s="18"/>
+      <c r="G102" s="18"/>
+      <c r="H102" s="18"/>
+      <c r="I102" s="5"/>
+    </row>
+    <row r="103" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B103" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="C103" s="18"/>
+      <c r="D103" s="18"/>
+      <c r="E103" s="18"/>
+      <c r="F103" s="18"/>
+      <c r="G103" s="18"/>
+      <c r="H103" s="18"/>
+      <c r="I103" s="5"/>
+    </row>
+    <row r="104" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B104" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C104" s="18"/>
+      <c r="D104" s="18"/>
+      <c r="E104" s="18"/>
+      <c r="F104" s="18"/>
+      <c r="G104" s="18"/>
+      <c r="H104" s="18"/>
+      <c r="I104" s="5"/>
+    </row>
+    <row r="105" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B105" s="4"/>
+      <c r="C105" s="18"/>
+      <c r="D105" s="18"/>
+      <c r="E105" s="18"/>
+      <c r="F105" s="18"/>
+      <c r="G105" s="18"/>
+      <c r="H105" s="18"/>
+      <c r="I105" s="5"/>
+    </row>
+    <row r="106" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B106" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C106" s="18"/>
+      <c r="D106" s="18"/>
+      <c r="E106" s="18"/>
+      <c r="F106" s="18"/>
+      <c r="G106" s="18"/>
+      <c r="H106" s="18"/>
+      <c r="I106" s="5"/>
+    </row>
+    <row r="107" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B107" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="C107" s="18"/>
+      <c r="D107" s="18"/>
+      <c r="E107" s="18"/>
+      <c r="F107" s="18"/>
+      <c r="G107" s="18"/>
+      <c r="H107" s="18"/>
+      <c r="I107" s="5"/>
+    </row>
+    <row r="108" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B108" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C108" s="18"/>
+      <c r="D108" s="18"/>
+      <c r="E108" s="18"/>
+      <c r="F108" s="18"/>
+      <c r="G108" s="18"/>
+      <c r="H108" s="18"/>
+      <c r="I108" s="5"/>
+    </row>
+    <row r="109" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B109" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C109" s="18"/>
+      <c r="D109" s="18"/>
+      <c r="E109" s="18"/>
+      <c r="F109" s="18"/>
+      <c r="G109" s="18"/>
+      <c r="H109" s="18"/>
+      <c r="I109" s="5"/>
+    </row>
+    <row r="110" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B110" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C110" s="18"/>
+      <c r="D110" s="18"/>
+      <c r="E110" s="18"/>
+      <c r="F110" s="18"/>
+      <c r="G110" s="18"/>
+      <c r="H110" s="18"/>
+      <c r="I110" s="5"/>
+    </row>
+    <row r="111" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B111" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="C111" s="18"/>
+      <c r="D111" s="18"/>
+      <c r="E111" s="18"/>
+      <c r="F111" s="18"/>
+      <c r="G111" s="18"/>
+      <c r="H111" s="18"/>
+      <c r="I111" s="5"/>
+    </row>
+    <row r="112" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B112" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C112" s="18"/>
+      <c r="D112" s="18"/>
+      <c r="E112" s="18"/>
+      <c r="F112" s="18"/>
+      <c r="G112" s="18"/>
+      <c r="H112" s="18"/>
+      <c r="I112" s="5"/>
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B113" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="C113" s="18"/>
+      <c r="D113" s="18"/>
+      <c r="E113" s="18"/>
+      <c r="F113" s="18"/>
+      <c r="G113" s="18"/>
+      <c r="H113" s="18"/>
+      <c r="I113" s="5"/>
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B114" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C114" s="18"/>
+      <c r="D114" s="18"/>
+      <c r="E114" s="18"/>
+      <c r="F114" s="18"/>
+      <c r="G114" s="18"/>
+      <c r="H114" s="18"/>
+      <c r="I114" s="5"/>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B115" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C115" s="7"/>
+      <c r="D115" s="7"/>
+      <c r="E115" s="7"/>
+      <c r="F115" s="7"/>
+      <c r="G115" s="7"/>
+      <c r="H115" s="7"/>
+      <c r="I115" s="8"/>
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A118" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>